<commit_message>
Minor fixes in data protocol specification protocol
</commit_message>
<xml_diff>
--- a/doc/DATA_PROTOCOL_SENSUS.xlsx
+++ b/doc/DATA_PROTOCOL_SENSUS.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Google Drive\PROROB\09 CLIENTI\Mind Music Lab AB\SOFTWARE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Google Drive\PROROB\09 CLIENTI\Mind Music Lab AB\GIT\sensei\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="23955" windowHeight="10800" tabRatio="655" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="23955" windowHeight="10800" tabRatio="655" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="GENERIC PACKET" sheetId="7" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="173">
   <si>
     <t>CMD</t>
   </si>
@@ -544,6 +544,9 @@
   </si>
   <si>
     <t># IEEE Float 32 bit little-endian</t>
+  </si>
+  <si>
+    <t>SLIDER_THRESHOLD</t>
   </si>
 </sst>
 </file>
@@ -940,7 +943,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1202,165 +1205,12 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1368,53 +1218,23 @@
     <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1423,62 +1243,257 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1869,350 +1884,350 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B2" s="144" t="s">
+      <c r="B2" s="123" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="145"/>
-      <c r="F2" s="146"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="125"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B4" s="108" t="s">
+      <c r="B4" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="108"/>
-      <c r="D4" s="100" t="s">
+      <c r="C4" s="126"/>
+      <c r="D4" s="135" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="100"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="100"/>
-      <c r="H4" s="100"/>
-      <c r="I4" s="100"/>
-      <c r="J4" s="100"/>
-      <c r="K4" s="100"/>
-      <c r="L4" s="100"/>
-      <c r="M4" s="100"/>
-      <c r="N4" s="100"/>
-      <c r="O4" s="100"/>
-      <c r="P4" s="100"/>
-      <c r="Q4" s="100"/>
-      <c r="R4" s="100"/>
-      <c r="S4" s="100"/>
-      <c r="T4" s="100"/>
-      <c r="U4" s="100"/>
-      <c r="V4" s="100"/>
-      <c r="W4" s="100"/>
-      <c r="X4" s="100"/>
+      <c r="E4" s="135"/>
+      <c r="F4" s="135"/>
+      <c r="G4" s="135"/>
+      <c r="H4" s="135"/>
+      <c r="I4" s="135"/>
+      <c r="J4" s="135"/>
+      <c r="K4" s="135"/>
+      <c r="L4" s="135"/>
+      <c r="M4" s="135"/>
+      <c r="N4" s="135"/>
+      <c r="O4" s="135"/>
+      <c r="P4" s="135"/>
+      <c r="Q4" s="135"/>
+      <c r="R4" s="135"/>
+      <c r="S4" s="135"/>
+      <c r="T4" s="135"/>
+      <c r="U4" s="135"/>
+      <c r="V4" s="135"/>
+      <c r="W4" s="135"/>
+      <c r="X4" s="135"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B5" s="109"/>
-      <c r="C5" s="109"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="100"/>
-      <c r="J5" s="100"/>
-      <c r="K5" s="100"/>
-      <c r="L5" s="100"/>
-      <c r="M5" s="100"/>
-      <c r="N5" s="100"/>
-      <c r="O5" s="100"/>
-      <c r="P5" s="100"/>
-      <c r="Q5" s="100"/>
-      <c r="R5" s="100"/>
-      <c r="S5" s="100"/>
-      <c r="T5" s="100"/>
-      <c r="U5" s="100"/>
-      <c r="V5" s="100"/>
-      <c r="W5" s="100"/>
-      <c r="X5" s="100"/>
+      <c r="B5" s="134"/>
+      <c r="C5" s="134"/>
+      <c r="D5" s="135"/>
+      <c r="E5" s="135"/>
+      <c r="F5" s="135"/>
+      <c r="G5" s="135"/>
+      <c r="H5" s="135"/>
+      <c r="I5" s="135"/>
+      <c r="J5" s="135"/>
+      <c r="K5" s="135"/>
+      <c r="L5" s="135"/>
+      <c r="M5" s="135"/>
+      <c r="N5" s="135"/>
+      <c r="O5" s="135"/>
+      <c r="P5" s="135"/>
+      <c r="Q5" s="135"/>
+      <c r="R5" s="135"/>
+      <c r="S5" s="135"/>
+      <c r="T5" s="135"/>
+      <c r="U5" s="135"/>
+      <c r="V5" s="135"/>
+      <c r="W5" s="135"/>
+      <c r="X5" s="135"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B6" s="110" t="s">
+      <c r="B6" s="137" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="110"/>
-      <c r="D6" s="100" t="s">
+      <c r="C6" s="137"/>
+      <c r="D6" s="135" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="100"/>
-      <c r="H6" s="100"/>
-      <c r="I6" s="100"/>
-      <c r="J6" s="100"/>
-      <c r="K6" s="100"/>
-      <c r="L6" s="100"/>
-      <c r="M6" s="100"/>
-      <c r="N6" s="100"/>
-      <c r="O6" s="100"/>
-      <c r="P6" s="100"/>
-      <c r="Q6" s="100"/>
-      <c r="R6" s="100"/>
-      <c r="S6" s="100"/>
-      <c r="T6" s="100"/>
-      <c r="U6" s="100"/>
-      <c r="V6" s="100"/>
-      <c r="W6" s="100"/>
-      <c r="X6" s="100"/>
+      <c r="E6" s="135"/>
+      <c r="F6" s="135"/>
+      <c r="G6" s="135"/>
+      <c r="H6" s="135"/>
+      <c r="I6" s="135"/>
+      <c r="J6" s="135"/>
+      <c r="K6" s="135"/>
+      <c r="L6" s="135"/>
+      <c r="M6" s="135"/>
+      <c r="N6" s="135"/>
+      <c r="O6" s="135"/>
+      <c r="P6" s="135"/>
+      <c r="Q6" s="135"/>
+      <c r="R6" s="135"/>
+      <c r="S6" s="135"/>
+      <c r="T6" s="135"/>
+      <c r="U6" s="135"/>
+      <c r="V6" s="135"/>
+      <c r="W6" s="135"/>
+      <c r="X6" s="135"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B7" s="99" t="s">
+      <c r="B7" s="138" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="99"/>
-      <c r="D7" s="100" t="s">
+      <c r="C7" s="138"/>
+      <c r="D7" s="135" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="100"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="100"/>
-      <c r="H7" s="100"/>
-      <c r="I7" s="100"/>
-      <c r="J7" s="100"/>
-      <c r="K7" s="100"/>
-      <c r="L7" s="100"/>
-      <c r="M7" s="100"/>
-      <c r="N7" s="100"/>
-      <c r="O7" s="100"/>
-      <c r="P7" s="100"/>
-      <c r="Q7" s="100"/>
-      <c r="R7" s="100"/>
-      <c r="S7" s="100"/>
-      <c r="T7" s="100"/>
-      <c r="U7" s="100"/>
-      <c r="V7" s="100"/>
-      <c r="W7" s="100"/>
-      <c r="X7" s="100"/>
+      <c r="E7" s="135"/>
+      <c r="F7" s="135"/>
+      <c r="G7" s="135"/>
+      <c r="H7" s="135"/>
+      <c r="I7" s="135"/>
+      <c r="J7" s="135"/>
+      <c r="K7" s="135"/>
+      <c r="L7" s="135"/>
+      <c r="M7" s="135"/>
+      <c r="N7" s="135"/>
+      <c r="O7" s="135"/>
+      <c r="P7" s="135"/>
+      <c r="Q7" s="135"/>
+      <c r="R7" s="135"/>
+      <c r="S7" s="135"/>
+      <c r="T7" s="135"/>
+      <c r="U7" s="135"/>
+      <c r="V7" s="135"/>
+      <c r="W7" s="135"/>
+      <c r="X7" s="135"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B8" s="101"/>
-      <c r="C8" s="102"/>
-      <c r="D8" s="103"/>
-      <c r="E8" s="104"/>
-      <c r="F8" s="104"/>
-      <c r="G8" s="104"/>
-      <c r="H8" s="104"/>
-      <c r="I8" s="104"/>
-      <c r="J8" s="104"/>
-      <c r="K8" s="104"/>
-      <c r="L8" s="104"/>
-      <c r="M8" s="104"/>
-      <c r="N8" s="104"/>
-      <c r="O8" s="104"/>
-      <c r="P8" s="104"/>
-      <c r="Q8" s="104"/>
-      <c r="R8" s="104"/>
-      <c r="S8" s="104"/>
-      <c r="T8" s="104"/>
-      <c r="U8" s="104"/>
-      <c r="V8" s="104"/>
-      <c r="W8" s="104"/>
-      <c r="X8" s="105"/>
+      <c r="B8" s="129"/>
+      <c r="C8" s="130"/>
+      <c r="D8" s="131"/>
+      <c r="E8" s="132"/>
+      <c r="F8" s="132"/>
+      <c r="G8" s="132"/>
+      <c r="H8" s="132"/>
+      <c r="I8" s="132"/>
+      <c r="J8" s="132"/>
+      <c r="K8" s="132"/>
+      <c r="L8" s="132"/>
+      <c r="M8" s="132"/>
+      <c r="N8" s="132"/>
+      <c r="O8" s="132"/>
+      <c r="P8" s="132"/>
+      <c r="Q8" s="132"/>
+      <c r="R8" s="132"/>
+      <c r="S8" s="132"/>
+      <c r="T8" s="132"/>
+      <c r="U8" s="132"/>
+      <c r="V8" s="132"/>
+      <c r="W8" s="132"/>
+      <c r="X8" s="133"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B9" s="106" t="s">
+      <c r="B9" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="107"/>
-      <c r="D9" s="103"/>
-      <c r="E9" s="104"/>
-      <c r="F9" s="104"/>
-      <c r="G9" s="104"/>
-      <c r="H9" s="104"/>
-      <c r="I9" s="104"/>
-      <c r="J9" s="104"/>
-      <c r="K9" s="104"/>
-      <c r="L9" s="104"/>
-      <c r="M9" s="104"/>
-      <c r="N9" s="104"/>
-      <c r="O9" s="104"/>
-      <c r="P9" s="104"/>
-      <c r="Q9" s="104"/>
-      <c r="R9" s="104"/>
-      <c r="S9" s="104"/>
-      <c r="T9" s="104"/>
-      <c r="U9" s="104"/>
-      <c r="V9" s="104"/>
-      <c r="W9" s="104"/>
-      <c r="X9" s="105"/>
+      <c r="C9" s="140"/>
+      <c r="D9" s="131"/>
+      <c r="E9" s="132"/>
+      <c r="F9" s="132"/>
+      <c r="G9" s="132"/>
+      <c r="H9" s="132"/>
+      <c r="I9" s="132"/>
+      <c r="J9" s="132"/>
+      <c r="K9" s="132"/>
+      <c r="L9" s="132"/>
+      <c r="M9" s="132"/>
+      <c r="N9" s="132"/>
+      <c r="O9" s="132"/>
+      <c r="P9" s="132"/>
+      <c r="Q9" s="132"/>
+      <c r="R9" s="132"/>
+      <c r="S9" s="132"/>
+      <c r="T9" s="132"/>
+      <c r="U9" s="132"/>
+      <c r="V9" s="132"/>
+      <c r="W9" s="132"/>
+      <c r="X9" s="133"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B10" s="101"/>
-      <c r="C10" s="102"/>
-      <c r="D10" s="103"/>
-      <c r="E10" s="104"/>
-      <c r="F10" s="104"/>
-      <c r="G10" s="104"/>
-      <c r="H10" s="104"/>
-      <c r="I10" s="104"/>
-      <c r="J10" s="104"/>
-      <c r="K10" s="104"/>
-      <c r="L10" s="104"/>
-      <c r="M10" s="104"/>
-      <c r="N10" s="104"/>
-      <c r="O10" s="104"/>
-      <c r="P10" s="104"/>
-      <c r="Q10" s="104"/>
-      <c r="R10" s="104"/>
-      <c r="S10" s="104"/>
-      <c r="T10" s="104"/>
-      <c r="U10" s="104"/>
-      <c r="V10" s="104"/>
-      <c r="W10" s="104"/>
-      <c r="X10" s="105"/>
+      <c r="B10" s="129"/>
+      <c r="C10" s="130"/>
+      <c r="D10" s="131"/>
+      <c r="E10" s="132"/>
+      <c r="F10" s="132"/>
+      <c r="G10" s="132"/>
+      <c r="H10" s="132"/>
+      <c r="I10" s="132"/>
+      <c r="J10" s="132"/>
+      <c r="K10" s="132"/>
+      <c r="L10" s="132"/>
+      <c r="M10" s="132"/>
+      <c r="N10" s="132"/>
+      <c r="O10" s="132"/>
+      <c r="P10" s="132"/>
+      <c r="Q10" s="132"/>
+      <c r="R10" s="132"/>
+      <c r="S10" s="132"/>
+      <c r="T10" s="132"/>
+      <c r="U10" s="132"/>
+      <c r="V10" s="132"/>
+      <c r="W10" s="132"/>
+      <c r="X10" s="133"/>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B11" s="113" t="s">
+      <c r="B11" s="136" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="113"/>
-      <c r="D11" s="100" t="s">
+      <c r="C11" s="136"/>
+      <c r="D11" s="135" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="100"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="100"/>
-      <c r="H11" s="100"/>
-      <c r="I11" s="100"/>
-      <c r="J11" s="100"/>
-      <c r="K11" s="100"/>
-      <c r="L11" s="100"/>
-      <c r="M11" s="100"/>
-      <c r="N11" s="100"/>
-      <c r="O11" s="100"/>
-      <c r="P11" s="100"/>
-      <c r="Q11" s="100"/>
-      <c r="R11" s="100"/>
-      <c r="S11" s="100"/>
-      <c r="T11" s="100"/>
-      <c r="U11" s="100"/>
-      <c r="V11" s="100"/>
-      <c r="W11" s="100"/>
-      <c r="X11" s="100"/>
+      <c r="E11" s="135"/>
+      <c r="F11" s="135"/>
+      <c r="G11" s="135"/>
+      <c r="H11" s="135"/>
+      <c r="I11" s="135"/>
+      <c r="J11" s="135"/>
+      <c r="K11" s="135"/>
+      <c r="L11" s="135"/>
+      <c r="M11" s="135"/>
+      <c r="N11" s="135"/>
+      <c r="O11" s="135"/>
+      <c r="P11" s="135"/>
+      <c r="Q11" s="135"/>
+      <c r="R11" s="135"/>
+      <c r="S11" s="135"/>
+      <c r="T11" s="135"/>
+      <c r="U11" s="135"/>
+      <c r="V11" s="135"/>
+      <c r="W11" s="135"/>
+      <c r="X11" s="135"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B12" s="112" t="s">
+      <c r="B12" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="112"/>
-      <c r="D12" s="100" t="s">
+      <c r="C12" s="128"/>
+      <c r="D12" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="100"/>
-      <c r="F12" s="100"/>
-      <c r="G12" s="100"/>
-      <c r="H12" s="100"/>
-      <c r="I12" s="100"/>
-      <c r="J12" s="100"/>
-      <c r="K12" s="100"/>
-      <c r="L12" s="100"/>
-      <c r="M12" s="100"/>
-      <c r="N12" s="100"/>
-      <c r="O12" s="100"/>
-      <c r="P12" s="100"/>
-      <c r="Q12" s="100"/>
-      <c r="R12" s="100"/>
-      <c r="S12" s="100"/>
-      <c r="T12" s="100"/>
-      <c r="U12" s="100"/>
-      <c r="V12" s="100"/>
-      <c r="W12" s="100"/>
-      <c r="X12" s="100"/>
+      <c r="E12" s="135"/>
+      <c r="F12" s="135"/>
+      <c r="G12" s="135"/>
+      <c r="H12" s="135"/>
+      <c r="I12" s="135"/>
+      <c r="J12" s="135"/>
+      <c r="K12" s="135"/>
+      <c r="L12" s="135"/>
+      <c r="M12" s="135"/>
+      <c r="N12" s="135"/>
+      <c r="O12" s="135"/>
+      <c r="P12" s="135"/>
+      <c r="Q12" s="135"/>
+      <c r="R12" s="135"/>
+      <c r="S12" s="135"/>
+      <c r="T12" s="135"/>
+      <c r="U12" s="135"/>
+      <c r="V12" s="135"/>
+      <c r="W12" s="135"/>
+      <c r="X12" s="135"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B13" s="111" t="s">
+      <c r="B13" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="111"/>
-      <c r="D13" s="100" t="s">
+      <c r="C13" s="127"/>
+      <c r="D13" s="135" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="100"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="100"/>
-      <c r="H13" s="100"/>
-      <c r="I13" s="100"/>
-      <c r="J13" s="100"/>
-      <c r="K13" s="100"/>
-      <c r="L13" s="100"/>
-      <c r="M13" s="100"/>
-      <c r="N13" s="100"/>
-      <c r="O13" s="100"/>
-      <c r="P13" s="100"/>
-      <c r="Q13" s="100"/>
-      <c r="R13" s="100"/>
-      <c r="S13" s="100"/>
-      <c r="T13" s="100"/>
-      <c r="U13" s="100"/>
-      <c r="V13" s="100"/>
-      <c r="W13" s="100"/>
-      <c r="X13" s="100"/>
+      <c r="E13" s="135"/>
+      <c r="F13" s="135"/>
+      <c r="G13" s="135"/>
+      <c r="H13" s="135"/>
+      <c r="I13" s="135"/>
+      <c r="J13" s="135"/>
+      <c r="K13" s="135"/>
+      <c r="L13" s="135"/>
+      <c r="M13" s="135"/>
+      <c r="N13" s="135"/>
+      <c r="O13" s="135"/>
+      <c r="P13" s="135"/>
+      <c r="Q13" s="135"/>
+      <c r="R13" s="135"/>
+      <c r="S13" s="135"/>
+      <c r="T13" s="135"/>
+      <c r="U13" s="135"/>
+      <c r="V13" s="135"/>
+      <c r="W13" s="135"/>
+      <c r="X13" s="135"/>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B14" s="109"/>
-      <c r="C14" s="109"/>
-      <c r="D14" s="100"/>
-      <c r="E14" s="100"/>
-      <c r="F14" s="100"/>
-      <c r="G14" s="100"/>
-      <c r="H14" s="100"/>
-      <c r="I14" s="100"/>
-      <c r="J14" s="100"/>
-      <c r="K14" s="100"/>
-      <c r="L14" s="100"/>
-      <c r="M14" s="100"/>
-      <c r="N14" s="100"/>
-      <c r="O14" s="100"/>
-      <c r="P14" s="100"/>
-      <c r="Q14" s="100"/>
-      <c r="R14" s="100"/>
-      <c r="S14" s="100"/>
-      <c r="T14" s="100"/>
-      <c r="U14" s="100"/>
-      <c r="V14" s="100"/>
-      <c r="W14" s="100"/>
-      <c r="X14" s="100"/>
+      <c r="B14" s="134"/>
+      <c r="C14" s="134"/>
+      <c r="D14" s="135"/>
+      <c r="E14" s="135"/>
+      <c r="F14" s="135"/>
+      <c r="G14" s="135"/>
+      <c r="H14" s="135"/>
+      <c r="I14" s="135"/>
+      <c r="J14" s="135"/>
+      <c r="K14" s="135"/>
+      <c r="L14" s="135"/>
+      <c r="M14" s="135"/>
+      <c r="N14" s="135"/>
+      <c r="O14" s="135"/>
+      <c r="P14" s="135"/>
+      <c r="Q14" s="135"/>
+      <c r="R14" s="135"/>
+      <c r="S14" s="135"/>
+      <c r="T14" s="135"/>
+      <c r="U14" s="135"/>
+      <c r="V14" s="135"/>
+      <c r="W14" s="135"/>
+      <c r="X14" s="135"/>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B15" s="108" t="s">
+      <c r="B15" s="126" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="108"/>
-      <c r="D15" s="100" t="s">
+      <c r="C15" s="126"/>
+      <c r="D15" s="135" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="100"/>
-      <c r="F15" s="100"/>
-      <c r="G15" s="100"/>
-      <c r="H15" s="100"/>
-      <c r="I15" s="100"/>
-      <c r="J15" s="100"/>
-      <c r="K15" s="100"/>
-      <c r="L15" s="100"/>
-      <c r="M15" s="100"/>
-      <c r="N15" s="100"/>
-      <c r="O15" s="100"/>
-      <c r="P15" s="100"/>
-      <c r="Q15" s="100"/>
-      <c r="R15" s="100"/>
-      <c r="S15" s="100"/>
-      <c r="T15" s="100"/>
-      <c r="U15" s="100"/>
-      <c r="V15" s="100"/>
-      <c r="W15" s="100"/>
-      <c r="X15" s="100"/>
+      <c r="E15" s="135"/>
+      <c r="F15" s="135"/>
+      <c r="G15" s="135"/>
+      <c r="H15" s="135"/>
+      <c r="I15" s="135"/>
+      <c r="J15" s="135"/>
+      <c r="K15" s="135"/>
+      <c r="L15" s="135"/>
+      <c r="M15" s="135"/>
+      <c r="N15" s="135"/>
+      <c r="O15" s="135"/>
+      <c r="P15" s="135"/>
+      <c r="Q15" s="135"/>
+      <c r="R15" s="135"/>
+      <c r="S15" s="135"/>
+      <c r="T15" s="135"/>
+      <c r="U15" s="135"/>
+      <c r="V15" s="135"/>
+      <c r="W15" s="135"/>
+      <c r="X15" s="135"/>
     </row>
     <row r="17" spans="3:67" x14ac:dyDescent="0.2">
-      <c r="D17" s="108" t="s">
+      <c r="D17" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="108"/>
-      <c r="F17" s="108"/>
+      <c r="E17" s="126"/>
+      <c r="F17" s="126"/>
       <c r="G17" s="88" t="s">
         <v>0</v>
       </c>
@@ -2271,24 +2286,24 @@
       <c r="BF17" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="BG17" s="112" t="s">
+      <c r="BG17" s="128" t="s">
         <v>7</v>
       </c>
-      <c r="BH17" s="112"/>
-      <c r="BI17" s="112"/>
-      <c r="BJ17" s="112"/>
-      <c r="BK17" s="111" t="s">
+      <c r="BH17" s="128"/>
+      <c r="BI17" s="128"/>
+      <c r="BJ17" s="128"/>
+      <c r="BK17" s="127" t="s">
         <v>5</v>
       </c>
-      <c r="BL17" s="111"/>
-      <c r="BM17" s="108" t="s">
+      <c r="BL17" s="127"/>
+      <c r="BM17" s="126" t="s">
         <v>6</v>
       </c>
-      <c r="BN17" s="108"/>
-      <c r="BO17" s="108"/>
+      <c r="BN17" s="126"/>
+      <c r="BO17" s="126"/>
     </row>
     <row r="18" spans="3:67" x14ac:dyDescent="0.2">
-      <c r="C18" s="155" t="s">
+      <c r="C18" s="104" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="9">
@@ -2486,6 +2501,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="D13:X13"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:X4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:X5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:X6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:X7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:X8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:X9"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="BK17:BL17"/>
@@ -2502,19 +2530,6 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:X12"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:X13"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:X4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:X5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:X6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:X7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:X8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:X9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2522,10 +2537,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L29"/>
+  <dimension ref="B2:L30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2541,11 +2556,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="129" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="147"/>
-      <c r="D2" s="102"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="130"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="16">
@@ -2583,7 +2598,7 @@
       <c r="B7" s="27">
         <v>5</v>
       </c>
-      <c r="C7" s="115" t="s">
+      <c r="C7" s="193" t="s">
         <v>78</v>
       </c>
       <c r="D7" s="29" t="s">
@@ -2601,7 +2616,7 @@
       <c r="B8" s="27">
         <v>6</v>
       </c>
-      <c r="C8" s="116"/>
+      <c r="C8" s="194"/>
       <c r="D8" s="30" t="s">
         <v>82</v>
       </c>
@@ -2660,7 +2675,7 @@
       <c r="B13" s="27">
         <v>5</v>
       </c>
-      <c r="C13" s="115" t="s">
+      <c r="C13" s="193" t="s">
         <v>78</v>
       </c>
       <c r="D13" s="29" t="s">
@@ -2680,7 +2695,7 @@
       <c r="B14" s="27">
         <v>6</v>
       </c>
-      <c r="C14" s="116"/>
+      <c r="C14" s="194"/>
       <c r="D14" s="30" t="s">
         <v>82</v>
       </c>
@@ -2747,17 +2762,17 @@
       <c r="D19" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="G19" s="135" t="s">
+      <c r="G19" s="190" t="s">
         <v>92</v>
       </c>
-      <c r="H19" s="136"/>
-      <c r="I19" s="137"/>
+      <c r="H19" s="191"/>
+      <c r="I19" s="192"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B20" s="27">
         <v>5</v>
       </c>
-      <c r="C20" s="115" t="s">
+      <c r="C20" s="193" t="s">
         <v>78</v>
       </c>
       <c r="D20" s="29" t="s">
@@ -2768,7 +2783,7 @@
       <c r="B21" s="27">
         <v>6</v>
       </c>
-      <c r="C21" s="116"/>
+      <c r="C21" s="194"/>
       <c r="D21" s="30" t="s">
         <v>82</v>
       </c>
@@ -2815,7 +2830,7 @@
       <c r="B24" s="27">
         <v>9</v>
       </c>
-      <c r="C24" s="138" t="s">
+      <c r="C24" s="195" t="s">
         <v>80</v>
       </c>
       <c r="D24" s="33" t="s">
@@ -2833,7 +2848,7 @@
       <c r="B25" s="27">
         <v>10</v>
       </c>
-      <c r="C25" s="139"/>
+      <c r="C25" s="196"/>
       <c r="D25" s="56" t="s">
         <v>82</v>
       </c>
@@ -2849,7 +2864,7 @@
       <c r="B26" s="16">
         <v>11</v>
       </c>
-      <c r="C26" s="139"/>
+      <c r="C26" s="196"/>
       <c r="D26" s="56" t="s">
         <v>84</v>
       </c>
@@ -2858,7 +2873,7 @@
       <c r="B27" s="16">
         <v>12</v>
       </c>
-      <c r="C27" s="140"/>
+      <c r="C27" s="197"/>
       <c r="D27" s="57" t="s">
         <v>83</v>
       </c>
@@ -2883,6 +2898,15 @@
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B29" s="16">
+        <v>14</v>
+      </c>
+      <c r="C29" s="198" t="s">
+        <v>172</v>
+      </c>
+      <c r="D29" s="200" t="s">
+        <v>81</v>
+      </c>
       <c r="G29" s="39" t="s">
         <v>108</v>
       </c>
@@ -2891,8 +2915,18 @@
         <v>1</v>
       </c>
     </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B30" s="16">
+        <v>15</v>
+      </c>
+      <c r="C30" s="199"/>
+      <c r="D30" s="201" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="C29:C30"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="G19:I19"/>
     <mergeCell ref="C7:C8"/>
@@ -2901,7 +2935,8 @@
     <mergeCell ref="C20:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2910,7 +2945,7 @@
   <dimension ref="B2:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21:E24"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3385,15 +3420,15 @@
       <c r="F44" s="3"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B45" s="181">
+      <c r="B45" s="117">
         <v>255</v>
       </c>
-      <c r="C45" s="181"/>
-      <c r="D45" s="181" t="s">
+      <c r="C45" s="117"/>
+      <c r="D45" s="117" t="s">
         <v>157</v>
       </c>
-      <c r="E45" s="181"/>
-      <c r="F45" s="182"/>
+      <c r="E45" s="117"/>
+      <c r="F45" s="118"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3418,11 +3453,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="151" t="s">
+      <c r="B2" s="141" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="151"/>
-      <c r="D2" s="151"/>
+      <c r="C2" s="141"/>
+      <c r="D2" s="141"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="16">
@@ -3442,7 +3477,7 @@
       <c r="C5" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="156" t="s">
+      <c r="D5" s="105" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3469,7 +3504,7 @@
   <dimension ref="B3:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B15" sqref="B15:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3507,135 +3542,135 @@
       <c r="B5" s="27">
         <v>5</v>
       </c>
-      <c r="C5" s="162" t="s">
+      <c r="C5" s="142" t="s">
         <v>123</v>
       </c>
-      <c r="D5" s="163" t="s">
+      <c r="D5" s="107" t="s">
         <v>81</v>
       </c>
-      <c r="F5" s="157" t="s">
+      <c r="F5" s="154" t="s">
         <v>158</v>
       </c>
-      <c r="G5" s="189"/>
-      <c r="H5" s="190"/>
+      <c r="G5" s="155"/>
+      <c r="H5" s="156"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="27">
         <v>6</v>
       </c>
-      <c r="C6" s="164"/>
-      <c r="D6" s="165" t="s">
+      <c r="C6" s="143"/>
+      <c r="D6" s="108" t="s">
         <v>82</v>
       </c>
-      <c r="F6" s="185" t="s">
+      <c r="F6" s="157" t="s">
         <v>161</v>
       </c>
-      <c r="G6" s="184"/>
-      <c r="H6" s="186"/>
+      <c r="G6" s="158"/>
+      <c r="H6" s="159"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="27">
         <v>7</v>
       </c>
-      <c r="C7" s="164"/>
-      <c r="D7" s="165" t="s">
+      <c r="C7" s="143"/>
+      <c r="D7" s="108" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="185" t="s">
+      <c r="F7" s="157" t="s">
         <v>162</v>
       </c>
-      <c r="G7" s="184"/>
-      <c r="H7" s="186"/>
+      <c r="G7" s="158"/>
+      <c r="H7" s="159"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" s="27">
         <v>8</v>
       </c>
-      <c r="C8" s="166"/>
-      <c r="D8" s="167" t="s">
+      <c r="C8" s="144"/>
+      <c r="D8" s="109" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="187" t="s">
+      <c r="F8" s="160" t="s">
         <v>163</v>
       </c>
-      <c r="G8" s="183"/>
-      <c r="H8" s="188"/>
+      <c r="G8" s="161"/>
+      <c r="H8" s="162"/>
     </row>
     <row r="9" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="27">
         <v>9</v>
       </c>
-      <c r="C9" s="168" t="s">
+      <c r="C9" s="151" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="169" t="s">
+      <c r="D9" s="110" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="158" t="s">
+      <c r="F9" s="145" t="s">
         <v>160</v>
       </c>
-      <c r="G9" s="161"/>
-      <c r="H9" s="180"/>
+      <c r="G9" s="146"/>
+      <c r="H9" s="147"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="27">
         <v>10</v>
       </c>
-      <c r="C10" s="170"/>
-      <c r="D10" s="171" t="s">
+      <c r="C10" s="152"/>
+      <c r="D10" s="111" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="158"/>
-      <c r="G10" s="161"/>
-      <c r="H10" s="180"/>
+      <c r="F10" s="145"/>
+      <c r="G10" s="146"/>
+      <c r="H10" s="147"/>
     </row>
     <row r="11" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="27">
         <v>11</v>
       </c>
-      <c r="C11" s="170"/>
-      <c r="D11" s="171" t="s">
+      <c r="C11" s="152"/>
+      <c r="D11" s="111" t="s">
         <v>84</v>
       </c>
-      <c r="F11" s="158"/>
-      <c r="G11" s="161"/>
-      <c r="H11" s="180"/>
+      <c r="F11" s="145"/>
+      <c r="G11" s="146"/>
+      <c r="H11" s="147"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" s="27">
         <v>12</v>
       </c>
-      <c r="C12" s="172"/>
-      <c r="D12" s="173" t="s">
+      <c r="C12" s="153"/>
+      <c r="D12" s="112" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="158"/>
-      <c r="G12" s="161"/>
-      <c r="H12" s="180"/>
+      <c r="F12" s="145"/>
+      <c r="G12" s="146"/>
+      <c r="H12" s="147"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="27">
         <v>13</v>
       </c>
-      <c r="C13" s="174" t="s">
+      <c r="C13" s="113" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="175"/>
-      <c r="F13" s="158"/>
-      <c r="G13" s="161"/>
-      <c r="H13" s="180"/>
+      <c r="D13" s="114"/>
+      <c r="F13" s="145"/>
+      <c r="G13" s="146"/>
+      <c r="H13" s="147"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="27">
         <v>14</v>
       </c>
-      <c r="C14" s="176" t="s">
+      <c r="C14" s="115" t="s">
         <v>20</v>
       </c>
-      <c r="D14" s="177"/>
-      <c r="F14" s="159"/>
-      <c r="G14" s="178"/>
-      <c r="H14" s="179"/>
+      <c r="D14" s="116"/>
+      <c r="F14" s="148"/>
+      <c r="G14" s="149"/>
+      <c r="H14" s="150"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3671,11 +3706,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="101" t="s">
+      <c r="B3" s="129" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="102"/>
-      <c r="D3" s="154"/>
+      <c r="C3" s="130"/>
+      <c r="D3" s="103"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="16">
@@ -3871,19 +3906,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="129" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="147"/>
-      <c r="D2" s="102"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="130"/>
     </row>
     <row r="5" spans="2:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="117" t="s">
+      <c r="B5" s="166" t="s">
         <v>152</v>
       </c>
-      <c r="C5" s="117"/>
-      <c r="E5" s="152"/>
-      <c r="F5" s="152"/>
+      <c r="C5" s="166"/>
+      <c r="E5" s="102"/>
+      <c r="F5" s="102"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="16">
@@ -3895,10 +3930,10 @@
       <c r="D6" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="114" t="s">
+      <c r="F6" s="165" t="s">
         <v>127</v>
       </c>
-      <c r="G6" s="114"/>
+      <c r="G6" s="165"/>
       <c r="H6" s="5"/>
       <c r="I6" s="76"/>
     </row>
@@ -3979,17 +4014,17 @@
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="153" t="s">
+      <c r="B13" s="164" t="s">
         <v>126</v>
       </c>
-      <c r="C13" s="153"/>
+      <c r="C13" s="164"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="148" t="s">
+      <c r="B14" s="167" t="s">
         <v>159</v>
       </c>
-      <c r="C14" s="149"/>
-      <c r="D14" s="150"/>
+      <c r="C14" s="168"/>
+      <c r="D14" s="169"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" s="16">
@@ -4122,8 +4157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -4138,18 +4173,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="129" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="147"/>
-      <c r="D2" s="102"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="130"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="117" t="s">
+      <c r="B5" s="166" t="s">
         <v>152</v>
       </c>
-      <c r="C5" s="117"/>
-      <c r="E5" s="152"/>
+      <c r="C5" s="166"/>
+      <c r="E5" s="102"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="16">
@@ -4222,10 +4257,10 @@
       <c r="B10" s="27">
         <v>7</v>
       </c>
-      <c r="C10" s="192" t="s">
+      <c r="C10" s="120" t="s">
         <v>129</v>
       </c>
-      <c r="D10" s="191"/>
+      <c r="D10" s="119"/>
       <c r="F10" s="14" t="s">
         <v>170</v>
       </c>
@@ -4235,10 +4270,10 @@
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="117" t="s">
+      <c r="B12" s="166" t="s">
         <v>152</v>
       </c>
-      <c r="C12" s="117"/>
+      <c r="C12" s="166"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="16">
@@ -4286,16 +4321,16 @@
       <c r="B17" s="27">
         <v>7</v>
       </c>
-      <c r="C17" s="192" t="s">
+      <c r="C17" s="120" t="s">
         <v>129</v>
       </c>
-      <c r="D17" s="191"/>
+      <c r="D17" s="119"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="117" t="s">
+      <c r="B19" s="166" t="s">
         <v>152</v>
       </c>
-      <c r="C19" s="117"/>
+      <c r="C19" s="166"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="16">
@@ -4335,7 +4370,7 @@
         <v>6</v>
       </c>
       <c r="C23" s="95"/>
-      <c r="D23" s="160" t="s">
+      <c r="D23" s="106" t="s">
         <v>82</v>
       </c>
     </row>
@@ -4343,7 +4378,7 @@
       <c r="B24" s="27">
         <v>7</v>
       </c>
-      <c r="C24" s="193" t="s">
+      <c r="C24" s="170" t="s">
         <v>129</v>
       </c>
       <c r="D24" s="52" t="s">
@@ -4354,16 +4389,16 @@
       <c r="B25" s="27">
         <v>8</v>
       </c>
-      <c r="C25" s="194"/>
+      <c r="C25" s="172"/>
       <c r="D25" s="53" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="117" t="s">
+      <c r="B27" s="166" t="s">
         <v>152</v>
       </c>
-      <c r="C27" s="117"/>
+      <c r="C27" s="166"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="16">
@@ -4403,7 +4438,7 @@
         <v>6</v>
       </c>
       <c r="C31" s="95"/>
-      <c r="D31" s="160" t="s">
+      <c r="D31" s="106" t="s">
         <v>82</v>
       </c>
     </row>
@@ -4411,7 +4446,7 @@
       <c r="B32" s="27">
         <v>7</v>
       </c>
-      <c r="C32" s="193" t="s">
+      <c r="C32" s="170" t="s">
         <v>129</v>
       </c>
       <c r="D32" s="52" t="s">
@@ -4422,8 +4457,8 @@
       <c r="B33" s="27">
         <v>8</v>
       </c>
-      <c r="C33" s="195"/>
-      <c r="D33" s="196" t="s">
+      <c r="C33" s="171"/>
+      <c r="D33" s="121" t="s">
         <v>82</v>
       </c>
     </row>
@@ -4431,8 +4466,8 @@
       <c r="B34" s="27">
         <v>9</v>
       </c>
-      <c r="C34" s="195"/>
-      <c r="D34" s="196" t="s">
+      <c r="C34" s="171"/>
+      <c r="D34" s="121" t="s">
         <v>84</v>
       </c>
     </row>
@@ -4440,7 +4475,7 @@
       <c r="B35" s="27">
         <v>10</v>
       </c>
-      <c r="C35" s="194"/>
+      <c r="C35" s="172"/>
       <c r="D35" s="53" t="s">
         <v>83</v>
       </c>
@@ -4451,14 +4486,15 @@
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="148" t="s">
+      <c r="B39" s="167" t="s">
         <v>159</v>
       </c>
-      <c r="C39" s="149"/>
-      <c r="D39" s="150"/>
+      <c r="C39" s="168"/>
+      <c r="D39" s="169"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="B2:D2"/>
     <mergeCell ref="C32:C35"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="B39:D39"/>
@@ -4466,7 +4502,6 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4493,11 +4528,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="129" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="147"/>
-      <c r="D2" s="102"/>
+      <c r="C2" s="163"/>
+      <c r="D2" s="130"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="61"/>
@@ -4505,10 +4540,10 @@
       <c r="D3" s="61"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="117" t="s">
+      <c r="B4" s="166" t="s">
         <v>152</v>
       </c>
-      <c r="C4" s="117"/>
+      <c r="C4" s="166"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="16">
@@ -4645,11 +4680,11 @@
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="148" t="s">
+      <c r="B14" s="167" t="s">
         <v>159</v>
       </c>
-      <c r="C14" s="149"/>
-      <c r="D14" s="150"/>
+      <c r="C14" s="168"/>
+      <c r="D14" s="169"/>
       <c r="F14" s="15" t="s">
         <v>56</v>
       </c>
@@ -4666,7 +4701,7 @@
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="48"/>
       <c r="C16" s="44"/>
-      <c r="D16" s="197"/>
+      <c r="D16" s="122"/>
       <c r="F16" s="13" t="s">
         <v>62</v>
       </c>
@@ -4696,11 +4731,11 @@
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="101" t="s">
+      <c r="B19" s="129" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="147"/>
-      <c r="D19" s="102"/>
+      <c r="C19" s="163"/>
+      <c r="D19" s="130"/>
       <c r="F19" s="15" t="s">
         <v>40</v>
       </c>
@@ -4713,10 +4748,10 @@
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="117" t="s">
+      <c r="B21" s="166" t="s">
         <v>152</v>
       </c>
-      <c r="C21" s="117"/>
+      <c r="C21" s="166"/>
       <c r="F21" s="98" t="s">
         <v>63</v>
       </c>
@@ -4782,11 +4817,11 @@
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="148" t="s">
+      <c r="B26" s="167" t="s">
         <v>159</v>
       </c>
-      <c r="C26" s="149"/>
-      <c r="D26" s="150"/>
+      <c r="C26" s="168"/>
+      <c r="D26" s="169"/>
       <c r="F26" s="15" t="s">
         <v>46</v>
       </c>
@@ -4938,36 +4973,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B2" s="144" t="s">
+      <c r="B2" s="123" t="s">
         <v>138</v>
       </c>
-      <c r="C2" s="145"/>
-      <c r="D2" s="146"/>
+      <c r="C2" s="124"/>
+      <c r="D2" s="125"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B4" s="117" t="s">
+      <c r="B4" s="166" t="s">
         <v>152</v>
       </c>
-      <c r="C4" s="117"/>
+      <c r="C4" s="166"/>
       <c r="E4" s="75"/>
-      <c r="G4" s="128" t="s">
+      <c r="G4" s="173" t="s">
         <v>171</v>
       </c>
-      <c r="H4" s="128"/>
-      <c r="I4" s="128"/>
-      <c r="J4" s="128"/>
-      <c r="K4" s="128"/>
-      <c r="L4" s="128"/>
-      <c r="M4" s="128"/>
-      <c r="N4" s="128"/>
-      <c r="O4" s="128"/>
-      <c r="P4" s="128"/>
-      <c r="Q4" s="128"/>
-      <c r="R4" s="128"/>
-      <c r="S4" s="128"/>
-      <c r="T4" s="128"/>
-      <c r="U4" s="128"/>
-      <c r="V4" s="128"/>
+      <c r="H4" s="173"/>
+      <c r="I4" s="173"/>
+      <c r="J4" s="173"/>
+      <c r="K4" s="173"/>
+      <c r="L4" s="173"/>
+      <c r="M4" s="173"/>
+      <c r="N4" s="173"/>
+      <c r="O4" s="173"/>
+      <c r="P4" s="173"/>
+      <c r="Q4" s="173"/>
+      <c r="R4" s="173"/>
+      <c r="S4" s="173"/>
+      <c r="T4" s="173"/>
+      <c r="U4" s="173"/>
+      <c r="V4" s="173"/>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B5" s="16">
@@ -5269,11 +5304,11 @@
       <c r="V11" s="15"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B12" s="148" t="s">
+      <c r="B12" s="167" t="s">
         <v>159</v>
       </c>
-      <c r="C12" s="149"/>
-      <c r="D12" s="150"/>
+      <c r="C12" s="168"/>
+      <c r="D12" s="169"/>
       <c r="F12" s="50"/>
       <c r="G12" s="75"/>
       <c r="H12" s="75"/>
@@ -5321,24 +5356,24 @@
       <c r="B15" s="70">
         <v>0</v>
       </c>
-      <c r="C15" s="132" t="s">
+      <c r="C15" s="184" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="141"/>
+      <c r="D15" s="99"/>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B16" s="70">
         <v>1</v>
       </c>
-      <c r="C16" s="133"/>
-      <c r="D16" s="142"/>
+      <c r="C16" s="185"/>
+      <c r="D16" s="100"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B17" s="70">
         <v>2</v>
       </c>
-      <c r="C17" s="134"/>
-      <c r="D17" s="143"/>
+      <c r="C17" s="186"/>
+      <c r="D17" s="101"/>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B18" s="16">
@@ -5366,7 +5401,7 @@
       <c r="B20" s="16">
         <v>5</v>
       </c>
-      <c r="C20" s="118" t="s">
+      <c r="C20" s="182" t="s">
         <v>131</v>
       </c>
       <c r="D20" s="62" t="s">
@@ -5377,7 +5412,7 @@
       <c r="B21" s="16">
         <v>6</v>
       </c>
-      <c r="C21" s="119"/>
+      <c r="C21" s="183"/>
       <c r="D21" s="63" t="s">
         <v>82</v>
       </c>
@@ -5386,7 +5421,7 @@
       <c r="B22" s="16">
         <v>7</v>
       </c>
-      <c r="C22" s="119"/>
+      <c r="C22" s="183"/>
       <c r="D22" s="63" t="s">
         <v>84</v>
       </c>
@@ -5395,7 +5430,7 @@
       <c r="B23" s="16">
         <v>8</v>
       </c>
-      <c r="C23" s="119"/>
+      <c r="C23" s="183"/>
       <c r="D23" s="64" t="s">
         <v>83</v>
       </c>
@@ -5404,7 +5439,7 @@
       <c r="B24" s="16">
         <v>9</v>
       </c>
-      <c r="C24" s="118" t="s">
+      <c r="C24" s="182" t="s">
         <v>132</v>
       </c>
       <c r="D24" s="62" t="s">
@@ -5415,7 +5450,7 @@
       <c r="B25" s="16">
         <v>10</v>
       </c>
-      <c r="C25" s="119"/>
+      <c r="C25" s="183"/>
       <c r="D25" s="63" t="s">
         <v>82</v>
       </c>
@@ -5441,7 +5476,7 @@
       <c r="B26" s="16">
         <v>11</v>
       </c>
-      <c r="C26" s="119"/>
+      <c r="C26" s="183"/>
       <c r="D26" s="63" t="s">
         <v>84</v>
       </c>
@@ -5450,7 +5485,7 @@
       <c r="B27" s="16">
         <v>12</v>
       </c>
-      <c r="C27" s="119"/>
+      <c r="C27" s="183"/>
       <c r="D27" s="64" t="s">
         <v>83</v>
       </c>
@@ -5459,7 +5494,7 @@
       <c r="B28" s="16">
         <v>13</v>
       </c>
-      <c r="C28" s="118" t="s">
+      <c r="C28" s="182" t="s">
         <v>133</v>
       </c>
       <c r="D28" s="62" t="s">
@@ -5470,7 +5505,7 @@
       <c r="B29" s="16">
         <v>14</v>
       </c>
-      <c r="C29" s="119"/>
+      <c r="C29" s="183"/>
       <c r="D29" s="63" t="s">
         <v>82</v>
       </c>
@@ -5479,7 +5514,7 @@
       <c r="B30" s="16">
         <v>15</v>
       </c>
-      <c r="C30" s="119"/>
+      <c r="C30" s="183"/>
       <c r="D30" s="63" t="s">
         <v>84</v>
       </c>
@@ -5488,7 +5523,7 @@
       <c r="B31" s="16">
         <v>16</v>
       </c>
-      <c r="C31" s="119"/>
+      <c r="C31" s="183"/>
       <c r="D31" s="64" t="s">
         <v>83</v>
       </c>
@@ -5497,7 +5532,7 @@
       <c r="B32" s="16">
         <v>17</v>
       </c>
-      <c r="C32" s="118" t="s">
+      <c r="C32" s="182" t="s">
         <v>134</v>
       </c>
       <c r="D32" s="62" t="s">
@@ -5508,7 +5543,7 @@
       <c r="B33" s="16">
         <v>18</v>
       </c>
-      <c r="C33" s="119"/>
+      <c r="C33" s="183"/>
       <c r="D33" s="63" t="s">
         <v>82</v>
       </c>
@@ -5517,7 +5552,7 @@
       <c r="B34" s="16">
         <v>19</v>
       </c>
-      <c r="C34" s="119"/>
+      <c r="C34" s="183"/>
       <c r="D34" s="63" t="s">
         <v>84</v>
       </c>
@@ -5543,7 +5578,7 @@
       <c r="B35" s="16">
         <v>20</v>
       </c>
-      <c r="C35" s="119"/>
+      <c r="C35" s="183"/>
       <c r="D35" s="64" t="s">
         <v>83</v>
       </c>
@@ -5569,7 +5604,7 @@
       <c r="B36" s="16">
         <v>21</v>
       </c>
-      <c r="C36" s="118" t="s">
+      <c r="C36" s="182" t="s">
         <v>139</v>
       </c>
       <c r="D36" s="62" t="s">
@@ -5597,7 +5632,7 @@
       <c r="B37" s="16">
         <v>22</v>
       </c>
-      <c r="C37" s="119"/>
+      <c r="C37" s="183"/>
       <c r="D37" s="63" t="s">
         <v>82</v>
       </c>
@@ -5623,7 +5658,7 @@
       <c r="B38" s="16">
         <v>23</v>
       </c>
-      <c r="C38" s="119"/>
+      <c r="C38" s="183"/>
       <c r="D38" s="63" t="s">
         <v>84</v>
       </c>
@@ -5645,7 +5680,7 @@
       <c r="B39" s="16">
         <v>24</v>
       </c>
-      <c r="C39" s="119"/>
+      <c r="C39" s="183"/>
       <c r="D39" s="64" t="s">
         <v>83</v>
       </c>
@@ -5667,7 +5702,7 @@
       <c r="B40" s="16">
         <v>25</v>
       </c>
-      <c r="C40" s="118" t="s">
+      <c r="C40" s="182" t="s">
         <v>140</v>
       </c>
       <c r="D40" s="62" t="s">
@@ -5691,7 +5726,7 @@
       <c r="B41" s="16">
         <v>26</v>
       </c>
-      <c r="C41" s="119"/>
+      <c r="C41" s="183"/>
       <c r="D41" s="63" t="s">
         <v>82</v>
       </c>
@@ -5717,7 +5752,7 @@
       <c r="B42" s="16">
         <v>27</v>
       </c>
-      <c r="C42" s="119"/>
+      <c r="C42" s="183"/>
       <c r="D42" s="63" t="s">
         <v>84</v>
       </c>
@@ -5743,7 +5778,7 @@
       <c r="B43" s="16">
         <v>28</v>
       </c>
-      <c r="C43" s="119"/>
+      <c r="C43" s="183"/>
       <c r="D43" s="64" t="s">
         <v>83</v>
       </c>
@@ -5769,7 +5804,7 @@
       <c r="B44" s="16">
         <v>29</v>
       </c>
-      <c r="C44" s="118" t="s">
+      <c r="C44" s="182" t="s">
         <v>141</v>
       </c>
       <c r="D44" s="62" t="s">
@@ -5797,7 +5832,7 @@
       <c r="B45" s="16">
         <v>30</v>
       </c>
-      <c r="C45" s="119"/>
+      <c r="C45" s="183"/>
       <c r="D45" s="63" t="s">
         <v>82</v>
       </c>
@@ -5806,7 +5841,7 @@
       <c r="B46" s="16">
         <v>31</v>
       </c>
-      <c r="C46" s="119"/>
+      <c r="C46" s="183"/>
       <c r="D46" s="63" t="s">
         <v>84</v>
       </c>
@@ -5815,7 +5850,7 @@
       <c r="B47" s="16">
         <v>32</v>
       </c>
-      <c r="C47" s="119"/>
+      <c r="C47" s="183"/>
       <c r="D47" s="64" t="s">
         <v>83</v>
       </c>
@@ -5824,7 +5859,7 @@
       <c r="B48" s="16">
         <v>33</v>
       </c>
-      <c r="C48" s="118" t="s">
+      <c r="C48" s="182" t="s">
         <v>142</v>
       </c>
       <c r="D48" s="62" t="s">
@@ -5835,7 +5870,7 @@
       <c r="B49" s="16">
         <v>34</v>
       </c>
-      <c r="C49" s="119"/>
+      <c r="C49" s="183"/>
       <c r="D49" s="63" t="s">
         <v>82</v>
       </c>
@@ -5844,7 +5879,7 @@
       <c r="B50" s="16">
         <v>35</v>
       </c>
-      <c r="C50" s="119"/>
+      <c r="C50" s="183"/>
       <c r="D50" s="63" t="s">
         <v>84</v>
       </c>
@@ -5853,7 +5888,7 @@
       <c r="B51" s="16">
         <v>36</v>
       </c>
-      <c r="C51" s="119"/>
+      <c r="C51" s="183"/>
       <c r="D51" s="64" t="s">
         <v>83</v>
       </c>
@@ -5862,7 +5897,7 @@
       <c r="B52" s="16">
         <v>37</v>
       </c>
-      <c r="C52" s="125" t="s">
+      <c r="C52" s="187" t="s">
         <v>143</v>
       </c>
       <c r="D52" s="62" t="s">
@@ -5873,7 +5908,7 @@
       <c r="B53" s="16">
         <v>38</v>
       </c>
-      <c r="C53" s="126"/>
+      <c r="C53" s="188"/>
       <c r="D53" s="63" t="s">
         <v>82</v>
       </c>
@@ -5882,7 +5917,7 @@
       <c r="B54" s="16">
         <v>39</v>
       </c>
-      <c r="C54" s="126"/>
+      <c r="C54" s="188"/>
       <c r="D54" s="63" t="s">
         <v>84</v>
       </c>
@@ -5891,7 +5926,7 @@
       <c r="B55" s="16">
         <v>40</v>
       </c>
-      <c r="C55" s="127"/>
+      <c r="C55" s="189"/>
       <c r="D55" s="64" t="s">
         <v>83</v>
       </c>
@@ -5900,7 +5935,7 @@
       <c r="B56" s="16">
         <v>41</v>
       </c>
-      <c r="C56" s="118" t="s">
+      <c r="C56" s="182" t="s">
         <v>144</v>
       </c>
       <c r="D56" s="62" t="s">
@@ -5911,7 +5946,7 @@
       <c r="B57" s="16">
         <v>42</v>
       </c>
-      <c r="C57" s="119"/>
+      <c r="C57" s="183"/>
       <c r="D57" s="63" t="s">
         <v>82</v>
       </c>
@@ -5920,7 +5955,7 @@
       <c r="B58" s="16">
         <v>43</v>
       </c>
-      <c r="C58" s="119"/>
+      <c r="C58" s="183"/>
       <c r="D58" s="63" t="s">
         <v>84</v>
       </c>
@@ -5929,7 +5964,7 @@
       <c r="B59" s="16">
         <v>44</v>
       </c>
-      <c r="C59" s="119"/>
+      <c r="C59" s="183"/>
       <c r="D59" s="64" t="s">
         <v>83</v>
       </c>
@@ -5938,7 +5973,7 @@
       <c r="B60" s="16">
         <v>45</v>
       </c>
-      <c r="C60" s="118" t="s">
+      <c r="C60" s="182" t="s">
         <v>145</v>
       </c>
       <c r="D60" s="62" t="s">
@@ -5949,7 +5984,7 @@
       <c r="B61" s="16">
         <v>46</v>
       </c>
-      <c r="C61" s="119"/>
+      <c r="C61" s="183"/>
       <c r="D61" s="63" t="s">
         <v>82</v>
       </c>
@@ -5958,7 +5993,7 @@
       <c r="B62" s="16">
         <v>47</v>
       </c>
-      <c r="C62" s="119"/>
+      <c r="C62" s="183"/>
       <c r="D62" s="63" t="s">
         <v>84</v>
       </c>
@@ -5967,7 +6002,7 @@
       <c r="B63" s="16">
         <v>48</v>
       </c>
-      <c r="C63" s="119"/>
+      <c r="C63" s="183"/>
       <c r="D63" s="64" t="s">
         <v>83</v>
       </c>
@@ -5976,7 +6011,7 @@
       <c r="B64" s="16">
         <v>49</v>
       </c>
-      <c r="C64" s="118" t="s">
+      <c r="C64" s="182" t="s">
         <v>146</v>
       </c>
       <c r="D64" s="62" t="s">
@@ -5987,7 +6022,7 @@
       <c r="B65" s="16">
         <v>50</v>
       </c>
-      <c r="C65" s="119"/>
+      <c r="C65" s="183"/>
       <c r="D65" s="63" t="s">
         <v>82</v>
       </c>
@@ -5996,7 +6031,7 @@
       <c r="B66" s="16">
         <v>51</v>
       </c>
-      <c r="C66" s="119"/>
+      <c r="C66" s="183"/>
       <c r="D66" s="63" t="s">
         <v>84</v>
       </c>
@@ -6005,7 +6040,7 @@
       <c r="B67" s="16">
         <v>52</v>
       </c>
-      <c r="C67" s="119"/>
+      <c r="C67" s="183"/>
       <c r="D67" s="64" t="s">
         <v>83</v>
       </c>
@@ -6032,7 +6067,7 @@
       <c r="B70" s="16">
         <v>55</v>
       </c>
-      <c r="C70" s="129" t="s">
+      <c r="C70" s="174" t="s">
         <v>7</v>
       </c>
       <c r="D70" s="58" t="s">
@@ -6043,7 +6078,7 @@
       <c r="B71" s="16">
         <v>56</v>
       </c>
-      <c r="C71" s="130"/>
+      <c r="C71" s="175"/>
       <c r="D71" s="59" t="s">
         <v>82</v>
       </c>
@@ -6052,7 +6087,7 @@
       <c r="B72" s="16">
         <v>57</v>
       </c>
-      <c r="C72" s="130"/>
+      <c r="C72" s="175"/>
       <c r="D72" s="59" t="s">
         <v>84</v>
       </c>
@@ -6061,7 +6096,7 @@
       <c r="B73" s="16">
         <v>58</v>
       </c>
-      <c r="C73" s="131"/>
+      <c r="C73" s="176"/>
       <c r="D73" s="60" t="s">
         <v>83</v>
       </c>
@@ -6070,7 +6105,7 @@
       <c r="B74" s="16">
         <v>59</v>
       </c>
-      <c r="C74" s="123" t="s">
+      <c r="C74" s="177" t="s">
         <v>5</v>
       </c>
       <c r="D74" s="68"/>
@@ -6079,14 +6114,14 @@
       <c r="B75" s="16">
         <v>60</v>
       </c>
-      <c r="C75" s="124"/>
+      <c r="C75" s="178"/>
       <c r="D75" s="69"/>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B76" s="16">
         <v>61</v>
       </c>
-      <c r="C76" s="120" t="s">
+      <c r="C76" s="179" t="s">
         <v>6</v>
       </c>
       <c r="D76" s="65"/>
@@ -6095,14 +6130,14 @@
       <c r="B77" s="16">
         <v>62</v>
       </c>
-      <c r="C77" s="121"/>
+      <c r="C77" s="180"/>
       <c r="D77" s="66"/>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B78" s="16">
         <v>63</v>
       </c>
-      <c r="C78" s="122"/>
+      <c r="C78" s="181"/>
       <c r="D78" s="67"/>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.2">
@@ -6114,7 +6149,7 @@
       <c r="B83" s="70">
         <v>0</v>
       </c>
-      <c r="C83" s="132" t="s">
+      <c r="C83" s="184" t="s">
         <v>2</v>
       </c>
       <c r="D83" s="65"/>
@@ -6123,14 +6158,14 @@
       <c r="B84" s="70">
         <v>1</v>
       </c>
-      <c r="C84" s="133"/>
+      <c r="C84" s="185"/>
       <c r="D84" s="66"/>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B85" s="70">
         <v>2</v>
       </c>
-      <c r="C85" s="134"/>
+      <c r="C85" s="186"/>
       <c r="D85" s="67"/>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.2">
@@ -6159,7 +6194,7 @@
       <c r="B88" s="16">
         <v>5</v>
       </c>
-      <c r="C88" s="118" t="s">
+      <c r="C88" s="182" t="s">
         <v>147</v>
       </c>
       <c r="D88" s="62" t="s">
@@ -6170,7 +6205,7 @@
       <c r="B89" s="16">
         <v>6</v>
       </c>
-      <c r="C89" s="119"/>
+      <c r="C89" s="183"/>
       <c r="D89" s="63" t="s">
         <v>82</v>
       </c>
@@ -6179,7 +6214,7 @@
       <c r="B90" s="16">
         <v>7</v>
       </c>
-      <c r="C90" s="119"/>
+      <c r="C90" s="183"/>
       <c r="D90" s="63" t="s">
         <v>84</v>
       </c>
@@ -6188,7 +6223,7 @@
       <c r="B91" s="16">
         <v>8</v>
       </c>
-      <c r="C91" s="119"/>
+      <c r="C91" s="183"/>
       <c r="D91" s="64" t="s">
         <v>83</v>
       </c>
@@ -6197,7 +6232,7 @@
       <c r="B92" s="16">
         <v>9</v>
       </c>
-      <c r="C92" s="118" t="s">
+      <c r="C92" s="182" t="s">
         <v>148</v>
       </c>
       <c r="D92" s="62" t="s">
@@ -6208,7 +6243,7 @@
       <c r="B93" s="16">
         <v>10</v>
       </c>
-      <c r="C93" s="119"/>
+      <c r="C93" s="183"/>
       <c r="D93" s="63" t="s">
         <v>82</v>
       </c>
@@ -6217,7 +6252,7 @@
       <c r="B94" s="16">
         <v>11</v>
       </c>
-      <c r="C94" s="119"/>
+      <c r="C94" s="183"/>
       <c r="D94" s="63" t="s">
         <v>84</v>
       </c>
@@ -6226,7 +6261,7 @@
       <c r="B95" s="16">
         <v>12</v>
       </c>
-      <c r="C95" s="119"/>
+      <c r="C95" s="183"/>
       <c r="D95" s="64" t="s">
         <v>83</v>
       </c>
@@ -6235,7 +6270,7 @@
       <c r="B96" s="16">
         <v>13</v>
       </c>
-      <c r="C96" s="118" t="s">
+      <c r="C96" s="182" t="s">
         <v>149</v>
       </c>
       <c r="D96" s="62" t="s">
@@ -6246,7 +6281,7 @@
       <c r="B97" s="16">
         <v>14</v>
       </c>
-      <c r="C97" s="119"/>
+      <c r="C97" s="183"/>
       <c r="D97" s="63" t="s">
         <v>82</v>
       </c>
@@ -6255,7 +6290,7 @@
       <c r="B98" s="16">
         <v>15</v>
       </c>
-      <c r="C98" s="119"/>
+      <c r="C98" s="183"/>
       <c r="D98" s="63" t="s">
         <v>84</v>
       </c>
@@ -6264,7 +6299,7 @@
       <c r="B99" s="16">
         <v>16</v>
       </c>
-      <c r="C99" s="119"/>
+      <c r="C99" s="183"/>
       <c r="D99" s="64" t="s">
         <v>83</v>
       </c>
@@ -6273,7 +6308,7 @@
       <c r="B100" s="16">
         <v>17</v>
       </c>
-      <c r="C100" s="118" t="s">
+      <c r="C100" s="182" t="s">
         <v>150</v>
       </c>
       <c r="D100" s="62" t="s">
@@ -6284,7 +6319,7 @@
       <c r="B101" s="16">
         <v>18</v>
       </c>
-      <c r="C101" s="119"/>
+      <c r="C101" s="183"/>
       <c r="D101" s="63" t="s">
         <v>82</v>
       </c>
@@ -6293,7 +6328,7 @@
       <c r="B102" s="16">
         <v>19</v>
       </c>
-      <c r="C102" s="119"/>
+      <c r="C102" s="183"/>
       <c r="D102" s="63" t="s">
         <v>84</v>
       </c>
@@ -6302,7 +6337,7 @@
       <c r="B103" s="16">
         <v>20</v>
       </c>
-      <c r="C103" s="119"/>
+      <c r="C103" s="183"/>
       <c r="D103" s="64" t="s">
         <v>83</v>
       </c>
@@ -6553,7 +6588,7 @@
       <c r="B138" s="16">
         <v>55</v>
       </c>
-      <c r="C138" s="129" t="s">
+      <c r="C138" s="174" t="s">
         <v>7</v>
       </c>
       <c r="D138" s="58" t="s">
@@ -6564,7 +6599,7 @@
       <c r="B139" s="16">
         <v>56</v>
       </c>
-      <c r="C139" s="130"/>
+      <c r="C139" s="175"/>
       <c r="D139" s="59" t="s">
         <v>82</v>
       </c>
@@ -6573,7 +6608,7 @@
       <c r="B140" s="16">
         <v>57</v>
       </c>
-      <c r="C140" s="130"/>
+      <c r="C140" s="175"/>
       <c r="D140" s="59" t="s">
         <v>84</v>
       </c>
@@ -6582,7 +6617,7 @@
       <c r="B141" s="16">
         <v>58</v>
       </c>
-      <c r="C141" s="131"/>
+      <c r="C141" s="176"/>
       <c r="D141" s="60" t="s">
         <v>83</v>
       </c>
@@ -6591,7 +6626,7 @@
       <c r="B142" s="16">
         <v>59</v>
       </c>
-      <c r="C142" s="123" t="s">
+      <c r="C142" s="177" t="s">
         <v>5</v>
       </c>
       <c r="D142" s="68"/>
@@ -6600,14 +6635,14 @@
       <c r="B143" s="16">
         <v>60</v>
       </c>
-      <c r="C143" s="124"/>
+      <c r="C143" s="178"/>
       <c r="D143" s="69"/>
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B144" s="16">
         <v>61</v>
       </c>
-      <c r="C144" s="120" t="s">
+      <c r="C144" s="179" t="s">
         <v>6</v>
       </c>
       <c r="D144" s="65"/>
@@ -6616,23 +6651,18 @@
       <c r="B145" s="16">
         <v>62</v>
       </c>
-      <c r="C145" s="121"/>
+      <c r="C145" s="180"/>
       <c r="D145" s="66"/>
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B146" s="16">
         <v>63</v>
       </c>
-      <c r="C146" s="122"/>
+      <c r="C146" s="181"/>
       <c r="D146" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="G4:V4"/>
-    <mergeCell ref="C138:C141"/>
     <mergeCell ref="C142:C143"/>
     <mergeCell ref="C144:C146"/>
     <mergeCell ref="C56:C59"/>
@@ -6643,15 +6673,20 @@
     <mergeCell ref="C92:C95"/>
     <mergeCell ref="C96:C99"/>
     <mergeCell ref="C100:C103"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="C76:C78"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="G4:V4"/>
+    <mergeCell ref="C138:C141"/>
     <mergeCell ref="C15:C17"/>
-    <mergeCell ref="C70:C73"/>
     <mergeCell ref="C20:C23"/>
     <mergeCell ref="C24:C27"/>
     <mergeCell ref="C28:C31"/>
     <mergeCell ref="C32:C35"/>
     <mergeCell ref="C36:C39"/>
-    <mergeCell ref="C76:C78"/>
-    <mergeCell ref="C74:C75"/>
     <mergeCell ref="C40:C43"/>
     <mergeCell ref="C44:C47"/>
     <mergeCell ref="C48:C51"/>

</xml_diff>

<commit_message>
Added DELTA_TICKS_CONT_MODE in CONFIGURE_PIN command
</commit_message>
<xml_diff>
--- a/doc/DATA_PROTOCOL_SENSUS.xlsx
+++ b/doc/DATA_PROTOCOL_SENSUS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="23955" windowHeight="10800" tabRatio="655" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="23955" windowHeight="10800" tabRatio="804" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="GENERIC PACKET" sheetId="7" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="176">
   <si>
     <t>CMD</t>
   </si>
@@ -547,6 +547,15 @@
   </si>
   <si>
     <t>SLIDER_THRESHOLD</t>
+  </si>
+  <si>
+    <t>DELTA_TICK_CONT_MODE</t>
+  </si>
+  <si>
+    <t>DELTA_TICKS_CONT_MODE</t>
+  </si>
+  <si>
+    <t>(uint16_t)</t>
   </si>
 </sst>
 </file>
@@ -610,7 +619,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="26">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -758,6 +767,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -943,7 +958,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="207">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1259,58 +1274,79 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1409,8 +1445,35 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1421,35 +1484,8 @@
     <xf numFmtId="0" fontId="2" fillId="20" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1475,25 +1511,19 @@
     <xf numFmtId="0" fontId="2" fillId="19" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1884,350 +1914,350 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B2" s="123" t="s">
+      <c r="B2" s="142" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="124"/>
-      <c r="D2" s="124"/>
-      <c r="E2" s="124"/>
-      <c r="F2" s="125"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="143"/>
+      <c r="E2" s="143"/>
+      <c r="F2" s="144"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B4" s="126" t="s">
+      <c r="B4" s="131" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="126"/>
-      <c r="D4" s="135" t="s">
+      <c r="C4" s="131"/>
+      <c r="D4" s="130" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="135"/>
-      <c r="F4" s="135"/>
-      <c r="G4" s="135"/>
-      <c r="H4" s="135"/>
-      <c r="I4" s="135"/>
-      <c r="J4" s="135"/>
-      <c r="K4" s="135"/>
-      <c r="L4" s="135"/>
-      <c r="M4" s="135"/>
-      <c r="N4" s="135"/>
-      <c r="O4" s="135"/>
-      <c r="P4" s="135"/>
-      <c r="Q4" s="135"/>
-      <c r="R4" s="135"/>
-      <c r="S4" s="135"/>
-      <c r="T4" s="135"/>
-      <c r="U4" s="135"/>
-      <c r="V4" s="135"/>
-      <c r="W4" s="135"/>
-      <c r="X4" s="135"/>
+      <c r="E4" s="130"/>
+      <c r="F4" s="130"/>
+      <c r="G4" s="130"/>
+      <c r="H4" s="130"/>
+      <c r="I4" s="130"/>
+      <c r="J4" s="130"/>
+      <c r="K4" s="130"/>
+      <c r="L4" s="130"/>
+      <c r="M4" s="130"/>
+      <c r="N4" s="130"/>
+      <c r="O4" s="130"/>
+      <c r="P4" s="130"/>
+      <c r="Q4" s="130"/>
+      <c r="R4" s="130"/>
+      <c r="S4" s="130"/>
+      <c r="T4" s="130"/>
+      <c r="U4" s="130"/>
+      <c r="V4" s="130"/>
+      <c r="W4" s="130"/>
+      <c r="X4" s="130"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B5" s="134"/>
-      <c r="C5" s="134"/>
-      <c r="D5" s="135"/>
-      <c r="E5" s="135"/>
-      <c r="F5" s="135"/>
-      <c r="G5" s="135"/>
-      <c r="H5" s="135"/>
-      <c r="I5" s="135"/>
-      <c r="J5" s="135"/>
-      <c r="K5" s="135"/>
-      <c r="L5" s="135"/>
-      <c r="M5" s="135"/>
-      <c r="N5" s="135"/>
-      <c r="O5" s="135"/>
-      <c r="P5" s="135"/>
-      <c r="Q5" s="135"/>
-      <c r="R5" s="135"/>
-      <c r="S5" s="135"/>
-      <c r="T5" s="135"/>
-      <c r="U5" s="135"/>
-      <c r="V5" s="135"/>
-      <c r="W5" s="135"/>
-      <c r="X5" s="135"/>
+      <c r="B5" s="132"/>
+      <c r="C5" s="132"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="130"/>
+      <c r="F5" s="130"/>
+      <c r="G5" s="130"/>
+      <c r="H5" s="130"/>
+      <c r="I5" s="130"/>
+      <c r="J5" s="130"/>
+      <c r="K5" s="130"/>
+      <c r="L5" s="130"/>
+      <c r="M5" s="130"/>
+      <c r="N5" s="130"/>
+      <c r="O5" s="130"/>
+      <c r="P5" s="130"/>
+      <c r="Q5" s="130"/>
+      <c r="R5" s="130"/>
+      <c r="S5" s="130"/>
+      <c r="T5" s="130"/>
+      <c r="U5" s="130"/>
+      <c r="V5" s="130"/>
+      <c r="W5" s="130"/>
+      <c r="X5" s="130"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B6" s="137" t="s">
+      <c r="B6" s="133" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="137"/>
-      <c r="D6" s="135" t="s">
+      <c r="C6" s="133"/>
+      <c r="D6" s="130" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="135"/>
-      <c r="F6" s="135"/>
-      <c r="G6" s="135"/>
-      <c r="H6" s="135"/>
-      <c r="I6" s="135"/>
-      <c r="J6" s="135"/>
-      <c r="K6" s="135"/>
-      <c r="L6" s="135"/>
-      <c r="M6" s="135"/>
-      <c r="N6" s="135"/>
-      <c r="O6" s="135"/>
-      <c r="P6" s="135"/>
-      <c r="Q6" s="135"/>
-      <c r="R6" s="135"/>
-      <c r="S6" s="135"/>
-      <c r="T6" s="135"/>
-      <c r="U6" s="135"/>
-      <c r="V6" s="135"/>
-      <c r="W6" s="135"/>
-      <c r="X6" s="135"/>
+      <c r="E6" s="130"/>
+      <c r="F6" s="130"/>
+      <c r="G6" s="130"/>
+      <c r="H6" s="130"/>
+      <c r="I6" s="130"/>
+      <c r="J6" s="130"/>
+      <c r="K6" s="130"/>
+      <c r="L6" s="130"/>
+      <c r="M6" s="130"/>
+      <c r="N6" s="130"/>
+      <c r="O6" s="130"/>
+      <c r="P6" s="130"/>
+      <c r="Q6" s="130"/>
+      <c r="R6" s="130"/>
+      <c r="S6" s="130"/>
+      <c r="T6" s="130"/>
+      <c r="U6" s="130"/>
+      <c r="V6" s="130"/>
+      <c r="W6" s="130"/>
+      <c r="X6" s="130"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B7" s="138" t="s">
+      <c r="B7" s="134" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="138"/>
-      <c r="D7" s="135" t="s">
+      <c r="C7" s="134"/>
+      <c r="D7" s="130" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="135"/>
-      <c r="F7" s="135"/>
-      <c r="G7" s="135"/>
-      <c r="H7" s="135"/>
-      <c r="I7" s="135"/>
-      <c r="J7" s="135"/>
-      <c r="K7" s="135"/>
-      <c r="L7" s="135"/>
-      <c r="M7" s="135"/>
-      <c r="N7" s="135"/>
-      <c r="O7" s="135"/>
-      <c r="P7" s="135"/>
-      <c r="Q7" s="135"/>
-      <c r="R7" s="135"/>
-      <c r="S7" s="135"/>
-      <c r="T7" s="135"/>
-      <c r="U7" s="135"/>
-      <c r="V7" s="135"/>
-      <c r="W7" s="135"/>
-      <c r="X7" s="135"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="130"/>
+      <c r="G7" s="130"/>
+      <c r="H7" s="130"/>
+      <c r="I7" s="130"/>
+      <c r="J7" s="130"/>
+      <c r="K7" s="130"/>
+      <c r="L7" s="130"/>
+      <c r="M7" s="130"/>
+      <c r="N7" s="130"/>
+      <c r="O7" s="130"/>
+      <c r="P7" s="130"/>
+      <c r="Q7" s="130"/>
+      <c r="R7" s="130"/>
+      <c r="S7" s="130"/>
+      <c r="T7" s="130"/>
+      <c r="U7" s="130"/>
+      <c r="V7" s="130"/>
+      <c r="W7" s="130"/>
+      <c r="X7" s="130"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B8" s="129"/>
-      <c r="C8" s="130"/>
-      <c r="D8" s="131"/>
-      <c r="E8" s="132"/>
-      <c r="F8" s="132"/>
-      <c r="G8" s="132"/>
-      <c r="H8" s="132"/>
-      <c r="I8" s="132"/>
-      <c r="J8" s="132"/>
-      <c r="K8" s="132"/>
-      <c r="L8" s="132"/>
-      <c r="M8" s="132"/>
-      <c r="N8" s="132"/>
-      <c r="O8" s="132"/>
-      <c r="P8" s="132"/>
-      <c r="Q8" s="132"/>
-      <c r="R8" s="132"/>
-      <c r="S8" s="132"/>
-      <c r="T8" s="132"/>
-      <c r="U8" s="132"/>
-      <c r="V8" s="132"/>
-      <c r="W8" s="132"/>
-      <c r="X8" s="133"/>
+      <c r="B8" s="135"/>
+      <c r="C8" s="136"/>
+      <c r="D8" s="137"/>
+      <c r="E8" s="138"/>
+      <c r="F8" s="138"/>
+      <c r="G8" s="138"/>
+      <c r="H8" s="138"/>
+      <c r="I8" s="138"/>
+      <c r="J8" s="138"/>
+      <c r="K8" s="138"/>
+      <c r="L8" s="138"/>
+      <c r="M8" s="138"/>
+      <c r="N8" s="138"/>
+      <c r="O8" s="138"/>
+      <c r="P8" s="138"/>
+      <c r="Q8" s="138"/>
+      <c r="R8" s="138"/>
+      <c r="S8" s="138"/>
+      <c r="T8" s="138"/>
+      <c r="U8" s="138"/>
+      <c r="V8" s="138"/>
+      <c r="W8" s="138"/>
+      <c r="X8" s="139"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B9" s="139" t="s">
+      <c r="B9" s="140" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="140"/>
-      <c r="D9" s="131"/>
-      <c r="E9" s="132"/>
-      <c r="F9" s="132"/>
-      <c r="G9" s="132"/>
-      <c r="H9" s="132"/>
-      <c r="I9" s="132"/>
-      <c r="J9" s="132"/>
-      <c r="K9" s="132"/>
-      <c r="L9" s="132"/>
-      <c r="M9" s="132"/>
-      <c r="N9" s="132"/>
-      <c r="O9" s="132"/>
-      <c r="P9" s="132"/>
-      <c r="Q9" s="132"/>
-      <c r="R9" s="132"/>
-      <c r="S9" s="132"/>
-      <c r="T9" s="132"/>
-      <c r="U9" s="132"/>
-      <c r="V9" s="132"/>
-      <c r="W9" s="132"/>
-      <c r="X9" s="133"/>
+      <c r="C9" s="141"/>
+      <c r="D9" s="137"/>
+      <c r="E9" s="138"/>
+      <c r="F9" s="138"/>
+      <c r="G9" s="138"/>
+      <c r="H9" s="138"/>
+      <c r="I9" s="138"/>
+      <c r="J9" s="138"/>
+      <c r="K9" s="138"/>
+      <c r="L9" s="138"/>
+      <c r="M9" s="138"/>
+      <c r="N9" s="138"/>
+      <c r="O9" s="138"/>
+      <c r="P9" s="138"/>
+      <c r="Q9" s="138"/>
+      <c r="R9" s="138"/>
+      <c r="S9" s="138"/>
+      <c r="T9" s="138"/>
+      <c r="U9" s="138"/>
+      <c r="V9" s="138"/>
+      <c r="W9" s="138"/>
+      <c r="X9" s="139"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B10" s="129"/>
-      <c r="C10" s="130"/>
-      <c r="D10" s="131"/>
-      <c r="E10" s="132"/>
-      <c r="F10" s="132"/>
-      <c r="G10" s="132"/>
-      <c r="H10" s="132"/>
-      <c r="I10" s="132"/>
-      <c r="J10" s="132"/>
-      <c r="K10" s="132"/>
-      <c r="L10" s="132"/>
-      <c r="M10" s="132"/>
-      <c r="N10" s="132"/>
-      <c r="O10" s="132"/>
-      <c r="P10" s="132"/>
-      <c r="Q10" s="132"/>
-      <c r="R10" s="132"/>
-      <c r="S10" s="132"/>
-      <c r="T10" s="132"/>
-      <c r="U10" s="132"/>
-      <c r="V10" s="132"/>
-      <c r="W10" s="132"/>
-      <c r="X10" s="133"/>
+      <c r="B10" s="135"/>
+      <c r="C10" s="136"/>
+      <c r="D10" s="137"/>
+      <c r="E10" s="138"/>
+      <c r="F10" s="138"/>
+      <c r="G10" s="138"/>
+      <c r="H10" s="138"/>
+      <c r="I10" s="138"/>
+      <c r="J10" s="138"/>
+      <c r="K10" s="138"/>
+      <c r="L10" s="138"/>
+      <c r="M10" s="138"/>
+      <c r="N10" s="138"/>
+      <c r="O10" s="138"/>
+      <c r="P10" s="138"/>
+      <c r="Q10" s="138"/>
+      <c r="R10" s="138"/>
+      <c r="S10" s="138"/>
+      <c r="T10" s="138"/>
+      <c r="U10" s="138"/>
+      <c r="V10" s="138"/>
+      <c r="W10" s="138"/>
+      <c r="X10" s="139"/>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B11" s="136" t="s">
+      <c r="B11" s="147" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="136"/>
-      <c r="D11" s="135" t="s">
+      <c r="C11" s="147"/>
+      <c r="D11" s="130" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="135"/>
-      <c r="F11" s="135"/>
-      <c r="G11" s="135"/>
-      <c r="H11" s="135"/>
-      <c r="I11" s="135"/>
-      <c r="J11" s="135"/>
-      <c r="K11" s="135"/>
-      <c r="L11" s="135"/>
-      <c r="M11" s="135"/>
-      <c r="N11" s="135"/>
-      <c r="O11" s="135"/>
-      <c r="P11" s="135"/>
-      <c r="Q11" s="135"/>
-      <c r="R11" s="135"/>
-      <c r="S11" s="135"/>
-      <c r="T11" s="135"/>
-      <c r="U11" s="135"/>
-      <c r="V11" s="135"/>
-      <c r="W11" s="135"/>
-      <c r="X11" s="135"/>
+      <c r="E11" s="130"/>
+      <c r="F11" s="130"/>
+      <c r="G11" s="130"/>
+      <c r="H11" s="130"/>
+      <c r="I11" s="130"/>
+      <c r="J11" s="130"/>
+      <c r="K11" s="130"/>
+      <c r="L11" s="130"/>
+      <c r="M11" s="130"/>
+      <c r="N11" s="130"/>
+      <c r="O11" s="130"/>
+      <c r="P11" s="130"/>
+      <c r="Q11" s="130"/>
+      <c r="R11" s="130"/>
+      <c r="S11" s="130"/>
+      <c r="T11" s="130"/>
+      <c r="U11" s="130"/>
+      <c r="V11" s="130"/>
+      <c r="W11" s="130"/>
+      <c r="X11" s="130"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B12" s="128" t="s">
+      <c r="B12" s="146" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="128"/>
-      <c r="D12" s="135" t="s">
+      <c r="C12" s="146"/>
+      <c r="D12" s="130" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="135"/>
-      <c r="F12" s="135"/>
-      <c r="G12" s="135"/>
-      <c r="H12" s="135"/>
-      <c r="I12" s="135"/>
-      <c r="J12" s="135"/>
-      <c r="K12" s="135"/>
-      <c r="L12" s="135"/>
-      <c r="M12" s="135"/>
-      <c r="N12" s="135"/>
-      <c r="O12" s="135"/>
-      <c r="P12" s="135"/>
-      <c r="Q12" s="135"/>
-      <c r="R12" s="135"/>
-      <c r="S12" s="135"/>
-      <c r="T12" s="135"/>
-      <c r="U12" s="135"/>
-      <c r="V12" s="135"/>
-      <c r="W12" s="135"/>
-      <c r="X12" s="135"/>
+      <c r="E12" s="130"/>
+      <c r="F12" s="130"/>
+      <c r="G12" s="130"/>
+      <c r="H12" s="130"/>
+      <c r="I12" s="130"/>
+      <c r="J12" s="130"/>
+      <c r="K12" s="130"/>
+      <c r="L12" s="130"/>
+      <c r="M12" s="130"/>
+      <c r="N12" s="130"/>
+      <c r="O12" s="130"/>
+      <c r="P12" s="130"/>
+      <c r="Q12" s="130"/>
+      <c r="R12" s="130"/>
+      <c r="S12" s="130"/>
+      <c r="T12" s="130"/>
+      <c r="U12" s="130"/>
+      <c r="V12" s="130"/>
+      <c r="W12" s="130"/>
+      <c r="X12" s="130"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B13" s="127" t="s">
+      <c r="B13" s="145" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="127"/>
-      <c r="D13" s="135" t="s">
+      <c r="C13" s="145"/>
+      <c r="D13" s="130" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="135"/>
-      <c r="F13" s="135"/>
-      <c r="G13" s="135"/>
-      <c r="H13" s="135"/>
-      <c r="I13" s="135"/>
-      <c r="J13" s="135"/>
-      <c r="K13" s="135"/>
-      <c r="L13" s="135"/>
-      <c r="M13" s="135"/>
-      <c r="N13" s="135"/>
-      <c r="O13" s="135"/>
-      <c r="P13" s="135"/>
-      <c r="Q13" s="135"/>
-      <c r="R13" s="135"/>
-      <c r="S13" s="135"/>
-      <c r="T13" s="135"/>
-      <c r="U13" s="135"/>
-      <c r="V13" s="135"/>
-      <c r="W13" s="135"/>
-      <c r="X13" s="135"/>
+      <c r="E13" s="130"/>
+      <c r="F13" s="130"/>
+      <c r="G13" s="130"/>
+      <c r="H13" s="130"/>
+      <c r="I13" s="130"/>
+      <c r="J13" s="130"/>
+      <c r="K13" s="130"/>
+      <c r="L13" s="130"/>
+      <c r="M13" s="130"/>
+      <c r="N13" s="130"/>
+      <c r="O13" s="130"/>
+      <c r="P13" s="130"/>
+      <c r="Q13" s="130"/>
+      <c r="R13" s="130"/>
+      <c r="S13" s="130"/>
+      <c r="T13" s="130"/>
+      <c r="U13" s="130"/>
+      <c r="V13" s="130"/>
+      <c r="W13" s="130"/>
+      <c r="X13" s="130"/>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B14" s="134"/>
-      <c r="C14" s="134"/>
-      <c r="D14" s="135"/>
-      <c r="E14" s="135"/>
-      <c r="F14" s="135"/>
-      <c r="G14" s="135"/>
-      <c r="H14" s="135"/>
-      <c r="I14" s="135"/>
-      <c r="J14" s="135"/>
-      <c r="K14" s="135"/>
-      <c r="L14" s="135"/>
-      <c r="M14" s="135"/>
-      <c r="N14" s="135"/>
-      <c r="O14" s="135"/>
-      <c r="P14" s="135"/>
-      <c r="Q14" s="135"/>
-      <c r="R14" s="135"/>
-      <c r="S14" s="135"/>
-      <c r="T14" s="135"/>
-      <c r="U14" s="135"/>
-      <c r="V14" s="135"/>
-      <c r="W14" s="135"/>
-      <c r="X14" s="135"/>
+      <c r="B14" s="132"/>
+      <c r="C14" s="132"/>
+      <c r="D14" s="130"/>
+      <c r="E14" s="130"/>
+      <c r="F14" s="130"/>
+      <c r="G14" s="130"/>
+      <c r="H14" s="130"/>
+      <c r="I14" s="130"/>
+      <c r="J14" s="130"/>
+      <c r="K14" s="130"/>
+      <c r="L14" s="130"/>
+      <c r="M14" s="130"/>
+      <c r="N14" s="130"/>
+      <c r="O14" s="130"/>
+      <c r="P14" s="130"/>
+      <c r="Q14" s="130"/>
+      <c r="R14" s="130"/>
+      <c r="S14" s="130"/>
+      <c r="T14" s="130"/>
+      <c r="U14" s="130"/>
+      <c r="V14" s="130"/>
+      <c r="W14" s="130"/>
+      <c r="X14" s="130"/>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.2">
-      <c r="B15" s="126" t="s">
+      <c r="B15" s="131" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="126"/>
-      <c r="D15" s="135" t="s">
+      <c r="C15" s="131"/>
+      <c r="D15" s="130" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="135"/>
-      <c r="F15" s="135"/>
-      <c r="G15" s="135"/>
-      <c r="H15" s="135"/>
-      <c r="I15" s="135"/>
-      <c r="J15" s="135"/>
-      <c r="K15" s="135"/>
-      <c r="L15" s="135"/>
-      <c r="M15" s="135"/>
-      <c r="N15" s="135"/>
-      <c r="O15" s="135"/>
-      <c r="P15" s="135"/>
-      <c r="Q15" s="135"/>
-      <c r="R15" s="135"/>
-      <c r="S15" s="135"/>
-      <c r="T15" s="135"/>
-      <c r="U15" s="135"/>
-      <c r="V15" s="135"/>
-      <c r="W15" s="135"/>
-      <c r="X15" s="135"/>
+      <c r="E15" s="130"/>
+      <c r="F15" s="130"/>
+      <c r="G15" s="130"/>
+      <c r="H15" s="130"/>
+      <c r="I15" s="130"/>
+      <c r="J15" s="130"/>
+      <c r="K15" s="130"/>
+      <c r="L15" s="130"/>
+      <c r="M15" s="130"/>
+      <c r="N15" s="130"/>
+      <c r="O15" s="130"/>
+      <c r="P15" s="130"/>
+      <c r="Q15" s="130"/>
+      <c r="R15" s="130"/>
+      <c r="S15" s="130"/>
+      <c r="T15" s="130"/>
+      <c r="U15" s="130"/>
+      <c r="V15" s="130"/>
+      <c r="W15" s="130"/>
+      <c r="X15" s="130"/>
     </row>
     <row r="17" spans="3:67" x14ac:dyDescent="0.2">
-      <c r="D17" s="126" t="s">
+      <c r="D17" s="131" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="126"/>
-      <c r="F17" s="126"/>
+      <c r="E17" s="131"/>
+      <c r="F17" s="131"/>
       <c r="G17" s="88" t="s">
         <v>0</v>
       </c>
@@ -2286,21 +2316,21 @@
       <c r="BF17" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="BG17" s="128" t="s">
+      <c r="BG17" s="146" t="s">
         <v>7</v>
       </c>
-      <c r="BH17" s="128"/>
-      <c r="BI17" s="128"/>
-      <c r="BJ17" s="128"/>
-      <c r="BK17" s="127" t="s">
+      <c r="BH17" s="146"/>
+      <c r="BI17" s="146"/>
+      <c r="BJ17" s="146"/>
+      <c r="BK17" s="145" t="s">
         <v>5</v>
       </c>
-      <c r="BL17" s="127"/>
-      <c r="BM17" s="126" t="s">
+      <c r="BL17" s="145"/>
+      <c r="BM17" s="131" t="s">
         <v>6</v>
       </c>
-      <c r="BN17" s="126"/>
-      <c r="BO17" s="126"/>
+      <c r="BN17" s="131"/>
+      <c r="BO17" s="131"/>
     </row>
     <row r="18" spans="3:67" x14ac:dyDescent="0.2">
       <c r="C18" s="104" t="s">
@@ -2501,19 +2531,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="D13:X13"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:X4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:X5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:X6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:X7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:X8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:X9"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="BK17:BL17"/>
@@ -2530,6 +2547,19 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:X12"/>
     <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:X13"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:X4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:X5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:X6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:X7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:X8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:X9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2537,17 +2567,17 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L30"/>
+  <dimension ref="B2:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="6.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.140625" style="4"/>
     <col min="7" max="8" width="30.7109375" style="4" customWidth="1"/>
@@ -2556,11 +2586,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B2" s="129" t="s">
+      <c r="B2" s="135" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="130"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="136"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B5" s="16">
@@ -2598,11 +2628,14 @@
       <c r="B7" s="27">
         <v>5</v>
       </c>
-      <c r="C7" s="193" t="s">
+      <c r="C7" s="200" t="s">
         <v>78</v>
       </c>
       <c r="D7" s="29" t="s">
         <v>81</v>
+      </c>
+      <c r="E7" s="206" t="s">
+        <v>175</v>
       </c>
       <c r="G7" s="15" t="s">
         <v>102</v>
@@ -2616,7 +2649,7 @@
       <c r="B8" s="27">
         <v>6</v>
       </c>
-      <c r="C8" s="194"/>
+      <c r="C8" s="201"/>
       <c r="D8" s="30" t="s">
         <v>82</v>
       </c>
@@ -2675,11 +2708,14 @@
       <c r="B13" s="27">
         <v>5</v>
       </c>
-      <c r="C13" s="193" t="s">
+      <c r="C13" s="200" t="s">
         <v>78</v>
       </c>
       <c r="D13" s="29" t="s">
         <v>81</v>
+      </c>
+      <c r="E13" s="206" t="s">
+        <v>175</v>
       </c>
       <c r="G13" s="15" t="s">
         <v>95</v>
@@ -2695,7 +2731,7 @@
       <c r="B14" s="27">
         <v>6</v>
       </c>
-      <c r="C14" s="194"/>
+      <c r="C14" s="201"/>
       <c r="D14" s="30" t="s">
         <v>82</v>
       </c>
@@ -2731,208 +2767,263 @@
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="G16" s="15" t="s">
+      <c r="B16" s="27">
+        <v>8</v>
+      </c>
+      <c r="C16" s="202" t="s">
+        <v>174</v>
+      </c>
+      <c r="D16" s="203" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="206" t="s">
+        <v>175</v>
+      </c>
+      <c r="G16" s="15"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="10"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B17" s="27">
+        <v>9</v>
+      </c>
+      <c r="C17" s="204"/>
+      <c r="D17" s="205" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" s="15"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="10"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="G18" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="H16" s="38" t="s">
+      <c r="H18" s="38" t="s">
         <v>87</v>
       </c>
-      <c r="I16" s="10">
+      <c r="I18" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B18" s="16">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B20" s="16">
         <v>3</v>
       </c>
-      <c r="C18" s="88" t="s">
+      <c r="C20" s="88" t="s">
         <v>0</v>
       </c>
-      <c r="G18" s="90" t="s">
+      <c r="G20" s="90" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B19" s="16">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B21" s="16">
         <v>4</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C21" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D19" s="31" t="s">
+      <c r="D21" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="G19" s="190" t="s">
+      <c r="G21" s="197" t="s">
         <v>92</v>
       </c>
-      <c r="H19" s="191"/>
-      <c r="I19" s="192"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B20" s="27">
+      <c r="H21" s="198"/>
+      <c r="I21" s="199"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B22" s="16">
         <v>5</v>
       </c>
-      <c r="C20" s="193" t="s">
+      <c r="C22" s="200" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D22" s="29" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B21" s="27">
+      <c r="E22" s="206" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B23" s="16">
         <v>6</v>
       </c>
-      <c r="C21" s="194"/>
-      <c r="D21" s="30" t="s">
+      <c r="C23" s="201"/>
+      <c r="D23" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G23" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B22" s="27">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B24" s="16">
         <v>7</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C24" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="40"/>
-      <c r="G22" s="15" t="s">
+      <c r="D24" s="40"/>
+      <c r="G24" s="15" t="s">
         <v>99</v>
-      </c>
-      <c r="H22" s="17"/>
-      <c r="I22" s="9">
-        <v>0</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B23" s="27">
-        <v>8</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" s="54"/>
-      <c r="G23" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="H23" s="17"/>
-      <c r="I23" s="9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B24" s="27">
-        <v>9</v>
-      </c>
-      <c r="C24" s="195" t="s">
-        <v>80</v>
-      </c>
-      <c r="D24" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="G24" s="15" t="s">
-        <v>105</v>
       </c>
       <c r="H24" s="17"/>
       <c r="I24" s="9">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B25" s="27">
-        <v>10</v>
-      </c>
-      <c r="C25" s="196"/>
-      <c r="D25" s="56" t="s">
-        <v>82</v>
+      <c r="B25" s="16">
+        <v>8</v>
+      </c>
+      <c r="C25" s="202" t="s">
+        <v>173</v>
+      </c>
+      <c r="D25" s="203" t="s">
+        <v>81</v>
+      </c>
+      <c r="E25" s="206" t="s">
+        <v>175</v>
       </c>
       <c r="G25" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="H25" s="38"/>
-      <c r="I25" s="10">
-        <v>3</v>
+        <v>100</v>
+      </c>
+      <c r="H25" s="17"/>
+      <c r="I25" s="9">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B26" s="16">
-        <v>11</v>
-      </c>
-      <c r="C26" s="196"/>
-      <c r="D26" s="56" t="s">
-        <v>84</v>
+        <v>9</v>
+      </c>
+      <c r="C26" s="204"/>
+      <c r="D26" s="205" t="s">
+        <v>82</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="H26" s="17"/>
+      <c r="I26" s="9">
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B27" s="16">
-        <v>12</v>
-      </c>
-      <c r="C27" s="197"/>
-      <c r="D27" s="57" t="s">
-        <v>83</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>86</v>
+        <v>10</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" s="54"/>
+      <c r="G27" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="H27" s="38"/>
+      <c r="I27" s="10">
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B28" s="16">
-        <v>13</v>
-      </c>
-      <c r="C28" s="37" t="s">
-        <v>86</v>
-      </c>
-      <c r="D28" s="55"/>
-      <c r="G28" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="H28" s="15"/>
-      <c r="I28" s="9">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="C28" s="123" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" s="33" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B29" s="16">
-        <v>14</v>
-      </c>
-      <c r="C29" s="198" t="s">
-        <v>172</v>
-      </c>
-      <c r="D29" s="200" t="s">
-        <v>81</v>
-      </c>
-      <c r="G29" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="H29" s="15"/>
-      <c r="I29" s="9">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="C29" s="124"/>
+      <c r="D29" s="56" t="s">
+        <v>82</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B30" s="16">
+        <v>13</v>
+      </c>
+      <c r="C30" s="124"/>
+      <c r="D30" s="56" t="s">
+        <v>84</v>
+      </c>
+      <c r="G30" s="39" t="s">
+        <v>109</v>
+      </c>
+      <c r="H30" s="15"/>
+      <c r="I30" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B31" s="16">
+        <v>14</v>
+      </c>
+      <c r="C31" s="125"/>
+      <c r="D31" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="G31" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="H31" s="15"/>
+      <c r="I31" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B32" s="16">
         <v>15</v>
       </c>
-      <c r="C30" s="199"/>
-      <c r="D30" s="201" t="s">
+      <c r="C32" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" s="55"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="16">
+        <v>16</v>
+      </c>
+      <c r="C33" s="126" t="s">
+        <v>172</v>
+      </c>
+      <c r="D33" s="128" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="16">
+        <v>17</v>
+      </c>
+      <c r="C34" s="127"/>
+      <c r="D34" s="129" t="s">
         <v>82</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="C29:C30"/>
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G21:I21"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C24:C27"/>
-    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C25:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3453,11 +3544,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="141" t="s">
+      <c r="B2" s="148" t="s">
         <v>126</v>
       </c>
-      <c r="C2" s="141"/>
-      <c r="D2" s="141"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="16">
@@ -3542,111 +3633,111 @@
       <c r="B5" s="27">
         <v>5</v>
       </c>
-      <c r="C5" s="142" t="s">
+      <c r="C5" s="149" t="s">
         <v>123</v>
       </c>
       <c r="D5" s="107" t="s">
         <v>81</v>
       </c>
-      <c r="F5" s="154" t="s">
+      <c r="F5" s="161" t="s">
         <v>158</v>
       </c>
-      <c r="G5" s="155"/>
-      <c r="H5" s="156"/>
+      <c r="G5" s="162"/>
+      <c r="H5" s="163"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="27">
         <v>6</v>
       </c>
-      <c r="C6" s="143"/>
+      <c r="C6" s="150"/>
       <c r="D6" s="108" t="s">
         <v>82</v>
       </c>
-      <c r="F6" s="157" t="s">
+      <c r="F6" s="164" t="s">
         <v>161</v>
       </c>
-      <c r="G6" s="158"/>
-      <c r="H6" s="159"/>
+      <c r="G6" s="165"/>
+      <c r="H6" s="166"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="27">
         <v>7</v>
       </c>
-      <c r="C7" s="143"/>
+      <c r="C7" s="150"/>
       <c r="D7" s="108" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="157" t="s">
+      <c r="F7" s="164" t="s">
         <v>162</v>
       </c>
-      <c r="G7" s="158"/>
-      <c r="H7" s="159"/>
+      <c r="G7" s="165"/>
+      <c r="H7" s="166"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" s="27">
         <v>8</v>
       </c>
-      <c r="C8" s="144"/>
+      <c r="C8" s="151"/>
       <c r="D8" s="109" t="s">
         <v>83</v>
       </c>
-      <c r="F8" s="160" t="s">
+      <c r="F8" s="167" t="s">
         <v>163</v>
       </c>
-      <c r="G8" s="161"/>
-      <c r="H8" s="162"/>
+      <c r="G8" s="168"/>
+      <c r="H8" s="169"/>
     </row>
     <row r="9" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="27">
         <v>9</v>
       </c>
-      <c r="C9" s="151" t="s">
+      <c r="C9" s="158" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="110" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="145" t="s">
+      <c r="F9" s="152" t="s">
         <v>160</v>
       </c>
-      <c r="G9" s="146"/>
-      <c r="H9" s="147"/>
+      <c r="G9" s="153"/>
+      <c r="H9" s="154"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="27">
         <v>10</v>
       </c>
-      <c r="C10" s="152"/>
+      <c r="C10" s="159"/>
       <c r="D10" s="111" t="s">
         <v>82</v>
       </c>
-      <c r="F10" s="145"/>
-      <c r="G10" s="146"/>
-      <c r="H10" s="147"/>
+      <c r="F10" s="152"/>
+      <c r="G10" s="153"/>
+      <c r="H10" s="154"/>
     </row>
     <row r="11" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="27">
         <v>11</v>
       </c>
-      <c r="C11" s="152"/>
+      <c r="C11" s="159"/>
       <c r="D11" s="111" t="s">
         <v>84</v>
       </c>
-      <c r="F11" s="145"/>
-      <c r="G11" s="146"/>
-      <c r="H11" s="147"/>
+      <c r="F11" s="152"/>
+      <c r="G11" s="153"/>
+      <c r="H11" s="154"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" s="27">
         <v>12</v>
       </c>
-      <c r="C12" s="153"/>
+      <c r="C12" s="160"/>
       <c r="D12" s="112" t="s">
         <v>83</v>
       </c>
-      <c r="F12" s="145"/>
-      <c r="G12" s="146"/>
-      <c r="H12" s="147"/>
+      <c r="F12" s="152"/>
+      <c r="G12" s="153"/>
+      <c r="H12" s="154"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="27">
@@ -3656,9 +3747,9 @@
         <v>0</v>
       </c>
       <c r="D13" s="114"/>
-      <c r="F13" s="145"/>
-      <c r="G13" s="146"/>
-      <c r="H13" s="147"/>
+      <c r="F13" s="152"/>
+      <c r="G13" s="153"/>
+      <c r="H13" s="154"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="27">
@@ -3668,9 +3759,9 @@
         <v>20</v>
       </c>
       <c r="D14" s="116"/>
-      <c r="F14" s="148"/>
-      <c r="G14" s="149"/>
-      <c r="H14" s="150"/>
+      <c r="F14" s="155"/>
+      <c r="G14" s="156"/>
+      <c r="H14" s="157"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3706,10 +3797,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="129" t="s">
+      <c r="B3" s="135" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="130"/>
+      <c r="C3" s="136"/>
       <c r="D3" s="103"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
@@ -3906,17 +3997,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B2" s="129" t="s">
+      <c r="B2" s="135" t="s">
         <v>71</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="130"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="136"/>
     </row>
     <row r="5" spans="2:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="166" t="s">
+      <c r="B5" s="173" t="s">
         <v>152</v>
       </c>
-      <c r="C5" s="166"/>
+      <c r="C5" s="173"/>
       <c r="E5" s="102"/>
       <c r="F5" s="102"/>
     </row>
@@ -3930,10 +4021,10 @@
       <c r="D6" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="F6" s="165" t="s">
+      <c r="F6" s="172" t="s">
         <v>127</v>
       </c>
-      <c r="G6" s="165"/>
+      <c r="G6" s="172"/>
       <c r="H6" s="5"/>
       <c r="I6" s="76"/>
     </row>
@@ -4014,17 +4105,17 @@
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="164" t="s">
+      <c r="B13" s="171" t="s">
         <v>126</v>
       </c>
-      <c r="C13" s="164"/>
+      <c r="C13" s="171"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="167" t="s">
+      <c r="B14" s="174" t="s">
         <v>159</v>
       </c>
-      <c r="C14" s="168"/>
-      <c r="D14" s="169"/>
+      <c r="C14" s="175"/>
+      <c r="D14" s="176"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B16" s="16">
@@ -4173,17 +4264,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="129" t="s">
+      <c r="B2" s="135" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="130"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="136"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="166" t="s">
+      <c r="B5" s="173" t="s">
         <v>152</v>
       </c>
-      <c r="C5" s="166"/>
+      <c r="C5" s="173"/>
       <c r="E5" s="102"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
@@ -4270,10 +4361,10 @@
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="166" t="s">
+      <c r="B12" s="173" t="s">
         <v>152</v>
       </c>
-      <c r="C12" s="166"/>
+      <c r="C12" s="173"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="16">
@@ -4327,10 +4418,10 @@
       <c r="D17" s="119"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B19" s="166" t="s">
+      <c r="B19" s="173" t="s">
         <v>152</v>
       </c>
-      <c r="C19" s="166"/>
+      <c r="C19" s="173"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="16">
@@ -4378,7 +4469,7 @@
       <c r="B24" s="27">
         <v>7</v>
       </c>
-      <c r="C24" s="170" t="s">
+      <c r="C24" s="177" t="s">
         <v>129</v>
       </c>
       <c r="D24" s="52" t="s">
@@ -4389,16 +4480,16 @@
       <c r="B25" s="27">
         <v>8</v>
       </c>
-      <c r="C25" s="172"/>
+      <c r="C25" s="179"/>
       <c r="D25" s="53" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="166" t="s">
+      <c r="B27" s="173" t="s">
         <v>152</v>
       </c>
-      <c r="C27" s="166"/>
+      <c r="C27" s="173"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="16">
@@ -4446,7 +4537,7 @@
       <c r="B32" s="27">
         <v>7</v>
       </c>
-      <c r="C32" s="170" t="s">
+      <c r="C32" s="177" t="s">
         <v>129</v>
       </c>
       <c r="D32" s="52" t="s">
@@ -4457,7 +4548,7 @@
       <c r="B33" s="27">
         <v>8</v>
       </c>
-      <c r="C33" s="171"/>
+      <c r="C33" s="178"/>
       <c r="D33" s="121" t="s">
         <v>82</v>
       </c>
@@ -4466,7 +4557,7 @@
       <c r="B34" s="27">
         <v>9</v>
       </c>
-      <c r="C34" s="171"/>
+      <c r="C34" s="178"/>
       <c r="D34" s="121" t="s">
         <v>84</v>
       </c>
@@ -4475,7 +4566,7 @@
       <c r="B35" s="27">
         <v>10</v>
       </c>
-      <c r="C35" s="172"/>
+      <c r="C35" s="179"/>
       <c r="D35" s="53" t="s">
         <v>83</v>
       </c>
@@ -4486,11 +4577,11 @@
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="167" t="s">
+      <c r="B39" s="174" t="s">
         <v>159</v>
       </c>
-      <c r="C39" s="168"/>
-      <c r="D39" s="169"/>
+      <c r="C39" s="175"/>
+      <c r="D39" s="176"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -4528,11 +4619,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="129" t="s">
+      <c r="B2" s="135" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="163"/>
-      <c r="D2" s="130"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="136"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="61"/>
@@ -4540,10 +4631,10 @@
       <c r="D3" s="61"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="166" t="s">
+      <c r="B4" s="173" t="s">
         <v>152</v>
       </c>
-      <c r="C4" s="166"/>
+      <c r="C4" s="173"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="16">
@@ -4680,11 +4771,11 @@
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="167" t="s">
+      <c r="B14" s="174" t="s">
         <v>159</v>
       </c>
-      <c r="C14" s="168"/>
-      <c r="D14" s="169"/>
+      <c r="C14" s="175"/>
+      <c r="D14" s="176"/>
       <c r="F14" s="15" t="s">
         <v>56</v>
       </c>
@@ -4731,11 +4822,11 @@
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B19" s="129" t="s">
+      <c r="B19" s="135" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="163"/>
-      <c r="D19" s="130"/>
+      <c r="C19" s="170"/>
+      <c r="D19" s="136"/>
       <c r="F19" s="15" t="s">
         <v>40</v>
       </c>
@@ -4748,10 +4839,10 @@
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="166" t="s">
+      <c r="B21" s="173" t="s">
         <v>152</v>
       </c>
-      <c r="C21" s="166"/>
+      <c r="C21" s="173"/>
       <c r="F21" s="98" t="s">
         <v>63</v>
       </c>
@@ -4817,11 +4908,11 @@
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="167" t="s">
+      <c r="B26" s="174" t="s">
         <v>159</v>
       </c>
-      <c r="C26" s="168"/>
-      <c r="D26" s="169"/>
+      <c r="C26" s="175"/>
+      <c r="D26" s="176"/>
       <c r="F26" s="15" t="s">
         <v>46</v>
       </c>
@@ -4973,36 +5064,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B2" s="123" t="s">
+      <c r="B2" s="142" t="s">
         <v>138</v>
       </c>
-      <c r="C2" s="124"/>
-      <c r="D2" s="125"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="144"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B4" s="166" t="s">
+      <c r="B4" s="173" t="s">
         <v>152</v>
       </c>
-      <c r="C4" s="166"/>
+      <c r="C4" s="173"/>
       <c r="E4" s="75"/>
-      <c r="G4" s="173" t="s">
+      <c r="G4" s="193" t="s">
         <v>171</v>
       </c>
-      <c r="H4" s="173"/>
-      <c r="I4" s="173"/>
-      <c r="J4" s="173"/>
-      <c r="K4" s="173"/>
-      <c r="L4" s="173"/>
-      <c r="M4" s="173"/>
-      <c r="N4" s="173"/>
-      <c r="O4" s="173"/>
-      <c r="P4" s="173"/>
-      <c r="Q4" s="173"/>
-      <c r="R4" s="173"/>
-      <c r="S4" s="173"/>
-      <c r="T4" s="173"/>
-      <c r="U4" s="173"/>
-      <c r="V4" s="173"/>
+      <c r="H4" s="193"/>
+      <c r="I4" s="193"/>
+      <c r="J4" s="193"/>
+      <c r="K4" s="193"/>
+      <c r="L4" s="193"/>
+      <c r="M4" s="193"/>
+      <c r="N4" s="193"/>
+      <c r="O4" s="193"/>
+      <c r="P4" s="193"/>
+      <c r="Q4" s="193"/>
+      <c r="R4" s="193"/>
+      <c r="S4" s="193"/>
+      <c r="T4" s="193"/>
+      <c r="U4" s="193"/>
+      <c r="V4" s="193"/>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B5" s="16">
@@ -5304,11 +5395,11 @@
       <c r="V11" s="15"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B12" s="167" t="s">
+      <c r="B12" s="174" t="s">
         <v>159</v>
       </c>
-      <c r="C12" s="168"/>
-      <c r="D12" s="169"/>
+      <c r="C12" s="175"/>
+      <c r="D12" s="176"/>
       <c r="F12" s="50"/>
       <c r="G12" s="75"/>
       <c r="H12" s="75"/>
@@ -5356,7 +5447,7 @@
       <c r="B15" s="70">
         <v>0</v>
       </c>
-      <c r="C15" s="184" t="s">
+      <c r="C15" s="187" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="99"/>
@@ -5365,14 +5456,14 @@
       <c r="B16" s="70">
         <v>1</v>
       </c>
-      <c r="C16" s="185"/>
+      <c r="C16" s="188"/>
       <c r="D16" s="100"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B17" s="70">
         <v>2</v>
       </c>
-      <c r="C17" s="186"/>
+      <c r="C17" s="189"/>
       <c r="D17" s="101"/>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.2">
@@ -5401,7 +5492,7 @@
       <c r="B20" s="16">
         <v>5</v>
       </c>
-      <c r="C20" s="182" t="s">
+      <c r="C20" s="185" t="s">
         <v>131</v>
       </c>
       <c r="D20" s="62" t="s">
@@ -5412,7 +5503,7 @@
       <c r="B21" s="16">
         <v>6</v>
       </c>
-      <c r="C21" s="183"/>
+      <c r="C21" s="186"/>
       <c r="D21" s="63" t="s">
         <v>82</v>
       </c>
@@ -5421,7 +5512,7 @@
       <c r="B22" s="16">
         <v>7</v>
       </c>
-      <c r="C22" s="183"/>
+      <c r="C22" s="186"/>
       <c r="D22" s="63" t="s">
         <v>84</v>
       </c>
@@ -5430,7 +5521,7 @@
       <c r="B23" s="16">
         <v>8</v>
       </c>
-      <c r="C23" s="183"/>
+      <c r="C23" s="186"/>
       <c r="D23" s="64" t="s">
         <v>83</v>
       </c>
@@ -5439,7 +5530,7 @@
       <c r="B24" s="16">
         <v>9</v>
       </c>
-      <c r="C24" s="182" t="s">
+      <c r="C24" s="185" t="s">
         <v>132</v>
       </c>
       <c r="D24" s="62" t="s">
@@ -5450,7 +5541,7 @@
       <c r="B25" s="16">
         <v>10</v>
       </c>
-      <c r="C25" s="183"/>
+      <c r="C25" s="186"/>
       <c r="D25" s="63" t="s">
         <v>82</v>
       </c>
@@ -5476,7 +5567,7 @@
       <c r="B26" s="16">
         <v>11</v>
       </c>
-      <c r="C26" s="183"/>
+      <c r="C26" s="186"/>
       <c r="D26" s="63" t="s">
         <v>84</v>
       </c>
@@ -5485,7 +5576,7 @@
       <c r="B27" s="16">
         <v>12</v>
       </c>
-      <c r="C27" s="183"/>
+      <c r="C27" s="186"/>
       <c r="D27" s="64" t="s">
         <v>83</v>
       </c>
@@ -5494,7 +5585,7 @@
       <c r="B28" s="16">
         <v>13</v>
       </c>
-      <c r="C28" s="182" t="s">
+      <c r="C28" s="185" t="s">
         <v>133</v>
       </c>
       <c r="D28" s="62" t="s">
@@ -5505,7 +5596,7 @@
       <c r="B29" s="16">
         <v>14</v>
       </c>
-      <c r="C29" s="183"/>
+      <c r="C29" s="186"/>
       <c r="D29" s="63" t="s">
         <v>82</v>
       </c>
@@ -5514,7 +5605,7 @@
       <c r="B30" s="16">
         <v>15</v>
       </c>
-      <c r="C30" s="183"/>
+      <c r="C30" s="186"/>
       <c r="D30" s="63" t="s">
         <v>84</v>
       </c>
@@ -5523,7 +5614,7 @@
       <c r="B31" s="16">
         <v>16</v>
       </c>
-      <c r="C31" s="183"/>
+      <c r="C31" s="186"/>
       <c r="D31" s="64" t="s">
         <v>83</v>
       </c>
@@ -5532,7 +5623,7 @@
       <c r="B32" s="16">
         <v>17</v>
       </c>
-      <c r="C32" s="182" t="s">
+      <c r="C32" s="185" t="s">
         <v>134</v>
       </c>
       <c r="D32" s="62" t="s">
@@ -5543,7 +5634,7 @@
       <c r="B33" s="16">
         <v>18</v>
       </c>
-      <c r="C33" s="183"/>
+      <c r="C33" s="186"/>
       <c r="D33" s="63" t="s">
         <v>82</v>
       </c>
@@ -5552,7 +5643,7 @@
       <c r="B34" s="16">
         <v>19</v>
       </c>
-      <c r="C34" s="183"/>
+      <c r="C34" s="186"/>
       <c r="D34" s="63" t="s">
         <v>84</v>
       </c>
@@ -5578,7 +5669,7 @@
       <c r="B35" s="16">
         <v>20</v>
       </c>
-      <c r="C35" s="183"/>
+      <c r="C35" s="186"/>
       <c r="D35" s="64" t="s">
         <v>83</v>
       </c>
@@ -5604,7 +5695,7 @@
       <c r="B36" s="16">
         <v>21</v>
       </c>
-      <c r="C36" s="182" t="s">
+      <c r="C36" s="185" t="s">
         <v>139</v>
       </c>
       <c r="D36" s="62" t="s">
@@ -5632,7 +5723,7 @@
       <c r="B37" s="16">
         <v>22</v>
       </c>
-      <c r="C37" s="183"/>
+      <c r="C37" s="186"/>
       <c r="D37" s="63" t="s">
         <v>82</v>
       </c>
@@ -5658,7 +5749,7 @@
       <c r="B38" s="16">
         <v>23</v>
       </c>
-      <c r="C38" s="183"/>
+      <c r="C38" s="186"/>
       <c r="D38" s="63" t="s">
         <v>84</v>
       </c>
@@ -5680,7 +5771,7 @@
       <c r="B39" s="16">
         <v>24</v>
       </c>
-      <c r="C39" s="183"/>
+      <c r="C39" s="186"/>
       <c r="D39" s="64" t="s">
         <v>83</v>
       </c>
@@ -5702,7 +5793,7 @@
       <c r="B40" s="16">
         <v>25</v>
       </c>
-      <c r="C40" s="182" t="s">
+      <c r="C40" s="185" t="s">
         <v>140</v>
       </c>
       <c r="D40" s="62" t="s">
@@ -5726,7 +5817,7 @@
       <c r="B41" s="16">
         <v>26</v>
       </c>
-      <c r="C41" s="183"/>
+      <c r="C41" s="186"/>
       <c r="D41" s="63" t="s">
         <v>82</v>
       </c>
@@ -5752,7 +5843,7 @@
       <c r="B42" s="16">
         <v>27</v>
       </c>
-      <c r="C42" s="183"/>
+      <c r="C42" s="186"/>
       <c r="D42" s="63" t="s">
         <v>84</v>
       </c>
@@ -5778,7 +5869,7 @@
       <c r="B43" s="16">
         <v>28</v>
       </c>
-      <c r="C43" s="183"/>
+      <c r="C43" s="186"/>
       <c r="D43" s="64" t="s">
         <v>83</v>
       </c>
@@ -5804,7 +5895,7 @@
       <c r="B44" s="16">
         <v>29</v>
       </c>
-      <c r="C44" s="182" t="s">
+      <c r="C44" s="185" t="s">
         <v>141</v>
       </c>
       <c r="D44" s="62" t="s">
@@ -5832,7 +5923,7 @@
       <c r="B45" s="16">
         <v>30</v>
       </c>
-      <c r="C45" s="183"/>
+      <c r="C45" s="186"/>
       <c r="D45" s="63" t="s">
         <v>82</v>
       </c>
@@ -5841,7 +5932,7 @@
       <c r="B46" s="16">
         <v>31</v>
       </c>
-      <c r="C46" s="183"/>
+      <c r="C46" s="186"/>
       <c r="D46" s="63" t="s">
         <v>84</v>
       </c>
@@ -5850,7 +5941,7 @@
       <c r="B47" s="16">
         <v>32</v>
       </c>
-      <c r="C47" s="183"/>
+      <c r="C47" s="186"/>
       <c r="D47" s="64" t="s">
         <v>83</v>
       </c>
@@ -5859,7 +5950,7 @@
       <c r="B48" s="16">
         <v>33</v>
       </c>
-      <c r="C48" s="182" t="s">
+      <c r="C48" s="185" t="s">
         <v>142</v>
       </c>
       <c r="D48" s="62" t="s">
@@ -5870,7 +5961,7 @@
       <c r="B49" s="16">
         <v>34</v>
       </c>
-      <c r="C49" s="183"/>
+      <c r="C49" s="186"/>
       <c r="D49" s="63" t="s">
         <v>82</v>
       </c>
@@ -5879,7 +5970,7 @@
       <c r="B50" s="16">
         <v>35</v>
       </c>
-      <c r="C50" s="183"/>
+      <c r="C50" s="186"/>
       <c r="D50" s="63" t="s">
         <v>84</v>
       </c>
@@ -5888,7 +5979,7 @@
       <c r="B51" s="16">
         <v>36</v>
       </c>
-      <c r="C51" s="183"/>
+      <c r="C51" s="186"/>
       <c r="D51" s="64" t="s">
         <v>83</v>
       </c>
@@ -5897,7 +5988,7 @@
       <c r="B52" s="16">
         <v>37</v>
       </c>
-      <c r="C52" s="187" t="s">
+      <c r="C52" s="194" t="s">
         <v>143</v>
       </c>
       <c r="D52" s="62" t="s">
@@ -5908,7 +5999,7 @@
       <c r="B53" s="16">
         <v>38</v>
       </c>
-      <c r="C53" s="188"/>
+      <c r="C53" s="195"/>
       <c r="D53" s="63" t="s">
         <v>82</v>
       </c>
@@ -5917,7 +6008,7 @@
       <c r="B54" s="16">
         <v>39</v>
       </c>
-      <c r="C54" s="188"/>
+      <c r="C54" s="195"/>
       <c r="D54" s="63" t="s">
         <v>84</v>
       </c>
@@ -5926,7 +6017,7 @@
       <c r="B55" s="16">
         <v>40</v>
       </c>
-      <c r="C55" s="189"/>
+      <c r="C55" s="196"/>
       <c r="D55" s="64" t="s">
         <v>83</v>
       </c>
@@ -5935,7 +6026,7 @@
       <c r="B56" s="16">
         <v>41</v>
       </c>
-      <c r="C56" s="182" t="s">
+      <c r="C56" s="185" t="s">
         <v>144</v>
       </c>
       <c r="D56" s="62" t="s">
@@ -5946,7 +6037,7 @@
       <c r="B57" s="16">
         <v>42</v>
       </c>
-      <c r="C57" s="183"/>
+      <c r="C57" s="186"/>
       <c r="D57" s="63" t="s">
         <v>82</v>
       </c>
@@ -5955,7 +6046,7 @@
       <c r="B58" s="16">
         <v>43</v>
       </c>
-      <c r="C58" s="183"/>
+      <c r="C58" s="186"/>
       <c r="D58" s="63" t="s">
         <v>84</v>
       </c>
@@ -5964,7 +6055,7 @@
       <c r="B59" s="16">
         <v>44</v>
       </c>
-      <c r="C59" s="183"/>
+      <c r="C59" s="186"/>
       <c r="D59" s="64" t="s">
         <v>83</v>
       </c>
@@ -5973,7 +6064,7 @@
       <c r="B60" s="16">
         <v>45</v>
       </c>
-      <c r="C60" s="182" t="s">
+      <c r="C60" s="185" t="s">
         <v>145</v>
       </c>
       <c r="D60" s="62" t="s">
@@ -5984,7 +6075,7 @@
       <c r="B61" s="16">
         <v>46</v>
       </c>
-      <c r="C61" s="183"/>
+      <c r="C61" s="186"/>
       <c r="D61" s="63" t="s">
         <v>82</v>
       </c>
@@ -5993,7 +6084,7 @@
       <c r="B62" s="16">
         <v>47</v>
       </c>
-      <c r="C62" s="183"/>
+      <c r="C62" s="186"/>
       <c r="D62" s="63" t="s">
         <v>84</v>
       </c>
@@ -6002,7 +6093,7 @@
       <c r="B63" s="16">
         <v>48</v>
       </c>
-      <c r="C63" s="183"/>
+      <c r="C63" s="186"/>
       <c r="D63" s="64" t="s">
         <v>83</v>
       </c>
@@ -6011,7 +6102,7 @@
       <c r="B64" s="16">
         <v>49</v>
       </c>
-      <c r="C64" s="182" t="s">
+      <c r="C64" s="185" t="s">
         <v>146</v>
       </c>
       <c r="D64" s="62" t="s">
@@ -6022,7 +6113,7 @@
       <c r="B65" s="16">
         <v>50</v>
       </c>
-      <c r="C65" s="183"/>
+      <c r="C65" s="186"/>
       <c r="D65" s="63" t="s">
         <v>82</v>
       </c>
@@ -6031,7 +6122,7 @@
       <c r="B66" s="16">
         <v>51</v>
       </c>
-      <c r="C66" s="183"/>
+      <c r="C66" s="186"/>
       <c r="D66" s="63" t="s">
         <v>84</v>
       </c>
@@ -6040,7 +6131,7 @@
       <c r="B67" s="16">
         <v>52</v>
       </c>
-      <c r="C67" s="183"/>
+      <c r="C67" s="186"/>
       <c r="D67" s="64" t="s">
         <v>83</v>
       </c>
@@ -6067,7 +6158,7 @@
       <c r="B70" s="16">
         <v>55</v>
       </c>
-      <c r="C70" s="174" t="s">
+      <c r="C70" s="190" t="s">
         <v>7</v>
       </c>
       <c r="D70" s="58" t="s">
@@ -6078,7 +6169,7 @@
       <c r="B71" s="16">
         <v>56</v>
       </c>
-      <c r="C71" s="175"/>
+      <c r="C71" s="191"/>
       <c r="D71" s="59" t="s">
         <v>82</v>
       </c>
@@ -6087,7 +6178,7 @@
       <c r="B72" s="16">
         <v>57</v>
       </c>
-      <c r="C72" s="175"/>
+      <c r="C72" s="191"/>
       <c r="D72" s="59" t="s">
         <v>84</v>
       </c>
@@ -6096,7 +6187,7 @@
       <c r="B73" s="16">
         <v>58</v>
       </c>
-      <c r="C73" s="176"/>
+      <c r="C73" s="192"/>
       <c r="D73" s="60" t="s">
         <v>83</v>
       </c>
@@ -6105,7 +6196,7 @@
       <c r="B74" s="16">
         <v>59</v>
       </c>
-      <c r="C74" s="177" t="s">
+      <c r="C74" s="180" t="s">
         <v>5</v>
       </c>
       <c r="D74" s="68"/>
@@ -6114,14 +6205,14 @@
       <c r="B75" s="16">
         <v>60</v>
       </c>
-      <c r="C75" s="178"/>
+      <c r="C75" s="181"/>
       <c r="D75" s="69"/>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B76" s="16">
         <v>61</v>
       </c>
-      <c r="C76" s="179" t="s">
+      <c r="C76" s="182" t="s">
         <v>6</v>
       </c>
       <c r="D76" s="65"/>
@@ -6130,14 +6221,14 @@
       <c r="B77" s="16">
         <v>62</v>
       </c>
-      <c r="C77" s="180"/>
+      <c r="C77" s="183"/>
       <c r="D77" s="66"/>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B78" s="16">
         <v>63</v>
       </c>
-      <c r="C78" s="181"/>
+      <c r="C78" s="184"/>
       <c r="D78" s="67"/>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.2">
@@ -6149,7 +6240,7 @@
       <c r="B83" s="70">
         <v>0</v>
       </c>
-      <c r="C83" s="184" t="s">
+      <c r="C83" s="187" t="s">
         <v>2</v>
       </c>
       <c r="D83" s="65"/>
@@ -6158,14 +6249,14 @@
       <c r="B84" s="70">
         <v>1</v>
       </c>
-      <c r="C84" s="185"/>
+      <c r="C84" s="188"/>
       <c r="D84" s="66"/>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B85" s="70">
         <v>2</v>
       </c>
-      <c r="C85" s="186"/>
+      <c r="C85" s="189"/>
       <c r="D85" s="67"/>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.2">
@@ -6194,7 +6285,7 @@
       <c r="B88" s="16">
         <v>5</v>
       </c>
-      <c r="C88" s="182" t="s">
+      <c r="C88" s="185" t="s">
         <v>147</v>
       </c>
       <c r="D88" s="62" t="s">
@@ -6205,7 +6296,7 @@
       <c r="B89" s="16">
         <v>6</v>
       </c>
-      <c r="C89" s="183"/>
+      <c r="C89" s="186"/>
       <c r="D89" s="63" t="s">
         <v>82</v>
       </c>
@@ -6214,7 +6305,7 @@
       <c r="B90" s="16">
         <v>7</v>
       </c>
-      <c r="C90" s="183"/>
+      <c r="C90" s="186"/>
       <c r="D90" s="63" t="s">
         <v>84</v>
       </c>
@@ -6223,7 +6314,7 @@
       <c r="B91" s="16">
         <v>8</v>
       </c>
-      <c r="C91" s="183"/>
+      <c r="C91" s="186"/>
       <c r="D91" s="64" t="s">
         <v>83</v>
       </c>
@@ -6232,7 +6323,7 @@
       <c r="B92" s="16">
         <v>9</v>
       </c>
-      <c r="C92" s="182" t="s">
+      <c r="C92" s="185" t="s">
         <v>148</v>
       </c>
       <c r="D92" s="62" t="s">
@@ -6243,7 +6334,7 @@
       <c r="B93" s="16">
         <v>10</v>
       </c>
-      <c r="C93" s="183"/>
+      <c r="C93" s="186"/>
       <c r="D93" s="63" t="s">
         <v>82</v>
       </c>
@@ -6252,7 +6343,7 @@
       <c r="B94" s="16">
         <v>11</v>
       </c>
-      <c r="C94" s="183"/>
+      <c r="C94" s="186"/>
       <c r="D94" s="63" t="s">
         <v>84</v>
       </c>
@@ -6261,7 +6352,7 @@
       <c r="B95" s="16">
         <v>12</v>
       </c>
-      <c r="C95" s="183"/>
+      <c r="C95" s="186"/>
       <c r="D95" s="64" t="s">
         <v>83</v>
       </c>
@@ -6270,7 +6361,7 @@
       <c r="B96" s="16">
         <v>13</v>
       </c>
-      <c r="C96" s="182" t="s">
+      <c r="C96" s="185" t="s">
         <v>149</v>
       </c>
       <c r="D96" s="62" t="s">
@@ -6281,7 +6372,7 @@
       <c r="B97" s="16">
         <v>14</v>
       </c>
-      <c r="C97" s="183"/>
+      <c r="C97" s="186"/>
       <c r="D97" s="63" t="s">
         <v>82</v>
       </c>
@@ -6290,7 +6381,7 @@
       <c r="B98" s="16">
         <v>15</v>
       </c>
-      <c r="C98" s="183"/>
+      <c r="C98" s="186"/>
       <c r="D98" s="63" t="s">
         <v>84</v>
       </c>
@@ -6299,7 +6390,7 @@
       <c r="B99" s="16">
         <v>16</v>
       </c>
-      <c r="C99" s="183"/>
+      <c r="C99" s="186"/>
       <c r="D99" s="64" t="s">
         <v>83</v>
       </c>
@@ -6308,7 +6399,7 @@
       <c r="B100" s="16">
         <v>17</v>
       </c>
-      <c r="C100" s="182" t="s">
+      <c r="C100" s="185" t="s">
         <v>150</v>
       </c>
       <c r="D100" s="62" t="s">
@@ -6319,7 +6410,7 @@
       <c r="B101" s="16">
         <v>18</v>
       </c>
-      <c r="C101" s="183"/>
+      <c r="C101" s="186"/>
       <c r="D101" s="63" t="s">
         <v>82</v>
       </c>
@@ -6328,7 +6419,7 @@
       <c r="B102" s="16">
         <v>19</v>
       </c>
-      <c r="C102" s="183"/>
+      <c r="C102" s="186"/>
       <c r="D102" s="63" t="s">
         <v>84</v>
       </c>
@@ -6337,7 +6428,7 @@
       <c r="B103" s="16">
         <v>20</v>
       </c>
-      <c r="C103" s="183"/>
+      <c r="C103" s="186"/>
       <c r="D103" s="64" t="s">
         <v>83</v>
       </c>
@@ -6588,7 +6679,7 @@
       <c r="B138" s="16">
         <v>55</v>
       </c>
-      <c r="C138" s="174" t="s">
+      <c r="C138" s="190" t="s">
         <v>7</v>
       </c>
       <c r="D138" s="58" t="s">
@@ -6599,7 +6690,7 @@
       <c r="B139" s="16">
         <v>56</v>
       </c>
-      <c r="C139" s="175"/>
+      <c r="C139" s="191"/>
       <c r="D139" s="59" t="s">
         <v>82</v>
       </c>
@@ -6608,7 +6699,7 @@
       <c r="B140" s="16">
         <v>57</v>
       </c>
-      <c r="C140" s="175"/>
+      <c r="C140" s="191"/>
       <c r="D140" s="59" t="s">
         <v>84</v>
       </c>
@@ -6617,7 +6708,7 @@
       <c r="B141" s="16">
         <v>58</v>
       </c>
-      <c r="C141" s="176"/>
+      <c r="C141" s="192"/>
       <c r="D141" s="60" t="s">
         <v>83</v>
       </c>
@@ -6626,7 +6717,7 @@
       <c r="B142" s="16">
         <v>59</v>
       </c>
-      <c r="C142" s="177" t="s">
+      <c r="C142" s="180" t="s">
         <v>5</v>
       </c>
       <c r="D142" s="68"/>
@@ -6635,14 +6726,14 @@
       <c r="B143" s="16">
         <v>60</v>
       </c>
-      <c r="C143" s="178"/>
+      <c r="C143" s="181"/>
       <c r="D143" s="69"/>
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B144" s="16">
         <v>61</v>
       </c>
-      <c r="C144" s="179" t="s">
+      <c r="C144" s="182" t="s">
         <v>6</v>
       </c>
       <c r="D144" s="65"/>
@@ -6651,31 +6742,18 @@
       <c r="B145" s="16">
         <v>62</v>
       </c>
-      <c r="C145" s="180"/>
+      <c r="C145" s="183"/>
       <c r="D145" s="66"/>
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B146" s="16">
         <v>63</v>
       </c>
-      <c r="C146" s="181"/>
+      <c r="C146" s="184"/>
       <c r="D146" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C142:C143"/>
-    <mergeCell ref="C144:C146"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="C60:C63"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="C83:C85"/>
-    <mergeCell ref="C88:C91"/>
-    <mergeCell ref="C92:C95"/>
-    <mergeCell ref="C96:C99"/>
-    <mergeCell ref="C100:C103"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="C76:C78"/>
-    <mergeCell ref="C74:C75"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B4:C4"/>
@@ -6691,6 +6769,19 @@
     <mergeCell ref="C44:C47"/>
     <mergeCell ref="C48:C51"/>
     <mergeCell ref="C52:C55"/>
+    <mergeCell ref="C142:C143"/>
+    <mergeCell ref="C144:C146"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="C60:C63"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="C88:C91"/>
+    <mergeCell ref="C92:C95"/>
+    <mergeCell ref="C96:C99"/>
+    <mergeCell ref="C100:C103"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="C76:C78"/>
+    <mergeCell ref="C74:C75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated CONFIGURE_PIN and GET_VALUE commands
</commit_message>
<xml_diff>
--- a/doc/DATA_PROTOCOL_SENSUS.xlsx
+++ b/doc/DATA_PROTOCOL_SENSUS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19840" tabRatio="804" activeTab="6"/>
+    <workbookView xWindow="1320" yWindow="460" windowWidth="28800" windowHeight="16840" tabRatio="804"/>
   </bookViews>
   <sheets>
     <sheet name="LIST_CMD" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="187">
   <si>
     <t>CMD</t>
   </si>
@@ -596,6 +596,9 @@
   </si>
   <si>
     <t>TICKS_DELAY_RT_TASK</t>
+  </si>
+  <si>
+    <t>CMD_VALUE</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1007,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="223">
+  <cellXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1344,12 +1347,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1407,6 +1404,9 @@
     <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1545,7 +1545,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1619,6 +1619,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1989,8 +1998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -2143,14 +2152,14 @@
       <c r="D14" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="E14" s="140"/>
+      <c r="E14" s="138"/>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B15" s="140"/>
-      <c r="C15" s="140"/>
-      <c r="D15" s="140"/>
-      <c r="E15" s="140"/>
+      <c r="B15" s="138"/>
+      <c r="C15" s="138"/>
+      <c r="D15" s="138"/>
+      <c r="E15" s="138"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.15">
@@ -2457,17 +2466,17 @@
       <c r="F42" s="2"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B43" s="133">
+      <c r="B43" s="131">
         <v>250</v>
       </c>
-      <c r="C43" s="133">
+      <c r="C43" s="131">
         <v>0</v>
       </c>
-      <c r="D43" s="133" t="s">
+      <c r="D43" s="131" t="s">
         <v>172</v>
       </c>
-      <c r="E43" s="133"/>
-      <c r="F43" s="134"/>
+      <c r="E43" s="131"/>
+      <c r="F43" s="132"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B44" s="83"/>
@@ -2477,9 +2486,13 @@
       <c r="F44" s="2"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B45" s="83"/>
+      <c r="B45" s="83">
+        <v>254</v>
+      </c>
       <c r="C45" s="83"/>
-      <c r="D45" s="83"/>
+      <c r="D45" s="83" t="s">
+        <v>186</v>
+      </c>
       <c r="E45" s="83"/>
       <c r="F45" s="3"/>
     </row>
@@ -2521,11 +2534,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B2" s="152" t="s">
+      <c r="B2" s="151" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="154"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="153"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B3" s="58"/>
@@ -2533,10 +2546,10 @@
       <c r="D3" s="58"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B4" s="155" t="s">
+      <c r="B4" s="154" t="s">
         <v>147</v>
       </c>
-      <c r="C4" s="155"/>
+      <c r="C4" s="154"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B5" s="15">
@@ -2673,11 +2686,11 @@
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B14" s="156" t="s">
+      <c r="B14" s="155" t="s">
         <v>154</v>
       </c>
-      <c r="C14" s="157"/>
-      <c r="D14" s="158"/>
+      <c r="C14" s="156"/>
+      <c r="D14" s="157"/>
       <c r="F14" s="14" t="s">
         <v>55</v>
       </c>
@@ -2724,11 +2737,11 @@
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B19" s="152" t="s">
+      <c r="B19" s="151" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="153"/>
-      <c r="D19" s="154"/>
+      <c r="C19" s="152"/>
+      <c r="D19" s="153"/>
       <c r="F19" s="14" t="s">
         <v>39</v>
       </c>
@@ -2741,10 +2754,10 @@
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B21" s="155" t="s">
+      <c r="B21" s="154" t="s">
         <v>147</v>
       </c>
-      <c r="C21" s="155"/>
+      <c r="C21" s="154"/>
       <c r="F21" s="90" t="s">
         <v>62</v>
       </c>
@@ -2810,11 +2823,11 @@
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B26" s="156" t="s">
+      <c r="B26" s="155" t="s">
         <v>154</v>
       </c>
-      <c r="C26" s="157"/>
-      <c r="D26" s="158"/>
+      <c r="C26" s="156"/>
+      <c r="D26" s="157"/>
       <c r="F26" s="14" t="s">
         <v>45</v>
       </c>
@@ -2966,36 +2979,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.15">
-      <c r="B2" s="159" t="s">
+      <c r="B2" s="158" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="160"/>
-      <c r="D2" s="161"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="160"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.15">
-      <c r="B4" s="155" t="s">
+      <c r="B4" s="154" t="s">
         <v>147</v>
       </c>
-      <c r="C4" s="155"/>
+      <c r="C4" s="154"/>
       <c r="E4" s="72"/>
-      <c r="G4" s="199" t="s">
+      <c r="G4" s="198" t="s">
         <v>162</v>
       </c>
-      <c r="H4" s="199"/>
-      <c r="I4" s="199"/>
-      <c r="J4" s="199"/>
-      <c r="K4" s="199"/>
-      <c r="L4" s="199"/>
-      <c r="M4" s="199"/>
-      <c r="N4" s="199"/>
-      <c r="O4" s="199"/>
-      <c r="P4" s="199"/>
-      <c r="Q4" s="199"/>
-      <c r="R4" s="199"/>
-      <c r="S4" s="199"/>
-      <c r="T4" s="199"/>
-      <c r="U4" s="199"/>
-      <c r="V4" s="199"/>
+      <c r="H4" s="198"/>
+      <c r="I4" s="198"/>
+      <c r="J4" s="198"/>
+      <c r="K4" s="198"/>
+      <c r="L4" s="198"/>
+      <c r="M4" s="198"/>
+      <c r="N4" s="198"/>
+      <c r="O4" s="198"/>
+      <c r="P4" s="198"/>
+      <c r="Q4" s="198"/>
+      <c r="R4" s="198"/>
+      <c r="S4" s="198"/>
+      <c r="T4" s="198"/>
+      <c r="U4" s="198"/>
+      <c r="V4" s="198"/>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B5" s="15">
@@ -3297,11 +3310,11 @@
       <c r="V11" s="14"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.15">
-      <c r="B12" s="156" t="s">
+      <c r="B12" s="155" t="s">
         <v>154</v>
       </c>
-      <c r="C12" s="157"/>
-      <c r="D12" s="158"/>
+      <c r="C12" s="156"/>
+      <c r="D12" s="157"/>
       <c r="F12" s="49"/>
       <c r="G12" s="72"/>
       <c r="H12" s="72"/>
@@ -3349,7 +3362,7 @@
       <c r="B15" s="67">
         <v>0</v>
       </c>
-      <c r="C15" s="203" t="s">
+      <c r="C15" s="202" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="91"/>
@@ -3358,14 +3371,14 @@
       <c r="B16" s="67">
         <v>1</v>
       </c>
-      <c r="C16" s="204"/>
+      <c r="C16" s="203"/>
       <c r="D16" s="92"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B17" s="67">
         <v>2</v>
       </c>
-      <c r="C17" s="205"/>
+      <c r="C17" s="204"/>
       <c r="D17" s="93"/>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.15">
@@ -3394,7 +3407,7 @@
       <c r="B20" s="15">
         <v>5</v>
       </c>
-      <c r="C20" s="206" t="s">
+      <c r="C20" s="205" t="s">
         <v>126</v>
       </c>
       <c r="D20" s="59" t="s">
@@ -3405,7 +3418,7 @@
       <c r="B21" s="15">
         <v>6</v>
       </c>
-      <c r="C21" s="207"/>
+      <c r="C21" s="206"/>
       <c r="D21" s="60" t="s">
         <v>80</v>
       </c>
@@ -3414,7 +3427,7 @@
       <c r="B22" s="15">
         <v>7</v>
       </c>
-      <c r="C22" s="207"/>
+      <c r="C22" s="206"/>
       <c r="D22" s="60" t="s">
         <v>82</v>
       </c>
@@ -3423,7 +3436,7 @@
       <c r="B23" s="15">
         <v>8</v>
       </c>
-      <c r="C23" s="207"/>
+      <c r="C23" s="206"/>
       <c r="D23" s="61" t="s">
         <v>81</v>
       </c>
@@ -3432,7 +3445,7 @@
       <c r="B24" s="15">
         <v>9</v>
       </c>
-      <c r="C24" s="206" t="s">
+      <c r="C24" s="205" t="s">
         <v>127</v>
       </c>
       <c r="D24" s="59" t="s">
@@ -3443,7 +3456,7 @@
       <c r="B25" s="15">
         <v>10</v>
       </c>
-      <c r="C25" s="207"/>
+      <c r="C25" s="206"/>
       <c r="D25" s="60" t="s">
         <v>80</v>
       </c>
@@ -3469,7 +3482,7 @@
       <c r="B26" s="15">
         <v>11</v>
       </c>
-      <c r="C26" s="207"/>
+      <c r="C26" s="206"/>
       <c r="D26" s="60" t="s">
         <v>82</v>
       </c>
@@ -3478,7 +3491,7 @@
       <c r="B27" s="15">
         <v>12</v>
       </c>
-      <c r="C27" s="207"/>
+      <c r="C27" s="206"/>
       <c r="D27" s="61" t="s">
         <v>81</v>
       </c>
@@ -3487,7 +3500,7 @@
       <c r="B28" s="15">
         <v>13</v>
       </c>
-      <c r="C28" s="206" t="s">
+      <c r="C28" s="205" t="s">
         <v>128</v>
       </c>
       <c r="D28" s="59" t="s">
@@ -3498,7 +3511,7 @@
       <c r="B29" s="15">
         <v>14</v>
       </c>
-      <c r="C29" s="207"/>
+      <c r="C29" s="206"/>
       <c r="D29" s="60" t="s">
         <v>80</v>
       </c>
@@ -3507,7 +3520,7 @@
       <c r="B30" s="15">
         <v>15</v>
       </c>
-      <c r="C30" s="207"/>
+      <c r="C30" s="206"/>
       <c r="D30" s="60" t="s">
         <v>82</v>
       </c>
@@ -3516,7 +3529,7 @@
       <c r="B31" s="15">
         <v>16</v>
       </c>
-      <c r="C31" s="207"/>
+      <c r="C31" s="206"/>
       <c r="D31" s="61" t="s">
         <v>81</v>
       </c>
@@ -3525,7 +3538,7 @@
       <c r="B32" s="15">
         <v>17</v>
       </c>
-      <c r="C32" s="206" t="s">
+      <c r="C32" s="205" t="s">
         <v>129</v>
       </c>
       <c r="D32" s="59" t="s">
@@ -3536,7 +3549,7 @@
       <c r="B33" s="15">
         <v>18</v>
       </c>
-      <c r="C33" s="207"/>
+      <c r="C33" s="206"/>
       <c r="D33" s="60" t="s">
         <v>80</v>
       </c>
@@ -3545,7 +3558,7 @@
       <c r="B34" s="15">
         <v>19</v>
       </c>
-      <c r="C34" s="207"/>
+      <c r="C34" s="206"/>
       <c r="D34" s="60" t="s">
         <v>82</v>
       </c>
@@ -3571,7 +3584,7 @@
       <c r="B35" s="15">
         <v>20</v>
       </c>
-      <c r="C35" s="207"/>
+      <c r="C35" s="206"/>
       <c r="D35" s="61" t="s">
         <v>81</v>
       </c>
@@ -3597,7 +3610,7 @@
       <c r="B36" s="15">
         <v>21</v>
       </c>
-      <c r="C36" s="206" t="s">
+      <c r="C36" s="205" t="s">
         <v>134</v>
       </c>
       <c r="D36" s="59" t="s">
@@ -3625,7 +3638,7 @@
       <c r="B37" s="15">
         <v>22</v>
       </c>
-      <c r="C37" s="207"/>
+      <c r="C37" s="206"/>
       <c r="D37" s="60" t="s">
         <v>80</v>
       </c>
@@ -3651,7 +3664,7 @@
       <c r="B38" s="15">
         <v>23</v>
       </c>
-      <c r="C38" s="207"/>
+      <c r="C38" s="206"/>
       <c r="D38" s="60" t="s">
         <v>82</v>
       </c>
@@ -3673,7 +3686,7 @@
       <c r="B39" s="15">
         <v>24</v>
       </c>
-      <c r="C39" s="207"/>
+      <c r="C39" s="206"/>
       <c r="D39" s="61" t="s">
         <v>81</v>
       </c>
@@ -3695,7 +3708,7 @@
       <c r="B40" s="15">
         <v>25</v>
       </c>
-      <c r="C40" s="206" t="s">
+      <c r="C40" s="205" t="s">
         <v>135</v>
       </c>
       <c r="D40" s="59" t="s">
@@ -3719,7 +3732,7 @@
       <c r="B41" s="15">
         <v>26</v>
       </c>
-      <c r="C41" s="207"/>
+      <c r="C41" s="206"/>
       <c r="D41" s="60" t="s">
         <v>80</v>
       </c>
@@ -3745,7 +3758,7 @@
       <c r="B42" s="15">
         <v>27</v>
       </c>
-      <c r="C42" s="207"/>
+      <c r="C42" s="206"/>
       <c r="D42" s="60" t="s">
         <v>82</v>
       </c>
@@ -3771,7 +3784,7 @@
       <c r="B43" s="15">
         <v>28</v>
       </c>
-      <c r="C43" s="207"/>
+      <c r="C43" s="206"/>
       <c r="D43" s="61" t="s">
         <v>81</v>
       </c>
@@ -3797,7 +3810,7 @@
       <c r="B44" s="15">
         <v>29</v>
       </c>
-      <c r="C44" s="206" t="s">
+      <c r="C44" s="205" t="s">
         <v>136</v>
       </c>
       <c r="D44" s="59" t="s">
@@ -3825,7 +3838,7 @@
       <c r="B45" s="15">
         <v>30</v>
       </c>
-      <c r="C45" s="207"/>
+      <c r="C45" s="206"/>
       <c r="D45" s="60" t="s">
         <v>80</v>
       </c>
@@ -3834,7 +3847,7 @@
       <c r="B46" s="15">
         <v>31</v>
       </c>
-      <c r="C46" s="207"/>
+      <c r="C46" s="206"/>
       <c r="D46" s="60" t="s">
         <v>82</v>
       </c>
@@ -3843,7 +3856,7 @@
       <c r="B47" s="15">
         <v>32</v>
       </c>
-      <c r="C47" s="207"/>
+      <c r="C47" s="206"/>
       <c r="D47" s="61" t="s">
         <v>81</v>
       </c>
@@ -3852,7 +3865,7 @@
       <c r="B48" s="15">
         <v>33</v>
       </c>
-      <c r="C48" s="206" t="s">
+      <c r="C48" s="205" t="s">
         <v>137</v>
       </c>
       <c r="D48" s="59" t="s">
@@ -3863,7 +3876,7 @@
       <c r="B49" s="15">
         <v>34</v>
       </c>
-      <c r="C49" s="207"/>
+      <c r="C49" s="206"/>
       <c r="D49" s="60" t="s">
         <v>80</v>
       </c>
@@ -3872,7 +3885,7 @@
       <c r="B50" s="15">
         <v>35</v>
       </c>
-      <c r="C50" s="207"/>
+      <c r="C50" s="206"/>
       <c r="D50" s="60" t="s">
         <v>82</v>
       </c>
@@ -3881,7 +3894,7 @@
       <c r="B51" s="15">
         <v>36</v>
       </c>
-      <c r="C51" s="207"/>
+      <c r="C51" s="206"/>
       <c r="D51" s="61" t="s">
         <v>81</v>
       </c>
@@ -3890,7 +3903,7 @@
       <c r="B52" s="15">
         <v>37</v>
       </c>
-      <c r="C52" s="208" t="s">
+      <c r="C52" s="207" t="s">
         <v>138</v>
       </c>
       <c r="D52" s="59" t="s">
@@ -3901,7 +3914,7 @@
       <c r="B53" s="15">
         <v>38</v>
       </c>
-      <c r="C53" s="209"/>
+      <c r="C53" s="208"/>
       <c r="D53" s="60" t="s">
         <v>80</v>
       </c>
@@ -3910,7 +3923,7 @@
       <c r="B54" s="15">
         <v>39</v>
       </c>
-      <c r="C54" s="209"/>
+      <c r="C54" s="208"/>
       <c r="D54" s="60" t="s">
         <v>82</v>
       </c>
@@ -3919,7 +3932,7 @@
       <c r="B55" s="15">
         <v>40</v>
       </c>
-      <c r="C55" s="210"/>
+      <c r="C55" s="209"/>
       <c r="D55" s="61" t="s">
         <v>81</v>
       </c>
@@ -3928,7 +3941,7 @@
       <c r="B56" s="15">
         <v>41</v>
       </c>
-      <c r="C56" s="206" t="s">
+      <c r="C56" s="205" t="s">
         <v>139</v>
       </c>
       <c r="D56" s="59" t="s">
@@ -3939,7 +3952,7 @@
       <c r="B57" s="15">
         <v>42</v>
       </c>
-      <c r="C57" s="207"/>
+      <c r="C57" s="206"/>
       <c r="D57" s="60" t="s">
         <v>80</v>
       </c>
@@ -3948,7 +3961,7 @@
       <c r="B58" s="15">
         <v>43</v>
       </c>
-      <c r="C58" s="207"/>
+      <c r="C58" s="206"/>
       <c r="D58" s="60" t="s">
         <v>82</v>
       </c>
@@ -3957,7 +3970,7 @@
       <c r="B59" s="15">
         <v>44</v>
       </c>
-      <c r="C59" s="207"/>
+      <c r="C59" s="206"/>
       <c r="D59" s="61" t="s">
         <v>81</v>
       </c>
@@ -3966,7 +3979,7 @@
       <c r="B60" s="15">
         <v>45</v>
       </c>
-      <c r="C60" s="206" t="s">
+      <c r="C60" s="205" t="s">
         <v>140</v>
       </c>
       <c r="D60" s="59" t="s">
@@ -3977,7 +3990,7 @@
       <c r="B61" s="15">
         <v>46</v>
       </c>
-      <c r="C61" s="207"/>
+      <c r="C61" s="206"/>
       <c r="D61" s="60" t="s">
         <v>80</v>
       </c>
@@ -3986,7 +3999,7 @@
       <c r="B62" s="15">
         <v>47</v>
       </c>
-      <c r="C62" s="207"/>
+      <c r="C62" s="206"/>
       <c r="D62" s="60" t="s">
         <v>82</v>
       </c>
@@ -3995,7 +4008,7 @@
       <c r="B63" s="15">
         <v>48</v>
       </c>
-      <c r="C63" s="207"/>
+      <c r="C63" s="206"/>
       <c r="D63" s="61" t="s">
         <v>81</v>
       </c>
@@ -4004,7 +4017,7 @@
       <c r="B64" s="15">
         <v>49</v>
       </c>
-      <c r="C64" s="206" t="s">
+      <c r="C64" s="205" t="s">
         <v>141</v>
       </c>
       <c r="D64" s="59" t="s">
@@ -4015,7 +4028,7 @@
       <c r="B65" s="15">
         <v>50</v>
       </c>
-      <c r="C65" s="207"/>
+      <c r="C65" s="206"/>
       <c r="D65" s="60" t="s">
         <v>80</v>
       </c>
@@ -4024,7 +4037,7 @@
       <c r="B66" s="15">
         <v>51</v>
       </c>
-      <c r="C66" s="207"/>
+      <c r="C66" s="206"/>
       <c r="D66" s="60" t="s">
         <v>82</v>
       </c>
@@ -4033,7 +4046,7 @@
       <c r="B67" s="15">
         <v>52</v>
       </c>
-      <c r="C67" s="207"/>
+      <c r="C67" s="206"/>
       <c r="D67" s="61" t="s">
         <v>81</v>
       </c>
@@ -4060,7 +4073,7 @@
       <c r="B70" s="15">
         <v>55</v>
       </c>
-      <c r="C70" s="200" t="s">
+      <c r="C70" s="199" t="s">
         <v>7</v>
       </c>
       <c r="D70" s="55" t="s">
@@ -4071,7 +4084,7 @@
       <c r="B71" s="15">
         <v>56</v>
       </c>
-      <c r="C71" s="201"/>
+      <c r="C71" s="200"/>
       <c r="D71" s="56" t="s">
         <v>80</v>
       </c>
@@ -4080,7 +4093,7 @@
       <c r="B72" s="15">
         <v>57</v>
       </c>
-      <c r="C72" s="201"/>
+      <c r="C72" s="200"/>
       <c r="D72" s="56" t="s">
         <v>82</v>
       </c>
@@ -4089,7 +4102,7 @@
       <c r="B73" s="15">
         <v>58</v>
       </c>
-      <c r="C73" s="202"/>
+      <c r="C73" s="201"/>
       <c r="D73" s="57" t="s">
         <v>81</v>
       </c>
@@ -4098,7 +4111,7 @@
       <c r="B74" s="15">
         <v>59</v>
       </c>
-      <c r="C74" s="211" t="s">
+      <c r="C74" s="210" t="s">
         <v>5</v>
       </c>
       <c r="D74" s="65"/>
@@ -4107,14 +4120,14 @@
       <c r="B75" s="15">
         <v>60</v>
       </c>
-      <c r="C75" s="212"/>
+      <c r="C75" s="211"/>
       <c r="D75" s="66"/>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B76" s="15">
         <v>61</v>
       </c>
-      <c r="C76" s="213" t="s">
+      <c r="C76" s="212" t="s">
         <v>6</v>
       </c>
       <c r="D76" s="62"/>
@@ -4123,14 +4136,14 @@
       <c r="B77" s="15">
         <v>62</v>
       </c>
-      <c r="C77" s="214"/>
+      <c r="C77" s="213"/>
       <c r="D77" s="63"/>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B78" s="15">
         <v>63</v>
       </c>
-      <c r="C78" s="215"/>
+      <c r="C78" s="214"/>
       <c r="D78" s="64"/>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.15">
@@ -4142,7 +4155,7 @@
       <c r="B83" s="67">
         <v>0</v>
       </c>
-      <c r="C83" s="203" t="s">
+      <c r="C83" s="202" t="s">
         <v>2</v>
       </c>
       <c r="D83" s="62"/>
@@ -4151,14 +4164,14 @@
       <c r="B84" s="67">
         <v>1</v>
       </c>
-      <c r="C84" s="204"/>
+      <c r="C84" s="203"/>
       <c r="D84" s="63"/>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B85" s="67">
         <v>2</v>
       </c>
-      <c r="C85" s="205"/>
+      <c r="C85" s="204"/>
       <c r="D85" s="64"/>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.15">
@@ -4187,7 +4200,7 @@
       <c r="B88" s="15">
         <v>5</v>
       </c>
-      <c r="C88" s="206" t="s">
+      <c r="C88" s="205" t="s">
         <v>142</v>
       </c>
       <c r="D88" s="59" t="s">
@@ -4198,7 +4211,7 @@
       <c r="B89" s="15">
         <v>6</v>
       </c>
-      <c r="C89" s="207"/>
+      <c r="C89" s="206"/>
       <c r="D89" s="60" t="s">
         <v>80</v>
       </c>
@@ -4207,7 +4220,7 @@
       <c r="B90" s="15">
         <v>7</v>
       </c>
-      <c r="C90" s="207"/>
+      <c r="C90" s="206"/>
       <c r="D90" s="60" t="s">
         <v>82</v>
       </c>
@@ -4216,7 +4229,7 @@
       <c r="B91" s="15">
         <v>8</v>
       </c>
-      <c r="C91" s="207"/>
+      <c r="C91" s="206"/>
       <c r="D91" s="61" t="s">
         <v>81</v>
       </c>
@@ -4225,7 +4238,7 @@
       <c r="B92" s="15">
         <v>9</v>
       </c>
-      <c r="C92" s="206" t="s">
+      <c r="C92" s="205" t="s">
         <v>143</v>
       </c>
       <c r="D92" s="59" t="s">
@@ -4236,7 +4249,7 @@
       <c r="B93" s="15">
         <v>10</v>
       </c>
-      <c r="C93" s="207"/>
+      <c r="C93" s="206"/>
       <c r="D93" s="60" t="s">
         <v>80</v>
       </c>
@@ -4245,7 +4258,7 @@
       <c r="B94" s="15">
         <v>11</v>
       </c>
-      <c r="C94" s="207"/>
+      <c r="C94" s="206"/>
       <c r="D94" s="60" t="s">
         <v>82</v>
       </c>
@@ -4254,7 +4267,7 @@
       <c r="B95" s="15">
         <v>12</v>
       </c>
-      <c r="C95" s="207"/>
+      <c r="C95" s="206"/>
       <c r="D95" s="61" t="s">
         <v>81</v>
       </c>
@@ -4263,7 +4276,7 @@
       <c r="B96" s="15">
         <v>13</v>
       </c>
-      <c r="C96" s="206" t="s">
+      <c r="C96" s="205" t="s">
         <v>144</v>
       </c>
       <c r="D96" s="59" t="s">
@@ -4274,7 +4287,7 @@
       <c r="B97" s="15">
         <v>14</v>
       </c>
-      <c r="C97" s="207"/>
+      <c r="C97" s="206"/>
       <c r="D97" s="60" t="s">
         <v>80</v>
       </c>
@@ -4283,7 +4296,7 @@
       <c r="B98" s="15">
         <v>15</v>
       </c>
-      <c r="C98" s="207"/>
+      <c r="C98" s="206"/>
       <c r="D98" s="60" t="s">
         <v>82</v>
       </c>
@@ -4292,7 +4305,7 @@
       <c r="B99" s="15">
         <v>16</v>
       </c>
-      <c r="C99" s="207"/>
+      <c r="C99" s="206"/>
       <c r="D99" s="61" t="s">
         <v>81</v>
       </c>
@@ -4301,7 +4314,7 @@
       <c r="B100" s="15">
         <v>17</v>
       </c>
-      <c r="C100" s="206" t="s">
+      <c r="C100" s="205" t="s">
         <v>145</v>
       </c>
       <c r="D100" s="59" t="s">
@@ -4312,7 +4325,7 @@
       <c r="B101" s="15">
         <v>18</v>
       </c>
-      <c r="C101" s="207"/>
+      <c r="C101" s="206"/>
       <c r="D101" s="60" t="s">
         <v>80</v>
       </c>
@@ -4321,7 +4334,7 @@
       <c r="B102" s="15">
         <v>19</v>
       </c>
-      <c r="C102" s="207"/>
+      <c r="C102" s="206"/>
       <c r="D102" s="60" t="s">
         <v>82</v>
       </c>
@@ -4330,7 +4343,7 @@
       <c r="B103" s="15">
         <v>20</v>
       </c>
-      <c r="C103" s="207"/>
+      <c r="C103" s="206"/>
       <c r="D103" s="61" t="s">
         <v>81</v>
       </c>
@@ -4581,7 +4594,7 @@
       <c r="B138" s="15">
         <v>55</v>
       </c>
-      <c r="C138" s="200" t="s">
+      <c r="C138" s="199" t="s">
         <v>7</v>
       </c>
       <c r="D138" s="55" t="s">
@@ -4592,7 +4605,7 @@
       <c r="B139" s="15">
         <v>56</v>
       </c>
-      <c r="C139" s="201"/>
+      <c r="C139" s="200"/>
       <c r="D139" s="56" t="s">
         <v>80</v>
       </c>
@@ -4601,7 +4614,7 @@
       <c r="B140" s="15">
         <v>57</v>
       </c>
-      <c r="C140" s="201"/>
+      <c r="C140" s="200"/>
       <c r="D140" s="56" t="s">
         <v>82</v>
       </c>
@@ -4610,7 +4623,7 @@
       <c r="B141" s="15">
         <v>58</v>
       </c>
-      <c r="C141" s="202"/>
+      <c r="C141" s="201"/>
       <c r="D141" s="57" t="s">
         <v>81</v>
       </c>
@@ -4619,7 +4632,7 @@
       <c r="B142" s="15">
         <v>59</v>
       </c>
-      <c r="C142" s="211" t="s">
+      <c r="C142" s="210" t="s">
         <v>5</v>
       </c>
       <c r="D142" s="65"/>
@@ -4628,14 +4641,14 @@
       <c r="B143" s="15">
         <v>60</v>
       </c>
-      <c r="C143" s="212"/>
+      <c r="C143" s="211"/>
       <c r="D143" s="66"/>
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B144" s="15">
         <v>61</v>
       </c>
-      <c r="C144" s="213" t="s">
+      <c r="C144" s="212" t="s">
         <v>6</v>
       </c>
       <c r="D144" s="62"/>
@@ -4644,14 +4657,14 @@
       <c r="B145" s="15">
         <v>62</v>
       </c>
-      <c r="C145" s="214"/>
+      <c r="C145" s="213"/>
       <c r="D145" s="63"/>
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B146" s="15">
         <v>63</v>
       </c>
-      <c r="C146" s="215"/>
+      <c r="C146" s="214"/>
       <c r="D146" s="64"/>
     </row>
   </sheetData>
@@ -4694,7 +4707,7 @@
   <dimension ref="B2:L35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="C28" sqref="C28:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -4710,11 +4723,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B2" s="152" t="s">
+      <c r="B2" s="151" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="154"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="153"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B5" s="15">
@@ -4752,7 +4765,7 @@
       <c r="B7" s="26">
         <v>5</v>
       </c>
-      <c r="C7" s="221" t="s">
+      <c r="C7" s="220" t="s">
         <v>76</v>
       </c>
       <c r="D7" s="28" t="s">
@@ -4773,7 +4786,7 @@
       <c r="B8" s="26">
         <v>6</v>
       </c>
-      <c r="C8" s="222"/>
+      <c r="C8" s="221"/>
       <c r="D8" s="29" t="s">
         <v>80</v>
       </c>
@@ -4832,7 +4845,7 @@
       <c r="B13" s="26">
         <v>5</v>
       </c>
-      <c r="C13" s="221" t="s">
+      <c r="C13" s="220" t="s">
         <v>76</v>
       </c>
       <c r="D13" s="28" t="s">
@@ -4855,7 +4868,7 @@
       <c r="B14" s="26">
         <v>6</v>
       </c>
-      <c r="C14" s="222"/>
+      <c r="C14" s="221"/>
       <c r="D14" s="29" t="s">
         <v>80</v>
       </c>
@@ -4894,7 +4907,7 @@
       <c r="B16" s="26">
         <v>8</v>
       </c>
-      <c r="C16" s="216" t="s">
+      <c r="C16" s="215" t="s">
         <v>165</v>
       </c>
       <c r="D16" s="124" t="s">
@@ -4917,7 +4930,7 @@
       <c r="B17" s="26">
         <v>9</v>
       </c>
-      <c r="C17" s="217"/>
+      <c r="C17" s="216"/>
       <c r="D17" s="125" t="s">
         <v>80</v>
       </c>
@@ -4946,17 +4959,17 @@
       <c r="D21" s="30" t="s">
         <v>71</v>
       </c>
-      <c r="G21" s="218" t="s">
+      <c r="G21" s="217" t="s">
         <v>90</v>
       </c>
-      <c r="H21" s="219"/>
-      <c r="I21" s="220"/>
+      <c r="H21" s="218"/>
+      <c r="I21" s="219"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B22" s="15">
         <v>5</v>
       </c>
-      <c r="C22" s="221" t="s">
+      <c r="C22" s="220" t="s">
         <v>76</v>
       </c>
       <c r="D22" s="28" t="s">
@@ -4970,7 +4983,7 @@
       <c r="B23" s="15">
         <v>6</v>
       </c>
-      <c r="C23" s="222"/>
+      <c r="C23" s="221"/>
       <c r="D23" s="29" t="s">
         <v>80</v>
       </c>
@@ -5001,7 +5014,7 @@
       <c r="B25" s="15">
         <v>8</v>
       </c>
-      <c r="C25" s="216" t="s">
+      <c r="C25" s="215" t="s">
         <v>164</v>
       </c>
       <c r="D25" s="124" t="s">
@@ -5022,7 +5035,7 @@
       <c r="B26" s="15">
         <v>9</v>
       </c>
-      <c r="C26" s="217"/>
+      <c r="C26" s="216"/>
       <c r="D26" s="125" t="s">
         <v>80</v>
       </c>
@@ -5038,7 +5051,7 @@
       <c r="B27" s="15">
         <v>10</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="222" t="s">
         <v>77</v>
       </c>
       <c r="D27" s="51"/>
@@ -5054,10 +5067,10 @@
       <c r="B28" s="15">
         <v>11</v>
       </c>
-      <c r="C28" s="113" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="32" t="s">
+      <c r="C28" s="223" t="s">
+        <v>171</v>
+      </c>
+      <c r="D28" s="224" t="s">
         <v>79</v>
       </c>
     </row>
@@ -5065,9 +5078,11 @@
       <c r="B29" s="15">
         <v>12</v>
       </c>
-      <c r="C29" s="114"/>
-      <c r="D29" s="53" t="s">
-        <v>80</v>
+      <c r="C29" s="113" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>79</v>
       </c>
       <c r="G29" s="11" t="s">
         <v>84</v>
@@ -5079,7 +5094,7 @@
       </c>
       <c r="C30" s="114"/>
       <c r="D30" s="53" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G30" s="38" t="s">
         <v>107</v>
@@ -5093,9 +5108,9 @@
       <c r="B31" s="15">
         <v>14</v>
       </c>
-      <c r="C31" s="115"/>
-      <c r="D31" s="54" t="s">
-        <v>81</v>
+      <c r="C31" s="114"/>
+      <c r="D31" s="53" t="s">
+        <v>82</v>
       </c>
       <c r="G31" s="38" t="s">
         <v>106</v>
@@ -5109,11 +5124,9 @@
       <c r="B32" s="15">
         <v>15</v>
       </c>
-      <c r="C32" s="131" t="s">
-        <v>171</v>
-      </c>
-      <c r="D32" s="132" t="s">
-        <v>79</v>
+      <c r="C32" s="115"/>
+      <c r="D32" s="54" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.15">
@@ -5175,11 +5188,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C4" s="152" t="s">
+      <c r="C4" s="151" t="s">
         <v>173</v>
       </c>
-      <c r="D4" s="153"/>
-      <c r="E4" s="154"/>
+      <c r="D4" s="152"/>
+      <c r="E4" s="153"/>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.2">
@@ -5195,10 +5208,10 @@
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C7" s="155" t="s">
+      <c r="C7" s="154" t="s">
         <v>147</v>
       </c>
-      <c r="D7" s="155"/>
+      <c r="D7" s="154"/>
       <c r="E7" s="4"/>
       <c r="F7" s="94"/>
     </row>
@@ -5206,7 +5219,7 @@
       <c r="C8" s="15">
         <v>3</v>
       </c>
-      <c r="D8" s="135" t="s">
+      <c r="D8" s="133" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="31" t="s">
@@ -5218,7 +5231,7 @@
       <c r="C9" s="50">
         <v>4</v>
       </c>
-      <c r="D9" s="136" t="s">
+      <c r="D9" s="134" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="40" t="s">
@@ -5253,11 +5266,11 @@
       <c r="F13" s="4"/>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C14" s="156" t="s">
+      <c r="C14" s="155" t="s">
         <v>154</v>
       </c>
-      <c r="D14" s="157"/>
-      <c r="E14" s="158"/>
+      <c r="D14" s="156"/>
+      <c r="E14" s="157"/>
       <c r="F14" s="4"/>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.2">
@@ -5270,7 +5283,7 @@
       <c r="C17" s="15">
         <v>3</v>
       </c>
-      <c r="D17" s="135" t="s">
+      <c r="D17" s="133" t="s">
         <v>0</v>
       </c>
       <c r="E17" s="31" t="s">
@@ -5281,7 +5294,7 @@
       <c r="C18" s="50">
         <v>4</v>
       </c>
-      <c r="D18" s="136" t="s">
+      <c r="D18" s="134" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="40" t="s">
@@ -5292,7 +5305,7 @@
       <c r="C19" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="D19" s="138" t="s">
+      <c r="D19" s="136" t="s">
         <v>76</v>
       </c>
       <c r="E19" s="28" t="s">
@@ -5303,7 +5316,7 @@
       <c r="C20" s="26" t="s">
         <v>174</v>
       </c>
-      <c r="D20" s="139"/>
+      <c r="D20" s="137"/>
       <c r="E20" s="29" t="s">
         <v>80</v>
       </c>
@@ -5312,10 +5325,10 @@
       <c r="C21" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="D21" s="137" t="s">
+      <c r="D21" s="135" t="s">
         <v>124</v>
       </c>
-      <c r="E21" s="137"/>
+      <c r="E21" s="135"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5350,350 +5363,350 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B2" s="159" t="s">
+      <c r="B2" s="158" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="160"/>
-      <c r="D2" s="160"/>
-      <c r="E2" s="160"/>
-      <c r="F2" s="161"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="160"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B4" s="162" t="s">
+      <c r="B4" s="161" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="162"/>
-      <c r="D4" s="169" t="s">
+      <c r="C4" s="161"/>
+      <c r="D4" s="168" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="169"/>
-      <c r="F4" s="169"/>
-      <c r="G4" s="169"/>
-      <c r="H4" s="169"/>
-      <c r="I4" s="169"/>
-      <c r="J4" s="169"/>
-      <c r="K4" s="169"/>
-      <c r="L4" s="169"/>
-      <c r="M4" s="169"/>
-      <c r="N4" s="169"/>
-      <c r="O4" s="169"/>
-      <c r="P4" s="169"/>
-      <c r="Q4" s="169"/>
-      <c r="R4" s="169"/>
-      <c r="S4" s="169"/>
-      <c r="T4" s="169"/>
-      <c r="U4" s="169"/>
-      <c r="V4" s="169"/>
-      <c r="W4" s="169"/>
-      <c r="X4" s="169"/>
+      <c r="E4" s="168"/>
+      <c r="F4" s="168"/>
+      <c r="G4" s="168"/>
+      <c r="H4" s="168"/>
+      <c r="I4" s="168"/>
+      <c r="J4" s="168"/>
+      <c r="K4" s="168"/>
+      <c r="L4" s="168"/>
+      <c r="M4" s="168"/>
+      <c r="N4" s="168"/>
+      <c r="O4" s="168"/>
+      <c r="P4" s="168"/>
+      <c r="Q4" s="168"/>
+      <c r="R4" s="168"/>
+      <c r="S4" s="168"/>
+      <c r="T4" s="168"/>
+      <c r="U4" s="168"/>
+      <c r="V4" s="168"/>
+      <c r="W4" s="168"/>
+      <c r="X4" s="168"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B5" s="168"/>
-      <c r="C5" s="168"/>
-      <c r="D5" s="169"/>
-      <c r="E5" s="169"/>
-      <c r="F5" s="169"/>
-      <c r="G5" s="169"/>
-      <c r="H5" s="169"/>
-      <c r="I5" s="169"/>
-      <c r="J5" s="169"/>
-      <c r="K5" s="169"/>
-      <c r="L5" s="169"/>
-      <c r="M5" s="169"/>
-      <c r="N5" s="169"/>
-      <c r="O5" s="169"/>
-      <c r="P5" s="169"/>
-      <c r="Q5" s="169"/>
-      <c r="R5" s="169"/>
-      <c r="S5" s="169"/>
-      <c r="T5" s="169"/>
-      <c r="U5" s="169"/>
-      <c r="V5" s="169"/>
-      <c r="W5" s="169"/>
-      <c r="X5" s="169"/>
+      <c r="B5" s="167"/>
+      <c r="C5" s="167"/>
+      <c r="D5" s="168"/>
+      <c r="E5" s="168"/>
+      <c r="F5" s="168"/>
+      <c r="G5" s="168"/>
+      <c r="H5" s="168"/>
+      <c r="I5" s="168"/>
+      <c r="J5" s="168"/>
+      <c r="K5" s="168"/>
+      <c r="L5" s="168"/>
+      <c r="M5" s="168"/>
+      <c r="N5" s="168"/>
+      <c r="O5" s="168"/>
+      <c r="P5" s="168"/>
+      <c r="Q5" s="168"/>
+      <c r="R5" s="168"/>
+      <c r="S5" s="168"/>
+      <c r="T5" s="168"/>
+      <c r="U5" s="168"/>
+      <c r="V5" s="168"/>
+      <c r="W5" s="168"/>
+      <c r="X5" s="168"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B6" s="171" t="s">
+      <c r="B6" s="170" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="171"/>
-      <c r="D6" s="169" t="s">
+      <c r="C6" s="170"/>
+      <c r="D6" s="168" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="169"/>
-      <c r="F6" s="169"/>
-      <c r="G6" s="169"/>
-      <c r="H6" s="169"/>
-      <c r="I6" s="169"/>
-      <c r="J6" s="169"/>
-      <c r="K6" s="169"/>
-      <c r="L6" s="169"/>
-      <c r="M6" s="169"/>
-      <c r="N6" s="169"/>
-      <c r="O6" s="169"/>
-      <c r="P6" s="169"/>
-      <c r="Q6" s="169"/>
-      <c r="R6" s="169"/>
-      <c r="S6" s="169"/>
-      <c r="T6" s="169"/>
-      <c r="U6" s="169"/>
-      <c r="V6" s="169"/>
-      <c r="W6" s="169"/>
-      <c r="X6" s="169"/>
+      <c r="E6" s="168"/>
+      <c r="F6" s="168"/>
+      <c r="G6" s="168"/>
+      <c r="H6" s="168"/>
+      <c r="I6" s="168"/>
+      <c r="J6" s="168"/>
+      <c r="K6" s="168"/>
+      <c r="L6" s="168"/>
+      <c r="M6" s="168"/>
+      <c r="N6" s="168"/>
+      <c r="O6" s="168"/>
+      <c r="P6" s="168"/>
+      <c r="Q6" s="168"/>
+      <c r="R6" s="168"/>
+      <c r="S6" s="168"/>
+      <c r="T6" s="168"/>
+      <c r="U6" s="168"/>
+      <c r="V6" s="168"/>
+      <c r="W6" s="168"/>
+      <c r="X6" s="168"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B7" s="172" t="s">
+      <c r="B7" s="171" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="172"/>
-      <c r="D7" s="169" t="s">
+      <c r="C7" s="171"/>
+      <c r="D7" s="168" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="169"/>
-      <c r="F7" s="169"/>
-      <c r="G7" s="169"/>
-      <c r="H7" s="169"/>
-      <c r="I7" s="169"/>
-      <c r="J7" s="169"/>
-      <c r="K7" s="169"/>
-      <c r="L7" s="169"/>
-      <c r="M7" s="169"/>
-      <c r="N7" s="169"/>
-      <c r="O7" s="169"/>
-      <c r="P7" s="169"/>
-      <c r="Q7" s="169"/>
-      <c r="R7" s="169"/>
-      <c r="S7" s="169"/>
-      <c r="T7" s="169"/>
-      <c r="U7" s="169"/>
-      <c r="V7" s="169"/>
-      <c r="W7" s="169"/>
-      <c r="X7" s="169"/>
+      <c r="E7" s="168"/>
+      <c r="F7" s="168"/>
+      <c r="G7" s="168"/>
+      <c r="H7" s="168"/>
+      <c r="I7" s="168"/>
+      <c r="J7" s="168"/>
+      <c r="K7" s="168"/>
+      <c r="L7" s="168"/>
+      <c r="M7" s="168"/>
+      <c r="N7" s="168"/>
+      <c r="O7" s="168"/>
+      <c r="P7" s="168"/>
+      <c r="Q7" s="168"/>
+      <c r="R7" s="168"/>
+      <c r="S7" s="168"/>
+      <c r="T7" s="168"/>
+      <c r="U7" s="168"/>
+      <c r="V7" s="168"/>
+      <c r="W7" s="168"/>
+      <c r="X7" s="168"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B8" s="152"/>
-      <c r="C8" s="154"/>
-      <c r="D8" s="165"/>
-      <c r="E8" s="166"/>
-      <c r="F8" s="166"/>
-      <c r="G8" s="166"/>
-      <c r="H8" s="166"/>
-      <c r="I8" s="166"/>
-      <c r="J8" s="166"/>
-      <c r="K8" s="166"/>
-      <c r="L8" s="166"/>
-      <c r="M8" s="166"/>
-      <c r="N8" s="166"/>
-      <c r="O8" s="166"/>
-      <c r="P8" s="166"/>
-      <c r="Q8" s="166"/>
-      <c r="R8" s="166"/>
-      <c r="S8" s="166"/>
-      <c r="T8" s="166"/>
-      <c r="U8" s="166"/>
-      <c r="V8" s="166"/>
-      <c r="W8" s="166"/>
-      <c r="X8" s="167"/>
+      <c r="B8" s="151"/>
+      <c r="C8" s="153"/>
+      <c r="D8" s="164"/>
+      <c r="E8" s="165"/>
+      <c r="F8" s="165"/>
+      <c r="G8" s="165"/>
+      <c r="H8" s="165"/>
+      <c r="I8" s="165"/>
+      <c r="J8" s="165"/>
+      <c r="K8" s="165"/>
+      <c r="L8" s="165"/>
+      <c r="M8" s="165"/>
+      <c r="N8" s="165"/>
+      <c r="O8" s="165"/>
+      <c r="P8" s="165"/>
+      <c r="Q8" s="165"/>
+      <c r="R8" s="165"/>
+      <c r="S8" s="165"/>
+      <c r="T8" s="165"/>
+      <c r="U8" s="165"/>
+      <c r="V8" s="165"/>
+      <c r="W8" s="165"/>
+      <c r="X8" s="166"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B9" s="173" t="s">
+      <c r="B9" s="172" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="174"/>
-      <c r="D9" s="165"/>
-      <c r="E9" s="166"/>
-      <c r="F9" s="166"/>
-      <c r="G9" s="166"/>
-      <c r="H9" s="166"/>
-      <c r="I9" s="166"/>
-      <c r="J9" s="166"/>
-      <c r="K9" s="166"/>
-      <c r="L9" s="166"/>
-      <c r="M9" s="166"/>
-      <c r="N9" s="166"/>
-      <c r="O9" s="166"/>
-      <c r="P9" s="166"/>
-      <c r="Q9" s="166"/>
-      <c r="R9" s="166"/>
-      <c r="S9" s="166"/>
-      <c r="T9" s="166"/>
-      <c r="U9" s="166"/>
-      <c r="V9" s="166"/>
-      <c r="W9" s="166"/>
-      <c r="X9" s="167"/>
+      <c r="C9" s="173"/>
+      <c r="D9" s="164"/>
+      <c r="E9" s="165"/>
+      <c r="F9" s="165"/>
+      <c r="G9" s="165"/>
+      <c r="H9" s="165"/>
+      <c r="I9" s="165"/>
+      <c r="J9" s="165"/>
+      <c r="K9" s="165"/>
+      <c r="L9" s="165"/>
+      <c r="M9" s="165"/>
+      <c r="N9" s="165"/>
+      <c r="O9" s="165"/>
+      <c r="P9" s="165"/>
+      <c r="Q9" s="165"/>
+      <c r="R9" s="165"/>
+      <c r="S9" s="165"/>
+      <c r="T9" s="165"/>
+      <c r="U9" s="165"/>
+      <c r="V9" s="165"/>
+      <c r="W9" s="165"/>
+      <c r="X9" s="166"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B10" s="152"/>
-      <c r="C10" s="154"/>
-      <c r="D10" s="165"/>
-      <c r="E10" s="166"/>
-      <c r="F10" s="166"/>
-      <c r="G10" s="166"/>
-      <c r="H10" s="166"/>
-      <c r="I10" s="166"/>
-      <c r="J10" s="166"/>
-      <c r="K10" s="166"/>
-      <c r="L10" s="166"/>
-      <c r="M10" s="166"/>
-      <c r="N10" s="166"/>
-      <c r="O10" s="166"/>
-      <c r="P10" s="166"/>
-      <c r="Q10" s="166"/>
-      <c r="R10" s="166"/>
-      <c r="S10" s="166"/>
-      <c r="T10" s="166"/>
-      <c r="U10" s="166"/>
-      <c r="V10" s="166"/>
-      <c r="W10" s="166"/>
-      <c r="X10" s="167"/>
+      <c r="B10" s="151"/>
+      <c r="C10" s="153"/>
+      <c r="D10" s="164"/>
+      <c r="E10" s="165"/>
+      <c r="F10" s="165"/>
+      <c r="G10" s="165"/>
+      <c r="H10" s="165"/>
+      <c r="I10" s="165"/>
+      <c r="J10" s="165"/>
+      <c r="K10" s="165"/>
+      <c r="L10" s="165"/>
+      <c r="M10" s="165"/>
+      <c r="N10" s="165"/>
+      <c r="O10" s="165"/>
+      <c r="P10" s="165"/>
+      <c r="Q10" s="165"/>
+      <c r="R10" s="165"/>
+      <c r="S10" s="165"/>
+      <c r="T10" s="165"/>
+      <c r="U10" s="165"/>
+      <c r="V10" s="165"/>
+      <c r="W10" s="165"/>
+      <c r="X10" s="166"/>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B11" s="170" t="s">
+      <c r="B11" s="169" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="170"/>
-      <c r="D11" s="169" t="s">
+      <c r="C11" s="169"/>
+      <c r="D11" s="168" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="169"/>
-      <c r="F11" s="169"/>
-      <c r="G11" s="169"/>
-      <c r="H11" s="169"/>
-      <c r="I11" s="169"/>
-      <c r="J11" s="169"/>
-      <c r="K11" s="169"/>
-      <c r="L11" s="169"/>
-      <c r="M11" s="169"/>
-      <c r="N11" s="169"/>
-      <c r="O11" s="169"/>
-      <c r="P11" s="169"/>
-      <c r="Q11" s="169"/>
-      <c r="R11" s="169"/>
-      <c r="S11" s="169"/>
-      <c r="T11" s="169"/>
-      <c r="U11" s="169"/>
-      <c r="V11" s="169"/>
-      <c r="W11" s="169"/>
-      <c r="X11" s="169"/>
+      <c r="E11" s="168"/>
+      <c r="F11" s="168"/>
+      <c r="G11" s="168"/>
+      <c r="H11" s="168"/>
+      <c r="I11" s="168"/>
+      <c r="J11" s="168"/>
+      <c r="K11" s="168"/>
+      <c r="L11" s="168"/>
+      <c r="M11" s="168"/>
+      <c r="N11" s="168"/>
+      <c r="O11" s="168"/>
+      <c r="P11" s="168"/>
+      <c r="Q11" s="168"/>
+      <c r="R11" s="168"/>
+      <c r="S11" s="168"/>
+      <c r="T11" s="168"/>
+      <c r="U11" s="168"/>
+      <c r="V11" s="168"/>
+      <c r="W11" s="168"/>
+      <c r="X11" s="168"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B12" s="164" t="s">
+      <c r="B12" s="163" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="164"/>
-      <c r="D12" s="169" t="s">
+      <c r="C12" s="163"/>
+      <c r="D12" s="168" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="169"/>
-      <c r="F12" s="169"/>
-      <c r="G12" s="169"/>
-      <c r="H12" s="169"/>
-      <c r="I12" s="169"/>
-      <c r="J12" s="169"/>
-      <c r="K12" s="169"/>
-      <c r="L12" s="169"/>
-      <c r="M12" s="169"/>
-      <c r="N12" s="169"/>
-      <c r="O12" s="169"/>
-      <c r="P12" s="169"/>
-      <c r="Q12" s="169"/>
-      <c r="R12" s="169"/>
-      <c r="S12" s="169"/>
-      <c r="T12" s="169"/>
-      <c r="U12" s="169"/>
-      <c r="V12" s="169"/>
-      <c r="W12" s="169"/>
-      <c r="X12" s="169"/>
+      <c r="E12" s="168"/>
+      <c r="F12" s="168"/>
+      <c r="G12" s="168"/>
+      <c r="H12" s="168"/>
+      <c r="I12" s="168"/>
+      <c r="J12" s="168"/>
+      <c r="K12" s="168"/>
+      <c r="L12" s="168"/>
+      <c r="M12" s="168"/>
+      <c r="N12" s="168"/>
+      <c r="O12" s="168"/>
+      <c r="P12" s="168"/>
+      <c r="Q12" s="168"/>
+      <c r="R12" s="168"/>
+      <c r="S12" s="168"/>
+      <c r="T12" s="168"/>
+      <c r="U12" s="168"/>
+      <c r="V12" s="168"/>
+      <c r="W12" s="168"/>
+      <c r="X12" s="168"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B13" s="163" t="s">
+      <c r="B13" s="162" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="163"/>
-      <c r="D13" s="169" t="s">
+      <c r="C13" s="162"/>
+      <c r="D13" s="168" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="169"/>
-      <c r="F13" s="169"/>
-      <c r="G13" s="169"/>
-      <c r="H13" s="169"/>
-      <c r="I13" s="169"/>
-      <c r="J13" s="169"/>
-      <c r="K13" s="169"/>
-      <c r="L13" s="169"/>
-      <c r="M13" s="169"/>
-      <c r="N13" s="169"/>
-      <c r="O13" s="169"/>
-      <c r="P13" s="169"/>
-      <c r="Q13" s="169"/>
-      <c r="R13" s="169"/>
-      <c r="S13" s="169"/>
-      <c r="T13" s="169"/>
-      <c r="U13" s="169"/>
-      <c r="V13" s="169"/>
-      <c r="W13" s="169"/>
-      <c r="X13" s="169"/>
+      <c r="E13" s="168"/>
+      <c r="F13" s="168"/>
+      <c r="G13" s="168"/>
+      <c r="H13" s="168"/>
+      <c r="I13" s="168"/>
+      <c r="J13" s="168"/>
+      <c r="K13" s="168"/>
+      <c r="L13" s="168"/>
+      <c r="M13" s="168"/>
+      <c r="N13" s="168"/>
+      <c r="O13" s="168"/>
+      <c r="P13" s="168"/>
+      <c r="Q13" s="168"/>
+      <c r="R13" s="168"/>
+      <c r="S13" s="168"/>
+      <c r="T13" s="168"/>
+      <c r="U13" s="168"/>
+      <c r="V13" s="168"/>
+      <c r="W13" s="168"/>
+      <c r="X13" s="168"/>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B14" s="168"/>
-      <c r="C14" s="168"/>
-      <c r="D14" s="169"/>
-      <c r="E14" s="169"/>
-      <c r="F14" s="169"/>
-      <c r="G14" s="169"/>
-      <c r="H14" s="169"/>
-      <c r="I14" s="169"/>
-      <c r="J14" s="169"/>
-      <c r="K14" s="169"/>
-      <c r="L14" s="169"/>
-      <c r="M14" s="169"/>
-      <c r="N14" s="169"/>
-      <c r="O14" s="169"/>
-      <c r="P14" s="169"/>
-      <c r="Q14" s="169"/>
-      <c r="R14" s="169"/>
-      <c r="S14" s="169"/>
-      <c r="T14" s="169"/>
-      <c r="U14" s="169"/>
-      <c r="V14" s="169"/>
-      <c r="W14" s="169"/>
-      <c r="X14" s="169"/>
+      <c r="B14" s="167"/>
+      <c r="C14" s="167"/>
+      <c r="D14" s="168"/>
+      <c r="E14" s="168"/>
+      <c r="F14" s="168"/>
+      <c r="G14" s="168"/>
+      <c r="H14" s="168"/>
+      <c r="I14" s="168"/>
+      <c r="J14" s="168"/>
+      <c r="K14" s="168"/>
+      <c r="L14" s="168"/>
+      <c r="M14" s="168"/>
+      <c r="N14" s="168"/>
+      <c r="O14" s="168"/>
+      <c r="P14" s="168"/>
+      <c r="Q14" s="168"/>
+      <c r="R14" s="168"/>
+      <c r="S14" s="168"/>
+      <c r="T14" s="168"/>
+      <c r="U14" s="168"/>
+      <c r="V14" s="168"/>
+      <c r="W14" s="168"/>
+      <c r="X14" s="168"/>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B15" s="162" t="s">
+      <c r="B15" s="161" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="162"/>
-      <c r="D15" s="169" t="s">
+      <c r="C15" s="161"/>
+      <c r="D15" s="168" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="169"/>
-      <c r="F15" s="169"/>
-      <c r="G15" s="169"/>
-      <c r="H15" s="169"/>
-      <c r="I15" s="169"/>
-      <c r="J15" s="169"/>
-      <c r="K15" s="169"/>
-      <c r="L15" s="169"/>
-      <c r="M15" s="169"/>
-      <c r="N15" s="169"/>
-      <c r="O15" s="169"/>
-      <c r="P15" s="169"/>
-      <c r="Q15" s="169"/>
-      <c r="R15" s="169"/>
-      <c r="S15" s="169"/>
-      <c r="T15" s="169"/>
-      <c r="U15" s="169"/>
-      <c r="V15" s="169"/>
-      <c r="W15" s="169"/>
-      <c r="X15" s="169"/>
+      <c r="E15" s="168"/>
+      <c r="F15" s="168"/>
+      <c r="G15" s="168"/>
+      <c r="H15" s="168"/>
+      <c r="I15" s="168"/>
+      <c r="J15" s="168"/>
+      <c r="K15" s="168"/>
+      <c r="L15" s="168"/>
+      <c r="M15" s="168"/>
+      <c r="N15" s="168"/>
+      <c r="O15" s="168"/>
+      <c r="P15" s="168"/>
+      <c r="Q15" s="168"/>
+      <c r="R15" s="168"/>
+      <c r="S15" s="168"/>
+      <c r="T15" s="168"/>
+      <c r="U15" s="168"/>
+      <c r="V15" s="168"/>
+      <c r="W15" s="168"/>
+      <c r="X15" s="168"/>
     </row>
     <row r="17" spans="3:67" x14ac:dyDescent="0.15">
-      <c r="D17" s="162" t="s">
+      <c r="D17" s="161" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="162"/>
-      <c r="F17" s="162"/>
+      <c r="E17" s="161"/>
+      <c r="F17" s="161"/>
       <c r="G17" s="85" t="s">
         <v>0</v>
       </c>
@@ -5752,21 +5765,21 @@
       <c r="BF17" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="BG17" s="164" t="s">
+      <c r="BG17" s="163" t="s">
         <v>7</v>
       </c>
-      <c r="BH17" s="164"/>
-      <c r="BI17" s="164"/>
-      <c r="BJ17" s="164"/>
-      <c r="BK17" s="163" t="s">
+      <c r="BH17" s="163"/>
+      <c r="BI17" s="163"/>
+      <c r="BJ17" s="163"/>
+      <c r="BK17" s="162" t="s">
         <v>5</v>
       </c>
-      <c r="BL17" s="163"/>
-      <c r="BM17" s="162" t="s">
+      <c r="BL17" s="162"/>
+      <c r="BM17" s="161" t="s">
         <v>6</v>
       </c>
-      <c r="BN17" s="162"/>
-      <c r="BO17" s="162"/>
+      <c r="BN17" s="161"/>
+      <c r="BO17" s="161"/>
     </row>
     <row r="18" spans="3:67" x14ac:dyDescent="0.15">
       <c r="C18" s="96" t="s">
@@ -5966,57 +5979,57 @@
       </c>
     </row>
     <row r="20" spans="3:67" x14ac:dyDescent="0.15">
-      <c r="I20" s="152" t="s">
+      <c r="I20" s="151" t="s">
         <v>170</v>
       </c>
-      <c r="J20" s="153"/>
-      <c r="K20" s="153"/>
-      <c r="L20" s="153"/>
-      <c r="M20" s="153"/>
-      <c r="N20" s="153"/>
-      <c r="O20" s="153"/>
-      <c r="P20" s="153"/>
-      <c r="Q20" s="153"/>
-      <c r="R20" s="153"/>
-      <c r="S20" s="153"/>
-      <c r="T20" s="153"/>
-      <c r="U20" s="153"/>
-      <c r="V20" s="153"/>
-      <c r="W20" s="153"/>
-      <c r="X20" s="153"/>
-      <c r="Y20" s="153"/>
-      <c r="Z20" s="153"/>
-      <c r="AA20" s="153"/>
-      <c r="AB20" s="153"/>
-      <c r="AC20" s="153"/>
-      <c r="AD20" s="153"/>
-      <c r="AE20" s="153"/>
-      <c r="AF20" s="153"/>
-      <c r="AG20" s="153"/>
-      <c r="AH20" s="153"/>
-      <c r="AI20" s="153"/>
-      <c r="AJ20" s="153"/>
-      <c r="AK20" s="153"/>
-      <c r="AL20" s="153"/>
-      <c r="AM20" s="153"/>
-      <c r="AN20" s="153"/>
-      <c r="AO20" s="153"/>
-      <c r="AP20" s="153"/>
-      <c r="AQ20" s="153"/>
-      <c r="AR20" s="153"/>
-      <c r="AS20" s="153"/>
-      <c r="AT20" s="153"/>
-      <c r="AU20" s="153"/>
-      <c r="AV20" s="153"/>
-      <c r="AW20" s="153"/>
-      <c r="AX20" s="153"/>
-      <c r="AY20" s="153"/>
-      <c r="AZ20" s="153"/>
-      <c r="BA20" s="153"/>
-      <c r="BB20" s="153"/>
-      <c r="BC20" s="153"/>
-      <c r="BD20" s="153"/>
-      <c r="BE20" s="154"/>
+      <c r="J20" s="152"/>
+      <c r="K20" s="152"/>
+      <c r="L20" s="152"/>
+      <c r="M20" s="152"/>
+      <c r="N20" s="152"/>
+      <c r="O20" s="152"/>
+      <c r="P20" s="152"/>
+      <c r="Q20" s="152"/>
+      <c r="R20" s="152"/>
+      <c r="S20" s="152"/>
+      <c r="T20" s="152"/>
+      <c r="U20" s="152"/>
+      <c r="V20" s="152"/>
+      <c r="W20" s="152"/>
+      <c r="X20" s="152"/>
+      <c r="Y20" s="152"/>
+      <c r="Z20" s="152"/>
+      <c r="AA20" s="152"/>
+      <c r="AB20" s="152"/>
+      <c r="AC20" s="152"/>
+      <c r="AD20" s="152"/>
+      <c r="AE20" s="152"/>
+      <c r="AF20" s="152"/>
+      <c r="AG20" s="152"/>
+      <c r="AH20" s="152"/>
+      <c r="AI20" s="152"/>
+      <c r="AJ20" s="152"/>
+      <c r="AK20" s="152"/>
+      <c r="AL20" s="152"/>
+      <c r="AM20" s="152"/>
+      <c r="AN20" s="152"/>
+      <c r="AO20" s="152"/>
+      <c r="AP20" s="152"/>
+      <c r="AQ20" s="152"/>
+      <c r="AR20" s="152"/>
+      <c r="AS20" s="152"/>
+      <c r="AT20" s="152"/>
+      <c r="AU20" s="152"/>
+      <c r="AV20" s="152"/>
+      <c r="AW20" s="152"/>
+      <c r="AX20" s="152"/>
+      <c r="AY20" s="152"/>
+      <c r="AZ20" s="152"/>
+      <c r="BA20" s="152"/>
+      <c r="BB20" s="152"/>
+      <c r="BC20" s="152"/>
+      <c r="BD20" s="152"/>
+      <c r="BE20" s="153"/>
     </row>
     <row r="21" spans="3:67" x14ac:dyDescent="0.15">
       <c r="I21" s="127">
@@ -6225,17 +6238,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B2" s="152" t="s">
+      <c r="B2" s="151" t="s">
         <v>167</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="154"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="153"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B5" s="155" t="s">
+      <c r="B5" s="154" t="s">
         <v>147</v>
       </c>
-      <c r="C5" s="155"/>
+      <c r="C5" s="154"/>
       <c r="E5" s="94"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.15">
@@ -6314,10 +6327,10 @@
       <c r="H10" s="77"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B12" s="155" t="s">
+      <c r="B12" s="154" t="s">
         <v>147</v>
       </c>
-      <c r="C12" s="155"/>
+      <c r="C12" s="154"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B13" s="15">
@@ -6376,11 +6389,11 @@
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B21" s="156" t="s">
+      <c r="B21" s="155" t="s">
         <v>154</v>
       </c>
-      <c r="C21" s="157"/>
-      <c r="D21" s="158"/>
+      <c r="C21" s="156"/>
+      <c r="D21" s="157"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -6410,11 +6423,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B2" s="175" t="s">
+      <c r="B2" s="174" t="s">
         <v>123</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B4" s="15">
@@ -6499,111 +6512,111 @@
       <c r="B5" s="26">
         <v>5</v>
       </c>
-      <c r="C5" s="176" t="s">
+      <c r="C5" s="175" t="s">
         <v>120</v>
       </c>
       <c r="D5" s="98" t="s">
         <v>79</v>
       </c>
-      <c r="F5" s="188" t="s">
+      <c r="F5" s="187" t="s">
         <v>153</v>
       </c>
-      <c r="G5" s="189"/>
-      <c r="H5" s="190"/>
+      <c r="G5" s="188"/>
+      <c r="H5" s="189"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B6" s="26">
         <v>6</v>
       </c>
-      <c r="C6" s="177"/>
+      <c r="C6" s="176"/>
       <c r="D6" s="99" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="191" t="s">
+      <c r="F6" s="190" t="s">
         <v>156</v>
       </c>
-      <c r="G6" s="192"/>
-      <c r="H6" s="193"/>
+      <c r="G6" s="191"/>
+      <c r="H6" s="192"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B7" s="26">
         <v>7</v>
       </c>
-      <c r="C7" s="177"/>
+      <c r="C7" s="176"/>
       <c r="D7" s="99" t="s">
         <v>82</v>
       </c>
-      <c r="F7" s="191" t="s">
+      <c r="F7" s="190" t="s">
         <v>157</v>
       </c>
-      <c r="G7" s="192"/>
-      <c r="H7" s="193"/>
+      <c r="G7" s="191"/>
+      <c r="H7" s="192"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B8" s="26">
         <v>8</v>
       </c>
-      <c r="C8" s="178"/>
+      <c r="C8" s="177"/>
       <c r="D8" s="100" t="s">
         <v>81</v>
       </c>
-      <c r="F8" s="194" t="s">
+      <c r="F8" s="193" t="s">
         <v>158</v>
       </c>
-      <c r="G8" s="195"/>
-      <c r="H8" s="196"/>
+      <c r="G8" s="194"/>
+      <c r="H8" s="195"/>
     </row>
     <row r="9" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="26">
         <v>9</v>
       </c>
-      <c r="C9" s="185" t="s">
+      <c r="C9" s="184" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="F9" s="179" t="s">
+      <c r="F9" s="178" t="s">
         <v>155</v>
       </c>
-      <c r="G9" s="180"/>
-      <c r="H9" s="181"/>
+      <c r="G9" s="179"/>
+      <c r="H9" s="180"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B10" s="26">
         <v>10</v>
       </c>
-      <c r="C10" s="186"/>
+      <c r="C10" s="185"/>
       <c r="D10" s="102" t="s">
         <v>80</v>
       </c>
-      <c r="F10" s="179"/>
-      <c r="G10" s="180"/>
-      <c r="H10" s="181"/>
+      <c r="F10" s="178"/>
+      <c r="G10" s="179"/>
+      <c r="H10" s="180"/>
     </row>
     <row r="11" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="26">
         <v>11</v>
       </c>
-      <c r="C11" s="186"/>
+      <c r="C11" s="185"/>
       <c r="D11" s="102" t="s">
         <v>82</v>
       </c>
-      <c r="F11" s="179"/>
-      <c r="G11" s="180"/>
-      <c r="H11" s="181"/>
+      <c r="F11" s="178"/>
+      <c r="G11" s="179"/>
+      <c r="H11" s="180"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B12" s="26">
         <v>12</v>
       </c>
-      <c r="C12" s="187"/>
+      <c r="C12" s="186"/>
       <c r="D12" s="103" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="179"/>
-      <c r="G12" s="180"/>
-      <c r="H12" s="181"/>
+      <c r="F12" s="178"/>
+      <c r="G12" s="179"/>
+      <c r="H12" s="180"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B13" s="26">
@@ -6613,9 +6626,9 @@
         <v>0</v>
       </c>
       <c r="D13" s="105"/>
-      <c r="F13" s="179"/>
-      <c r="G13" s="180"/>
-      <c r="H13" s="181"/>
+      <c r="F13" s="178"/>
+      <c r="G13" s="179"/>
+      <c r="H13" s="180"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B14" s="26">
@@ -6625,9 +6638,9 @@
         <v>20</v>
       </c>
       <c r="D14" s="107"/>
-      <c r="F14" s="182"/>
-      <c r="G14" s="183"/>
-      <c r="H14" s="184"/>
+      <c r="F14" s="181"/>
+      <c r="G14" s="182"/>
+      <c r="H14" s="183"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -6647,7 +6660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -6663,10 +6676,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B3" s="152" t="s">
+      <c r="B3" s="151" t="s">
         <v>175</v>
       </c>
-      <c r="C3" s="154"/>
+      <c r="C3" s="153"/>
       <c r="D3" s="95"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.15">
@@ -6724,7 +6737,7 @@
       <c r="B8" s="15">
         <v>6</v>
       </c>
-      <c r="C8" s="141" t="s">
+      <c r="C8" s="139" t="s">
         <v>176</v>
       </c>
       <c r="D8" s="28" t="s">
@@ -6742,7 +6755,7 @@
       <c r="B9" s="26">
         <v>7</v>
       </c>
-      <c r="C9" s="142"/>
+      <c r="C9" s="140"/>
       <c r="D9" s="29" t="s">
         <v>80</v>
       </c>
@@ -6758,7 +6771,7 @@
       <c r="B10" s="15">
         <v>8</v>
       </c>
-      <c r="C10" s="141" t="s">
+      <c r="C10" s="139" t="s">
         <v>177</v>
       </c>
       <c r="D10" s="28" t="s">
@@ -6776,7 +6789,7 @@
       <c r="B11" s="15">
         <v>9</v>
       </c>
-      <c r="C11" s="142"/>
+      <c r="C11" s="140"/>
       <c r="D11" s="29" t="s">
         <v>80</v>
       </c>
@@ -6882,10 +6895,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:I21"/>
+  <dimension ref="B2:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C22" sqref="C22:D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -6899,17 +6912,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B2" s="152" t="s">
+      <c r="B2" s="151" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="154"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="153"/>
     </row>
     <row r="5" spans="2:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="155" t="s">
+      <c r="B5" s="154" t="s">
         <v>147</v>
       </c>
-      <c r="C5" s="155"/>
+      <c r="C5" s="154"/>
       <c r="E5" s="94"/>
       <c r="F5" s="94"/>
     </row>
@@ -6923,10 +6936,10 @@
       <c r="D6" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="F6" s="198" t="s">
+      <c r="F6" s="197" t="s">
         <v>124</v>
       </c>
-      <c r="G6" s="198"/>
+      <c r="G6" s="197"/>
       <c r="H6" s="5"/>
       <c r="I6" s="73"/>
     </row>
@@ -7005,16 +7018,16 @@
       <c r="B12" s="75" t="s">
         <v>146</v>
       </c>
-      <c r="F12" s="151" t="s">
+      <c r="F12" s="149" t="s">
         <v>10</v>
       </c>
       <c r="G12" s="43"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B13" s="197" t="s">
+      <c r="B13" s="196" t="s">
         <v>123</v>
       </c>
-      <c r="C13" s="197"/>
+      <c r="C13" s="196"/>
       <c r="F13" s="13" t="s">
         <v>184</v>
       </c>
@@ -7024,11 +7037,11 @@
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B14" s="156" t="s">
+      <c r="B14" s="155" t="s">
         <v>154</v>
       </c>
-      <c r="C14" s="157"/>
-      <c r="D14" s="158"/>
+      <c r="C14" s="156"/>
+      <c r="D14" s="157"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B16" s="15">
@@ -7076,20 +7089,31 @@
       <c r="B20" s="15">
         <v>7</v>
       </c>
-      <c r="C20" s="147" t="s">
+      <c r="C20" s="145" t="s">
         <v>183</v>
       </c>
-      <c r="D20" s="148" t="s">
+      <c r="D20" s="146" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B21" s="15">
+        <v>7</v>
+      </c>
+      <c r="C21" s="147"/>
+      <c r="D21" s="148" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B22" s="15">
         <v>8</v>
       </c>
-      <c r="C21" s="149"/>
-      <c r="D21" s="150" t="s">
-        <v>80</v>
+      <c r="C22" s="150" t="s">
+        <v>124</v>
+      </c>
+      <c r="D22" s="55" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -7125,17 +7149,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B2" s="152" t="s">
+      <c r="B2" s="151" t="s">
         <v>160</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="154"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="153"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B5" s="155" t="s">
+      <c r="B5" s="154" t="s">
         <v>147</v>
       </c>
-      <c r="C5" s="155"/>
+      <c r="C5" s="154"/>
       <c r="E5" s="94"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.15">
@@ -7201,10 +7225,10 @@
       <c r="B10" s="26">
         <v>7</v>
       </c>
-      <c r="C10" s="143" t="s">
+      <c r="C10" s="141" t="s">
         <v>125</v>
       </c>
-      <c r="D10" s="144" t="s">
+      <c r="D10" s="142" t="s">
         <v>79</v>
       </c>
       <c r="F10" s="49"/>
@@ -7215,8 +7239,8 @@
       <c r="B11" s="26">
         <v>7</v>
       </c>
-      <c r="C11" s="145"/>
-      <c r="D11" s="146" t="s">
+      <c r="C11" s="143"/>
+      <c r="D11" s="144" t="s">
         <v>80</v>
       </c>
     </row>
@@ -7226,11 +7250,11 @@
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B15" s="156" t="s">
+      <c r="B15" s="155" t="s">
         <v>154</v>
       </c>
-      <c r="C15" s="157"/>
-      <c r="D15" s="158"/>
+      <c r="C15" s="156"/>
+      <c r="D15" s="157"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Removed some items on ImuGetData enum
</commit_message>
<xml_diff>
--- a/doc/DATA_PROTOCOL_SENSUS.xlsx
+++ b/doc/DATA_PROTOCOL_SENSUS.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="191">
   <si>
     <t>CMD</t>
   </si>
@@ -236,9 +236,6 @@
     <t>IMU_COMPASS_DISABLE</t>
   </si>
   <si>
-    <t>accelerometer, gyroscope, magnetometer (normalized)</t>
-  </si>
-  <si>
     <t>quaternions</t>
   </si>
   <si>
@@ -434,9 +431,6 @@
     <t>GET_ALL_DATA</t>
   </si>
   <si>
-    <t>quaternions, linear acceleration</t>
-  </si>
-  <si>
     <t>quaternions,linear acceleration,accelerometer, gyroscope, magnetometer</t>
   </si>
   <si>
@@ -614,16 +608,10 @@
     <t>IMU_GET_ALL_DATA</t>
   </si>
   <si>
-    <t>IMU_GET_DATA_COMPONENT_SENSOR_NORMALIZED</t>
-  </si>
-  <si>
     <t>IMU_GET_DATA_QUATERNION</t>
   </si>
   <si>
     <t>IMU_GET_DATA_LINEARACCELERATION</t>
-  </si>
-  <si>
-    <t>IMU_GET_DATA_QUATERNION_LINEARACCELERATION</t>
   </si>
 </sst>
 </file>
@@ -1483,6 +1471,13 @@
     <xf numFmtId="0" fontId="4" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1624,6 +1619,27 @@
     <xf numFmtId="0" fontId="2" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1674,34 +1690,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2070,10 +2058,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F46"/>
+  <dimension ref="B2:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="E33" sqref="E33:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
@@ -2109,7 +2097,7 @@
       </c>
       <c r="C3" s="16"/>
       <c r="D3" s="16" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E3" s="16"/>
       <c r="F3" s="17"/>
@@ -2120,7 +2108,7 @@
       </c>
       <c r="C4" s="16"/>
       <c r="D4" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="17"/>
@@ -2131,7 +2119,7 @@
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="16" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="17"/>
@@ -2142,7 +2130,7 @@
       </c>
       <c r="C6" s="16"/>
       <c r="D6" s="16" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E6" s="16"/>
       <c r="F6" s="17"/>
@@ -2169,10 +2157,10 @@
         <v>0</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F9" s="21"/>
     </row>
@@ -2183,7 +2171,7 @@
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F10" s="21"/>
     </row>
@@ -2194,7 +2182,7 @@
       </c>
       <c r="D11" s="20"/>
       <c r="E11" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F11" s="21"/>
     </row>
@@ -2205,7 +2193,7 @@
       </c>
       <c r="D12" s="20"/>
       <c r="E12" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F12" s="21"/>
     </row>
@@ -2224,17 +2212,17 @@
         <v>0</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="E14" s="137"/>
-      <c r="F14" s="2"/>
+        <v>171</v>
+      </c>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B15" s="137"/>
       <c r="C15" s="137"/>
       <c r="D15" s="137"/>
-      <c r="E15" s="137"/>
-      <c r="F15" s="2"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B16" s="20">
@@ -2244,7 +2232,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E16" s="20"/>
       <c r="F16" s="21"/>
@@ -2264,10 +2252,10 @@
         <v>0</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F18" s="21"/>
     </row>
@@ -2278,7 +2266,7 @@
       </c>
       <c r="D19" s="20"/>
       <c r="E19" s="20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F19" s="21"/>
     </row>
@@ -2297,10 +2285,10 @@
         <v>0</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E21" s="20" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F21" s="21"/>
     </row>
@@ -2319,10 +2307,10 @@
         <v>0</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F23" s="20"/>
     </row>
@@ -2333,7 +2321,7 @@
       </c>
       <c r="D24" s="20"/>
       <c r="E24" s="20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F24" s="20"/>
     </row>
@@ -2352,7 +2340,7 @@
         <v>0</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E26" s="18"/>
       <c r="F26" s="19"/>
@@ -2365,7 +2353,7 @@
         <v>0</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E27" s="18"/>
       <c r="F27" s="19"/>
@@ -2440,10 +2428,10 @@
         <v>27</v>
       </c>
       <c r="E33" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="F33" s="19" t="s">
         <v>130</v>
-      </c>
-      <c r="F33" s="19" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.15">
@@ -2453,10 +2441,10 @@
       </c>
       <c r="D34" s="18"/>
       <c r="E34" s="18" t="s">
-        <v>28</v>
+        <v>189</v>
       </c>
       <c r="F34" s="19" t="s">
-        <v>30</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.15">
@@ -2466,10 +2454,10 @@
       </c>
       <c r="D35" s="18"/>
       <c r="E35" s="18" t="s">
-        <v>31</v>
+        <v>190</v>
       </c>
       <c r="F35" s="19" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.15">
@@ -2479,44 +2467,38 @@
       </c>
       <c r="D36" s="18"/>
       <c r="E36" s="18" t="s">
-        <v>32</v>
+        <v>187</v>
       </c>
       <c r="F36" s="19" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B37" s="18"/>
-      <c r="C37" s="18">
-        <v>4</v>
-      </c>
-      <c r="D37" s="18"/>
-      <c r="E37" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="F37" s="19" t="s">
-        <v>67</v>
-      </c>
+      <c r="B37" s="82"/>
+      <c r="C37" s="82"/>
+      <c r="D37" s="82"/>
+      <c r="E37" s="82"/>
+      <c r="F37" s="2"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B38" s="18"/>
-      <c r="C38" s="18">
-        <v>5</v>
-      </c>
-      <c r="D38" s="18"/>
-      <c r="E38" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F38" s="19" t="s">
-        <v>131</v>
-      </c>
+      <c r="B38" s="82"/>
+      <c r="C38" s="82"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="82"/>
+      <c r="F38" s="2"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B39" s="82"/>
-      <c r="C39" s="82"/>
-      <c r="D39" s="82"/>
-      <c r="E39" s="82"/>
-      <c r="F39" s="2"/>
+      <c r="B39" s="130">
+        <v>250</v>
+      </c>
+      <c r="C39" s="130">
+        <v>0</v>
+      </c>
+      <c r="D39" s="130" t="s">
+        <v>170</v>
+      </c>
+      <c r="E39" s="130"/>
+      <c r="F39" s="131"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B40" s="82"/>
@@ -2526,62 +2508,28 @@
       <c r="F40" s="2"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B41" s="82"/>
-      <c r="C41" s="82"/>
-      <c r="D41" s="82"/>
-      <c r="E41" s="82"/>
-      <c r="F41" s="2"/>
+      <c r="B41" s="164">
+        <v>254</v>
+      </c>
+      <c r="C41" s="164">
+        <v>0</v>
+      </c>
+      <c r="D41" s="164" t="s">
+        <v>184</v>
+      </c>
+      <c r="E41" s="164"/>
+      <c r="F41" s="165"/>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B42" s="82"/>
-      <c r="C42" s="82"/>
-      <c r="D42" s="82"/>
-      <c r="E42" s="82"/>
-      <c r="F42" s="2"/>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B43" s="130">
-        <v>250</v>
-      </c>
-      <c r="C43" s="130">
-        <v>0</v>
-      </c>
-      <c r="D43" s="130" t="s">
-        <v>172</v>
-      </c>
-      <c r="E43" s="130"/>
-      <c r="F43" s="131"/>
-    </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B44" s="82"/>
-      <c r="C44" s="82"/>
-      <c r="D44" s="82"/>
-      <c r="E44" s="82"/>
-      <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B45" s="164">
-        <v>254</v>
-      </c>
-      <c r="C45" s="164">
-        <v>0</v>
-      </c>
-      <c r="D45" s="164" t="s">
-        <v>186</v>
-      </c>
-      <c r="E45" s="164"/>
-      <c r="F45" s="165"/>
-    </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B46" s="107">
+      <c r="B42" s="107">
         <v>255</v>
       </c>
-      <c r="C46" s="107"/>
-      <c r="D46" s="107" t="s">
-        <v>152</v>
-      </c>
-      <c r="E46" s="107"/>
-      <c r="F46" s="108"/>
+      <c r="C42" s="107"/>
+      <c r="D42" s="107" t="s">
+        <v>150</v>
+      </c>
+      <c r="E42" s="107"/>
+      <c r="F42" s="108"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2609,17 +2557,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B2" s="166" t="s">
-        <v>160</v>
-      </c>
-      <c r="C2" s="167"/>
-      <c r="D2" s="168"/>
+      <c r="B2" s="169" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="170"/>
+      <c r="D2" s="171"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B5" s="169" t="s">
-        <v>147</v>
-      </c>
-      <c r="C5" s="169"/>
+      <c r="B5" s="172" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="172"/>
       <c r="E5" s="93"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.15">
@@ -2630,7 +2578,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F6" s="85" t="s">
         <v>10</v>
@@ -2645,10 +2593,10 @@
         <v>10</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="7">
@@ -2660,10 +2608,10 @@
         <v>5</v>
       </c>
       <c r="C8" s="87" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F8" s="48"/>
       <c r="G8" s="48"/>
@@ -2675,7 +2623,7 @@
       </c>
       <c r="C9" s="88"/>
       <c r="D9" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F9" s="48"/>
       <c r="G9" s="48"/>
@@ -2686,10 +2634,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="140" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D10" s="141" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F10" s="48"/>
       <c r="G10" s="48"/>
@@ -2701,20 +2649,20 @@
       </c>
       <c r="C11" s="142"/>
       <c r="D11" s="143" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B14" s="74" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B15" s="170" t="s">
-        <v>154</v>
-      </c>
-      <c r="C15" s="171"/>
-      <c r="D15" s="172"/>
+      <c r="B15" s="173" t="s">
+        <v>152</v>
+      </c>
+      <c r="C15" s="174"/>
+      <c r="D15" s="175"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2747,11 +2695,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.15">
-      <c r="B2" s="166" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" s="167"/>
-      <c r="D2" s="168"/>
+      <c r="B2" s="169" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="170"/>
+      <c r="D2" s="171"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B5" s="14">
@@ -2761,10 +2709,10 @@
         <v>0</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G5" s="26" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.15">
@@ -2775,10 +2723,10 @@
         <v>10</v>
       </c>
       <c r="D6" s="29" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H6" s="13"/>
       <c r="I6" s="7">
@@ -2789,17 +2737,17 @@
       <c r="B7" s="25">
         <v>5</v>
       </c>
-      <c r="C7" s="235" t="s">
-        <v>76</v>
+      <c r="C7" s="221" t="s">
+        <v>75</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E7" s="125" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H7" s="13"/>
       <c r="I7" s="7">
@@ -2810,12 +2758,12 @@
       <c r="B8" s="25">
         <v>6</v>
       </c>
-      <c r="C8" s="236"/>
+      <c r="C8" s="222"/>
       <c r="D8" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H8" s="13"/>
       <c r="I8" s="7">
@@ -2824,7 +2772,7 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.15">
       <c r="G9" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H9" s="13"/>
       <c r="I9" s="7">
@@ -2839,10 +2787,10 @@
         <v>0</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.15">
@@ -2853,13 +2801,13 @@
         <v>10</v>
       </c>
       <c r="D12" s="29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I12" s="7">
         <v>0</v>
@@ -2869,20 +2817,20 @@
       <c r="B13" s="25">
         <v>5</v>
       </c>
-      <c r="C13" s="235" t="s">
-        <v>76</v>
+      <c r="C13" s="221" t="s">
+        <v>75</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E13" s="125" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I13" s="7">
         <v>1</v>
@@ -2892,15 +2840,15 @@
       <c r="B14" s="25">
         <v>6</v>
       </c>
-      <c r="C14" s="236"/>
+      <c r="C14" s="222"/>
       <c r="D14" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H14" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I14" s="7">
         <v>2</v>
@@ -2911,40 +2859,40 @@
         <v>7</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D15" s="38"/>
       <c r="G15" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H15" s="36" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I15" s="8">
         <v>3</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B16" s="25">
         <v>8</v>
       </c>
-      <c r="C16" s="230" t="s">
-        <v>165</v>
+      <c r="C16" s="216" t="s">
+        <v>163</v>
       </c>
       <c r="D16" s="123" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E16" s="125" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H16" s="36" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I16" s="8">
         <v>4</v>
@@ -2954,9 +2902,9 @@
       <c r="B17" s="25">
         <v>9</v>
       </c>
-      <c r="C17" s="231"/>
+      <c r="C17" s="217"/>
       <c r="D17" s="124" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="36"/>
@@ -2970,7 +2918,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="86" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.15">
@@ -2981,38 +2929,38 @@
         <v>10</v>
       </c>
       <c r="D21" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" s="232" t="s">
-        <v>90</v>
-      </c>
-      <c r="H21" s="233"/>
-      <c r="I21" s="234"/>
+        <v>70</v>
+      </c>
+      <c r="G21" s="218" t="s">
+        <v>89</v>
+      </c>
+      <c r="H21" s="219"/>
+      <c r="I21" s="220"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B22" s="14">
         <v>5</v>
       </c>
-      <c r="C22" s="235" t="s">
-        <v>76</v>
+      <c r="C22" s="221" t="s">
+        <v>75</v>
       </c>
       <c r="D22" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E22" s="125" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B23" s="14">
         <v>6</v>
       </c>
-      <c r="C23" s="236"/>
+      <c r="C23" s="222"/>
       <c r="D23" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.15">
@@ -3020,35 +2968,35 @@
         <v>7</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D24" s="38"/>
       <c r="G24" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H24" s="15"/>
       <c r="I24" s="7">
         <v>0</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B25" s="14">
         <v>8</v>
       </c>
-      <c r="C25" s="230" t="s">
+      <c r="C25" s="216" t="s">
+        <v>162</v>
+      </c>
+      <c r="D25" s="123" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="125" t="s">
         <v>164</v>
       </c>
-      <c r="D25" s="123" t="s">
-        <v>79</v>
-      </c>
-      <c r="E25" s="125" t="s">
-        <v>166</v>
-      </c>
       <c r="G25" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H25" s="15"/>
       <c r="I25" s="7">
@@ -3059,12 +3007,12 @@
       <c r="B26" s="14">
         <v>9</v>
       </c>
-      <c r="C26" s="231"/>
+      <c r="C26" s="217"/>
       <c r="D26" s="124" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H26" s="15"/>
       <c r="I26" s="7">
@@ -3076,11 +3024,11 @@
         <v>10</v>
       </c>
       <c r="C27" s="154" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D27" s="50"/>
       <c r="G27" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H27" s="36"/>
       <c r="I27" s="8">
@@ -3092,10 +3040,10 @@
         <v>11</v>
       </c>
       <c r="C28" s="155" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D28" s="156" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.15">
@@ -3103,13 +3051,13 @@
         <v>12</v>
       </c>
       <c r="C29" s="112" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="31" t="s">
         <v>78</v>
       </c>
-      <c r="D29" s="31" t="s">
-        <v>79</v>
-      </c>
       <c r="G29" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.15">
@@ -3118,10 +3066,10 @@
       </c>
       <c r="C30" s="113"/>
       <c r="D30" s="52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G30" s="37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H30" s="13"/>
       <c r="I30" s="7">
@@ -3134,10 +3082,10 @@
       </c>
       <c r="C31" s="113"/>
       <c r="D31" s="52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G31" s="37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H31" s="13"/>
       <c r="I31" s="7">
@@ -3150,7 +3098,7 @@
       </c>
       <c r="C32" s="114"/>
       <c r="D32" s="53" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.15">
@@ -3158,7 +3106,7 @@
         <v>16</v>
       </c>
       <c r="C33" s="35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D33" s="51"/>
     </row>
@@ -3167,10 +3115,10 @@
         <v>17</v>
       </c>
       <c r="C34" s="115" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D34" s="117" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.15">
@@ -3179,7 +3127,7 @@
       </c>
       <c r="C35" s="116"/>
       <c r="D35" s="118" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -3203,13 +3151,13 @@
   <dimension ref="B2:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="9.1640625" style="3"/>
-    <col min="2" max="2" width="6.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.5" style="3" bestFit="1" customWidth="1"/>
@@ -3220,11 +3168,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B2" s="166" t="s">
+      <c r="B2" s="169" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="167"/>
-      <c r="D2" s="168"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="171"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B3" s="57"/>
@@ -3232,10 +3180,10 @@
       <c r="D3" s="57"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B4" s="169" t="s">
-        <v>147</v>
-      </c>
-      <c r="C4" s="169"/>
+      <c r="B4" s="172" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="172"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B5" s="14">
@@ -3352,11 +3300,11 @@
       <c r="B12" s="14">
         <v>10</v>
       </c>
-      <c r="C12" s="230" t="s">
-        <v>165</v>
+      <c r="C12" s="216" t="s">
+        <v>163</v>
       </c>
       <c r="D12" s="123" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E12" s="125"/>
       <c r="F12" s="13" t="s">
@@ -3373,9 +3321,9 @@
       <c r="B13" s="14">
         <v>11</v>
       </c>
-      <c r="C13" s="231"/>
+      <c r="C13" s="217"/>
       <c r="D13" s="124" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F13" s="13" t="s">
         <v>54</v>
@@ -3389,10 +3337,10 @@
       <c r="B14" s="14">
         <v>12</v>
       </c>
-      <c r="C14" s="237" t="s">
-        <v>187</v>
-      </c>
-      <c r="D14" s="238"/>
+      <c r="C14" s="166" t="s">
+        <v>185</v>
+      </c>
+      <c r="D14" s="167"/>
       <c r="F14" s="13" t="s">
         <v>55</v>
       </c>
@@ -3406,10 +3354,10 @@
         <v>13</v>
       </c>
       <c r="C15" s="112" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F15" s="71"/>
       <c r="G15" s="75"/>
@@ -3421,7 +3369,7 @@
       </c>
       <c r="C16" s="113"/>
       <c r="D16" s="52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>61</v>
@@ -3434,7 +3382,7 @@
       </c>
       <c r="C17" s="113"/>
       <c r="D17" s="52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F17" s="13" t="s">
         <v>38</v>
@@ -3452,7 +3400,7 @@
       </c>
       <c r="C18" s="114"/>
       <c r="D18" s="53" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>40</v>
@@ -3477,7 +3425,7 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B21" s="74" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F21" s="89" t="s">
         <v>62</v>
@@ -3485,11 +3433,11 @@
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B22" s="170" t="s">
-        <v>154</v>
-      </c>
-      <c r="C22" s="171"/>
-      <c r="D22" s="172"/>
+      <c r="B22" s="173" t="s">
+        <v>152</v>
+      </c>
+      <c r="C22" s="174"/>
+      <c r="D22" s="175"/>
       <c r="F22" s="13" t="s">
         <v>41</v>
       </c>
@@ -3543,11 +3491,11 @@
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B27" s="166" t="s">
+      <c r="B27" s="169" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="167"/>
-      <c r="D27" s="168"/>
+      <c r="C27" s="170"/>
+      <c r="D27" s="171"/>
       <c r="F27" s="13" t="s">
         <v>46</v>
       </c>
@@ -3565,9 +3513,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="24" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B29" s="157" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C29" s="157"/>
       <c r="F29" s="13" t="s">
@@ -3616,7 +3564,7 @@
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B33" s="74" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F33" s="13" t="s">
         <v>63</v>
@@ -3628,14 +3576,14 @@
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B34" s="158" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C34" s="159"/>
       <c r="D34" s="160"/>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="F35" s="239" t="s">
-        <v>187</v>
+      <c r="F35" s="168" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.15">
@@ -3648,8 +3596,8 @@
       <c r="D36" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="F36" s="13" t="s">
-        <v>190</v>
+      <c r="F36" s="12" t="s">
+        <v>188</v>
       </c>
       <c r="G36" s="13"/>
       <c r="H36" s="7">
@@ -3666,7 +3614,7 @@
       <c r="D37" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="F37" s="13" t="s">
+      <c r="F37" s="12" t="s">
         <v>189</v>
       </c>
       <c r="G37" s="13"/>
@@ -3682,8 +3630,8 @@
         <v>3</v>
       </c>
       <c r="D38" s="34"/>
-      <c r="F38" s="13" t="s">
-        <v>191</v>
+      <c r="F38" s="12" t="s">
+        <v>190</v>
       </c>
       <c r="G38" s="13"/>
       <c r="H38" s="7">
@@ -3698,8 +3646,8 @@
         <v>60</v>
       </c>
       <c r="D39" s="40"/>
-      <c r="F39" s="13" t="s">
-        <v>192</v>
+      <c r="F39" s="12" t="s">
+        <v>187</v>
       </c>
       <c r="G39" s="13"/>
       <c r="H39" s="7">
@@ -3714,13 +3662,6 @@
         <v>61</v>
       </c>
       <c r="D40" s="33"/>
-      <c r="F40" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="G40" s="13"/>
-      <c r="H40" s="7">
-        <v>4</v>
-      </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B41" s="14">
@@ -3730,13 +3671,6 @@
         <v>62</v>
       </c>
       <c r="D41" s="41"/>
-      <c r="F41" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="G41" s="13"/>
-      <c r="H41" s="7">
-        <v>5</v>
-      </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B42" s="14">
@@ -3751,41 +3685,44 @@
       <c r="B43" s="14">
         <v>10</v>
       </c>
-      <c r="C43" s="230" t="s">
-        <v>165</v>
+      <c r="C43" s="216" t="s">
+        <v>163</v>
       </c>
       <c r="D43" s="123" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B44" s="14">
         <v>11</v>
       </c>
-      <c r="C44" s="231"/>
+      <c r="C44" s="217"/>
       <c r="D44" s="124" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B45" s="14">
         <v>12</v>
       </c>
-      <c r="C45" s="237" t="s">
-        <v>187</v>
-      </c>
-      <c r="D45" s="238"/>
+      <c r="C45" s="166" t="s">
+        <v>185</v>
+      </c>
+      <c r="D45" s="167"/>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B46" s="14">
         <v>13</v>
       </c>
       <c r="C46" s="112" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>79</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="F46" s="71"/>
+      <c r="G46" s="71"/>
+      <c r="H46" s="76"/>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B47" s="14">
@@ -3793,7 +3730,7 @@
       </c>
       <c r="C47" s="113"/>
       <c r="D47" s="52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.15">
@@ -3802,7 +3739,7 @@
       </c>
       <c r="C48" s="113"/>
       <c r="D48" s="52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.15">
@@ -3811,7 +3748,7 @@
       </c>
       <c r="C49" s="114"/>
       <c r="D49" s="53" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -3848,36 +3785,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.15">
-      <c r="B2" s="174" t="s">
-        <v>133</v>
-      </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="176"/>
+      <c r="B2" s="177" t="s">
+        <v>131</v>
+      </c>
+      <c r="C2" s="178"/>
+      <c r="D2" s="179"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.15">
-      <c r="B4" s="169" t="s">
-        <v>147</v>
-      </c>
-      <c r="C4" s="169"/>
+      <c r="B4" s="172" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="172"/>
       <c r="E4" s="71"/>
-      <c r="G4" s="213" t="s">
-        <v>162</v>
-      </c>
-      <c r="H4" s="213"/>
-      <c r="I4" s="213"/>
-      <c r="J4" s="213"/>
-      <c r="K4" s="213"/>
-      <c r="L4" s="213"/>
-      <c r="M4" s="213"/>
-      <c r="N4" s="213"/>
-      <c r="O4" s="213"/>
-      <c r="P4" s="213"/>
-      <c r="Q4" s="213"/>
-      <c r="R4" s="213"/>
-      <c r="S4" s="213"/>
-      <c r="T4" s="213"/>
-      <c r="U4" s="213"/>
-      <c r="V4" s="213"/>
+      <c r="G4" s="223" t="s">
+        <v>160</v>
+      </c>
+      <c r="H4" s="223"/>
+      <c r="I4" s="223"/>
+      <c r="J4" s="223"/>
+      <c r="K4" s="223"/>
+      <c r="L4" s="223"/>
+      <c r="M4" s="223"/>
+      <c r="N4" s="223"/>
+      <c r="O4" s="223"/>
+      <c r="P4" s="223"/>
+      <c r="Q4" s="223"/>
+      <c r="R4" s="223"/>
+      <c r="S4" s="223"/>
+      <c r="T4" s="223"/>
+      <c r="U4" s="223"/>
+      <c r="V4" s="223"/>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B5" s="14">
@@ -3950,59 +3887,59 @@
         <v>10</v>
       </c>
       <c r="D6" s="73" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E6" s="71"/>
       <c r="F6" s="77" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G6" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="H6" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="I6" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="J6" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="J6" s="13" t="s">
-        <v>129</v>
-      </c>
       <c r="K6" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="M6" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="N6" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="M6" s="13" t="s">
+      <c r="O6" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="N6" s="13" t="s">
+      <c r="P6" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="O6" s="13" t="s">
+      <c r="Q6" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="P6" s="13" t="s">
+      <c r="R6" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="Q6" s="13" t="s">
+      <c r="S6" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="R6" s="13" t="s">
+      <c r="T6" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="S6" s="13" t="s">
+      <c r="U6" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="T6" s="13" t="s">
+      <c r="V6" s="13" t="s">
         <v>143</v>
-      </c>
-      <c r="U6" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="V6" s="13" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.15">
@@ -4010,31 +3947,31 @@
         <v>28</v>
       </c>
       <c r="G7" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="I7" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="H7" s="13" t="s">
+      <c r="J7" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="K7" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="J7" s="13" t="s">
+      <c r="L7" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="M7" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="N7" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="M7" s="13" t="s">
+      <c r="O7" s="13" t="s">
         <v>143</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="O7" s="13" t="s">
-        <v>145</v>
       </c>
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
@@ -4049,31 +3986,31 @@
         <v>31</v>
       </c>
       <c r="G8" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="I8" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="J8" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="K8" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="J8" s="13" t="s">
+      <c r="L8" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="M8" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="N8" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="M8" s="13" t="s">
+      <c r="O8" s="13" t="s">
         <v>143</v>
-      </c>
-      <c r="N8" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="O8" s="13" t="s">
-        <v>145</v>
       </c>
       <c r="P8" s="13"/>
       <c r="Q8" s="13"/>
@@ -4088,16 +4025,16 @@
         <v>32</v>
       </c>
       <c r="G9" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="H9" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H9" s="13" t="s">
+      <c r="I9" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="J9" s="13" t="s">
         <v>128</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>129</v>
       </c>
       <c r="K9" s="13"/>
       <c r="L9" s="13"/>
@@ -4114,19 +4051,19 @@
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B10" s="74" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F10" s="77" t="s">
         <v>33</v>
       </c>
       <c r="G10" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="I10" s="13" t="s">
         <v>134</v>
-      </c>
-      <c r="H10" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>136</v>
       </c>
       <c r="J10" s="13"/>
       <c r="K10" s="13"/>
@@ -4148,25 +4085,25 @@
         <v>29</v>
       </c>
       <c r="G11" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="H11" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="I11" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="J11" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="J11" s="13" t="s">
-        <v>129</v>
-      </c>
       <c r="K11" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="M11" s="13" t="s">
         <v>134</v>
-      </c>
-      <c r="L11" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="M11" s="13" t="s">
-        <v>136</v>
       </c>
       <c r="N11" s="13"/>
       <c r="O11" s="13"/>
@@ -4179,11 +4116,11 @@
       <c r="V11" s="13"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.15">
-      <c r="B12" s="170" t="s">
-        <v>154</v>
-      </c>
-      <c r="C12" s="171"/>
-      <c r="D12" s="172"/>
+      <c r="B12" s="173" t="s">
+        <v>152</v>
+      </c>
+      <c r="C12" s="174"/>
+      <c r="D12" s="175"/>
       <c r="F12" s="48"/>
       <c r="G12" s="71"/>
       <c r="H12" s="71"/>
@@ -4224,14 +4161,14 @@
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B14" s="78" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B15" s="66">
         <v>0</v>
       </c>
-      <c r="C15" s="217" t="s">
+      <c r="C15" s="227" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="90"/>
@@ -4240,14 +4177,14 @@
       <c r="B16" s="66">
         <v>1</v>
       </c>
-      <c r="C16" s="218"/>
+      <c r="C16" s="228"/>
       <c r="D16" s="91"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B17" s="66">
         <v>2</v>
       </c>
-      <c r="C17" s="219"/>
+      <c r="C17" s="229"/>
       <c r="D17" s="92"/>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.15">
@@ -4269,65 +4206,65 @@
         <v>10</v>
       </c>
       <c r="D19" s="73" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B20" s="14">
         <v>5</v>
       </c>
-      <c r="C20" s="220" t="s">
-        <v>126</v>
+      <c r="C20" s="230" t="s">
+        <v>125</v>
       </c>
       <c r="D20" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B21" s="14">
         <v>6</v>
       </c>
-      <c r="C21" s="221"/>
+      <c r="C21" s="231"/>
       <c r="D21" s="59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B22" s="14">
         <v>7</v>
       </c>
-      <c r="C22" s="221"/>
+      <c r="C22" s="231"/>
       <c r="D22" s="59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B23" s="14">
         <v>8</v>
       </c>
-      <c r="C23" s="221"/>
+      <c r="C23" s="231"/>
       <c r="D23" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B24" s="14">
         <v>9</v>
       </c>
-      <c r="C24" s="220" t="s">
-        <v>127</v>
+      <c r="C24" s="230" t="s">
+        <v>126</v>
       </c>
       <c r="D24" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B25" s="14">
         <v>10</v>
       </c>
-      <c r="C25" s="221"/>
+      <c r="C25" s="231"/>
       <c r="D25" s="59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F25" s="48"/>
       <c r="G25" s="72"/>
@@ -4351,85 +4288,85 @@
       <c r="B26" s="14">
         <v>11</v>
       </c>
-      <c r="C26" s="221"/>
+      <c r="C26" s="231"/>
       <c r="D26" s="59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B27" s="14">
         <v>12</v>
       </c>
-      <c r="C27" s="221"/>
+      <c r="C27" s="231"/>
       <c r="D27" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B28" s="14">
         <v>13</v>
       </c>
-      <c r="C28" s="220" t="s">
-        <v>128</v>
+      <c r="C28" s="230" t="s">
+        <v>127</v>
       </c>
       <c r="D28" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B29" s="14">
         <v>14</v>
       </c>
-      <c r="C29" s="221"/>
+      <c r="C29" s="231"/>
       <c r="D29" s="59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B30" s="14">
         <v>15</v>
       </c>
-      <c r="C30" s="221"/>
+      <c r="C30" s="231"/>
       <c r="D30" s="59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B31" s="14">
         <v>16</v>
       </c>
-      <c r="C31" s="221"/>
+      <c r="C31" s="231"/>
       <c r="D31" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="2:22" x14ac:dyDescent="0.15">
       <c r="B32" s="14">
         <v>17</v>
       </c>
-      <c r="C32" s="220" t="s">
-        <v>129</v>
+      <c r="C32" s="230" t="s">
+        <v>128</v>
       </c>
       <c r="D32" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B33" s="14">
         <v>18</v>
       </c>
-      <c r="C33" s="221"/>
+      <c r="C33" s="231"/>
       <c r="D33" s="59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B34" s="14">
         <v>19</v>
       </c>
-      <c r="C34" s="221"/>
+      <c r="C34" s="231"/>
       <c r="D34" s="59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G34" s="71"/>
       <c r="H34" s="71"/>
@@ -4453,9 +4390,9 @@
       <c r="B35" s="14">
         <v>20</v>
       </c>
-      <c r="C35" s="221"/>
+      <c r="C35" s="231"/>
       <c r="D35" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G35" s="71"/>
       <c r="H35" s="71"/>
@@ -4479,11 +4416,11 @@
       <c r="B36" s="14">
         <v>21</v>
       </c>
-      <c r="C36" s="220" t="s">
-        <v>134</v>
+      <c r="C36" s="230" t="s">
+        <v>132</v>
       </c>
       <c r="D36" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G36" s="71"/>
       <c r="H36" s="71"/>
@@ -4507,9 +4444,9 @@
       <c r="B37" s="14">
         <v>22</v>
       </c>
-      <c r="C37" s="221"/>
+      <c r="C37" s="231"/>
       <c r="D37" s="59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G37" s="71"/>
       <c r="H37" s="71"/>
@@ -4533,9 +4470,9 @@
       <c r="B38" s="14">
         <v>23</v>
       </c>
-      <c r="C38" s="221"/>
+      <c r="C38" s="231"/>
       <c r="D38" s="59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K38" s="71"/>
       <c r="L38" s="71"/>
@@ -4555,9 +4492,9 @@
       <c r="B39" s="14">
         <v>24</v>
       </c>
-      <c r="C39" s="221"/>
+      <c r="C39" s="231"/>
       <c r="D39" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K39" s="71"/>
       <c r="L39" s="71"/>
@@ -4577,11 +4514,11 @@
       <c r="B40" s="14">
         <v>25</v>
       </c>
-      <c r="C40" s="220" t="s">
-        <v>135</v>
+      <c r="C40" s="230" t="s">
+        <v>133</v>
       </c>
       <c r="D40" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K40" s="71"/>
       <c r="L40" s="71"/>
@@ -4601,9 +4538,9 @@
       <c r="B41" s="14">
         <v>26</v>
       </c>
-      <c r="C41" s="221"/>
+      <c r="C41" s="231"/>
       <c r="D41" s="59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G41" s="71"/>
       <c r="H41" s="71"/>
@@ -4627,9 +4564,9 @@
       <c r="B42" s="14">
         <v>27</v>
       </c>
-      <c r="C42" s="221"/>
+      <c r="C42" s="231"/>
       <c r="D42" s="59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G42" s="71"/>
       <c r="H42" s="71"/>
@@ -4653,9 +4590,9 @@
       <c r="B43" s="14">
         <v>28</v>
       </c>
-      <c r="C43" s="221"/>
+      <c r="C43" s="231"/>
       <c r="D43" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G43" s="71"/>
       <c r="H43" s="71"/>
@@ -4679,11 +4616,11 @@
       <c r="B44" s="14">
         <v>29</v>
       </c>
-      <c r="C44" s="220" t="s">
-        <v>136</v>
+      <c r="C44" s="230" t="s">
+        <v>134</v>
       </c>
       <c r="D44" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G44" s="71"/>
       <c r="H44" s="71"/>
@@ -4707,217 +4644,217 @@
       <c r="B45" s="14">
         <v>30</v>
       </c>
-      <c r="C45" s="221"/>
+      <c r="C45" s="231"/>
       <c r="D45" s="59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="46" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B46" s="14">
         <v>31</v>
       </c>
-      <c r="C46" s="221"/>
+      <c r="C46" s="231"/>
       <c r="D46" s="59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="47" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B47" s="14">
         <v>32</v>
       </c>
-      <c r="C47" s="221"/>
+      <c r="C47" s="231"/>
       <c r="D47" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="48" spans="2:23" x14ac:dyDescent="0.15">
       <c r="B48" s="14">
         <v>33</v>
       </c>
-      <c r="C48" s="220" t="s">
-        <v>137</v>
+      <c r="C48" s="230" t="s">
+        <v>135</v>
       </c>
       <c r="D48" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B49" s="14">
         <v>34</v>
       </c>
-      <c r="C49" s="221"/>
+      <c r="C49" s="231"/>
       <c r="D49" s="59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B50" s="14">
         <v>35</v>
       </c>
-      <c r="C50" s="221"/>
+      <c r="C50" s="231"/>
       <c r="D50" s="59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B51" s="14">
         <v>36</v>
       </c>
-      <c r="C51" s="221"/>
+      <c r="C51" s="231"/>
       <c r="D51" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B52" s="14">
         <v>37</v>
       </c>
-      <c r="C52" s="222" t="s">
-        <v>138</v>
+      <c r="C52" s="232" t="s">
+        <v>136</v>
       </c>
       <c r="D52" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B53" s="14">
         <v>38</v>
       </c>
-      <c r="C53" s="223"/>
+      <c r="C53" s="233"/>
       <c r="D53" s="59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B54" s="14">
         <v>39</v>
       </c>
-      <c r="C54" s="223"/>
+      <c r="C54" s="233"/>
       <c r="D54" s="59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B55" s="14">
         <v>40</v>
       </c>
-      <c r="C55" s="224"/>
+      <c r="C55" s="234"/>
       <c r="D55" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B56" s="14">
         <v>41</v>
       </c>
-      <c r="C56" s="220" t="s">
-        <v>139</v>
+      <c r="C56" s="230" t="s">
+        <v>137</v>
       </c>
       <c r="D56" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B57" s="14">
         <v>42</v>
       </c>
-      <c r="C57" s="221"/>
+      <c r="C57" s="231"/>
       <c r="D57" s="59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B58" s="14">
         <v>43</v>
       </c>
-      <c r="C58" s="221"/>
+      <c r="C58" s="231"/>
       <c r="D58" s="59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B59" s="14">
         <v>44</v>
       </c>
-      <c r="C59" s="221"/>
+      <c r="C59" s="231"/>
       <c r="D59" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B60" s="14">
         <v>45</v>
       </c>
-      <c r="C60" s="220" t="s">
-        <v>140</v>
+      <c r="C60" s="230" t="s">
+        <v>138</v>
       </c>
       <c r="D60" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B61" s="14">
         <v>46</v>
       </c>
-      <c r="C61" s="221"/>
+      <c r="C61" s="231"/>
       <c r="D61" s="59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B62" s="14">
         <v>47</v>
       </c>
-      <c r="C62" s="221"/>
+      <c r="C62" s="231"/>
       <c r="D62" s="59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B63" s="14">
         <v>48</v>
       </c>
-      <c r="C63" s="221"/>
+      <c r="C63" s="231"/>
       <c r="D63" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B64" s="14">
         <v>49</v>
       </c>
-      <c r="C64" s="220" t="s">
-        <v>141</v>
+      <c r="C64" s="230" t="s">
+        <v>139</v>
       </c>
       <c r="D64" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B65" s="14">
         <v>50</v>
       </c>
-      <c r="C65" s="221"/>
+      <c r="C65" s="231"/>
       <c r="D65" s="59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B66" s="14">
         <v>51</v>
       </c>
-      <c r="C66" s="221"/>
+      <c r="C66" s="231"/>
       <c r="D66" s="59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B67" s="14">
         <v>52</v>
       </c>
-      <c r="C67" s="221"/>
+      <c r="C67" s="231"/>
       <c r="D67" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.15">
@@ -4942,45 +4879,45 @@
       <c r="B70" s="14">
         <v>55</v>
       </c>
-      <c r="C70" s="214" t="s">
+      <c r="C70" s="224" t="s">
         <v>7</v>
       </c>
       <c r="D70" s="54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B71" s="14">
         <v>56</v>
       </c>
-      <c r="C71" s="215"/>
+      <c r="C71" s="225"/>
       <c r="D71" s="55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B72" s="14">
         <v>57</v>
       </c>
-      <c r="C72" s="215"/>
+      <c r="C72" s="225"/>
       <c r="D72" s="55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B73" s="14">
         <v>58</v>
       </c>
-      <c r="C73" s="216"/>
+      <c r="C73" s="226"/>
       <c r="D73" s="56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B74" s="14">
         <v>59</v>
       </c>
-      <c r="C74" s="225" t="s">
+      <c r="C74" s="235" t="s">
         <v>5</v>
       </c>
       <c r="D74" s="64"/>
@@ -4989,14 +4926,14 @@
       <c r="B75" s="14">
         <v>60</v>
       </c>
-      <c r="C75" s="226"/>
+      <c r="C75" s="236"/>
       <c r="D75" s="65"/>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B76" s="14">
         <v>61</v>
       </c>
-      <c r="C76" s="227" t="s">
+      <c r="C76" s="237" t="s">
         <v>6</v>
       </c>
       <c r="D76" s="61"/>
@@ -5005,26 +4942,26 @@
       <c r="B77" s="14">
         <v>62</v>
       </c>
-      <c r="C77" s="228"/>
+      <c r="C77" s="238"/>
       <c r="D77" s="62"/>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B78" s="14">
         <v>63</v>
       </c>
-      <c r="C78" s="229"/>
+      <c r="C78" s="239"/>
       <c r="D78" s="63"/>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B82" s="78" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B83" s="66">
         <v>0</v>
       </c>
-      <c r="C83" s="217" t="s">
+      <c r="C83" s="227" t="s">
         <v>2</v>
       </c>
       <c r="D83" s="61"/>
@@ -5033,14 +4970,14 @@
       <c r="B84" s="66">
         <v>1</v>
       </c>
-      <c r="C84" s="218"/>
+      <c r="C84" s="228"/>
       <c r="D84" s="62"/>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B85" s="66">
         <v>2</v>
       </c>
-      <c r="C85" s="219"/>
+      <c r="C85" s="229"/>
       <c r="D85" s="63"/>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.15">
@@ -5062,159 +4999,159 @@
         <v>10</v>
       </c>
       <c r="D87" s="73" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B88" s="14">
         <v>5</v>
       </c>
-      <c r="C88" s="220" t="s">
-        <v>142</v>
+      <c r="C88" s="230" t="s">
+        <v>140</v>
       </c>
       <c r="D88" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B89" s="14">
         <v>6</v>
       </c>
-      <c r="C89" s="221"/>
+      <c r="C89" s="231"/>
       <c r="D89" s="59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B90" s="14">
         <v>7</v>
       </c>
-      <c r="C90" s="221"/>
+      <c r="C90" s="231"/>
       <c r="D90" s="59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B91" s="14">
         <v>8</v>
       </c>
-      <c r="C91" s="221"/>
+      <c r="C91" s="231"/>
       <c r="D91" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B92" s="14">
         <v>9</v>
       </c>
-      <c r="C92" s="220" t="s">
-        <v>143</v>
+      <c r="C92" s="230" t="s">
+        <v>141</v>
       </c>
       <c r="D92" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B93" s="14">
         <v>10</v>
       </c>
-      <c r="C93" s="221"/>
+      <c r="C93" s="231"/>
       <c r="D93" s="59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B94" s="14">
         <v>11</v>
       </c>
-      <c r="C94" s="221"/>
+      <c r="C94" s="231"/>
       <c r="D94" s="59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B95" s="14">
         <v>12</v>
       </c>
-      <c r="C95" s="221"/>
+      <c r="C95" s="231"/>
       <c r="D95" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B96" s="14">
         <v>13</v>
       </c>
-      <c r="C96" s="220" t="s">
-        <v>144</v>
+      <c r="C96" s="230" t="s">
+        <v>142</v>
       </c>
       <c r="D96" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B97" s="14">
         <v>14</v>
       </c>
-      <c r="C97" s="221"/>
+      <c r="C97" s="231"/>
       <c r="D97" s="59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B98" s="14">
         <v>15</v>
       </c>
-      <c r="C98" s="221"/>
+      <c r="C98" s="231"/>
       <c r="D98" s="59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B99" s="14">
         <v>16</v>
       </c>
-      <c r="C99" s="221"/>
+      <c r="C99" s="231"/>
       <c r="D99" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B100" s="14">
         <v>17</v>
       </c>
-      <c r="C100" s="220" t="s">
-        <v>145</v>
+      <c r="C100" s="230" t="s">
+        <v>143</v>
       </c>
       <c r="D100" s="58" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B101" s="14">
         <v>18</v>
       </c>
-      <c r="C101" s="221"/>
+      <c r="C101" s="231"/>
       <c r="D101" s="59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B102" s="14">
         <v>19</v>
       </c>
-      <c r="C102" s="221"/>
+      <c r="C102" s="231"/>
       <c r="D102" s="59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="103" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B103" s="14">
         <v>20</v>
       </c>
-      <c r="C103" s="221"/>
+      <c r="C103" s="231"/>
       <c r="D103" s="60" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="104" spans="2:4" x14ac:dyDescent="0.15">
@@ -5463,45 +5400,45 @@
       <c r="B138" s="14">
         <v>55</v>
       </c>
-      <c r="C138" s="214" t="s">
+      <c r="C138" s="224" t="s">
         <v>7</v>
       </c>
       <c r="D138" s="54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="139" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B139" s="14">
         <v>56</v>
       </c>
-      <c r="C139" s="215"/>
+      <c r="C139" s="225"/>
       <c r="D139" s="55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="140" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B140" s="14">
         <v>57</v>
       </c>
-      <c r="C140" s="215"/>
+      <c r="C140" s="225"/>
       <c r="D140" s="55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="141" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B141" s="14">
         <v>58</v>
       </c>
-      <c r="C141" s="216"/>
+      <c r="C141" s="226"/>
       <c r="D141" s="56" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="142" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B142" s="14">
         <v>59</v>
       </c>
-      <c r="C142" s="225" t="s">
+      <c r="C142" s="235" t="s">
         <v>5</v>
       </c>
       <c r="D142" s="64"/>
@@ -5510,14 +5447,14 @@
       <c r="B143" s="14">
         <v>60</v>
       </c>
-      <c r="C143" s="226"/>
+      <c r="C143" s="236"/>
       <c r="D143" s="65"/>
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B144" s="14">
         <v>61</v>
       </c>
-      <c r="C144" s="227" t="s">
+      <c r="C144" s="237" t="s">
         <v>6</v>
       </c>
       <c r="D144" s="61"/>
@@ -5526,14 +5463,14 @@
       <c r="B145" s="14">
         <v>62</v>
       </c>
-      <c r="C145" s="228"/>
+      <c r="C145" s="238"/>
       <c r="D145" s="62"/>
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B146" s="14">
         <v>63</v>
       </c>
-      <c r="C146" s="229"/>
+      <c r="C146" s="239"/>
       <c r="D146" s="63"/>
     </row>
   </sheetData>
@@ -5585,11 +5522,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C4" s="166" t="s">
-        <v>173</v>
-      </c>
-      <c r="D4" s="167"/>
-      <c r="E4" s="168"/>
+      <c r="C4" s="169" t="s">
+        <v>171</v>
+      </c>
+      <c r="D4" s="170"/>
+      <c r="E4" s="171"/>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.2">
@@ -5605,10 +5542,10 @@
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C7" s="169" t="s">
-        <v>147</v>
-      </c>
-      <c r="D7" s="169"/>
+      <c r="C7" s="172" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="172"/>
       <c r="E7" s="3"/>
       <c r="F7" s="93"/>
     </row>
@@ -5620,7 +5557,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F8" s="3"/>
     </row>
@@ -5656,18 +5593,18 @@
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C13" s="74" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C14" s="170" t="s">
-        <v>154</v>
-      </c>
-      <c r="D14" s="171"/>
-      <c r="E14" s="172"/>
+      <c r="C14" s="173" t="s">
+        <v>152</v>
+      </c>
+      <c r="D14" s="174"/>
+      <c r="E14" s="175"/>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.2">
@@ -5684,7 +5621,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="3:5" s="3" customFormat="1" ht="12" x14ac:dyDescent="0.15">
@@ -5700,30 +5637,30 @@
     </row>
     <row r="19" spans="3:5" s="3" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="C19" s="25" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D19" s="135" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="3:5" s="3" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="C20" s="25" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D20" s="136"/>
       <c r="E20" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="21" spans="3:5" s="3" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="C21" s="14" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D21" s="134" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E21" s="134"/>
     </row>
@@ -5753,11 +5690,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C4" s="166" t="s">
-        <v>186</v>
-      </c>
-      <c r="D4" s="167"/>
-      <c r="E4" s="168"/>
+      <c r="C4" s="169" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="170"/>
+      <c r="E4" s="171"/>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C5" s="3"/>
@@ -5771,24 +5708,24 @@
     </row>
     <row r="7" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C7" s="74" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C8" s="173" t="s">
-        <v>123</v>
-      </c>
-      <c r="D8" s="173"/>
+      <c r="C8" s="176" t="s">
+        <v>122</v>
+      </c>
+      <c r="D8" s="176"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="C9" s="170" t="s">
-        <v>154</v>
-      </c>
-      <c r="D9" s="171"/>
-      <c r="E9" s="172"/>
+      <c r="C9" s="173" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="174"/>
+      <c r="E9" s="175"/>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C10" s="3"/>
@@ -5803,7 +5740,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.2">
@@ -5822,10 +5759,10 @@
         <v>5</v>
       </c>
       <c r="D13" s="152" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="3:5" x14ac:dyDescent="0.2">
@@ -5834,7 +5771,7 @@
       </c>
       <c r="D14" s="153"/>
       <c r="E14" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.2">
@@ -5842,10 +5779,10 @@
         <v>7</v>
       </c>
       <c r="D15" s="144" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E15" s="145" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.2">
@@ -5854,7 +5791,7 @@
       </c>
       <c r="D16" s="146"/>
       <c r="E16" s="147" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.2">
@@ -5862,10 +5799,10 @@
         <v>8</v>
       </c>
       <c r="D17" s="149" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E17" s="54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -5901,350 +5838,350 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B2" s="174" t="s">
+      <c r="B2" s="177" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="175"/>
-      <c r="D2" s="175"/>
-      <c r="E2" s="175"/>
-      <c r="F2" s="176"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
+      <c r="F2" s="179"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B4" s="177" t="s">
+      <c r="B4" s="180" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="177"/>
-      <c r="D4" s="184" t="s">
+      <c r="C4" s="180"/>
+      <c r="D4" s="187" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="184"/>
-      <c r="F4" s="184"/>
-      <c r="G4" s="184"/>
-      <c r="H4" s="184"/>
-      <c r="I4" s="184"/>
-      <c r="J4" s="184"/>
-      <c r="K4" s="184"/>
-      <c r="L4" s="184"/>
-      <c r="M4" s="184"/>
-      <c r="N4" s="184"/>
-      <c r="O4" s="184"/>
-      <c r="P4" s="184"/>
-      <c r="Q4" s="184"/>
-      <c r="R4" s="184"/>
-      <c r="S4" s="184"/>
-      <c r="T4" s="184"/>
-      <c r="U4" s="184"/>
-      <c r="V4" s="184"/>
-      <c r="W4" s="184"/>
-      <c r="X4" s="184"/>
+      <c r="E4" s="187"/>
+      <c r="F4" s="187"/>
+      <c r="G4" s="187"/>
+      <c r="H4" s="187"/>
+      <c r="I4" s="187"/>
+      <c r="J4" s="187"/>
+      <c r="K4" s="187"/>
+      <c r="L4" s="187"/>
+      <c r="M4" s="187"/>
+      <c r="N4" s="187"/>
+      <c r="O4" s="187"/>
+      <c r="P4" s="187"/>
+      <c r="Q4" s="187"/>
+      <c r="R4" s="187"/>
+      <c r="S4" s="187"/>
+      <c r="T4" s="187"/>
+      <c r="U4" s="187"/>
+      <c r="V4" s="187"/>
+      <c r="W4" s="187"/>
+      <c r="X4" s="187"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B5" s="183"/>
-      <c r="C5" s="183"/>
-      <c r="D5" s="184"/>
-      <c r="E5" s="184"/>
-      <c r="F5" s="184"/>
-      <c r="G5" s="184"/>
-      <c r="H5" s="184"/>
-      <c r="I5" s="184"/>
-      <c r="J5" s="184"/>
-      <c r="K5" s="184"/>
-      <c r="L5" s="184"/>
-      <c r="M5" s="184"/>
-      <c r="N5" s="184"/>
-      <c r="O5" s="184"/>
-      <c r="P5" s="184"/>
-      <c r="Q5" s="184"/>
-      <c r="R5" s="184"/>
-      <c r="S5" s="184"/>
-      <c r="T5" s="184"/>
-      <c r="U5" s="184"/>
-      <c r="V5" s="184"/>
-      <c r="W5" s="184"/>
-      <c r="X5" s="184"/>
+      <c r="B5" s="186"/>
+      <c r="C5" s="186"/>
+      <c r="D5" s="187"/>
+      <c r="E5" s="187"/>
+      <c r="F5" s="187"/>
+      <c r="G5" s="187"/>
+      <c r="H5" s="187"/>
+      <c r="I5" s="187"/>
+      <c r="J5" s="187"/>
+      <c r="K5" s="187"/>
+      <c r="L5" s="187"/>
+      <c r="M5" s="187"/>
+      <c r="N5" s="187"/>
+      <c r="O5" s="187"/>
+      <c r="P5" s="187"/>
+      <c r="Q5" s="187"/>
+      <c r="R5" s="187"/>
+      <c r="S5" s="187"/>
+      <c r="T5" s="187"/>
+      <c r="U5" s="187"/>
+      <c r="V5" s="187"/>
+      <c r="W5" s="187"/>
+      <c r="X5" s="187"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B6" s="186" t="s">
+      <c r="B6" s="189" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="186"/>
-      <c r="D6" s="184" t="s">
+      <c r="C6" s="189"/>
+      <c r="D6" s="187" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="184"/>
-      <c r="F6" s="184"/>
-      <c r="G6" s="184"/>
-      <c r="H6" s="184"/>
-      <c r="I6" s="184"/>
-      <c r="J6" s="184"/>
-      <c r="K6" s="184"/>
-      <c r="L6" s="184"/>
-      <c r="M6" s="184"/>
-      <c r="N6" s="184"/>
-      <c r="O6" s="184"/>
-      <c r="P6" s="184"/>
-      <c r="Q6" s="184"/>
-      <c r="R6" s="184"/>
-      <c r="S6" s="184"/>
-      <c r="T6" s="184"/>
-      <c r="U6" s="184"/>
-      <c r="V6" s="184"/>
-      <c r="W6" s="184"/>
-      <c r="X6" s="184"/>
+      <c r="E6" s="187"/>
+      <c r="F6" s="187"/>
+      <c r="G6" s="187"/>
+      <c r="H6" s="187"/>
+      <c r="I6" s="187"/>
+      <c r="J6" s="187"/>
+      <c r="K6" s="187"/>
+      <c r="L6" s="187"/>
+      <c r="M6" s="187"/>
+      <c r="N6" s="187"/>
+      <c r="O6" s="187"/>
+      <c r="P6" s="187"/>
+      <c r="Q6" s="187"/>
+      <c r="R6" s="187"/>
+      <c r="S6" s="187"/>
+      <c r="T6" s="187"/>
+      <c r="U6" s="187"/>
+      <c r="V6" s="187"/>
+      <c r="W6" s="187"/>
+      <c r="X6" s="187"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B7" s="187" t="s">
+      <c r="B7" s="190" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="187"/>
-      <c r="D7" s="184" t="s">
+      <c r="C7" s="190"/>
+      <c r="D7" s="187" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="184"/>
-      <c r="F7" s="184"/>
-      <c r="G7" s="184"/>
-      <c r="H7" s="184"/>
-      <c r="I7" s="184"/>
-      <c r="J7" s="184"/>
-      <c r="K7" s="184"/>
-      <c r="L7" s="184"/>
-      <c r="M7" s="184"/>
-      <c r="N7" s="184"/>
-      <c r="O7" s="184"/>
-      <c r="P7" s="184"/>
-      <c r="Q7" s="184"/>
-      <c r="R7" s="184"/>
-      <c r="S7" s="184"/>
-      <c r="T7" s="184"/>
-      <c r="U7" s="184"/>
-      <c r="V7" s="184"/>
-      <c r="W7" s="184"/>
-      <c r="X7" s="184"/>
+      <c r="E7" s="187"/>
+      <c r="F7" s="187"/>
+      <c r="G7" s="187"/>
+      <c r="H7" s="187"/>
+      <c r="I7" s="187"/>
+      <c r="J7" s="187"/>
+      <c r="K7" s="187"/>
+      <c r="L7" s="187"/>
+      <c r="M7" s="187"/>
+      <c r="N7" s="187"/>
+      <c r="O7" s="187"/>
+      <c r="P7" s="187"/>
+      <c r="Q7" s="187"/>
+      <c r="R7" s="187"/>
+      <c r="S7" s="187"/>
+      <c r="T7" s="187"/>
+      <c r="U7" s="187"/>
+      <c r="V7" s="187"/>
+      <c r="W7" s="187"/>
+      <c r="X7" s="187"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B8" s="166"/>
-      <c r="C8" s="168"/>
-      <c r="D8" s="180"/>
-      <c r="E8" s="181"/>
-      <c r="F8" s="181"/>
-      <c r="G8" s="181"/>
-      <c r="H8" s="181"/>
-      <c r="I8" s="181"/>
-      <c r="J8" s="181"/>
-      <c r="K8" s="181"/>
-      <c r="L8" s="181"/>
-      <c r="M8" s="181"/>
-      <c r="N8" s="181"/>
-      <c r="O8" s="181"/>
-      <c r="P8" s="181"/>
-      <c r="Q8" s="181"/>
-      <c r="R8" s="181"/>
-      <c r="S8" s="181"/>
-      <c r="T8" s="181"/>
-      <c r="U8" s="181"/>
-      <c r="V8" s="181"/>
-      <c r="W8" s="181"/>
-      <c r="X8" s="182"/>
+      <c r="B8" s="169"/>
+      <c r="C8" s="171"/>
+      <c r="D8" s="183"/>
+      <c r="E8" s="184"/>
+      <c r="F8" s="184"/>
+      <c r="G8" s="184"/>
+      <c r="H8" s="184"/>
+      <c r="I8" s="184"/>
+      <c r="J8" s="184"/>
+      <c r="K8" s="184"/>
+      <c r="L8" s="184"/>
+      <c r="M8" s="184"/>
+      <c r="N8" s="184"/>
+      <c r="O8" s="184"/>
+      <c r="P8" s="184"/>
+      <c r="Q8" s="184"/>
+      <c r="R8" s="184"/>
+      <c r="S8" s="184"/>
+      <c r="T8" s="184"/>
+      <c r="U8" s="184"/>
+      <c r="V8" s="184"/>
+      <c r="W8" s="184"/>
+      <c r="X8" s="185"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B9" s="188" t="s">
+      <c r="B9" s="191" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="189"/>
-      <c r="D9" s="180"/>
-      <c r="E9" s="181"/>
-      <c r="F9" s="181"/>
-      <c r="G9" s="181"/>
-      <c r="H9" s="181"/>
-      <c r="I9" s="181"/>
-      <c r="J9" s="181"/>
-      <c r="K9" s="181"/>
-      <c r="L9" s="181"/>
-      <c r="M9" s="181"/>
-      <c r="N9" s="181"/>
-      <c r="O9" s="181"/>
-      <c r="P9" s="181"/>
-      <c r="Q9" s="181"/>
-      <c r="R9" s="181"/>
-      <c r="S9" s="181"/>
-      <c r="T9" s="181"/>
-      <c r="U9" s="181"/>
-      <c r="V9" s="181"/>
-      <c r="W9" s="181"/>
-      <c r="X9" s="182"/>
+      <c r="C9" s="192"/>
+      <c r="D9" s="183"/>
+      <c r="E9" s="184"/>
+      <c r="F9" s="184"/>
+      <c r="G9" s="184"/>
+      <c r="H9" s="184"/>
+      <c r="I9" s="184"/>
+      <c r="J9" s="184"/>
+      <c r="K9" s="184"/>
+      <c r="L9" s="184"/>
+      <c r="M9" s="184"/>
+      <c r="N9" s="184"/>
+      <c r="O9" s="184"/>
+      <c r="P9" s="184"/>
+      <c r="Q9" s="184"/>
+      <c r="R9" s="184"/>
+      <c r="S9" s="184"/>
+      <c r="T9" s="184"/>
+      <c r="U9" s="184"/>
+      <c r="V9" s="184"/>
+      <c r="W9" s="184"/>
+      <c r="X9" s="185"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B10" s="166"/>
-      <c r="C10" s="168"/>
-      <c r="D10" s="180"/>
-      <c r="E10" s="181"/>
-      <c r="F10" s="181"/>
-      <c r="G10" s="181"/>
-      <c r="H10" s="181"/>
-      <c r="I10" s="181"/>
-      <c r="J10" s="181"/>
-      <c r="K10" s="181"/>
-      <c r="L10" s="181"/>
-      <c r="M10" s="181"/>
-      <c r="N10" s="181"/>
-      <c r="O10" s="181"/>
-      <c r="P10" s="181"/>
-      <c r="Q10" s="181"/>
-      <c r="R10" s="181"/>
-      <c r="S10" s="181"/>
-      <c r="T10" s="181"/>
-      <c r="U10" s="181"/>
-      <c r="V10" s="181"/>
-      <c r="W10" s="181"/>
-      <c r="X10" s="182"/>
+      <c r="B10" s="169"/>
+      <c r="C10" s="171"/>
+      <c r="D10" s="183"/>
+      <c r="E10" s="184"/>
+      <c r="F10" s="184"/>
+      <c r="G10" s="184"/>
+      <c r="H10" s="184"/>
+      <c r="I10" s="184"/>
+      <c r="J10" s="184"/>
+      <c r="K10" s="184"/>
+      <c r="L10" s="184"/>
+      <c r="M10" s="184"/>
+      <c r="N10" s="184"/>
+      <c r="O10" s="184"/>
+      <c r="P10" s="184"/>
+      <c r="Q10" s="184"/>
+      <c r="R10" s="184"/>
+      <c r="S10" s="184"/>
+      <c r="T10" s="184"/>
+      <c r="U10" s="184"/>
+      <c r="V10" s="184"/>
+      <c r="W10" s="184"/>
+      <c r="X10" s="185"/>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B11" s="185" t="s">
+      <c r="B11" s="188" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="185"/>
-      <c r="D11" s="184" t="s">
+      <c r="C11" s="188"/>
+      <c r="D11" s="187" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="184"/>
-      <c r="F11" s="184"/>
-      <c r="G11" s="184"/>
-      <c r="H11" s="184"/>
-      <c r="I11" s="184"/>
-      <c r="J11" s="184"/>
-      <c r="K11" s="184"/>
-      <c r="L11" s="184"/>
-      <c r="M11" s="184"/>
-      <c r="N11" s="184"/>
-      <c r="O11" s="184"/>
-      <c r="P11" s="184"/>
-      <c r="Q11" s="184"/>
-      <c r="R11" s="184"/>
-      <c r="S11" s="184"/>
-      <c r="T11" s="184"/>
-      <c r="U11" s="184"/>
-      <c r="V11" s="184"/>
-      <c r="W11" s="184"/>
-      <c r="X11" s="184"/>
+      <c r="E11" s="187"/>
+      <c r="F11" s="187"/>
+      <c r="G11" s="187"/>
+      <c r="H11" s="187"/>
+      <c r="I11" s="187"/>
+      <c r="J11" s="187"/>
+      <c r="K11" s="187"/>
+      <c r="L11" s="187"/>
+      <c r="M11" s="187"/>
+      <c r="N11" s="187"/>
+      <c r="O11" s="187"/>
+      <c r="P11" s="187"/>
+      <c r="Q11" s="187"/>
+      <c r="R11" s="187"/>
+      <c r="S11" s="187"/>
+      <c r="T11" s="187"/>
+      <c r="U11" s="187"/>
+      <c r="V11" s="187"/>
+      <c r="W11" s="187"/>
+      <c r="X11" s="187"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B12" s="179" t="s">
+      <c r="B12" s="182" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="179"/>
-      <c r="D12" s="184" t="s">
+      <c r="C12" s="182"/>
+      <c r="D12" s="187" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="184"/>
-      <c r="F12" s="184"/>
-      <c r="G12" s="184"/>
-      <c r="H12" s="184"/>
-      <c r="I12" s="184"/>
-      <c r="J12" s="184"/>
-      <c r="K12" s="184"/>
-      <c r="L12" s="184"/>
-      <c r="M12" s="184"/>
-      <c r="N12" s="184"/>
-      <c r="O12" s="184"/>
-      <c r="P12" s="184"/>
-      <c r="Q12" s="184"/>
-      <c r="R12" s="184"/>
-      <c r="S12" s="184"/>
-      <c r="T12" s="184"/>
-      <c r="U12" s="184"/>
-      <c r="V12" s="184"/>
-      <c r="W12" s="184"/>
-      <c r="X12" s="184"/>
+      <c r="E12" s="187"/>
+      <c r="F12" s="187"/>
+      <c r="G12" s="187"/>
+      <c r="H12" s="187"/>
+      <c r="I12" s="187"/>
+      <c r="J12" s="187"/>
+      <c r="K12" s="187"/>
+      <c r="L12" s="187"/>
+      <c r="M12" s="187"/>
+      <c r="N12" s="187"/>
+      <c r="O12" s="187"/>
+      <c r="P12" s="187"/>
+      <c r="Q12" s="187"/>
+      <c r="R12" s="187"/>
+      <c r="S12" s="187"/>
+      <c r="T12" s="187"/>
+      <c r="U12" s="187"/>
+      <c r="V12" s="187"/>
+      <c r="W12" s="187"/>
+      <c r="X12" s="187"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B13" s="178" t="s">
+      <c r="B13" s="181" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="178"/>
-      <c r="D13" s="184" t="s">
+      <c r="C13" s="181"/>
+      <c r="D13" s="187" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="184"/>
-      <c r="F13" s="184"/>
-      <c r="G13" s="184"/>
-      <c r="H13" s="184"/>
-      <c r="I13" s="184"/>
-      <c r="J13" s="184"/>
-      <c r="K13" s="184"/>
-      <c r="L13" s="184"/>
-      <c r="M13" s="184"/>
-      <c r="N13" s="184"/>
-      <c r="O13" s="184"/>
-      <c r="P13" s="184"/>
-      <c r="Q13" s="184"/>
-      <c r="R13" s="184"/>
-      <c r="S13" s="184"/>
-      <c r="T13" s="184"/>
-      <c r="U13" s="184"/>
-      <c r="V13" s="184"/>
-      <c r="W13" s="184"/>
-      <c r="X13" s="184"/>
+      <c r="E13" s="187"/>
+      <c r="F13" s="187"/>
+      <c r="G13" s="187"/>
+      <c r="H13" s="187"/>
+      <c r="I13" s="187"/>
+      <c r="J13" s="187"/>
+      <c r="K13" s="187"/>
+      <c r="L13" s="187"/>
+      <c r="M13" s="187"/>
+      <c r="N13" s="187"/>
+      <c r="O13" s="187"/>
+      <c r="P13" s="187"/>
+      <c r="Q13" s="187"/>
+      <c r="R13" s="187"/>
+      <c r="S13" s="187"/>
+      <c r="T13" s="187"/>
+      <c r="U13" s="187"/>
+      <c r="V13" s="187"/>
+      <c r="W13" s="187"/>
+      <c r="X13" s="187"/>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B14" s="183"/>
-      <c r="C14" s="183"/>
-      <c r="D14" s="184"/>
-      <c r="E14" s="184"/>
-      <c r="F14" s="184"/>
-      <c r="G14" s="184"/>
-      <c r="H14" s="184"/>
-      <c r="I14" s="184"/>
-      <c r="J14" s="184"/>
-      <c r="K14" s="184"/>
-      <c r="L14" s="184"/>
-      <c r="M14" s="184"/>
-      <c r="N14" s="184"/>
-      <c r="O14" s="184"/>
-      <c r="P14" s="184"/>
-      <c r="Q14" s="184"/>
-      <c r="R14" s="184"/>
-      <c r="S14" s="184"/>
-      <c r="T14" s="184"/>
-      <c r="U14" s="184"/>
-      <c r="V14" s="184"/>
-      <c r="W14" s="184"/>
-      <c r="X14" s="184"/>
+      <c r="B14" s="186"/>
+      <c r="C14" s="186"/>
+      <c r="D14" s="187"/>
+      <c r="E14" s="187"/>
+      <c r="F14" s="187"/>
+      <c r="G14" s="187"/>
+      <c r="H14" s="187"/>
+      <c r="I14" s="187"/>
+      <c r="J14" s="187"/>
+      <c r="K14" s="187"/>
+      <c r="L14" s="187"/>
+      <c r="M14" s="187"/>
+      <c r="N14" s="187"/>
+      <c r="O14" s="187"/>
+      <c r="P14" s="187"/>
+      <c r="Q14" s="187"/>
+      <c r="R14" s="187"/>
+      <c r="S14" s="187"/>
+      <c r="T14" s="187"/>
+      <c r="U14" s="187"/>
+      <c r="V14" s="187"/>
+      <c r="W14" s="187"/>
+      <c r="X14" s="187"/>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B15" s="177" t="s">
+      <c r="B15" s="180" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="177"/>
-      <c r="D15" s="184" t="s">
+      <c r="C15" s="180"/>
+      <c r="D15" s="187" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="184"/>
-      <c r="F15" s="184"/>
-      <c r="G15" s="184"/>
-      <c r="H15" s="184"/>
-      <c r="I15" s="184"/>
-      <c r="J15" s="184"/>
-      <c r="K15" s="184"/>
-      <c r="L15" s="184"/>
-      <c r="M15" s="184"/>
-      <c r="N15" s="184"/>
-      <c r="O15" s="184"/>
-      <c r="P15" s="184"/>
-      <c r="Q15" s="184"/>
-      <c r="R15" s="184"/>
-      <c r="S15" s="184"/>
-      <c r="T15" s="184"/>
-      <c r="U15" s="184"/>
-      <c r="V15" s="184"/>
-      <c r="W15" s="184"/>
-      <c r="X15" s="184"/>
+      <c r="E15" s="187"/>
+      <c r="F15" s="187"/>
+      <c r="G15" s="187"/>
+      <c r="H15" s="187"/>
+      <c r="I15" s="187"/>
+      <c r="J15" s="187"/>
+      <c r="K15" s="187"/>
+      <c r="L15" s="187"/>
+      <c r="M15" s="187"/>
+      <c r="N15" s="187"/>
+      <c r="O15" s="187"/>
+      <c r="P15" s="187"/>
+      <c r="Q15" s="187"/>
+      <c r="R15" s="187"/>
+      <c r="S15" s="187"/>
+      <c r="T15" s="187"/>
+      <c r="U15" s="187"/>
+      <c r="V15" s="187"/>
+      <c r="W15" s="187"/>
+      <c r="X15" s="187"/>
     </row>
     <row r="17" spans="3:67" x14ac:dyDescent="0.15">
-      <c r="D17" s="177" t="s">
+      <c r="D17" s="180" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="177"/>
-      <c r="F17" s="177"/>
+      <c r="E17" s="180"/>
+      <c r="F17" s="180"/>
       <c r="G17" s="84" t="s">
         <v>0</v>
       </c>
@@ -6303,21 +6240,21 @@
       <c r="BF17" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="BG17" s="179" t="s">
+      <c r="BG17" s="182" t="s">
         <v>7</v>
       </c>
-      <c r="BH17" s="179"/>
-      <c r="BI17" s="179"/>
-      <c r="BJ17" s="179"/>
-      <c r="BK17" s="178" t="s">
+      <c r="BH17" s="182"/>
+      <c r="BI17" s="182"/>
+      <c r="BJ17" s="182"/>
+      <c r="BK17" s="181" t="s">
         <v>5</v>
       </c>
-      <c r="BL17" s="178"/>
-      <c r="BM17" s="177" t="s">
+      <c r="BL17" s="181"/>
+      <c r="BM17" s="180" t="s">
         <v>6</v>
       </c>
-      <c r="BN17" s="177"/>
-      <c r="BO17" s="177"/>
+      <c r="BN17" s="180"/>
+      <c r="BO17" s="180"/>
     </row>
     <row r="18" spans="3:67" x14ac:dyDescent="0.15">
       <c r="C18" s="95" t="s">
@@ -6517,57 +6454,57 @@
       </c>
     </row>
     <row r="20" spans="3:67" x14ac:dyDescent="0.15">
-      <c r="I20" s="166" t="s">
-        <v>170</v>
-      </c>
-      <c r="J20" s="167"/>
-      <c r="K20" s="167"/>
-      <c r="L20" s="167"/>
-      <c r="M20" s="167"/>
-      <c r="N20" s="167"/>
-      <c r="O20" s="167"/>
-      <c r="P20" s="167"/>
-      <c r="Q20" s="167"/>
-      <c r="R20" s="167"/>
-      <c r="S20" s="167"/>
-      <c r="T20" s="167"/>
-      <c r="U20" s="167"/>
-      <c r="V20" s="167"/>
-      <c r="W20" s="167"/>
-      <c r="X20" s="167"/>
-      <c r="Y20" s="167"/>
-      <c r="Z20" s="167"/>
-      <c r="AA20" s="167"/>
-      <c r="AB20" s="167"/>
-      <c r="AC20" s="167"/>
-      <c r="AD20" s="167"/>
-      <c r="AE20" s="167"/>
-      <c r="AF20" s="167"/>
-      <c r="AG20" s="167"/>
-      <c r="AH20" s="167"/>
-      <c r="AI20" s="167"/>
-      <c r="AJ20" s="167"/>
-      <c r="AK20" s="167"/>
-      <c r="AL20" s="167"/>
-      <c r="AM20" s="167"/>
-      <c r="AN20" s="167"/>
-      <c r="AO20" s="167"/>
-      <c r="AP20" s="167"/>
-      <c r="AQ20" s="167"/>
-      <c r="AR20" s="167"/>
-      <c r="AS20" s="167"/>
-      <c r="AT20" s="167"/>
-      <c r="AU20" s="167"/>
-      <c r="AV20" s="167"/>
-      <c r="AW20" s="167"/>
-      <c r="AX20" s="167"/>
-      <c r="AY20" s="167"/>
-      <c r="AZ20" s="167"/>
-      <c r="BA20" s="167"/>
-      <c r="BB20" s="167"/>
-      <c r="BC20" s="167"/>
-      <c r="BD20" s="167"/>
-      <c r="BE20" s="168"/>
+      <c r="I20" s="169" t="s">
+        <v>168</v>
+      </c>
+      <c r="J20" s="170"/>
+      <c r="K20" s="170"/>
+      <c r="L20" s="170"/>
+      <c r="M20" s="170"/>
+      <c r="N20" s="170"/>
+      <c r="O20" s="170"/>
+      <c r="P20" s="170"/>
+      <c r="Q20" s="170"/>
+      <c r="R20" s="170"/>
+      <c r="S20" s="170"/>
+      <c r="T20" s="170"/>
+      <c r="U20" s="170"/>
+      <c r="V20" s="170"/>
+      <c r="W20" s="170"/>
+      <c r="X20" s="170"/>
+      <c r="Y20" s="170"/>
+      <c r="Z20" s="170"/>
+      <c r="AA20" s="170"/>
+      <c r="AB20" s="170"/>
+      <c r="AC20" s="170"/>
+      <c r="AD20" s="170"/>
+      <c r="AE20" s="170"/>
+      <c r="AF20" s="170"/>
+      <c r="AG20" s="170"/>
+      <c r="AH20" s="170"/>
+      <c r="AI20" s="170"/>
+      <c r="AJ20" s="170"/>
+      <c r="AK20" s="170"/>
+      <c r="AL20" s="170"/>
+      <c r="AM20" s="170"/>
+      <c r="AN20" s="170"/>
+      <c r="AO20" s="170"/>
+      <c r="AP20" s="170"/>
+      <c r="AQ20" s="170"/>
+      <c r="AR20" s="170"/>
+      <c r="AS20" s="170"/>
+      <c r="AT20" s="170"/>
+      <c r="AU20" s="170"/>
+      <c r="AV20" s="170"/>
+      <c r="AW20" s="170"/>
+      <c r="AX20" s="170"/>
+      <c r="AY20" s="170"/>
+      <c r="AZ20" s="170"/>
+      <c r="BA20" s="170"/>
+      <c r="BB20" s="170"/>
+      <c r="BC20" s="170"/>
+      <c r="BD20" s="170"/>
+      <c r="BE20" s="171"/>
     </row>
     <row r="21" spans="3:67" x14ac:dyDescent="0.15">
       <c r="I21" s="126">
@@ -6776,17 +6713,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B2" s="166" t="s">
-        <v>167</v>
-      </c>
-      <c r="C2" s="167"/>
-      <c r="D2" s="168"/>
+      <c r="B2" s="169" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="170"/>
+      <c r="D2" s="171"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B5" s="169" t="s">
-        <v>147</v>
-      </c>
-      <c r="C5" s="169"/>
+      <c r="B5" s="172" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="172"/>
       <c r="E5" s="93"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.15">
@@ -6797,7 +6734,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F6" s="120" t="s">
         <v>10</v>
@@ -6812,10 +6749,10 @@
         <v>10</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="7">
@@ -6827,13 +6764,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="121" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="7">
@@ -6846,7 +6783,7 @@
       </c>
       <c r="C9" s="122"/>
       <c r="D9" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F9" s="48"/>
       <c r="G9" s="48"/>
@@ -6857,7 +6794,7 @@
         <v>7</v>
       </c>
       <c r="C10" s="110" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D10" s="109"/>
       <c r="F10" s="48"/>
@@ -6865,10 +6802,10 @@
       <c r="H10" s="76"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B12" s="169" t="s">
-        <v>147</v>
-      </c>
-      <c r="C12" s="169"/>
+      <c r="B12" s="172" t="s">
+        <v>145</v>
+      </c>
+      <c r="C12" s="172"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B13" s="14">
@@ -6878,7 +6815,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.15">
@@ -6889,7 +6826,7 @@
         <v>10</v>
       </c>
       <c r="D14" s="39" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.15">
@@ -6897,10 +6834,10 @@
         <v>5</v>
       </c>
       <c r="C15" s="121" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.15">
@@ -6909,7 +6846,7 @@
       </c>
       <c r="C16" s="122"/>
       <c r="D16" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.15">
@@ -6917,21 +6854,21 @@
         <v>7</v>
       </c>
       <c r="C17" s="110" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D17" s="109"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B20" s="74" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B21" s="170" t="s">
-        <v>154</v>
-      </c>
-      <c r="C21" s="171"/>
-      <c r="D21" s="172"/>
+      <c r="B21" s="173" t="s">
+        <v>152</v>
+      </c>
+      <c r="C21" s="174"/>
+      <c r="D21" s="175"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -6961,11 +6898,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B2" s="190" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" s="190"/>
-      <c r="D2" s="190"/>
+      <c r="B2" s="193" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B4" s="14">
@@ -6991,7 +6928,7 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B6" s="80" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C6" s="89" t="s">
         <v>18</v>
@@ -7032,7 +6969,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.15">
@@ -7050,111 +6987,111 @@
       <c r="B5" s="25">
         <v>5</v>
       </c>
-      <c r="C5" s="191" t="s">
-        <v>120</v>
+      <c r="C5" s="194" t="s">
+        <v>119</v>
       </c>
       <c r="D5" s="97" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" s="203" t="s">
-        <v>153</v>
-      </c>
-      <c r="G5" s="204"/>
-      <c r="H5" s="205"/>
+        <v>78</v>
+      </c>
+      <c r="F5" s="206" t="s">
+        <v>151</v>
+      </c>
+      <c r="G5" s="207"/>
+      <c r="H5" s="208"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B6" s="25">
         <v>6</v>
       </c>
-      <c r="C6" s="192"/>
+      <c r="C6" s="195"/>
       <c r="D6" s="98" t="s">
-        <v>80</v>
-      </c>
-      <c r="F6" s="206" t="s">
-        <v>156</v>
-      </c>
-      <c r="G6" s="207"/>
-      <c r="H6" s="208"/>
+        <v>79</v>
+      </c>
+      <c r="F6" s="209" t="s">
+        <v>154</v>
+      </c>
+      <c r="G6" s="210"/>
+      <c r="H6" s="211"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B7" s="25">
         <v>7</v>
       </c>
-      <c r="C7" s="192"/>
+      <c r="C7" s="195"/>
       <c r="D7" s="98" t="s">
-        <v>82</v>
-      </c>
-      <c r="F7" s="206" t="s">
-        <v>157</v>
-      </c>
-      <c r="G7" s="207"/>
-      <c r="H7" s="208"/>
+        <v>81</v>
+      </c>
+      <c r="F7" s="209" t="s">
+        <v>155</v>
+      </c>
+      <c r="G7" s="210"/>
+      <c r="H7" s="211"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B8" s="25">
         <v>8</v>
       </c>
-      <c r="C8" s="193"/>
+      <c r="C8" s="196"/>
       <c r="D8" s="99" t="s">
-        <v>81</v>
-      </c>
-      <c r="F8" s="209" t="s">
-        <v>158</v>
-      </c>
-      <c r="G8" s="210"/>
-      <c r="H8" s="211"/>
+        <v>80</v>
+      </c>
+      <c r="F8" s="212" t="s">
+        <v>156</v>
+      </c>
+      <c r="G8" s="213"/>
+      <c r="H8" s="214"/>
     </row>
     <row r="9" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="25">
         <v>9</v>
       </c>
-      <c r="C9" s="200" t="s">
+      <c r="C9" s="203" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="100" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" s="194" t="s">
-        <v>155</v>
-      </c>
-      <c r="G9" s="195"/>
-      <c r="H9" s="196"/>
+        <v>78</v>
+      </c>
+      <c r="F9" s="197" t="s">
+        <v>153</v>
+      </c>
+      <c r="G9" s="198"/>
+      <c r="H9" s="199"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B10" s="25">
         <v>10</v>
       </c>
-      <c r="C10" s="201"/>
+      <c r="C10" s="204"/>
       <c r="D10" s="101" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="194"/>
-      <c r="G10" s="195"/>
-      <c r="H10" s="196"/>
+        <v>79</v>
+      </c>
+      <c r="F10" s="197"/>
+      <c r="G10" s="198"/>
+      <c r="H10" s="199"/>
     </row>
     <row r="11" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="25">
         <v>11</v>
       </c>
-      <c r="C11" s="201"/>
+      <c r="C11" s="204"/>
       <c r="D11" s="101" t="s">
-        <v>82</v>
-      </c>
-      <c r="F11" s="194"/>
-      <c r="G11" s="195"/>
-      <c r="H11" s="196"/>
+        <v>81</v>
+      </c>
+      <c r="F11" s="197"/>
+      <c r="G11" s="198"/>
+      <c r="H11" s="199"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B12" s="25">
         <v>12</v>
       </c>
-      <c r="C12" s="202"/>
+      <c r="C12" s="205"/>
       <c r="D12" s="102" t="s">
-        <v>81</v>
-      </c>
-      <c r="F12" s="194"/>
-      <c r="G12" s="195"/>
-      <c r="H12" s="196"/>
+        <v>80</v>
+      </c>
+      <c r="F12" s="197"/>
+      <c r="G12" s="198"/>
+      <c r="H12" s="199"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B13" s="25">
@@ -7164,9 +7101,9 @@
         <v>0</v>
       </c>
       <c r="D13" s="104"/>
-      <c r="F13" s="194"/>
-      <c r="G13" s="195"/>
-      <c r="H13" s="196"/>
+      <c r="F13" s="197"/>
+      <c r="G13" s="198"/>
+      <c r="H13" s="199"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B14" s="25">
@@ -7176,9 +7113,9 @@
         <v>20</v>
       </c>
       <c r="D14" s="106"/>
-      <c r="F14" s="197"/>
-      <c r="G14" s="198"/>
-      <c r="H14" s="199"/>
+      <c r="F14" s="200"/>
+      <c r="G14" s="201"/>
+      <c r="H14" s="202"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -7214,10 +7151,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.15">
-      <c r="B3" s="166" t="s">
-        <v>175</v>
-      </c>
-      <c r="C3" s="168"/>
+      <c r="B3" s="169" t="s">
+        <v>173</v>
+      </c>
+      <c r="C3" s="171"/>
       <c r="D3" s="94"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.15">
@@ -7228,10 +7165,10 @@
         <v>0</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F5" s="45" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H5" s="4"/>
     </row>
@@ -7246,7 +7183,7 @@
         <v>4</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G6" s="13"/>
       <c r="H6" s="7">
@@ -7258,14 +7195,14 @@
         <v>5</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D7" s="43"/>
       <c r="F7" s="13" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H7" s="7">
         <v>1</v>
@@ -7276,13 +7213,13 @@
         <v>6</v>
       </c>
       <c r="C8" s="138" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="7">
@@ -7295,10 +7232,10 @@
       </c>
       <c r="C9" s="139"/>
       <c r="D9" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="7">
@@ -7310,13 +7247,13 @@
         <v>8</v>
       </c>
       <c r="C10" s="138" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="7">
@@ -7329,10 +7266,10 @@
       </c>
       <c r="C11" s="139"/>
       <c r="D11" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G11" s="13"/>
       <c r="H11" s="7">
@@ -7342,7 +7279,7 @@
     <row r="12" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B12" s="46"/>
       <c r="F12" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G12" s="13"/>
       <c r="H12" s="7"/>
@@ -7350,7 +7287,7 @@
     <row r="13" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B13" s="46"/>
       <c r="F13" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G13" s="13"/>
       <c r="H13" s="7">
@@ -7360,7 +7297,7 @@
     <row r="14" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B14" s="46"/>
       <c r="F14" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G14" s="13"/>
       <c r="H14" s="7"/>
@@ -7368,7 +7305,7 @@
     <row r="15" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B15" s="46"/>
       <c r="F15" s="13" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G15" s="13"/>
       <c r="H15" s="7">
@@ -7377,14 +7314,14 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.15">
       <c r="F16" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="7"/>
     </row>
     <row r="17" spans="6:8" x14ac:dyDescent="0.15">
       <c r="F17" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G17" s="13"/>
       <c r="H17" s="7">
@@ -7393,14 +7330,14 @@
     </row>
     <row r="18" spans="6:8" x14ac:dyDescent="0.15">
       <c r="F18" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="7"/>
     </row>
     <row r="19" spans="6:8" x14ac:dyDescent="0.15">
       <c r="F19" s="13" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G19" s="13"/>
       <c r="H19" s="7">
@@ -7409,14 +7346,14 @@
     </row>
     <row r="20" spans="6:8" x14ac:dyDescent="0.15">
       <c r="F20" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="7"/>
     </row>
     <row r="21" spans="6:8" x14ac:dyDescent="0.15">
       <c r="F21" s="13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G21" s="13"/>
       <c r="H21" s="7">
@@ -7450,17 +7387,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B2" s="166" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="167"/>
-      <c r="D2" s="168"/>
+      <c r="B2" s="169" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="170"/>
+      <c r="D2" s="171"/>
     </row>
     <row r="5" spans="2:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="169" t="s">
-        <v>147</v>
-      </c>
-      <c r="C5" s="169"/>
+      <c r="B5" s="172" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="172"/>
       <c r="E5" s="93"/>
       <c r="F5" s="93"/>
     </row>
@@ -7472,12 +7409,12 @@
         <v>0</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="F6" s="212" t="s">
-        <v>124</v>
-      </c>
-      <c r="G6" s="212"/>
+        <v>69</v>
+      </c>
+      <c r="F6" s="215" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" s="215"/>
       <c r="H6" s="4"/>
       <c r="I6" s="72"/>
     </row>
@@ -7489,10 +7426,10 @@
         <v>10</v>
       </c>
       <c r="D7" s="39" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="7">
@@ -7505,13 +7442,13 @@
         <v>5</v>
       </c>
       <c r="C8" s="87" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G8" s="13"/>
       <c r="H8" s="7">
@@ -7525,10 +7462,10 @@
       </c>
       <c r="C9" s="88"/>
       <c r="D9" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="7">
@@ -7538,7 +7475,7 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.15">
       <c r="F10" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="7">
@@ -7554,7 +7491,7 @@
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B12" s="74" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F12" s="148" t="s">
         <v>10</v>
@@ -7562,12 +7499,12 @@
       <c r="G12" s="42"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B13" s="173" t="s">
-        <v>123</v>
-      </c>
-      <c r="C13" s="173"/>
+      <c r="B13" s="176" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="176"/>
       <c r="F13" s="12" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="7">
@@ -7575,11 +7512,11 @@
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.15">
-      <c r="B14" s="170" t="s">
-        <v>154</v>
-      </c>
-      <c r="C14" s="171"/>
-      <c r="D14" s="172"/>
+      <c r="B14" s="173" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" s="174"/>
+      <c r="D14" s="175"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.15">
       <c r="B16" s="14">
@@ -7589,7 +7526,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.15">
@@ -7600,7 +7537,7 @@
         <v>10</v>
       </c>
       <c r="D17" s="39" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.15">
@@ -7608,10 +7545,10 @@
         <v>5</v>
       </c>
       <c r="C18" s="87" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D18" s="27" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.15">
@@ -7620,7 +7557,7 @@
       </c>
       <c r="C19" s="88"/>
       <c r="D19" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.15">
@@ -7628,10 +7565,10 @@
         <v>7</v>
       </c>
       <c r="C20" s="144" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D20" s="145" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.15">
@@ -7640,7 +7577,7 @@
       </c>
       <c r="C21" s="146"/>
       <c r="D21" s="147" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.15">
@@ -7648,10 +7585,10 @@
         <v>8</v>
       </c>
       <c r="C22" s="149" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D22" s="54" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added IMU_RESET_TO_FACTORY_SETTINGS command and RESET_IMU_FACTORY_SETTINGS_ON_STARTUP define
</commit_message>
<xml_diff>
--- a/doc/DATA_PROTOCOL_SENSUS.xlsx
+++ b/doc/DATA_PROTOCOL_SENSUS.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Simone/Documents/Dropbox/Mind Music Lab AB/GIT/sensei/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simone.minto\Dropbox\PROROB\09 CLIENTI\Mind Music Lab AB\01 SENSEI\GIT\sensei-bitbucket\sensei\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="804" activeTab="11"/>
+    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="804"/>
   </bookViews>
   <sheets>
     <sheet name="LIST_CMD" sheetId="2" r:id="rId1"/>
@@ -28,9 +28,6 @@
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -39,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="192">
   <si>
     <t>CMD</t>
   </si>
@@ -612,6 +609,9 @@
   </si>
   <si>
     <t>IMU_GET_DATA_LINEARACCELERATION</t>
+  </si>
+  <si>
+    <t>IMU_RESET_TO_FACTORY_SETTINGS</t>
   </si>
 </sst>
 </file>
@@ -1026,7 +1026,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="240">
+  <cellXfs count="242">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1502,52 +1502,52 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1640,8 +1640,35 @@
     <xf numFmtId="0" fontId="2" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1652,20 +1679,8 @@
     <xf numFmtId="0" fontId="2" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1676,24 +1691,15 @@
     <xf numFmtId="0" fontId="2" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2058,23 +2064,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F42"/>
+  <dimension ref="B2:F44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33:E36"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.5" style="1" customWidth="1"/>
-    <col min="2" max="3" width="9.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.453125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="9.453125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="73" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="1"/>
+    <col min="7" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="14" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:6" ht="13" x14ac:dyDescent="0.3">
       <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
@@ -2091,7 +2097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="16">
         <v>0</v>
       </c>
@@ -2102,7 +2108,7 @@
       <c r="E3" s="16"/>
       <c r="F3" s="17"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" s="16">
         <v>1</v>
       </c>
@@ -2113,7 +2119,7 @@
       <c r="E4" s="16"/>
       <c r="F4" s="17"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="16">
         <v>2</v>
       </c>
@@ -2124,7 +2130,7 @@
       <c r="E5" s="16"/>
       <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="16">
         <v>3</v>
       </c>
@@ -2135,21 +2141,21 @@
       <c r="E6" s="16"/>
       <c r="F6" s="17"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" s="82"/>
       <c r="C7" s="82"/>
       <c r="D7" s="82"/>
       <c r="E7" s="82"/>
       <c r="F7" s="2"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="82"/>
       <c r="C8" s="82"/>
       <c r="D8" s="82"/>
       <c r="E8" s="82"/>
       <c r="F8" s="2"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="20">
         <v>100</v>
       </c>
@@ -2164,7 +2170,7 @@
       </c>
       <c r="F9" s="21"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="20"/>
       <c r="C10" s="20">
         <v>1</v>
@@ -2175,7 +2181,7 @@
       </c>
       <c r="F10" s="21"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="20"/>
       <c r="C11" s="20">
         <v>2</v>
@@ -2186,7 +2192,7 @@
       </c>
       <c r="F11" s="21"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="20"/>
       <c r="C12" s="20">
         <v>3</v>
@@ -2197,14 +2203,14 @@
       </c>
       <c r="F12" s="21"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="82"/>
       <c r="C13" s="82"/>
       <c r="D13" s="82"/>
       <c r="E13" s="82"/>
       <c r="F13" s="2"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="20">
         <v>101</v>
       </c>
@@ -2217,14 +2223,14 @@
       <c r="E14" s="20"/>
       <c r="F14" s="20"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" s="137"/>
       <c r="C15" s="137"/>
       <c r="D15" s="137"/>
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="20">
         <v>102</v>
       </c>
@@ -2237,14 +2243,14 @@
       <c r="E16" s="20"/>
       <c r="F16" s="21"/>
     </row>
-    <row r="17" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" s="12"/>
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
       <c r="E17" s="12"/>
       <c r="F17" s="23"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="20">
         <v>103</v>
       </c>
@@ -2259,7 +2265,7 @@
       </c>
       <c r="F18" s="21"/>
     </row>
-    <row r="19" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B19" s="20"/>
       <c r="C19" s="20">
         <v>1</v>
@@ -2270,14 +2276,14 @@
       </c>
       <c r="F19" s="21"/>
     </row>
-    <row r="20" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
       <c r="E20" s="12"/>
       <c r="F20" s="23"/>
     </row>
-    <row r="21" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:6" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" s="20">
         <v>104</v>
       </c>
@@ -2292,14 +2298,14 @@
       </c>
       <c r="F21" s="21"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="12"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
       <c r="E22" s="12"/>
       <c r="F22" s="23"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="20">
         <v>105</v>
       </c>
@@ -2314,7 +2320,7 @@
       </c>
       <c r="F23" s="20"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="20"/>
       <c r="C24" s="20">
         <v>1</v>
@@ -2325,14 +2331,14 @@
       </c>
       <c r="F24" s="20"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="129"/>
       <c r="C25" s="129"/>
       <c r="D25" s="129"/>
       <c r="E25" s="129"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="18">
         <v>200</v>
       </c>
@@ -2345,7 +2351,7 @@
       <c r="E26" s="18"/>
       <c r="F26" s="19"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="18">
         <v>201</v>
       </c>
@@ -2358,7 +2364,7 @@
       <c r="E27" s="18"/>
       <c r="F27" s="19"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="18">
         <v>202</v>
       </c>
@@ -2371,7 +2377,7 @@
       <c r="E28" s="18"/>
       <c r="F28" s="19"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="18">
         <v>203</v>
       </c>
@@ -2384,7 +2390,7 @@
       <c r="E29" s="18"/>
       <c r="F29" s="19"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="18">
         <v>204</v>
       </c>
@@ -2397,7 +2403,7 @@
       <c r="E30" s="18"/>
       <c r="F30" s="19"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B31" s="18">
         <v>205</v>
       </c>
@@ -2410,14 +2416,14 @@
       <c r="E31" s="18"/>
       <c r="F31" s="19"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B32" s="82"/>
       <c r="C32" s="82"/>
       <c r="D32" s="82"/>
       <c r="E32" s="82"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="18">
         <v>206</v>
       </c>
@@ -2434,7 +2440,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B34" s="18"/>
       <c r="C34" s="18">
         <v>1</v>
@@ -2447,7 +2453,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B35" s="18"/>
       <c r="C35" s="18">
         <v>2</v>
@@ -2460,7 +2466,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B36" s="18"/>
       <c r="C36" s="18">
         <v>3</v>
@@ -2473,63 +2479,83 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B37" s="82"/>
-      <c r="C37" s="82"/>
-      <c r="D37" s="82"/>
-      <c r="E37" s="82"/>
-      <c r="F37" s="2"/>
-    </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B38" s="82"/>
-      <c r="C38" s="82"/>
-      <c r="D38" s="82"/>
-      <c r="E38" s="82"/>
-      <c r="F38" s="2"/>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B39" s="130">
-        <v>250</v>
-      </c>
-      <c r="C39" s="130">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B37" s="240"/>
+      <c r="C37" s="240"/>
+      <c r="D37" s="240"/>
+      <c r="E37" s="240"/>
+      <c r="F37" s="241"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B38" s="18">
+        <v>207</v>
+      </c>
+      <c r="C38" s="18">
         <v>0</v>
       </c>
-      <c r="D39" s="130" t="s">
-        <v>170</v>
-      </c>
-      <c r="E39" s="130"/>
-      <c r="F39" s="131"/>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="D38" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="E38" s="18"/>
+      <c r="F38" s="19"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B39" s="82"/>
+      <c r="C39" s="82"/>
+      <c r="D39" s="82"/>
+      <c r="E39" s="82"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="82"/>
       <c r="C40" s="82"/>
       <c r="D40" s="82"/>
       <c r="E40" s="82"/>
       <c r="F40" s="2"/>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B41" s="164">
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B41" s="130">
+        <v>250</v>
+      </c>
+      <c r="C41" s="130">
+        <v>0</v>
+      </c>
+      <c r="D41" s="130" t="s">
+        <v>170</v>
+      </c>
+      <c r="E41" s="130"/>
+      <c r="F41" s="131"/>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B42" s="82"/>
+      <c r="C42" s="82"/>
+      <c r="D42" s="82"/>
+      <c r="E42" s="82"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B43" s="164">
         <v>254</v>
       </c>
-      <c r="C41" s="164">
+      <c r="C43" s="164">
         <v>0</v>
       </c>
-      <c r="D41" s="164" t="s">
+      <c r="D43" s="164" t="s">
         <v>184</v>
       </c>
-      <c r="E41" s="164"/>
-      <c r="F41" s="165"/>
-    </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B42" s="107">
+      <c r="E43" s="164"/>
+      <c r="F43" s="165"/>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B44" s="107">
         <v>255</v>
       </c>
-      <c r="C42" s="107"/>
-      <c r="D42" s="107" t="s">
+      <c r="C44" s="107"/>
+      <c r="D44" s="107" t="s">
         <v>150</v>
       </c>
-      <c r="E42" s="107"/>
-      <c r="F42" s="108"/>
+      <c r="E44" s="107"/>
+      <c r="F44" s="108"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2545,32 +2571,32 @@
       <selection activeCell="F6" sqref="F6:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" style="3"/>
-    <col min="3" max="4" width="19.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="3"/>
-    <col min="6" max="7" width="20.5" style="3" customWidth="1"/>
-    <col min="8" max="8" width="2.5" style="3" customWidth="1"/>
-    <col min="9" max="9" width="3.5" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="3"/>
+    <col min="1" max="2" width="8.81640625" style="3"/>
+    <col min="3" max="4" width="19.6328125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" style="3"/>
+    <col min="6" max="7" width="20.453125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="2.453125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="3.453125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="169" t="s">
         <v>158</v>
       </c>
       <c r="C2" s="170"/>
       <c r="D2" s="171"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="172" t="s">
         <v>145</v>
       </c>
       <c r="C5" s="172"/>
       <c r="E5" s="93"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="14">
         <v>3</v>
       </c>
@@ -2585,7 +2611,7 @@
       </c>
       <c r="G6" s="42"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="49">
         <v>4</v>
       </c>
@@ -2603,7 +2629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="25">
         <v>5</v>
       </c>
@@ -2617,7 +2643,7 @@
       <c r="G8" s="48"/>
       <c r="H8" s="76"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="25">
         <v>6</v>
       </c>
@@ -2629,7 +2655,7 @@
       <c r="G9" s="48"/>
       <c r="H9" s="76"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="25">
         <v>7</v>
       </c>
@@ -2643,7 +2669,7 @@
       <c r="G10" s="48"/>
       <c r="H10" s="76"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="25">
         <v>7</v>
       </c>
@@ -2652,12 +2678,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="74" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="173" t="s">
         <v>152</v>
       </c>
@@ -2682,26 +2708,26 @@
       <selection activeCell="C29" sqref="C29:D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="3"/>
-    <col min="2" max="2" width="6.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" style="3"/>
+    <col min="2" max="2" width="6.453125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="8.83203125" style="3"/>
-    <col min="7" max="8" width="30.6640625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="3.1640625" style="4" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="3"/>
+    <col min="4" max="4" width="32.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="8.81640625" style="3"/>
+    <col min="7" max="8" width="30.6328125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="3.1796875" style="4" customWidth="1"/>
+    <col min="10" max="16384" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" s="169" t="s">
         <v>68</v>
       </c>
       <c r="C2" s="170"/>
       <c r="D2" s="171"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" s="14">
         <v>3</v>
       </c>
@@ -2715,7 +2741,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="14">
         <v>4</v>
       </c>
@@ -2733,7 +2759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="25">
         <v>5</v>
       </c>
@@ -2754,7 +2780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="25">
         <v>6</v>
       </c>
@@ -2770,7 +2796,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="G9" s="13" t="s">
         <v>101</v>
       </c>
@@ -2779,7 +2805,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="14">
         <v>3</v>
       </c>
@@ -2793,7 +2819,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="14">
         <v>4</v>
       </c>
@@ -2813,7 +2839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="25">
         <v>5</v>
       </c>
@@ -2836,7 +2862,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="25">
         <v>6</v>
       </c>
@@ -2854,7 +2880,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="25">
         <v>7</v>
       </c>
@@ -2875,7 +2901,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" s="25">
         <v>8</v>
       </c>
@@ -2898,7 +2924,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B17" s="25">
         <v>9</v>
       </c>
@@ -2910,7 +2936,7 @@
       <c r="H17" s="36"/>
       <c r="I17" s="8"/>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="14">
         <v>3</v>
       </c>
@@ -2921,7 +2947,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="14">
         <v>4</v>
       </c>
@@ -2937,7 +2963,7 @@
       <c r="H21" s="219"/>
       <c r="I21" s="220"/>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" s="14">
         <v>5</v>
       </c>
@@ -2951,7 +2977,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B23" s="14">
         <v>6</v>
       </c>
@@ -2963,7 +2989,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" s="14">
         <v>7</v>
       </c>
@@ -2982,7 +3008,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B25" s="14">
         <v>8</v>
       </c>
@@ -3003,7 +3029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" s="14">
         <v>9</v>
       </c>
@@ -3019,7 +3045,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B27" s="14">
         <v>10</v>
       </c>
@@ -3035,7 +3061,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" s="14">
         <v>11</v>
       </c>
@@ -3046,7 +3072,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" s="14">
         <v>12</v>
       </c>
@@ -3060,7 +3086,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B30" s="14">
         <v>13</v>
       </c>
@@ -3076,7 +3102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B31" s="14">
         <v>14</v>
       </c>
@@ -3092,7 +3118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B32" s="14">
         <v>15</v>
       </c>
@@ -3101,7 +3127,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B33" s="14">
         <v>16</v>
       </c>
@@ -3110,7 +3136,7 @@
       </c>
       <c r="D33" s="51"/>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B34" s="14">
         <v>17</v>
       </c>
@@ -3121,7 +3147,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B35" s="14">
         <v>18</v>
       </c>
@@ -3150,42 +3176,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="3"/>
-    <col min="2" max="2" width="11.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1796875" style="3"/>
+    <col min="2" max="2" width="11.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.453125" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27" style="3" customWidth="1"/>
-    <col min="8" max="8" width="2.6640625" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.1640625" style="3"/>
+    <col min="8" max="8" width="2.6328125" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="169" t="s">
         <v>24</v>
       </c>
       <c r="C2" s="170"/>
       <c r="D2" s="171"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="57"/>
       <c r="C3" s="57"/>
       <c r="D3" s="57"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="172" t="s">
         <v>145</v>
       </c>
       <c r="C4" s="172"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="14">
         <v>3</v>
       </c>
@@ -3199,7 +3225,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="14">
         <v>4</v>
       </c>
@@ -3219,7 +3245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="14">
         <v>5</v>
       </c>
@@ -3237,7 +3263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="14">
         <v>6</v>
       </c>
@@ -3255,7 +3281,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="14">
         <v>7</v>
       </c>
@@ -3273,7 +3299,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="14">
         <v>8</v>
       </c>
@@ -3283,7 +3309,7 @@
       <c r="D10" s="41"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="14">
         <v>9</v>
       </c>
@@ -3296,7 +3322,7 @@
       </c>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="14">
         <v>10</v>
       </c>
@@ -3317,7 +3343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="14">
         <v>11</v>
       </c>
@@ -3333,7 +3359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="14">
         <v>12</v>
       </c>
@@ -3349,7 +3375,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="14">
         <v>13</v>
       </c>
@@ -3363,7 +3389,7 @@
       <c r="G15" s="75"/>
       <c r="H15" s="76"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="14">
         <v>14</v>
       </c>
@@ -3376,7 +3402,7 @@
       </c>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="14">
         <v>15</v>
       </c>
@@ -3394,7 +3420,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="14">
         <v>16</v>
       </c>
@@ -3410,7 +3436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="46"/>
       <c r="F19" s="13" t="s">
         <v>39</v>
@@ -3420,10 +3446,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="74" t="s">
         <v>144</v>
       </c>
@@ -3432,7 +3458,7 @@
       </c>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="173" t="s">
         <v>152</v>
       </c>
@@ -3448,7 +3474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F23" s="13" t="s">
         <v>42</v>
       </c>
@@ -3457,7 +3483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="46"/>
       <c r="C24" s="42"/>
       <c r="D24" s="111"/>
@@ -3469,7 +3495,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="46"/>
       <c r="C25" s="42"/>
       <c r="D25" s="46"/>
@@ -3481,7 +3507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F26" s="13" t="s">
         <v>45</v>
       </c>
@@ -3490,7 +3516,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="169" t="s">
         <v>23</v>
       </c>
@@ -3504,7 +3530,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F28" s="13" t="s">
         <v>47</v>
       </c>
@@ -3513,7 +3539,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:8" ht="24" x14ac:dyDescent="0.3">
       <c r="B29" s="157" t="s">
         <v>145</v>
       </c>
@@ -3526,7 +3552,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" s="14">
         <v>3</v>
       </c>
@@ -3538,7 +3564,7 @@
       </c>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" s="14">
         <v>4</v>
       </c>
@@ -3553,7 +3579,7 @@
       </c>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F32" s="13" t="s">
         <v>64</v>
       </c>
@@ -3562,7 +3588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B33" s="74" t="s">
         <v>144</v>
       </c>
@@ -3574,19 +3600,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B34" s="158" t="s">
         <v>152</v>
       </c>
       <c r="C34" s="159"/>
       <c r="D34" s="160"/>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F35" s="168" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B36" s="14">
         <v>3</v>
       </c>
@@ -3604,7 +3630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B37" s="14">
         <v>4</v>
       </c>
@@ -3622,7 +3648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B38" s="14">
         <v>5</v>
       </c>
@@ -3638,7 +3664,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:8" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B39" s="14">
         <v>6</v>
       </c>
@@ -3654,7 +3680,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B40" s="14">
         <v>7</v>
       </c>
@@ -3663,7 +3689,7 @@
       </c>
       <c r="D40" s="33"/>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B41" s="14">
         <v>8</v>
       </c>
@@ -3672,7 +3698,7 @@
       </c>
       <c r="D41" s="41"/>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B42" s="14">
         <v>9</v>
       </c>
@@ -3681,7 +3707,7 @@
       </c>
       <c r="D42" s="32"/>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B43" s="14">
         <v>10</v>
       </c>
@@ -3692,7 +3718,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B44" s="14">
         <v>11</v>
       </c>
@@ -3701,7 +3727,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B45" s="14">
         <v>12</v>
       </c>
@@ -3710,7 +3736,7 @@
       </c>
       <c r="D45" s="167"/>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B46" s="14">
         <v>13</v>
       </c>
@@ -3724,7 +3750,7 @@
       <c r="G46" s="71"/>
       <c r="H46" s="76"/>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B47" s="14">
         <v>14</v>
       </c>
@@ -3733,7 +3759,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B48" s="14">
         <v>15</v>
       </c>
@@ -3742,7 +3768,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" s="14">
         <v>16</v>
       </c>
@@ -3773,50 +3799,50 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.6640625" style="3"/>
-    <col min="3" max="3" width="12.5" style="3" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" style="3"/>
-    <col min="6" max="6" width="37.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="22" width="3.6640625" style="3" customWidth="1"/>
-    <col min="23" max="16384" width="8.6640625" style="3"/>
+    <col min="1" max="2" width="8.6328125" style="3"/>
+    <col min="3" max="3" width="12.453125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6328125" style="3"/>
+    <col min="6" max="6" width="37.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="22" width="3.6328125" style="3" customWidth="1"/>
+    <col min="23" max="16384" width="8.6328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.15">
-      <c r="B2" s="177" t="s">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B2" s="187" t="s">
         <v>131</v>
       </c>
-      <c r="C2" s="178"/>
-      <c r="D2" s="179"/>
-    </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.15">
+      <c r="C2" s="188"/>
+      <c r="D2" s="189"/>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B4" s="172" t="s">
         <v>145</v>
       </c>
       <c r="C4" s="172"/>
       <c r="E4" s="71"/>
-      <c r="G4" s="223" t="s">
+      <c r="G4" s="236" t="s">
         <v>160</v>
       </c>
-      <c r="H4" s="223"/>
-      <c r="I4" s="223"/>
-      <c r="J4" s="223"/>
-      <c r="K4" s="223"/>
-      <c r="L4" s="223"/>
-      <c r="M4" s="223"/>
-      <c r="N4" s="223"/>
-      <c r="O4" s="223"/>
-      <c r="P4" s="223"/>
-      <c r="Q4" s="223"/>
-      <c r="R4" s="223"/>
-      <c r="S4" s="223"/>
-      <c r="T4" s="223"/>
-      <c r="U4" s="223"/>
-      <c r="V4" s="223"/>
-    </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.15">
+      <c r="H4" s="236"/>
+      <c r="I4" s="236"/>
+      <c r="J4" s="236"/>
+      <c r="K4" s="236"/>
+      <c r="L4" s="236"/>
+      <c r="M4" s="236"/>
+      <c r="N4" s="236"/>
+      <c r="O4" s="236"/>
+      <c r="P4" s="236"/>
+      <c r="Q4" s="236"/>
+      <c r="R4" s="236"/>
+      <c r="S4" s="236"/>
+      <c r="T4" s="236"/>
+      <c r="U4" s="236"/>
+      <c r="V4" s="236"/>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B5" s="14">
         <v>3</v>
       </c>
@@ -3879,7 +3905,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B6" s="14">
         <v>4</v>
       </c>
@@ -3942,7 +3968,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.3">
       <c r="F7" s="77" t="s">
         <v>28</v>
       </c>
@@ -3981,7 +4007,7 @@
       <c r="U7" s="13"/>
       <c r="V7" s="13"/>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
       <c r="F8" s="77" t="s">
         <v>31</v>
       </c>
@@ -4020,7 +4046,7 @@
       <c r="U8" s="13"/>
       <c r="V8" s="13"/>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
       <c r="F9" s="77" t="s">
         <v>32</v>
       </c>
@@ -4049,7 +4075,7 @@
       <c r="U9" s="13"/>
       <c r="V9" s="13"/>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B10" s="74" t="s">
         <v>144</v>
       </c>
@@ -4079,7 +4105,7 @@
       <c r="U10" s="13"/>
       <c r="V10" s="13"/>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B11" s="74"/>
       <c r="F11" s="77" t="s">
         <v>29</v>
@@ -4115,7 +4141,7 @@
       <c r="U11" s="13"/>
       <c r="V11" s="13"/>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B12" s="173" t="s">
         <v>152</v>
       </c>
@@ -4139,7 +4165,7 @@
       <c r="U12" s="71"/>
       <c r="V12" s="71"/>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B13" s="74"/>
       <c r="F13" s="48"/>
       <c r="G13" s="71"/>
@@ -4159,35 +4185,35 @@
       <c r="U13" s="71"/>
       <c r="V13" s="71"/>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B14" s="78" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B15" s="66">
         <v>0</v>
       </c>
-      <c r="C15" s="227" t="s">
+      <c r="C15" s="230" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="90"/>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B16" s="66">
         <v>1</v>
       </c>
-      <c r="C16" s="228"/>
+      <c r="C16" s="231"/>
       <c r="D16" s="91"/>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B17" s="66">
         <v>2</v>
       </c>
-      <c r="C17" s="229"/>
+      <c r="C17" s="232"/>
       <c r="D17" s="92"/>
     </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B18" s="14">
         <v>3</v>
       </c>
@@ -4198,7 +4224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B19" s="14">
         <v>4</v>
       </c>
@@ -4209,60 +4235,60 @@
         <v>129</v>
       </c>
     </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B20" s="14">
         <v>5</v>
       </c>
-      <c r="C20" s="230" t="s">
+      <c r="C20" s="228" t="s">
         <v>125</v>
       </c>
       <c r="D20" s="58" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B21" s="14">
         <v>6</v>
       </c>
-      <c r="C21" s="231"/>
+      <c r="C21" s="229"/>
       <c r="D21" s="59" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B22" s="14">
         <v>7</v>
       </c>
-      <c r="C22" s="231"/>
+      <c r="C22" s="229"/>
       <c r="D22" s="59" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B23" s="14">
         <v>8</v>
       </c>
-      <c r="C23" s="231"/>
+      <c r="C23" s="229"/>
       <c r="D23" s="60" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B24" s="14">
         <v>9</v>
       </c>
-      <c r="C24" s="230" t="s">
+      <c r="C24" s="228" t="s">
         <v>126</v>
       </c>
       <c r="D24" s="58" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B25" s="14">
         <v>10</v>
       </c>
-      <c r="C25" s="231"/>
+      <c r="C25" s="229"/>
       <c r="D25" s="59" t="s">
         <v>79</v>
       </c>
@@ -4284,87 +4310,87 @@
       <c r="U25" s="72"/>
       <c r="V25" s="72"/>
     </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B26" s="14">
         <v>11</v>
       </c>
-      <c r="C26" s="231"/>
+      <c r="C26" s="229"/>
       <c r="D26" s="59" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="27" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B27" s="14">
         <v>12</v>
       </c>
-      <c r="C27" s="231"/>
+      <c r="C27" s="229"/>
       <c r="D27" s="60" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B28" s="14">
         <v>13</v>
       </c>
-      <c r="C28" s="230" t="s">
+      <c r="C28" s="228" t="s">
         <v>127</v>
       </c>
       <c r="D28" s="58" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B29" s="14">
         <v>14</v>
       </c>
-      <c r="C29" s="231"/>
+      <c r="C29" s="229"/>
       <c r="D29" s="59" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B30" s="14">
         <v>15</v>
       </c>
-      <c r="C30" s="231"/>
+      <c r="C30" s="229"/>
       <c r="D30" s="59" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B31" s="14">
         <v>16</v>
       </c>
-      <c r="C31" s="231"/>
+      <c r="C31" s="229"/>
       <c r="D31" s="60" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B32" s="14">
         <v>17</v>
       </c>
-      <c r="C32" s="230" t="s">
+      <c r="C32" s="228" t="s">
         <v>128</v>
       </c>
       <c r="D32" s="58" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B33" s="14">
         <v>18</v>
       </c>
-      <c r="C33" s="231"/>
+      <c r="C33" s="229"/>
       <c r="D33" s="59" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B34" s="14">
         <v>19</v>
       </c>
-      <c r="C34" s="231"/>
+      <c r="C34" s="229"/>
       <c r="D34" s="59" t="s">
         <v>81</v>
       </c>
@@ -4386,11 +4412,11 @@
       <c r="V34" s="71"/>
       <c r="W34" s="71"/>
     </row>
-    <row r="35" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B35" s="14">
         <v>20</v>
       </c>
-      <c r="C35" s="231"/>
+      <c r="C35" s="229"/>
       <c r="D35" s="60" t="s">
         <v>80</v>
       </c>
@@ -4412,11 +4438,11 @@
       <c r="V35" s="71"/>
       <c r="W35" s="71"/>
     </row>
-    <row r="36" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B36" s="14">
         <v>21</v>
       </c>
-      <c r="C36" s="230" t="s">
+      <c r="C36" s="228" t="s">
         <v>132</v>
       </c>
       <c r="D36" s="58" t="s">
@@ -4440,11 +4466,11 @@
       <c r="V36" s="71"/>
       <c r="W36" s="71"/>
     </row>
-    <row r="37" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B37" s="14">
         <v>22</v>
       </c>
-      <c r="C37" s="231"/>
+      <c r="C37" s="229"/>
       <c r="D37" s="59" t="s">
         <v>79</v>
       </c>
@@ -4466,11 +4492,11 @@
       <c r="V37" s="71"/>
       <c r="W37" s="71"/>
     </row>
-    <row r="38" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B38" s="14">
         <v>23</v>
       </c>
-      <c r="C38" s="231"/>
+      <c r="C38" s="229"/>
       <c r="D38" s="59" t="s">
         <v>81</v>
       </c>
@@ -4488,11 +4514,11 @@
       <c r="V38" s="71"/>
       <c r="W38" s="71"/>
     </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B39" s="14">
         <v>24</v>
       </c>
-      <c r="C39" s="231"/>
+      <c r="C39" s="229"/>
       <c r="D39" s="60" t="s">
         <v>80</v>
       </c>
@@ -4510,11 +4536,11 @@
       <c r="V39" s="71"/>
       <c r="W39" s="71"/>
     </row>
-    <row r="40" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B40" s="14">
         <v>25</v>
       </c>
-      <c r="C40" s="230" t="s">
+      <c r="C40" s="228" t="s">
         <v>133</v>
       </c>
       <c r="D40" s="58" t="s">
@@ -4534,11 +4560,11 @@
       <c r="V40" s="71"/>
       <c r="W40" s="71"/>
     </row>
-    <row r="41" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="41" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B41" s="14">
         <v>26</v>
       </c>
-      <c r="C41" s="231"/>
+      <c r="C41" s="229"/>
       <c r="D41" s="59" t="s">
         <v>79</v>
       </c>
@@ -4560,11 +4586,11 @@
       <c r="V41" s="71"/>
       <c r="W41" s="71"/>
     </row>
-    <row r="42" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B42" s="14">
         <v>27</v>
       </c>
-      <c r="C42" s="231"/>
+      <c r="C42" s="229"/>
       <c r="D42" s="59" t="s">
         <v>81</v>
       </c>
@@ -4586,11 +4612,11 @@
       <c r="V42" s="71"/>
       <c r="W42" s="71"/>
     </row>
-    <row r="43" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="43" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B43" s="14">
         <v>28</v>
       </c>
-      <c r="C43" s="231"/>
+      <c r="C43" s="229"/>
       <c r="D43" s="60" t="s">
         <v>80</v>
       </c>
@@ -4612,11 +4638,11 @@
       <c r="V43" s="71"/>
       <c r="W43" s="71"/>
     </row>
-    <row r="44" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="44" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B44" s="14">
         <v>29</v>
       </c>
-      <c r="C44" s="230" t="s">
+      <c r="C44" s="228" t="s">
         <v>134</v>
       </c>
       <c r="D44" s="58" t="s">
@@ -4640,231 +4666,231 @@
       <c r="V44" s="71"/>
       <c r="W44" s="71"/>
     </row>
-    <row r="45" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B45" s="14">
         <v>30</v>
       </c>
-      <c r="C45" s="231"/>
+      <c r="C45" s="229"/>
       <c r="D45" s="59" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="46" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B46" s="14">
         <v>31</v>
       </c>
-      <c r="C46" s="231"/>
+      <c r="C46" s="229"/>
       <c r="D46" s="59" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="47" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B47" s="14">
         <v>32</v>
       </c>
-      <c r="C47" s="231"/>
+      <c r="C47" s="229"/>
       <c r="D47" s="60" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="2:23" x14ac:dyDescent="0.15">
+    <row r="48" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B48" s="14">
         <v>33</v>
       </c>
-      <c r="C48" s="230" t="s">
+      <c r="C48" s="228" t="s">
         <v>135</v>
       </c>
       <c r="D48" s="58" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B49" s="14">
         <v>34</v>
       </c>
-      <c r="C49" s="231"/>
+      <c r="C49" s="229"/>
       <c r="D49" s="59" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B50" s="14">
         <v>35</v>
       </c>
-      <c r="C50" s="231"/>
+      <c r="C50" s="229"/>
       <c r="D50" s="59" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B51" s="14">
         <v>36</v>
       </c>
-      <c r="C51" s="231"/>
+      <c r="C51" s="229"/>
       <c r="D51" s="60" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B52" s="14">
         <v>37</v>
       </c>
-      <c r="C52" s="232" t="s">
+      <c r="C52" s="237" t="s">
         <v>136</v>
       </c>
       <c r="D52" s="58" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B53" s="14">
         <v>38</v>
       </c>
-      <c r="C53" s="233"/>
+      <c r="C53" s="238"/>
       <c r="D53" s="59" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B54" s="14">
         <v>39</v>
       </c>
-      <c r="C54" s="233"/>
+      <c r="C54" s="238"/>
       <c r="D54" s="59" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B55" s="14">
         <v>40</v>
       </c>
-      <c r="C55" s="234"/>
+      <c r="C55" s="239"/>
       <c r="D55" s="60" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B56" s="14">
         <v>41</v>
       </c>
-      <c r="C56" s="230" t="s">
+      <c r="C56" s="228" t="s">
         <v>137</v>
       </c>
       <c r="D56" s="58" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B57" s="14">
         <v>42</v>
       </c>
-      <c r="C57" s="231"/>
+      <c r="C57" s="229"/>
       <c r="D57" s="59" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B58" s="14">
         <v>43</v>
       </c>
-      <c r="C58" s="231"/>
+      <c r="C58" s="229"/>
       <c r="D58" s="59" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B59" s="14">
         <v>44</v>
       </c>
-      <c r="C59" s="231"/>
+      <c r="C59" s="229"/>
       <c r="D59" s="60" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B60" s="14">
         <v>45</v>
       </c>
-      <c r="C60" s="230" t="s">
+      <c r="C60" s="228" t="s">
         <v>138</v>
       </c>
       <c r="D60" s="58" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B61" s="14">
         <v>46</v>
       </c>
-      <c r="C61" s="231"/>
+      <c r="C61" s="229"/>
       <c r="D61" s="59" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="62" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B62" s="14">
         <v>47</v>
       </c>
-      <c r="C62" s="231"/>
+      <c r="C62" s="229"/>
       <c r="D62" s="59" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B63" s="14">
         <v>48</v>
       </c>
-      <c r="C63" s="231"/>
+      <c r="C63" s="229"/>
       <c r="D63" s="60" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B64" s="14">
         <v>49</v>
       </c>
-      <c r="C64" s="230" t="s">
+      <c r="C64" s="228" t="s">
         <v>139</v>
       </c>
       <c r="D64" s="58" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="65" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B65" s="14">
         <v>50</v>
       </c>
-      <c r="C65" s="231"/>
+      <c r="C65" s="229"/>
       <c r="D65" s="59" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="66" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="66" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B66" s="14">
         <v>51</v>
       </c>
-      <c r="C66" s="231"/>
+      <c r="C66" s="229"/>
       <c r="D66" s="59" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="67" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="67" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B67" s="14">
         <v>52</v>
       </c>
-      <c r="C67" s="231"/>
+      <c r="C67" s="229"/>
       <c r="D67" s="60" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="68" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="68" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B68" s="14">
         <v>53</v>
       </c>
       <c r="C68" s="68"/>
       <c r="D68" s="68"/>
     </row>
-    <row r="69" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="69" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B69" s="14">
         <v>54</v>
       </c>
@@ -4875,112 +4901,112 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="70" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B70" s="14">
         <v>55</v>
       </c>
-      <c r="C70" s="224" t="s">
+      <c r="C70" s="233" t="s">
         <v>7</v>
       </c>
       <c r="D70" s="54" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="71" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="71" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B71" s="14">
         <v>56</v>
       </c>
-      <c r="C71" s="225"/>
+      <c r="C71" s="234"/>
       <c r="D71" s="55" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="72" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="72" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B72" s="14">
         <v>57</v>
       </c>
-      <c r="C72" s="225"/>
+      <c r="C72" s="234"/>
       <c r="D72" s="55" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="73" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="73" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B73" s="14">
         <v>58</v>
       </c>
-      <c r="C73" s="226"/>
+      <c r="C73" s="235"/>
       <c r="D73" s="56" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="74" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B74" s="14">
         <v>59</v>
       </c>
-      <c r="C74" s="235" t="s">
+      <c r="C74" s="223" t="s">
         <v>5</v>
       </c>
       <c r="D74" s="64"/>
     </row>
-    <row r="75" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="75" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B75" s="14">
         <v>60</v>
       </c>
-      <c r="C75" s="236"/>
+      <c r="C75" s="224"/>
       <c r="D75" s="65"/>
     </row>
-    <row r="76" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="76" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B76" s="14">
         <v>61</v>
       </c>
-      <c r="C76" s="237" t="s">
+      <c r="C76" s="225" t="s">
         <v>6</v>
       </c>
       <c r="D76" s="61"/>
     </row>
-    <row r="77" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="77" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B77" s="14">
         <v>62</v>
       </c>
-      <c r="C77" s="238"/>
+      <c r="C77" s="226"/>
       <c r="D77" s="62"/>
     </row>
-    <row r="78" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="78" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B78" s="14">
         <v>63</v>
       </c>
-      <c r="C78" s="239"/>
+      <c r="C78" s="227"/>
       <c r="D78" s="63"/>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B82" s="78" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="83" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B83" s="66">
         <v>0</v>
       </c>
-      <c r="C83" s="227" t="s">
+      <c r="C83" s="230" t="s">
         <v>2</v>
       </c>
       <c r="D83" s="61"/>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="84" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B84" s="66">
         <v>1</v>
       </c>
-      <c r="C84" s="228"/>
+      <c r="C84" s="231"/>
       <c r="D84" s="62"/>
     </row>
-    <row r="85" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="85" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B85" s="66">
         <v>2</v>
       </c>
-      <c r="C85" s="229"/>
+      <c r="C85" s="232"/>
       <c r="D85" s="63"/>
     </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="86" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B86" s="14">
         <v>3</v>
       </c>
@@ -4991,7 +5017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="87" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B87" s="14">
         <v>4</v>
       </c>
@@ -5002,390 +5028,390 @@
         <v>129</v>
       </c>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="88" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B88" s="14">
         <v>5</v>
       </c>
-      <c r="C88" s="230" t="s">
+      <c r="C88" s="228" t="s">
         <v>140</v>
       </c>
       <c r="D88" s="58" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B89" s="14">
         <v>6</v>
       </c>
-      <c r="C89" s="231"/>
+      <c r="C89" s="229"/>
       <c r="D89" s="59" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B90" s="14">
         <v>7</v>
       </c>
-      <c r="C90" s="231"/>
+      <c r="C90" s="229"/>
       <c r="D90" s="59" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="91" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B91" s="14">
         <v>8</v>
       </c>
-      <c r="C91" s="231"/>
+      <c r="C91" s="229"/>
       <c r="D91" s="60" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="92" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B92" s="14">
         <v>9</v>
       </c>
-      <c r="C92" s="230" t="s">
+      <c r="C92" s="228" t="s">
         <v>141</v>
       </c>
       <c r="D92" s="58" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B93" s="14">
         <v>10</v>
       </c>
-      <c r="C93" s="231"/>
+      <c r="C93" s="229"/>
       <c r="D93" s="59" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="94" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B94" s="14">
         <v>11</v>
       </c>
-      <c r="C94" s="231"/>
+      <c r="C94" s="229"/>
       <c r="D94" s="59" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="95" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="95" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B95" s="14">
         <v>12</v>
       </c>
-      <c r="C95" s="231"/>
+      <c r="C95" s="229"/>
       <c r="D95" s="60" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="96" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B96" s="14">
         <v>13</v>
       </c>
-      <c r="C96" s="230" t="s">
+      <c r="C96" s="228" t="s">
         <v>142</v>
       </c>
       <c r="D96" s="58" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="97" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="97" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B97" s="14">
         <v>14</v>
       </c>
-      <c r="C97" s="231"/>
+      <c r="C97" s="229"/>
       <c r="D97" s="59" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="98" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="98" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B98" s="14">
         <v>15</v>
       </c>
-      <c r="C98" s="231"/>
+      <c r="C98" s="229"/>
       <c r="D98" s="59" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="99" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="99" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B99" s="14">
         <v>16</v>
       </c>
-      <c r="C99" s="231"/>
+      <c r="C99" s="229"/>
       <c r="D99" s="60" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="100" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="100" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B100" s="14">
         <v>17</v>
       </c>
-      <c r="C100" s="230" t="s">
+      <c r="C100" s="228" t="s">
         <v>143</v>
       </c>
       <c r="D100" s="58" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="101" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B101" s="14">
         <v>18</v>
       </c>
-      <c r="C101" s="231"/>
+      <c r="C101" s="229"/>
       <c r="D101" s="59" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B102" s="14">
         <v>19</v>
       </c>
-      <c r="C102" s="231"/>
+      <c r="C102" s="229"/>
       <c r="D102" s="59" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B103" s="14">
         <v>20</v>
       </c>
-      <c r="C103" s="231"/>
+      <c r="C103" s="229"/>
       <c r="D103" s="60" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="104" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B104" s="14">
         <v>21</v>
       </c>
       <c r="C104" s="70"/>
       <c r="D104" s="69"/>
     </row>
-    <row r="105" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="105" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B105" s="14">
         <v>22</v>
       </c>
       <c r="C105" s="70"/>
       <c r="D105" s="69"/>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B106" s="14">
         <v>23</v>
       </c>
       <c r="C106" s="70"/>
       <c r="D106" s="69"/>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="107" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B107" s="14">
         <v>24</v>
       </c>
       <c r="C107" s="70"/>
       <c r="D107" s="69"/>
     </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="108" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B108" s="14">
         <v>25</v>
       </c>
       <c r="C108" s="70"/>
       <c r="D108" s="69"/>
     </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B109" s="14">
         <v>26</v>
       </c>
       <c r="C109" s="70"/>
       <c r="D109" s="69"/>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B110" s="14">
         <v>27</v>
       </c>
       <c r="C110" s="70"/>
       <c r="D110" s="69"/>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B111" s="14">
         <v>28</v>
       </c>
       <c r="C111" s="70"/>
       <c r="D111" s="69"/>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B112" s="14">
         <v>29</v>
       </c>
       <c r="C112" s="70"/>
       <c r="D112" s="69"/>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="113" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B113" s="14">
         <v>30</v>
       </c>
       <c r="C113" s="70"/>
       <c r="D113" s="69"/>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="114" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B114" s="14">
         <v>31</v>
       </c>
       <c r="C114" s="70"/>
       <c r="D114" s="69"/>
     </row>
-    <row r="115" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="115" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B115" s="14">
         <v>32</v>
       </c>
       <c r="C115" s="70"/>
       <c r="D115" s="69"/>
     </row>
-    <row r="116" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="116" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B116" s="14">
         <v>33</v>
       </c>
       <c r="C116" s="70"/>
       <c r="D116" s="69"/>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="117" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B117" s="14">
         <v>34</v>
       </c>
       <c r="C117" s="70"/>
       <c r="D117" s="69"/>
     </row>
-    <row r="118" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="118" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B118" s="14">
         <v>35</v>
       </c>
       <c r="C118" s="70"/>
       <c r="D118" s="69"/>
     </row>
-    <row r="119" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="119" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B119" s="14">
         <v>36</v>
       </c>
       <c r="C119" s="70"/>
       <c r="D119" s="69"/>
     </row>
-    <row r="120" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="120" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B120" s="14">
         <v>37</v>
       </c>
       <c r="C120" s="70"/>
       <c r="D120" s="69"/>
     </row>
-    <row r="121" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="121" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B121" s="14">
         <v>38</v>
       </c>
       <c r="C121" s="70"/>
       <c r="D121" s="69"/>
     </row>
-    <row r="122" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="122" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B122" s="14">
         <v>39</v>
       </c>
       <c r="C122" s="70"/>
       <c r="D122" s="69"/>
     </row>
-    <row r="123" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="123" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B123" s="14">
         <v>40</v>
       </c>
       <c r="C123" s="70"/>
       <c r="D123" s="69"/>
     </row>
-    <row r="124" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="124" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B124" s="14">
         <v>41</v>
       </c>
       <c r="C124" s="13"/>
       <c r="D124" s="13"/>
     </row>
-    <row r="125" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="125" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B125" s="14">
         <v>42</v>
       </c>
       <c r="C125" s="13"/>
       <c r="D125" s="13"/>
     </row>
-    <row r="126" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="126" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B126" s="14">
         <v>43</v>
       </c>
       <c r="C126" s="13"/>
       <c r="D126" s="13"/>
     </row>
-    <row r="127" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="127" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B127" s="14">
         <v>44</v>
       </c>
       <c r="C127" s="13"/>
       <c r="D127" s="13"/>
     </row>
-    <row r="128" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="128" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B128" s="14">
         <v>45</v>
       </c>
       <c r="C128" s="13"/>
       <c r="D128" s="13"/>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="129" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B129" s="14">
         <v>46</v>
       </c>
       <c r="C129" s="13"/>
       <c r="D129" s="13"/>
     </row>
-    <row r="130" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="130" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B130" s="14">
         <v>47</v>
       </c>
       <c r="C130" s="13"/>
       <c r="D130" s="13"/>
     </row>
-    <row r="131" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="131" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B131" s="14">
         <v>48</v>
       </c>
       <c r="C131" s="13"/>
       <c r="D131" s="13"/>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="132" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B132" s="14">
         <v>49</v>
       </c>
       <c r="C132" s="13"/>
       <c r="D132" s="13"/>
     </row>
-    <row r="133" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="133" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B133" s="14">
         <v>50</v>
       </c>
       <c r="C133" s="13"/>
       <c r="D133" s="13"/>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="134" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B134" s="14">
         <v>51</v>
       </c>
       <c r="C134" s="13"/>
       <c r="D134" s="13"/>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="135" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B135" s="14">
         <v>52</v>
       </c>
       <c r="C135" s="13"/>
       <c r="D135" s="13"/>
     </row>
-    <row r="136" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="136" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B136" s="14">
         <v>53</v>
       </c>
       <c r="C136" s="13"/>
       <c r="D136" s="13"/>
     </row>
-    <row r="137" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="137" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B137" s="14">
         <v>54</v>
       </c>
@@ -5396,98 +5422,85 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="138" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B138" s="14">
         <v>55</v>
       </c>
-      <c r="C138" s="224" t="s">
+      <c r="C138" s="233" t="s">
         <v>7</v>
       </c>
       <c r="D138" s="54" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="139" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B139" s="14">
         <v>56</v>
       </c>
-      <c r="C139" s="225"/>
+      <c r="C139" s="234"/>
       <c r="D139" s="55" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="140" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="140" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B140" s="14">
         <v>57</v>
       </c>
-      <c r="C140" s="225"/>
+      <c r="C140" s="234"/>
       <c r="D140" s="55" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="141" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="141" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B141" s="14">
         <v>58</v>
       </c>
-      <c r="C141" s="226"/>
+      <c r="C141" s="235"/>
       <c r="D141" s="56" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="142" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B142" s="14">
         <v>59</v>
       </c>
-      <c r="C142" s="235" t="s">
+      <c r="C142" s="223" t="s">
         <v>5</v>
       </c>
       <c r="D142" s="64"/>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="143" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B143" s="14">
         <v>60</v>
       </c>
-      <c r="C143" s="236"/>
+      <c r="C143" s="224"/>
       <c r="D143" s="65"/>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="144" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B144" s="14">
         <v>61</v>
       </c>
-      <c r="C144" s="237" t="s">
+      <c r="C144" s="225" t="s">
         <v>6</v>
       </c>
       <c r="D144" s="61"/>
     </row>
-    <row r="145" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="145" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B145" s="14">
         <v>62</v>
       </c>
-      <c r="C145" s="238"/>
+      <c r="C145" s="226"/>
       <c r="D145" s="62"/>
     </row>
-    <row r="146" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="146" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B146" s="14">
         <v>63</v>
       </c>
-      <c r="C146" s="239"/>
+      <c r="C146" s="227"/>
       <c r="D146" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C142:C143"/>
-    <mergeCell ref="C144:C146"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="C60:C63"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="C83:C85"/>
-    <mergeCell ref="C88:C91"/>
-    <mergeCell ref="C92:C95"/>
-    <mergeCell ref="C96:C99"/>
-    <mergeCell ref="C100:C103"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="C76:C78"/>
-    <mergeCell ref="C74:C75"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B4:C4"/>
@@ -5503,6 +5516,19 @@
     <mergeCell ref="C44:C47"/>
     <mergeCell ref="C48:C51"/>
     <mergeCell ref="C52:C55"/>
+    <mergeCell ref="C142:C143"/>
+    <mergeCell ref="C144:C146"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="C60:C63"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="C88:C91"/>
+    <mergeCell ref="C92:C95"/>
+    <mergeCell ref="C96:C99"/>
+    <mergeCell ref="C100:C103"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="C76:C78"/>
+    <mergeCell ref="C74:C75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5516,12 +5542,12 @@
       <selection activeCell="C4" sqref="C4:E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C4" s="169" t="s">
         <v>171</v>
       </c>
@@ -5529,19 +5555,19 @@
       <c r="E4" s="171"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C7" s="172" t="s">
         <v>145</v>
       </c>
@@ -5549,7 +5575,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="93"/>
     </row>
-    <row r="8" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C8" s="14">
         <v>3</v>
       </c>
@@ -5561,7 +5587,7 @@
       </c>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C9" s="49">
         <v>4</v>
       </c>
@@ -5573,25 +5599,25 @@
       </c>
       <c r="F9" s="3"/>
     </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C13" s="74" t="s">
         <v>144</v>
       </c>
@@ -5599,7 +5625,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C14" s="173" t="s">
         <v>152</v>
       </c>
@@ -5607,13 +5633,13 @@
       <c r="E14" s="175"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="17" spans="3:5" s="3" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="17" spans="3:5" s="3" customFormat="1" ht="12" x14ac:dyDescent="0.3">
       <c r="C17" s="14">
         <v>3</v>
       </c>
@@ -5624,7 +5650,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="18" spans="3:5" s="3" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="18" spans="3:5" s="3" customFormat="1" ht="12" x14ac:dyDescent="0.3">
       <c r="C18" s="49">
         <v>4</v>
       </c>
@@ -5635,7 +5661,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="3:5" s="3" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="19" spans="3:5" s="3" customFormat="1" ht="12" x14ac:dyDescent="0.3">
       <c r="C19" s="25" t="s">
         <v>172</v>
       </c>
@@ -5646,7 +5672,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="3:5" s="3" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="20" spans="3:5" s="3" customFormat="1" ht="12" x14ac:dyDescent="0.3">
       <c r="C20" s="25" t="s">
         <v>172</v>
       </c>
@@ -5655,7 +5681,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="3:5" s="3" customFormat="1" ht="12" x14ac:dyDescent="0.15">
+    <row r="21" spans="3:5" s="3" customFormat="1" ht="12" x14ac:dyDescent="0.3">
       <c r="C21" s="14" t="s">
         <v>172</v>
       </c>
@@ -5682,57 +5708,57 @@
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C4" s="169" t="s">
         <v>184</v>
       </c>
       <c r="D4" s="170"/>
       <c r="E4" s="171"/>
     </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
     </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C7" s="74" t="s">
         <v>144</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
     </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C8" s="176" t="s">
         <v>122</v>
       </c>
       <c r="D8" s="176"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C9" s="173" t="s">
         <v>152</v>
       </c>
       <c r="D9" s="174"/>
       <c r="E9" s="175"/>
     </row>
-    <row r="10" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C11" s="14">
         <v>3</v>
       </c>
@@ -5743,7 +5769,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="12" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C12" s="49">
         <v>4</v>
       </c>
@@ -5754,7 +5780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C13" s="25">
         <v>5</v>
       </c>
@@ -5765,7 +5791,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C14" s="25">
         <v>6</v>
       </c>
@@ -5774,7 +5800,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C15" s="14">
         <v>7</v>
       </c>
@@ -5785,7 +5811,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C16" s="14">
         <v>7</v>
       </c>
@@ -5794,7 +5820,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C17" s="14">
         <v>8</v>
       </c>
@@ -5823,365 +5849,365 @@
       <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" style="3" customWidth="1"/>
-    <col min="2" max="2" width="5.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5" style="3" customWidth="1"/>
-    <col min="4" max="6" width="2.6640625" style="4" customWidth="1"/>
-    <col min="7" max="8" width="7.6640625" style="4" customWidth="1"/>
-    <col min="9" max="54" width="2.6640625" style="5" customWidth="1"/>
-    <col min="55" max="57" width="2.6640625" style="4" customWidth="1"/>
-    <col min="58" max="58" width="12.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="59" max="67" width="2.6640625" style="4" customWidth="1"/>
-    <col min="68" max="16384" width="9.1640625" style="3"/>
+    <col min="2" max="2" width="5.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" style="3" customWidth="1"/>
+    <col min="4" max="6" width="2.6328125" style="4" customWidth="1"/>
+    <col min="7" max="8" width="7.6328125" style="4" customWidth="1"/>
+    <col min="9" max="54" width="2.6328125" style="5" customWidth="1"/>
+    <col min="55" max="57" width="2.6328125" style="4" customWidth="1"/>
+    <col min="58" max="58" width="12.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="59" max="67" width="2.6328125" style="4" customWidth="1"/>
+    <col min="68" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B2" s="177" t="s">
+    <row r="2" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B2" s="187" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="178"/>
-      <c r="D2" s="178"/>
-      <c r="E2" s="178"/>
-      <c r="F2" s="179"/>
-    </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B4" s="180" t="s">
+      <c r="C2" s="188"/>
+      <c r="D2" s="188"/>
+      <c r="E2" s="188"/>
+      <c r="F2" s="189"/>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B4" s="178" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="180"/>
-      <c r="D4" s="187" t="s">
+      <c r="C4" s="178"/>
+      <c r="D4" s="177" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="187"/>
-      <c r="F4" s="187"/>
-      <c r="G4" s="187"/>
-      <c r="H4" s="187"/>
-      <c r="I4" s="187"/>
-      <c r="J4" s="187"/>
-      <c r="K4" s="187"/>
-      <c r="L4" s="187"/>
-      <c r="M4" s="187"/>
-      <c r="N4" s="187"/>
-      <c r="O4" s="187"/>
-      <c r="P4" s="187"/>
-      <c r="Q4" s="187"/>
-      <c r="R4" s="187"/>
-      <c r="S4" s="187"/>
-      <c r="T4" s="187"/>
-      <c r="U4" s="187"/>
-      <c r="V4" s="187"/>
-      <c r="W4" s="187"/>
-      <c r="X4" s="187"/>
-    </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B5" s="186"/>
-      <c r="C5" s="186"/>
-      <c r="D5" s="187"/>
-      <c r="E5" s="187"/>
-      <c r="F5" s="187"/>
-      <c r="G5" s="187"/>
-      <c r="H5" s="187"/>
-      <c r="I5" s="187"/>
-      <c r="J5" s="187"/>
-      <c r="K5" s="187"/>
-      <c r="L5" s="187"/>
-      <c r="M5" s="187"/>
-      <c r="N5" s="187"/>
-      <c r="O5" s="187"/>
-      <c r="P5" s="187"/>
-      <c r="Q5" s="187"/>
-      <c r="R5" s="187"/>
-      <c r="S5" s="187"/>
-      <c r="T5" s="187"/>
-      <c r="U5" s="187"/>
-      <c r="V5" s="187"/>
-      <c r="W5" s="187"/>
-      <c r="X5" s="187"/>
-    </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B6" s="189" t="s">
+      <c r="E4" s="177"/>
+      <c r="F4" s="177"/>
+      <c r="G4" s="177"/>
+      <c r="H4" s="177"/>
+      <c r="I4" s="177"/>
+      <c r="J4" s="177"/>
+      <c r="K4" s="177"/>
+      <c r="L4" s="177"/>
+      <c r="M4" s="177"/>
+      <c r="N4" s="177"/>
+      <c r="O4" s="177"/>
+      <c r="P4" s="177"/>
+      <c r="Q4" s="177"/>
+      <c r="R4" s="177"/>
+      <c r="S4" s="177"/>
+      <c r="T4" s="177"/>
+      <c r="U4" s="177"/>
+      <c r="V4" s="177"/>
+      <c r="W4" s="177"/>
+      <c r="X4" s="177"/>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B5" s="179"/>
+      <c r="C5" s="179"/>
+      <c r="D5" s="177"/>
+      <c r="E5" s="177"/>
+      <c r="F5" s="177"/>
+      <c r="G5" s="177"/>
+      <c r="H5" s="177"/>
+      <c r="I5" s="177"/>
+      <c r="J5" s="177"/>
+      <c r="K5" s="177"/>
+      <c r="L5" s="177"/>
+      <c r="M5" s="177"/>
+      <c r="N5" s="177"/>
+      <c r="O5" s="177"/>
+      <c r="P5" s="177"/>
+      <c r="Q5" s="177"/>
+      <c r="R5" s="177"/>
+      <c r="S5" s="177"/>
+      <c r="T5" s="177"/>
+      <c r="U5" s="177"/>
+      <c r="V5" s="177"/>
+      <c r="W5" s="177"/>
+      <c r="X5" s="177"/>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B6" s="180" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="189"/>
-      <c r="D6" s="187" t="s">
+      <c r="C6" s="180"/>
+      <c r="D6" s="177" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="187"/>
-      <c r="F6" s="187"/>
-      <c r="G6" s="187"/>
-      <c r="H6" s="187"/>
-      <c r="I6" s="187"/>
-      <c r="J6" s="187"/>
-      <c r="K6" s="187"/>
-      <c r="L6" s="187"/>
-      <c r="M6" s="187"/>
-      <c r="N6" s="187"/>
-      <c r="O6" s="187"/>
-      <c r="P6" s="187"/>
-      <c r="Q6" s="187"/>
-      <c r="R6" s="187"/>
-      <c r="S6" s="187"/>
-      <c r="T6" s="187"/>
-      <c r="U6" s="187"/>
-      <c r="V6" s="187"/>
-      <c r="W6" s="187"/>
-      <c r="X6" s="187"/>
-    </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B7" s="190" t="s">
+      <c r="E6" s="177"/>
+      <c r="F6" s="177"/>
+      <c r="G6" s="177"/>
+      <c r="H6" s="177"/>
+      <c r="I6" s="177"/>
+      <c r="J6" s="177"/>
+      <c r="K6" s="177"/>
+      <c r="L6" s="177"/>
+      <c r="M6" s="177"/>
+      <c r="N6" s="177"/>
+      <c r="O6" s="177"/>
+      <c r="P6" s="177"/>
+      <c r="Q6" s="177"/>
+      <c r="R6" s="177"/>
+      <c r="S6" s="177"/>
+      <c r="T6" s="177"/>
+      <c r="U6" s="177"/>
+      <c r="V6" s="177"/>
+      <c r="W6" s="177"/>
+      <c r="X6" s="177"/>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B7" s="181" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="190"/>
-      <c r="D7" s="187" t="s">
+      <c r="C7" s="181"/>
+      <c r="D7" s="177" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="187"/>
-      <c r="F7" s="187"/>
-      <c r="G7" s="187"/>
-      <c r="H7" s="187"/>
-      <c r="I7" s="187"/>
-      <c r="J7" s="187"/>
-      <c r="K7" s="187"/>
-      <c r="L7" s="187"/>
-      <c r="M7" s="187"/>
-      <c r="N7" s="187"/>
-      <c r="O7" s="187"/>
-      <c r="P7" s="187"/>
-      <c r="Q7" s="187"/>
-      <c r="R7" s="187"/>
-      <c r="S7" s="187"/>
-      <c r="T7" s="187"/>
-      <c r="U7" s="187"/>
-      <c r="V7" s="187"/>
-      <c r="W7" s="187"/>
-      <c r="X7" s="187"/>
-    </row>
-    <row r="8" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="E7" s="177"/>
+      <c r="F7" s="177"/>
+      <c r="G7" s="177"/>
+      <c r="H7" s="177"/>
+      <c r="I7" s="177"/>
+      <c r="J7" s="177"/>
+      <c r="K7" s="177"/>
+      <c r="L7" s="177"/>
+      <c r="M7" s="177"/>
+      <c r="N7" s="177"/>
+      <c r="O7" s="177"/>
+      <c r="P7" s="177"/>
+      <c r="Q7" s="177"/>
+      <c r="R7" s="177"/>
+      <c r="S7" s="177"/>
+      <c r="T7" s="177"/>
+      <c r="U7" s="177"/>
+      <c r="V7" s="177"/>
+      <c r="W7" s="177"/>
+      <c r="X7" s="177"/>
+    </row>
+    <row r="8" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B8" s="169"/>
       <c r="C8" s="171"/>
-      <c r="D8" s="183"/>
-      <c r="E8" s="184"/>
-      <c r="F8" s="184"/>
-      <c r="G8" s="184"/>
-      <c r="H8" s="184"/>
-      <c r="I8" s="184"/>
-      <c r="J8" s="184"/>
-      <c r="K8" s="184"/>
-      <c r="L8" s="184"/>
-      <c r="M8" s="184"/>
-      <c r="N8" s="184"/>
-      <c r="O8" s="184"/>
-      <c r="P8" s="184"/>
-      <c r="Q8" s="184"/>
-      <c r="R8" s="184"/>
-      <c r="S8" s="184"/>
-      <c r="T8" s="184"/>
-      <c r="U8" s="184"/>
-      <c r="V8" s="184"/>
-      <c r="W8" s="184"/>
-      <c r="X8" s="185"/>
-    </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B9" s="191" t="s">
+      <c r="D8" s="182"/>
+      <c r="E8" s="183"/>
+      <c r="F8" s="183"/>
+      <c r="G8" s="183"/>
+      <c r="H8" s="183"/>
+      <c r="I8" s="183"/>
+      <c r="J8" s="183"/>
+      <c r="K8" s="183"/>
+      <c r="L8" s="183"/>
+      <c r="M8" s="183"/>
+      <c r="N8" s="183"/>
+      <c r="O8" s="183"/>
+      <c r="P8" s="183"/>
+      <c r="Q8" s="183"/>
+      <c r="R8" s="183"/>
+      <c r="S8" s="183"/>
+      <c r="T8" s="183"/>
+      <c r="U8" s="183"/>
+      <c r="V8" s="183"/>
+      <c r="W8" s="183"/>
+      <c r="X8" s="184"/>
+    </row>
+    <row r="9" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B9" s="185" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="192"/>
-      <c r="D9" s="183"/>
-      <c r="E9" s="184"/>
-      <c r="F9" s="184"/>
-      <c r="G9" s="184"/>
-      <c r="H9" s="184"/>
-      <c r="I9" s="184"/>
-      <c r="J9" s="184"/>
-      <c r="K9" s="184"/>
-      <c r="L9" s="184"/>
-      <c r="M9" s="184"/>
-      <c r="N9" s="184"/>
-      <c r="O9" s="184"/>
-      <c r="P9" s="184"/>
-      <c r="Q9" s="184"/>
-      <c r="R9" s="184"/>
-      <c r="S9" s="184"/>
-      <c r="T9" s="184"/>
-      <c r="U9" s="184"/>
-      <c r="V9" s="184"/>
-      <c r="W9" s="184"/>
-      <c r="X9" s="185"/>
-    </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.15">
+      <c r="C9" s="186"/>
+      <c r="D9" s="182"/>
+      <c r="E9" s="183"/>
+      <c r="F9" s="183"/>
+      <c r="G9" s="183"/>
+      <c r="H9" s="183"/>
+      <c r="I9" s="183"/>
+      <c r="J9" s="183"/>
+      <c r="K9" s="183"/>
+      <c r="L9" s="183"/>
+      <c r="M9" s="183"/>
+      <c r="N9" s="183"/>
+      <c r="O9" s="183"/>
+      <c r="P9" s="183"/>
+      <c r="Q9" s="183"/>
+      <c r="R9" s="183"/>
+      <c r="S9" s="183"/>
+      <c r="T9" s="183"/>
+      <c r="U9" s="183"/>
+      <c r="V9" s="183"/>
+      <c r="W9" s="183"/>
+      <c r="X9" s="184"/>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B10" s="169"/>
       <c r="C10" s="171"/>
-      <c r="D10" s="183"/>
-      <c r="E10" s="184"/>
-      <c r="F10" s="184"/>
-      <c r="G10" s="184"/>
-      <c r="H10" s="184"/>
-      <c r="I10" s="184"/>
-      <c r="J10" s="184"/>
-      <c r="K10" s="184"/>
-      <c r="L10" s="184"/>
-      <c r="M10" s="184"/>
-      <c r="N10" s="184"/>
-      <c r="O10" s="184"/>
-      <c r="P10" s="184"/>
-      <c r="Q10" s="184"/>
-      <c r="R10" s="184"/>
-      <c r="S10" s="184"/>
-      <c r="T10" s="184"/>
-      <c r="U10" s="184"/>
-      <c r="V10" s="184"/>
-      <c r="W10" s="184"/>
-      <c r="X10" s="185"/>
-    </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B11" s="188" t="s">
+      <c r="D10" s="182"/>
+      <c r="E10" s="183"/>
+      <c r="F10" s="183"/>
+      <c r="G10" s="183"/>
+      <c r="H10" s="183"/>
+      <c r="I10" s="183"/>
+      <c r="J10" s="183"/>
+      <c r="K10" s="183"/>
+      <c r="L10" s="183"/>
+      <c r="M10" s="183"/>
+      <c r="N10" s="183"/>
+      <c r="O10" s="183"/>
+      <c r="P10" s="183"/>
+      <c r="Q10" s="183"/>
+      <c r="R10" s="183"/>
+      <c r="S10" s="183"/>
+      <c r="T10" s="183"/>
+      <c r="U10" s="183"/>
+      <c r="V10" s="183"/>
+      <c r="W10" s="183"/>
+      <c r="X10" s="184"/>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B11" s="192" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="188"/>
-      <c r="D11" s="187" t="s">
+      <c r="C11" s="192"/>
+      <c r="D11" s="177" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="187"/>
-      <c r="F11" s="187"/>
-      <c r="G11" s="187"/>
-      <c r="H11" s="187"/>
-      <c r="I11" s="187"/>
-      <c r="J11" s="187"/>
-      <c r="K11" s="187"/>
-      <c r="L11" s="187"/>
-      <c r="M11" s="187"/>
-      <c r="N11" s="187"/>
-      <c r="O11" s="187"/>
-      <c r="P11" s="187"/>
-      <c r="Q11" s="187"/>
-      <c r="R11" s="187"/>
-      <c r="S11" s="187"/>
-      <c r="T11" s="187"/>
-      <c r="U11" s="187"/>
-      <c r="V11" s="187"/>
-      <c r="W11" s="187"/>
-      <c r="X11" s="187"/>
-    </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B12" s="182" t="s">
+      <c r="E11" s="177"/>
+      <c r="F11" s="177"/>
+      <c r="G11" s="177"/>
+      <c r="H11" s="177"/>
+      <c r="I11" s="177"/>
+      <c r="J11" s="177"/>
+      <c r="K11" s="177"/>
+      <c r="L11" s="177"/>
+      <c r="M11" s="177"/>
+      <c r="N11" s="177"/>
+      <c r="O11" s="177"/>
+      <c r="P11" s="177"/>
+      <c r="Q11" s="177"/>
+      <c r="R11" s="177"/>
+      <c r="S11" s="177"/>
+      <c r="T11" s="177"/>
+      <c r="U11" s="177"/>
+      <c r="V11" s="177"/>
+      <c r="W11" s="177"/>
+      <c r="X11" s="177"/>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B12" s="191" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="182"/>
-      <c r="D12" s="187" t="s">
+      <c r="C12" s="191"/>
+      <c r="D12" s="177" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="187"/>
-      <c r="F12" s="187"/>
-      <c r="G12" s="187"/>
-      <c r="H12" s="187"/>
-      <c r="I12" s="187"/>
-      <c r="J12" s="187"/>
-      <c r="K12" s="187"/>
-      <c r="L12" s="187"/>
-      <c r="M12" s="187"/>
-      <c r="N12" s="187"/>
-      <c r="O12" s="187"/>
-      <c r="P12" s="187"/>
-      <c r="Q12" s="187"/>
-      <c r="R12" s="187"/>
-      <c r="S12" s="187"/>
-      <c r="T12" s="187"/>
-      <c r="U12" s="187"/>
-      <c r="V12" s="187"/>
-      <c r="W12" s="187"/>
-      <c r="X12" s="187"/>
-    </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B13" s="181" t="s">
+      <c r="E12" s="177"/>
+      <c r="F12" s="177"/>
+      <c r="G12" s="177"/>
+      <c r="H12" s="177"/>
+      <c r="I12" s="177"/>
+      <c r="J12" s="177"/>
+      <c r="K12" s="177"/>
+      <c r="L12" s="177"/>
+      <c r="M12" s="177"/>
+      <c r="N12" s="177"/>
+      <c r="O12" s="177"/>
+      <c r="P12" s="177"/>
+      <c r="Q12" s="177"/>
+      <c r="R12" s="177"/>
+      <c r="S12" s="177"/>
+      <c r="T12" s="177"/>
+      <c r="U12" s="177"/>
+      <c r="V12" s="177"/>
+      <c r="W12" s="177"/>
+      <c r="X12" s="177"/>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B13" s="190" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="181"/>
-      <c r="D13" s="187" t="s">
+      <c r="C13" s="190"/>
+      <c r="D13" s="177" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="187"/>
-      <c r="F13" s="187"/>
-      <c r="G13" s="187"/>
-      <c r="H13" s="187"/>
-      <c r="I13" s="187"/>
-      <c r="J13" s="187"/>
-      <c r="K13" s="187"/>
-      <c r="L13" s="187"/>
-      <c r="M13" s="187"/>
-      <c r="N13" s="187"/>
-      <c r="O13" s="187"/>
-      <c r="P13" s="187"/>
-      <c r="Q13" s="187"/>
-      <c r="R13" s="187"/>
-      <c r="S13" s="187"/>
-      <c r="T13" s="187"/>
-      <c r="U13" s="187"/>
-      <c r="V13" s="187"/>
-      <c r="W13" s="187"/>
-      <c r="X13" s="187"/>
-    </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B14" s="186"/>
-      <c r="C14" s="186"/>
-      <c r="D14" s="187"/>
-      <c r="E14" s="187"/>
-      <c r="F14" s="187"/>
-      <c r="G14" s="187"/>
-      <c r="H14" s="187"/>
-      <c r="I14" s="187"/>
-      <c r="J14" s="187"/>
-      <c r="K14" s="187"/>
-      <c r="L14" s="187"/>
-      <c r="M14" s="187"/>
-      <c r="N14" s="187"/>
-      <c r="O14" s="187"/>
-      <c r="P14" s="187"/>
-      <c r="Q14" s="187"/>
-      <c r="R14" s="187"/>
-      <c r="S14" s="187"/>
-      <c r="T14" s="187"/>
-      <c r="U14" s="187"/>
-      <c r="V14" s="187"/>
-      <c r="W14" s="187"/>
-      <c r="X14" s="187"/>
-    </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.15">
-      <c r="B15" s="180" t="s">
+      <c r="E13" s="177"/>
+      <c r="F13" s="177"/>
+      <c r="G13" s="177"/>
+      <c r="H13" s="177"/>
+      <c r="I13" s="177"/>
+      <c r="J13" s="177"/>
+      <c r="K13" s="177"/>
+      <c r="L13" s="177"/>
+      <c r="M13" s="177"/>
+      <c r="N13" s="177"/>
+      <c r="O13" s="177"/>
+      <c r="P13" s="177"/>
+      <c r="Q13" s="177"/>
+      <c r="R13" s="177"/>
+      <c r="S13" s="177"/>
+      <c r="T13" s="177"/>
+      <c r="U13" s="177"/>
+      <c r="V13" s="177"/>
+      <c r="W13" s="177"/>
+      <c r="X13" s="177"/>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B14" s="179"/>
+      <c r="C14" s="179"/>
+      <c r="D14" s="177"/>
+      <c r="E14" s="177"/>
+      <c r="F14" s="177"/>
+      <c r="G14" s="177"/>
+      <c r="H14" s="177"/>
+      <c r="I14" s="177"/>
+      <c r="J14" s="177"/>
+      <c r="K14" s="177"/>
+      <c r="L14" s="177"/>
+      <c r="M14" s="177"/>
+      <c r="N14" s="177"/>
+      <c r="O14" s="177"/>
+      <c r="P14" s="177"/>
+      <c r="Q14" s="177"/>
+      <c r="R14" s="177"/>
+      <c r="S14" s="177"/>
+      <c r="T14" s="177"/>
+      <c r="U14" s="177"/>
+      <c r="V14" s="177"/>
+      <c r="W14" s="177"/>
+      <c r="X14" s="177"/>
+    </row>
+    <row r="15" spans="2:24" x14ac:dyDescent="0.3">
+      <c r="B15" s="178" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="180"/>
-      <c r="D15" s="187" t="s">
+      <c r="C15" s="178"/>
+      <c r="D15" s="177" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="187"/>
-      <c r="F15" s="187"/>
-      <c r="G15" s="187"/>
-      <c r="H15" s="187"/>
-      <c r="I15" s="187"/>
-      <c r="J15" s="187"/>
-      <c r="K15" s="187"/>
-      <c r="L15" s="187"/>
-      <c r="M15" s="187"/>
-      <c r="N15" s="187"/>
-      <c r="O15" s="187"/>
-      <c r="P15" s="187"/>
-      <c r="Q15" s="187"/>
-      <c r="R15" s="187"/>
-      <c r="S15" s="187"/>
-      <c r="T15" s="187"/>
-      <c r="U15" s="187"/>
-      <c r="V15" s="187"/>
-      <c r="W15" s="187"/>
-      <c r="X15" s="187"/>
-    </row>
-    <row r="17" spans="3:67" x14ac:dyDescent="0.15">
-      <c r="D17" s="180" t="s">
+      <c r="E15" s="177"/>
+      <c r="F15" s="177"/>
+      <c r="G15" s="177"/>
+      <c r="H15" s="177"/>
+      <c r="I15" s="177"/>
+      <c r="J15" s="177"/>
+      <c r="K15" s="177"/>
+      <c r="L15" s="177"/>
+      <c r="M15" s="177"/>
+      <c r="N15" s="177"/>
+      <c r="O15" s="177"/>
+      <c r="P15" s="177"/>
+      <c r="Q15" s="177"/>
+      <c r="R15" s="177"/>
+      <c r="S15" s="177"/>
+      <c r="T15" s="177"/>
+      <c r="U15" s="177"/>
+      <c r="V15" s="177"/>
+      <c r="W15" s="177"/>
+      <c r="X15" s="177"/>
+    </row>
+    <row r="17" spans="3:67" x14ac:dyDescent="0.3">
+      <c r="D17" s="178" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="180"/>
-      <c r="F17" s="180"/>
+      <c r="E17" s="178"/>
+      <c r="F17" s="178"/>
       <c r="G17" s="84" t="s">
         <v>0</v>
       </c>
@@ -6240,23 +6266,23 @@
       <c r="BF17" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="BG17" s="182" t="s">
+      <c r="BG17" s="191" t="s">
         <v>7</v>
       </c>
-      <c r="BH17" s="182"/>
-      <c r="BI17" s="182"/>
-      <c r="BJ17" s="182"/>
-      <c r="BK17" s="181" t="s">
+      <c r="BH17" s="191"/>
+      <c r="BI17" s="191"/>
+      <c r="BJ17" s="191"/>
+      <c r="BK17" s="190" t="s">
         <v>5</v>
       </c>
-      <c r="BL17" s="181"/>
-      <c r="BM17" s="180" t="s">
+      <c r="BL17" s="190"/>
+      <c r="BM17" s="178" t="s">
         <v>6</v>
       </c>
-      <c r="BN17" s="180"/>
-      <c r="BO17" s="180"/>
-    </row>
-    <row r="18" spans="3:67" x14ac:dyDescent="0.15">
+      <c r="BN17" s="178"/>
+      <c r="BO17" s="178"/>
+    </row>
+    <row r="18" spans="3:67" x14ac:dyDescent="0.3">
       <c r="C18" s="95" t="s">
         <v>8</v>
       </c>
@@ -6453,7 +6479,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="20" spans="3:67" x14ac:dyDescent="0.15">
+    <row r="20" spans="3:67" x14ac:dyDescent="0.3">
       <c r="I20" s="169" t="s">
         <v>168</v>
       </c>
@@ -6506,7 +6532,7 @@
       <c r="BD20" s="170"/>
       <c r="BE20" s="171"/>
     </row>
-    <row r="21" spans="3:67" x14ac:dyDescent="0.15">
+    <row r="21" spans="3:67" x14ac:dyDescent="0.3">
       <c r="I21" s="126">
         <v>1</v>
       </c>
@@ -6657,20 +6683,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="I20:BE20"/>
-    <mergeCell ref="D13:X13"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:X4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:X5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:X6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:X7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:X8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:X9"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="BK17:BL17"/>
@@ -6687,6 +6699,20 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:X12"/>
     <mergeCell ref="B13:C13"/>
+    <mergeCell ref="I20:BE20"/>
+    <mergeCell ref="D13:X13"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:X4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:X5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:X6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:X7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:X8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:X9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6701,32 +6727,32 @@
       <selection activeCell="B2" sqref="B2:H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" style="3"/>
-    <col min="3" max="4" width="19.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="3"/>
-    <col min="6" max="7" width="20.5" style="3" customWidth="1"/>
-    <col min="8" max="8" width="2.5" style="3" customWidth="1"/>
-    <col min="9" max="9" width="3.5" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="8.83203125" style="3"/>
+    <col min="1" max="2" width="8.81640625" style="3"/>
+    <col min="3" max="4" width="19.6328125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" style="3"/>
+    <col min="6" max="7" width="20.453125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="2.453125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="3.453125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="169" t="s">
         <v>165</v>
       </c>
       <c r="C2" s="170"/>
       <c r="D2" s="171"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="172" t="s">
         <v>145</v>
       </c>
       <c r="C5" s="172"/>
       <c r="E5" s="93"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="14">
         <v>3</v>
       </c>
@@ -6741,7 +6767,7 @@
       </c>
       <c r="G6" s="42"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="49">
         <v>4</v>
       </c>
@@ -6759,7 +6785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="25">
         <v>5</v>
       </c>
@@ -6777,7 +6803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="25">
         <v>6</v>
       </c>
@@ -6789,7 +6815,7 @@
       <c r="G9" s="48"/>
       <c r="H9" s="76"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="25">
         <v>7</v>
       </c>
@@ -6801,13 +6827,13 @@
       <c r="G10" s="48"/>
       <c r="H10" s="76"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="172" t="s">
         <v>145</v>
       </c>
       <c r="C12" s="172"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="14">
         <v>3</v>
       </c>
@@ -6818,7 +6844,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="49">
         <v>4</v>
       </c>
@@ -6829,7 +6855,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="25">
         <v>5</v>
       </c>
@@ -6840,7 +6866,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="25">
         <v>6</v>
       </c>
@@ -6849,7 +6875,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="25">
         <v>7</v>
       </c>
@@ -6858,12 +6884,12 @@
       </c>
       <c r="D17" s="109"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="74" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="173" t="s">
         <v>152</v>
       </c>
@@ -6889,22 +6915,22 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" style="3"/>
-    <col min="3" max="3" width="13.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.83203125" style="3"/>
+    <col min="1" max="2" width="8.81640625" style="3"/>
+    <col min="3" max="3" width="13.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B2" s="193" t="s">
         <v>122</v>
       </c>
       <c r="C2" s="193"/>
       <c r="D2" s="193"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="14">
         <v>3</v>
       </c>
@@ -6915,7 +6941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" s="14">
         <v>4</v>
       </c>
@@ -6926,7 +6952,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B6" s="80" t="s">
         <v>148</v>
       </c>
@@ -6935,7 +6961,7 @@
       </c>
       <c r="D6" s="47"/>
     </row>
-    <row r="8" spans="2:4" s="72" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="8" spans="2:4" s="72" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:D2"/>
@@ -6952,16 +6978,16 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="3"/>
-    <col min="2" max="4" width="11.83203125" style="3" customWidth="1"/>
-    <col min="5" max="7" width="8.83203125" style="3"/>
-    <col min="8" max="8" width="14.83203125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="3"/>
+    <col min="1" max="1" width="8.81640625" style="3"/>
+    <col min="2" max="4" width="11.81640625" style="3" customWidth="1"/>
+    <col min="5" max="7" width="8.81640625" style="3"/>
+    <col min="8" max="8" width="14.81640625" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="14">
         <v>3</v>
       </c>
@@ -6972,7 +6998,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="14">
         <v>4</v>
       </c>
@@ -6983,7 +7009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="25">
         <v>5</v>
       </c>
@@ -6999,7 +7025,7 @@
       <c r="G5" s="207"/>
       <c r="H5" s="208"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="25">
         <v>6</v>
       </c>
@@ -7013,7 +7039,7 @@
       <c r="G6" s="210"/>
       <c r="H6" s="211"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="25">
         <v>7</v>
       </c>
@@ -7027,7 +7053,7 @@
       <c r="G7" s="210"/>
       <c r="H7" s="211"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="25">
         <v>8</v>
       </c>
@@ -7041,7 +7067,7 @@
       <c r="G8" s="213"/>
       <c r="H8" s="214"/>
     </row>
-    <row r="9" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="25">
         <v>9</v>
       </c>
@@ -7057,7 +7083,7 @@
       <c r="G9" s="198"/>
       <c r="H9" s="199"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="25">
         <v>10</v>
       </c>
@@ -7069,7 +7095,7 @@
       <c r="G10" s="198"/>
       <c r="H10" s="199"/>
     </row>
-    <row r="11" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="25">
         <v>11</v>
       </c>
@@ -7081,7 +7107,7 @@
       <c r="G11" s="198"/>
       <c r="H11" s="199"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="25">
         <v>12</v>
       </c>
@@ -7093,7 +7119,7 @@
       <c r="G12" s="198"/>
       <c r="H12" s="199"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="25">
         <v>13</v>
       </c>
@@ -7105,7 +7131,7 @@
       <c r="G13" s="198"/>
       <c r="H13" s="199"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="25">
         <v>14</v>
       </c>
@@ -7139,25 +7165,25 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" style="3"/>
-    <col min="3" max="3" width="17.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="3"/>
-    <col min="6" max="7" width="30.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="3.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="3"/>
+    <col min="1" max="2" width="8.81640625" style="3"/>
+    <col min="3" max="3" width="17.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.81640625" style="3"/>
+    <col min="6" max="7" width="30.6328125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="3.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="169" t="s">
         <v>173</v>
       </c>
       <c r="C3" s="171"/>
       <c r="D3" s="94"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="14">
         <v>3</v>
       </c>
@@ -7172,7 +7198,7 @@
       </c>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="14">
         <v>4</v>
       </c>
@@ -7190,7 +7216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="25">
         <v>5</v>
       </c>
@@ -7208,7 +7234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="14">
         <v>6</v>
       </c>
@@ -7226,7 +7252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="25">
         <v>7</v>
       </c>
@@ -7242,7 +7268,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="14">
         <v>8</v>
       </c>
@@ -7260,7 +7286,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="14">
         <v>9</v>
       </c>
@@ -7276,7 +7302,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="46"/>
       <c r="F12" s="13" t="s">
         <v>118</v>
@@ -7284,7 +7310,7 @@
       <c r="G12" s="13"/>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="46"/>
       <c r="F13" s="13" t="s">
         <v>111</v>
@@ -7294,7 +7320,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="46"/>
       <c r="F14" s="13" t="s">
         <v>118</v>
@@ -7302,7 +7328,7 @@
       <c r="G14" s="13"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="46"/>
       <c r="F15" s="13" t="s">
         <v>112</v>
@@ -7312,14 +7338,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="F16" s="13" t="s">
         <v>118</v>
       </c>
       <c r="G16" s="13"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="6:8" x14ac:dyDescent="0.15">
+    <row r="17" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F17" s="13" t="s">
         <v>114</v>
       </c>
@@ -7328,14 +7354,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="6:8" x14ac:dyDescent="0.15">
+    <row r="18" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F18" s="13" t="s">
         <v>118</v>
       </c>
       <c r="G18" s="13"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="6:8" x14ac:dyDescent="0.15">
+    <row r="19" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F19" s="13" t="s">
         <v>115</v>
       </c>
@@ -7344,14 +7370,14 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="6:8" x14ac:dyDescent="0.15">
+    <row r="20" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F20" s="13" t="s">
         <v>118</v>
       </c>
       <c r="G20" s="13"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="6:8" x14ac:dyDescent="0.15">
+    <row r="21" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F21" s="13" t="s">
         <v>116</v>
       </c>
@@ -7376,24 +7402,24 @@
       <selection activeCell="B2" sqref="B2:D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" style="3"/>
+    <col min="1" max="2" width="8.81640625" style="3"/>
     <col min="3" max="4" width="21" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="3"/>
+    <col min="5" max="5" width="8.81640625" style="3"/>
     <col min="6" max="7" width="19" style="3" customWidth="1"/>
     <col min="8" max="8" width="3" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="8.83203125" style="3"/>
+    <col min="9" max="16384" width="8.81640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B2" s="169" t="s">
         <v>69</v>
       </c>
       <c r="C2" s="170"/>
       <c r="D2" s="171"/>
     </row>
-    <row r="5" spans="2:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="172" t="s">
         <v>145</v>
       </c>
@@ -7401,7 +7427,7 @@
       <c r="E5" s="93"/>
       <c r="F5" s="93"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="14">
         <v>3</v>
       </c>
@@ -7418,7 +7444,7 @@
       <c r="H6" s="4"/>
       <c r="I6" s="72"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="49">
         <v>4</v>
       </c>
@@ -7437,7 +7463,7 @@
       </c>
       <c r="I7" s="72"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="25">
         <v>5</v>
       </c>
@@ -7456,7 +7482,7 @@
       </c>
       <c r="I8" s="72"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="25">
         <v>6</v>
       </c>
@@ -7473,7 +7499,7 @@
       </c>
       <c r="I9" s="72"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F10" s="13" t="s">
         <v>101</v>
       </c>
@@ -7483,13 +7509,13 @@
       </c>
       <c r="I10" s="72"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="F11" s="72"/>
       <c r="G11" s="72"/>
       <c r="H11" s="46"/>
       <c r="I11" s="72"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="74" t="s">
         <v>144</v>
       </c>
@@ -7498,7 +7524,7 @@
       </c>
       <c r="G12" s="42"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="176" t="s">
         <v>122</v>
       </c>
@@ -7511,14 +7537,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="173" t="s">
         <v>152</v>
       </c>
       <c r="C14" s="174"/>
       <c r="D14" s="175"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.15">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="14">
         <v>3</v>
       </c>
@@ -7529,7 +7555,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B17" s="49">
         <v>4</v>
       </c>
@@ -7540,7 +7566,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="25">
         <v>5</v>
       </c>
@@ -7551,7 +7577,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="25">
         <v>6</v>
       </c>
@@ -7560,7 +7586,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="14">
         <v>7</v>
       </c>
@@ -7571,7 +7597,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B21" s="14">
         <v>7</v>
       </c>
@@ -7580,7 +7606,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B22" s="14">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Added IMU_RESET_TO_FACTORY_SETTINGS and IMU_REBOOT commands
</commit_message>
<xml_diff>
--- a/doc/DATA_PROTOCOL_SENSUS.xlsx
+++ b/doc/DATA_PROTOCOL_SENSUS.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="193">
   <si>
     <t>CMD</t>
   </si>
@@ -612,6 +612,9 @@
   </si>
   <si>
     <t>IMU_RESET_TO_FACTORY_SETTINGS</t>
+  </si>
+  <si>
+    <t>IMU_REBOOT</t>
   </si>
 </sst>
 </file>
@@ -1478,6 +1481,12 @@
     <xf numFmtId="0" fontId="2" fillId="28" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1502,13 +1511,40 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1517,37 +1553,10 @@
     <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1640,6 +1649,42 @@
     <xf numFmtId="0" fontId="2" fillId="18" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1654,48 +1699,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2067,7 +2070,7 @@
   <dimension ref="B2:F44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12" x14ac:dyDescent="0.3"/>
@@ -2480,11 +2483,11 @@
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B37" s="240"/>
-      <c r="C37" s="240"/>
-      <c r="D37" s="240"/>
-      <c r="E37" s="240"/>
-      <c r="F37" s="241"/>
+      <c r="B37" s="169"/>
+      <c r="C37" s="169"/>
+      <c r="D37" s="169"/>
+      <c r="E37" s="169"/>
+      <c r="F37" s="170"/>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B38" s="18">
@@ -2500,11 +2503,17 @@
       <c r="F38" s="19"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B39" s="82"/>
-      <c r="C39" s="82"/>
-      <c r="D39" s="82"/>
-      <c r="E39" s="82"/>
-      <c r="F39" s="2"/>
+      <c r="B39" s="18">
+        <v>208</v>
+      </c>
+      <c r="C39" s="18">
+        <v>0</v>
+      </c>
+      <c r="D39" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="E39" s="18"/>
+      <c r="F39" s="19"/>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B40" s="82"/>
@@ -2583,17 +2592,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="169" t="s">
+      <c r="B2" s="171" t="s">
         <v>158</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="171"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="173"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="172" t="s">
+      <c r="B5" s="174" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="172"/>
+      <c r="C5" s="174"/>
       <c r="E5" s="93"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
@@ -2684,11 +2693,11 @@
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="173" t="s">
+      <c r="B15" s="175" t="s">
         <v>152</v>
       </c>
-      <c r="C15" s="174"/>
-      <c r="D15" s="175"/>
+      <c r="C15" s="176"/>
+      <c r="D15" s="177"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2721,11 +2730,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.3">
-      <c r="B2" s="169" t="s">
+      <c r="B2" s="171" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="171"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="173"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" s="14">
@@ -2763,7 +2772,7 @@
       <c r="B7" s="25">
         <v>5</v>
       </c>
-      <c r="C7" s="221" t="s">
+      <c r="C7" s="223" t="s">
         <v>75</v>
       </c>
       <c r="D7" s="27" t="s">
@@ -2784,7 +2793,7 @@
       <c r="B8" s="25">
         <v>6</v>
       </c>
-      <c r="C8" s="222"/>
+      <c r="C8" s="224"/>
       <c r="D8" s="28" t="s">
         <v>79</v>
       </c>
@@ -2843,7 +2852,7 @@
       <c r="B13" s="25">
         <v>5</v>
       </c>
-      <c r="C13" s="221" t="s">
+      <c r="C13" s="223" t="s">
         <v>75</v>
       </c>
       <c r="D13" s="27" t="s">
@@ -2866,7 +2875,7 @@
       <c r="B14" s="25">
         <v>6</v>
       </c>
-      <c r="C14" s="222"/>
+      <c r="C14" s="224"/>
       <c r="D14" s="28" t="s">
         <v>79</v>
       </c>
@@ -2905,7 +2914,7 @@
       <c r="B16" s="25">
         <v>8</v>
       </c>
-      <c r="C16" s="216" t="s">
+      <c r="C16" s="218" t="s">
         <v>163</v>
       </c>
       <c r="D16" s="123" t="s">
@@ -2928,7 +2937,7 @@
       <c r="B17" s="25">
         <v>9</v>
       </c>
-      <c r="C17" s="217"/>
+      <c r="C17" s="219"/>
       <c r="D17" s="124" t="s">
         <v>79</v>
       </c>
@@ -2957,17 +2966,17 @@
       <c r="D21" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="G21" s="218" t="s">
+      <c r="G21" s="220" t="s">
         <v>89</v>
       </c>
-      <c r="H21" s="219"/>
-      <c r="I21" s="220"/>
+      <c r="H21" s="221"/>
+      <c r="I21" s="222"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" s="14">
         <v>5</v>
       </c>
-      <c r="C22" s="221" t="s">
+      <c r="C22" s="223" t="s">
         <v>75</v>
       </c>
       <c r="D22" s="27" t="s">
@@ -2981,7 +2990,7 @@
       <c r="B23" s="14">
         <v>6</v>
       </c>
-      <c r="C23" s="222"/>
+      <c r="C23" s="224"/>
       <c r="D23" s="28" t="s">
         <v>79</v>
       </c>
@@ -3012,7 +3021,7 @@
       <c r="B25" s="14">
         <v>8</v>
       </c>
-      <c r="C25" s="216" t="s">
+      <c r="C25" s="218" t="s">
         <v>162</v>
       </c>
       <c r="D25" s="123" t="s">
@@ -3033,7 +3042,7 @@
       <c r="B26" s="14">
         <v>9</v>
       </c>
-      <c r="C26" s="217"/>
+      <c r="C26" s="219"/>
       <c r="D26" s="124" t="s">
         <v>79</v>
       </c>
@@ -3194,11 +3203,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="169" t="s">
+      <c r="B2" s="171" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="171"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="173"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="57"/>
@@ -3206,10 +3215,10 @@
       <c r="D3" s="57"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="174" t="s">
         <v>145</v>
       </c>
-      <c r="C4" s="172"/>
+      <c r="C4" s="174"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="14">
@@ -3326,7 +3335,7 @@
       <c r="B12" s="14">
         <v>10</v>
       </c>
-      <c r="C12" s="216" t="s">
+      <c r="C12" s="218" t="s">
         <v>163</v>
       </c>
       <c r="D12" s="123" t="s">
@@ -3347,7 +3356,7 @@
       <c r="B13" s="14">
         <v>11</v>
       </c>
-      <c r="C13" s="217"/>
+      <c r="C13" s="219"/>
       <c r="D13" s="124" t="s">
         <v>79</v>
       </c>
@@ -3459,11 +3468,11 @@
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="173" t="s">
+      <c r="B22" s="175" t="s">
         <v>152</v>
       </c>
-      <c r="C22" s="174"/>
-      <c r="D22" s="175"/>
+      <c r="C22" s="176"/>
+      <c r="D22" s="177"/>
       <c r="F22" s="13" t="s">
         <v>41</v>
       </c>
@@ -3517,11 +3526,11 @@
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="169" t="s">
+      <c r="B27" s="171" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="170"/>
-      <c r="D27" s="171"/>
+      <c r="C27" s="172"/>
+      <c r="D27" s="173"/>
       <c r="F27" s="13" t="s">
         <v>46</v>
       </c>
@@ -3711,7 +3720,7 @@
       <c r="B43" s="14">
         <v>10</v>
       </c>
-      <c r="C43" s="216" t="s">
+      <c r="C43" s="218" t="s">
         <v>163</v>
       </c>
       <c r="D43" s="123" t="s">
@@ -3722,7 +3731,7 @@
       <c r="B44" s="14">
         <v>11</v>
       </c>
-      <c r="C44" s="217"/>
+      <c r="C44" s="219"/>
       <c r="D44" s="124" t="s">
         <v>79</v>
       </c>
@@ -3811,36 +3820,36 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B2" s="187" t="s">
+      <c r="B2" s="179" t="s">
         <v>131</v>
       </c>
-      <c r="C2" s="188"/>
-      <c r="D2" s="189"/>
+      <c r="C2" s="180"/>
+      <c r="D2" s="181"/>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B4" s="172" t="s">
+      <c r="B4" s="174" t="s">
         <v>145</v>
       </c>
-      <c r="C4" s="172"/>
+      <c r="C4" s="174"/>
       <c r="E4" s="71"/>
-      <c r="G4" s="236" t="s">
+      <c r="G4" s="225" t="s">
         <v>160</v>
       </c>
-      <c r="H4" s="236"/>
-      <c r="I4" s="236"/>
-      <c r="J4" s="236"/>
-      <c r="K4" s="236"/>
-      <c r="L4" s="236"/>
-      <c r="M4" s="236"/>
-      <c r="N4" s="236"/>
-      <c r="O4" s="236"/>
-      <c r="P4" s="236"/>
-      <c r="Q4" s="236"/>
-      <c r="R4" s="236"/>
-      <c r="S4" s="236"/>
-      <c r="T4" s="236"/>
-      <c r="U4" s="236"/>
-      <c r="V4" s="236"/>
+      <c r="H4" s="225"/>
+      <c r="I4" s="225"/>
+      <c r="J4" s="225"/>
+      <c r="K4" s="225"/>
+      <c r="L4" s="225"/>
+      <c r="M4" s="225"/>
+      <c r="N4" s="225"/>
+      <c r="O4" s="225"/>
+      <c r="P4" s="225"/>
+      <c r="Q4" s="225"/>
+      <c r="R4" s="225"/>
+      <c r="S4" s="225"/>
+      <c r="T4" s="225"/>
+      <c r="U4" s="225"/>
+      <c r="V4" s="225"/>
     </row>
     <row r="5" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B5" s="14">
@@ -4142,11 +4151,11 @@
       <c r="V11" s="13"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B12" s="173" t="s">
+      <c r="B12" s="175" t="s">
         <v>152</v>
       </c>
-      <c r="C12" s="174"/>
-      <c r="D12" s="175"/>
+      <c r="C12" s="176"/>
+      <c r="D12" s="177"/>
       <c r="F12" s="48"/>
       <c r="G12" s="71"/>
       <c r="H12" s="71"/>
@@ -4194,7 +4203,7 @@
       <c r="B15" s="66">
         <v>0</v>
       </c>
-      <c r="C15" s="230" t="s">
+      <c r="C15" s="229" t="s">
         <v>2</v>
       </c>
       <c r="D15" s="90"/>
@@ -4203,14 +4212,14 @@
       <c r="B16" s="66">
         <v>1</v>
       </c>
-      <c r="C16" s="231"/>
+      <c r="C16" s="230"/>
       <c r="D16" s="91"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B17" s="66">
         <v>2</v>
       </c>
-      <c r="C17" s="232"/>
+      <c r="C17" s="231"/>
       <c r="D17" s="92"/>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.3">
@@ -4239,7 +4248,7 @@
       <c r="B20" s="14">
         <v>5</v>
       </c>
-      <c r="C20" s="228" t="s">
+      <c r="C20" s="232" t="s">
         <v>125</v>
       </c>
       <c r="D20" s="58" t="s">
@@ -4250,7 +4259,7 @@
       <c r="B21" s="14">
         <v>6</v>
       </c>
-      <c r="C21" s="229"/>
+      <c r="C21" s="233"/>
       <c r="D21" s="59" t="s">
         <v>79</v>
       </c>
@@ -4259,7 +4268,7 @@
       <c r="B22" s="14">
         <v>7</v>
       </c>
-      <c r="C22" s="229"/>
+      <c r="C22" s="233"/>
       <c r="D22" s="59" t="s">
         <v>81</v>
       </c>
@@ -4268,7 +4277,7 @@
       <c r="B23" s="14">
         <v>8</v>
       </c>
-      <c r="C23" s="229"/>
+      <c r="C23" s="233"/>
       <c r="D23" s="60" t="s">
         <v>80</v>
       </c>
@@ -4277,7 +4286,7 @@
       <c r="B24" s="14">
         <v>9</v>
       </c>
-      <c r="C24" s="228" t="s">
+      <c r="C24" s="232" t="s">
         <v>126</v>
       </c>
       <c r="D24" s="58" t="s">
@@ -4288,7 +4297,7 @@
       <c r="B25" s="14">
         <v>10</v>
       </c>
-      <c r="C25" s="229"/>
+      <c r="C25" s="233"/>
       <c r="D25" s="59" t="s">
         <v>79</v>
       </c>
@@ -4314,7 +4323,7 @@
       <c r="B26" s="14">
         <v>11</v>
       </c>
-      <c r="C26" s="229"/>
+      <c r="C26" s="233"/>
       <c r="D26" s="59" t="s">
         <v>81</v>
       </c>
@@ -4323,7 +4332,7 @@
       <c r="B27" s="14">
         <v>12</v>
       </c>
-      <c r="C27" s="229"/>
+      <c r="C27" s="233"/>
       <c r="D27" s="60" t="s">
         <v>80</v>
       </c>
@@ -4332,7 +4341,7 @@
       <c r="B28" s="14">
         <v>13</v>
       </c>
-      <c r="C28" s="228" t="s">
+      <c r="C28" s="232" t="s">
         <v>127</v>
       </c>
       <c r="D28" s="58" t="s">
@@ -4343,7 +4352,7 @@
       <c r="B29" s="14">
         <v>14</v>
       </c>
-      <c r="C29" s="229"/>
+      <c r="C29" s="233"/>
       <c r="D29" s="59" t="s">
         <v>79</v>
       </c>
@@ -4352,7 +4361,7 @@
       <c r="B30" s="14">
         <v>15</v>
       </c>
-      <c r="C30" s="229"/>
+      <c r="C30" s="233"/>
       <c r="D30" s="59" t="s">
         <v>81</v>
       </c>
@@ -4361,7 +4370,7 @@
       <c r="B31" s="14">
         <v>16</v>
       </c>
-      <c r="C31" s="229"/>
+      <c r="C31" s="233"/>
       <c r="D31" s="60" t="s">
         <v>80</v>
       </c>
@@ -4370,7 +4379,7 @@
       <c r="B32" s="14">
         <v>17</v>
       </c>
-      <c r="C32" s="228" t="s">
+      <c r="C32" s="232" t="s">
         <v>128</v>
       </c>
       <c r="D32" s="58" t="s">
@@ -4381,7 +4390,7 @@
       <c r="B33" s="14">
         <v>18</v>
       </c>
-      <c r="C33" s="229"/>
+      <c r="C33" s="233"/>
       <c r="D33" s="59" t="s">
         <v>79</v>
       </c>
@@ -4390,7 +4399,7 @@
       <c r="B34" s="14">
         <v>19</v>
       </c>
-      <c r="C34" s="229"/>
+      <c r="C34" s="233"/>
       <c r="D34" s="59" t="s">
         <v>81</v>
       </c>
@@ -4416,7 +4425,7 @@
       <c r="B35" s="14">
         <v>20</v>
       </c>
-      <c r="C35" s="229"/>
+      <c r="C35" s="233"/>
       <c r="D35" s="60" t="s">
         <v>80</v>
       </c>
@@ -4442,7 +4451,7 @@
       <c r="B36" s="14">
         <v>21</v>
       </c>
-      <c r="C36" s="228" t="s">
+      <c r="C36" s="232" t="s">
         <v>132</v>
       </c>
       <c r="D36" s="58" t="s">
@@ -4470,7 +4479,7 @@
       <c r="B37" s="14">
         <v>22</v>
       </c>
-      <c r="C37" s="229"/>
+      <c r="C37" s="233"/>
       <c r="D37" s="59" t="s">
         <v>79</v>
       </c>
@@ -4496,7 +4505,7 @@
       <c r="B38" s="14">
         <v>23</v>
       </c>
-      <c r="C38" s="229"/>
+      <c r="C38" s="233"/>
       <c r="D38" s="59" t="s">
         <v>81</v>
       </c>
@@ -4518,7 +4527,7 @@
       <c r="B39" s="14">
         <v>24</v>
       </c>
-      <c r="C39" s="229"/>
+      <c r="C39" s="233"/>
       <c r="D39" s="60" t="s">
         <v>80</v>
       </c>
@@ -4540,7 +4549,7 @@
       <c r="B40" s="14">
         <v>25</v>
       </c>
-      <c r="C40" s="228" t="s">
+      <c r="C40" s="232" t="s">
         <v>133</v>
       </c>
       <c r="D40" s="58" t="s">
@@ -4564,7 +4573,7 @@
       <c r="B41" s="14">
         <v>26</v>
       </c>
-      <c r="C41" s="229"/>
+      <c r="C41" s="233"/>
       <c r="D41" s="59" t="s">
         <v>79</v>
       </c>
@@ -4590,7 +4599,7 @@
       <c r="B42" s="14">
         <v>27</v>
       </c>
-      <c r="C42" s="229"/>
+      <c r="C42" s="233"/>
       <c r="D42" s="59" t="s">
         <v>81</v>
       </c>
@@ -4616,7 +4625,7 @@
       <c r="B43" s="14">
         <v>28</v>
       </c>
-      <c r="C43" s="229"/>
+      <c r="C43" s="233"/>
       <c r="D43" s="60" t="s">
         <v>80</v>
       </c>
@@ -4642,7 +4651,7 @@
       <c r="B44" s="14">
         <v>29</v>
       </c>
-      <c r="C44" s="228" t="s">
+      <c r="C44" s="232" t="s">
         <v>134</v>
       </c>
       <c r="D44" s="58" t="s">
@@ -4670,7 +4679,7 @@
       <c r="B45" s="14">
         <v>30</v>
       </c>
-      <c r="C45" s="229"/>
+      <c r="C45" s="233"/>
       <c r="D45" s="59" t="s">
         <v>79</v>
       </c>
@@ -4679,7 +4688,7 @@
       <c r="B46" s="14">
         <v>31</v>
       </c>
-      <c r="C46" s="229"/>
+      <c r="C46" s="233"/>
       <c r="D46" s="59" t="s">
         <v>81</v>
       </c>
@@ -4688,7 +4697,7 @@
       <c r="B47" s="14">
         <v>32</v>
       </c>
-      <c r="C47" s="229"/>
+      <c r="C47" s="233"/>
       <c r="D47" s="60" t="s">
         <v>80</v>
       </c>
@@ -4697,7 +4706,7 @@
       <c r="B48" s="14">
         <v>33</v>
       </c>
-      <c r="C48" s="228" t="s">
+      <c r="C48" s="232" t="s">
         <v>135</v>
       </c>
       <c r="D48" s="58" t="s">
@@ -4708,7 +4717,7 @@
       <c r="B49" s="14">
         <v>34</v>
       </c>
-      <c r="C49" s="229"/>
+      <c r="C49" s="233"/>
       <c r="D49" s="59" t="s">
         <v>79</v>
       </c>
@@ -4717,7 +4726,7 @@
       <c r="B50" s="14">
         <v>35</v>
       </c>
-      <c r="C50" s="229"/>
+      <c r="C50" s="233"/>
       <c r="D50" s="59" t="s">
         <v>81</v>
       </c>
@@ -4726,7 +4735,7 @@
       <c r="B51" s="14">
         <v>36</v>
       </c>
-      <c r="C51" s="229"/>
+      <c r="C51" s="233"/>
       <c r="D51" s="60" t="s">
         <v>80</v>
       </c>
@@ -4735,7 +4744,7 @@
       <c r="B52" s="14">
         <v>37</v>
       </c>
-      <c r="C52" s="237" t="s">
+      <c r="C52" s="234" t="s">
         <v>136</v>
       </c>
       <c r="D52" s="58" t="s">
@@ -4746,7 +4755,7 @@
       <c r="B53" s="14">
         <v>38</v>
       </c>
-      <c r="C53" s="238"/>
+      <c r="C53" s="235"/>
       <c r="D53" s="59" t="s">
         <v>79</v>
       </c>
@@ -4755,7 +4764,7 @@
       <c r="B54" s="14">
         <v>39</v>
       </c>
-      <c r="C54" s="238"/>
+      <c r="C54" s="235"/>
       <c r="D54" s="59" t="s">
         <v>81</v>
       </c>
@@ -4764,7 +4773,7 @@
       <c r="B55" s="14">
         <v>40</v>
       </c>
-      <c r="C55" s="239"/>
+      <c r="C55" s="236"/>
       <c r="D55" s="60" t="s">
         <v>80</v>
       </c>
@@ -4773,7 +4782,7 @@
       <c r="B56" s="14">
         <v>41</v>
       </c>
-      <c r="C56" s="228" t="s">
+      <c r="C56" s="232" t="s">
         <v>137</v>
       </c>
       <c r="D56" s="58" t="s">
@@ -4784,7 +4793,7 @@
       <c r="B57" s="14">
         <v>42</v>
       </c>
-      <c r="C57" s="229"/>
+      <c r="C57" s="233"/>
       <c r="D57" s="59" t="s">
         <v>79</v>
       </c>
@@ -4793,7 +4802,7 @@
       <c r="B58" s="14">
         <v>43</v>
       </c>
-      <c r="C58" s="229"/>
+      <c r="C58" s="233"/>
       <c r="D58" s="59" t="s">
         <v>81</v>
       </c>
@@ -4802,7 +4811,7 @@
       <c r="B59" s="14">
         <v>44</v>
       </c>
-      <c r="C59" s="229"/>
+      <c r="C59" s="233"/>
       <c r="D59" s="60" t="s">
         <v>80</v>
       </c>
@@ -4811,7 +4820,7 @@
       <c r="B60" s="14">
         <v>45</v>
       </c>
-      <c r="C60" s="228" t="s">
+      <c r="C60" s="232" t="s">
         <v>138</v>
       </c>
       <c r="D60" s="58" t="s">
@@ -4822,7 +4831,7 @@
       <c r="B61" s="14">
         <v>46</v>
       </c>
-      <c r="C61" s="229"/>
+      <c r="C61" s="233"/>
       <c r="D61" s="59" t="s">
         <v>79</v>
       </c>
@@ -4831,7 +4840,7 @@
       <c r="B62" s="14">
         <v>47</v>
       </c>
-      <c r="C62" s="229"/>
+      <c r="C62" s="233"/>
       <c r="D62" s="59" t="s">
         <v>81</v>
       </c>
@@ -4840,7 +4849,7 @@
       <c r="B63" s="14">
         <v>48</v>
       </c>
-      <c r="C63" s="229"/>
+      <c r="C63" s="233"/>
       <c r="D63" s="60" t="s">
         <v>80</v>
       </c>
@@ -4849,7 +4858,7 @@
       <c r="B64" s="14">
         <v>49</v>
       </c>
-      <c r="C64" s="228" t="s">
+      <c r="C64" s="232" t="s">
         <v>139</v>
       </c>
       <c r="D64" s="58" t="s">
@@ -4860,7 +4869,7 @@
       <c r="B65" s="14">
         <v>50</v>
       </c>
-      <c r="C65" s="229"/>
+      <c r="C65" s="233"/>
       <c r="D65" s="59" t="s">
         <v>79</v>
       </c>
@@ -4869,7 +4878,7 @@
       <c r="B66" s="14">
         <v>51</v>
       </c>
-      <c r="C66" s="229"/>
+      <c r="C66" s="233"/>
       <c r="D66" s="59" t="s">
         <v>81</v>
       </c>
@@ -4878,7 +4887,7 @@
       <c r="B67" s="14">
         <v>52</v>
       </c>
-      <c r="C67" s="229"/>
+      <c r="C67" s="233"/>
       <c r="D67" s="60" t="s">
         <v>80</v>
       </c>
@@ -4905,7 +4914,7 @@
       <c r="B70" s="14">
         <v>55</v>
       </c>
-      <c r="C70" s="233" t="s">
+      <c r="C70" s="226" t="s">
         <v>7</v>
       </c>
       <c r="D70" s="54" t="s">
@@ -4916,7 +4925,7 @@
       <c r="B71" s="14">
         <v>56</v>
       </c>
-      <c r="C71" s="234"/>
+      <c r="C71" s="227"/>
       <c r="D71" s="55" t="s">
         <v>79</v>
       </c>
@@ -4925,7 +4934,7 @@
       <c r="B72" s="14">
         <v>57</v>
       </c>
-      <c r="C72" s="234"/>
+      <c r="C72" s="227"/>
       <c r="D72" s="55" t="s">
         <v>81</v>
       </c>
@@ -4934,7 +4943,7 @@
       <c r="B73" s="14">
         <v>58</v>
       </c>
-      <c r="C73" s="235"/>
+      <c r="C73" s="228"/>
       <c r="D73" s="56" t="s">
         <v>80</v>
       </c>
@@ -4943,7 +4952,7 @@
       <c r="B74" s="14">
         <v>59</v>
       </c>
-      <c r="C74" s="223" t="s">
+      <c r="C74" s="237" t="s">
         <v>5</v>
       </c>
       <c r="D74" s="64"/>
@@ -4952,14 +4961,14 @@
       <c r="B75" s="14">
         <v>60</v>
       </c>
-      <c r="C75" s="224"/>
+      <c r="C75" s="238"/>
       <c r="D75" s="65"/>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B76" s="14">
         <v>61</v>
       </c>
-      <c r="C76" s="225" t="s">
+      <c r="C76" s="239" t="s">
         <v>6</v>
       </c>
       <c r="D76" s="61"/>
@@ -4968,14 +4977,14 @@
       <c r="B77" s="14">
         <v>62</v>
       </c>
-      <c r="C77" s="226"/>
+      <c r="C77" s="240"/>
       <c r="D77" s="62"/>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B78" s="14">
         <v>63</v>
       </c>
-      <c r="C78" s="227"/>
+      <c r="C78" s="241"/>
       <c r="D78" s="63"/>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.3">
@@ -4987,7 +4996,7 @@
       <c r="B83" s="66">
         <v>0</v>
       </c>
-      <c r="C83" s="230" t="s">
+      <c r="C83" s="229" t="s">
         <v>2</v>
       </c>
       <c r="D83" s="61"/>
@@ -4996,14 +5005,14 @@
       <c r="B84" s="66">
         <v>1</v>
       </c>
-      <c r="C84" s="231"/>
+      <c r="C84" s="230"/>
       <c r="D84" s="62"/>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B85" s="66">
         <v>2</v>
       </c>
-      <c r="C85" s="232"/>
+      <c r="C85" s="231"/>
       <c r="D85" s="63"/>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.3">
@@ -5032,7 +5041,7 @@
       <c r="B88" s="14">
         <v>5</v>
       </c>
-      <c r="C88" s="228" t="s">
+      <c r="C88" s="232" t="s">
         <v>140</v>
       </c>
       <c r="D88" s="58" t="s">
@@ -5043,7 +5052,7 @@
       <c r="B89" s="14">
         <v>6</v>
       </c>
-      <c r="C89" s="229"/>
+      <c r="C89" s="233"/>
       <c r="D89" s="59" t="s">
         <v>79</v>
       </c>
@@ -5052,7 +5061,7 @@
       <c r="B90" s="14">
         <v>7</v>
       </c>
-      <c r="C90" s="229"/>
+      <c r="C90" s="233"/>
       <c r="D90" s="59" t="s">
         <v>81</v>
       </c>
@@ -5061,7 +5070,7 @@
       <c r="B91" s="14">
         <v>8</v>
       </c>
-      <c r="C91" s="229"/>
+      <c r="C91" s="233"/>
       <c r="D91" s="60" t="s">
         <v>80</v>
       </c>
@@ -5070,7 +5079,7 @@
       <c r="B92" s="14">
         <v>9</v>
       </c>
-      <c r="C92" s="228" t="s">
+      <c r="C92" s="232" t="s">
         <v>141</v>
       </c>
       <c r="D92" s="58" t="s">
@@ -5081,7 +5090,7 @@
       <c r="B93" s="14">
         <v>10</v>
       </c>
-      <c r="C93" s="229"/>
+      <c r="C93" s="233"/>
       <c r="D93" s="59" t="s">
         <v>79</v>
       </c>
@@ -5090,7 +5099,7 @@
       <c r="B94" s="14">
         <v>11</v>
       </c>
-      <c r="C94" s="229"/>
+      <c r="C94" s="233"/>
       <c r="D94" s="59" t="s">
         <v>81</v>
       </c>
@@ -5099,7 +5108,7 @@
       <c r="B95" s="14">
         <v>12</v>
       </c>
-      <c r="C95" s="229"/>
+      <c r="C95" s="233"/>
       <c r="D95" s="60" t="s">
         <v>80</v>
       </c>
@@ -5108,7 +5117,7 @@
       <c r="B96" s="14">
         <v>13</v>
       </c>
-      <c r="C96" s="228" t="s">
+      <c r="C96" s="232" t="s">
         <v>142</v>
       </c>
       <c r="D96" s="58" t="s">
@@ -5119,7 +5128,7 @@
       <c r="B97" s="14">
         <v>14</v>
       </c>
-      <c r="C97" s="229"/>
+      <c r="C97" s="233"/>
       <c r="D97" s="59" t="s">
         <v>79</v>
       </c>
@@ -5128,7 +5137,7 @@
       <c r="B98" s="14">
         <v>15</v>
       </c>
-      <c r="C98" s="229"/>
+      <c r="C98" s="233"/>
       <c r="D98" s="59" t="s">
         <v>81</v>
       </c>
@@ -5137,7 +5146,7 @@
       <c r="B99" s="14">
         <v>16</v>
       </c>
-      <c r="C99" s="229"/>
+      <c r="C99" s="233"/>
       <c r="D99" s="60" t="s">
         <v>80</v>
       </c>
@@ -5146,7 +5155,7 @@
       <c r="B100" s="14">
         <v>17</v>
       </c>
-      <c r="C100" s="228" t="s">
+      <c r="C100" s="232" t="s">
         <v>143</v>
       </c>
       <c r="D100" s="58" t="s">
@@ -5157,7 +5166,7 @@
       <c r="B101" s="14">
         <v>18</v>
       </c>
-      <c r="C101" s="229"/>
+      <c r="C101" s="233"/>
       <c r="D101" s="59" t="s">
         <v>79</v>
       </c>
@@ -5166,7 +5175,7 @@
       <c r="B102" s="14">
         <v>19</v>
       </c>
-      <c r="C102" s="229"/>
+      <c r="C102" s="233"/>
       <c r="D102" s="59" t="s">
         <v>81</v>
       </c>
@@ -5175,7 +5184,7 @@
       <c r="B103" s="14">
         <v>20</v>
       </c>
-      <c r="C103" s="229"/>
+      <c r="C103" s="233"/>
       <c r="D103" s="60" t="s">
         <v>80</v>
       </c>
@@ -5426,7 +5435,7 @@
       <c r="B138" s="14">
         <v>55</v>
       </c>
-      <c r="C138" s="233" t="s">
+      <c r="C138" s="226" t="s">
         <v>7</v>
       </c>
       <c r="D138" s="54" t="s">
@@ -5437,7 +5446,7 @@
       <c r="B139" s="14">
         <v>56</v>
       </c>
-      <c r="C139" s="234"/>
+      <c r="C139" s="227"/>
       <c r="D139" s="55" t="s">
         <v>79</v>
       </c>
@@ -5446,7 +5455,7 @@
       <c r="B140" s="14">
         <v>57</v>
       </c>
-      <c r="C140" s="234"/>
+      <c r="C140" s="227"/>
       <c r="D140" s="55" t="s">
         <v>81</v>
       </c>
@@ -5455,7 +5464,7 @@
       <c r="B141" s="14">
         <v>58</v>
       </c>
-      <c r="C141" s="235"/>
+      <c r="C141" s="228"/>
       <c r="D141" s="56" t="s">
         <v>80</v>
       </c>
@@ -5464,7 +5473,7 @@
       <c r="B142" s="14">
         <v>59</v>
       </c>
-      <c r="C142" s="223" t="s">
+      <c r="C142" s="237" t="s">
         <v>5</v>
       </c>
       <c r="D142" s="64"/>
@@ -5473,14 +5482,14 @@
       <c r="B143" s="14">
         <v>60</v>
       </c>
-      <c r="C143" s="224"/>
+      <c r="C143" s="238"/>
       <c r="D143" s="65"/>
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B144" s="14">
         <v>61</v>
       </c>
-      <c r="C144" s="225" t="s">
+      <c r="C144" s="239" t="s">
         <v>6</v>
       </c>
       <c r="D144" s="61"/>
@@ -5489,18 +5498,31 @@
       <c r="B145" s="14">
         <v>62</v>
       </c>
-      <c r="C145" s="226"/>
+      <c r="C145" s="240"/>
       <c r="D145" s="62"/>
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B146" s="14">
         <v>63</v>
       </c>
-      <c r="C146" s="227"/>
+      <c r="C146" s="241"/>
       <c r="D146" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="C142:C143"/>
+    <mergeCell ref="C144:C146"/>
+    <mergeCell ref="C56:C59"/>
+    <mergeCell ref="C60:C63"/>
+    <mergeCell ref="C64:C67"/>
+    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="C88:C91"/>
+    <mergeCell ref="C92:C95"/>
+    <mergeCell ref="C96:C99"/>
+    <mergeCell ref="C100:C103"/>
+    <mergeCell ref="C70:C73"/>
+    <mergeCell ref="C76:C78"/>
+    <mergeCell ref="C74:C75"/>
     <mergeCell ref="B12:D12"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B4:C4"/>
@@ -5516,19 +5538,6 @@
     <mergeCell ref="C44:C47"/>
     <mergeCell ref="C48:C51"/>
     <mergeCell ref="C52:C55"/>
-    <mergeCell ref="C142:C143"/>
-    <mergeCell ref="C144:C146"/>
-    <mergeCell ref="C56:C59"/>
-    <mergeCell ref="C60:C63"/>
-    <mergeCell ref="C64:C67"/>
-    <mergeCell ref="C83:C85"/>
-    <mergeCell ref="C88:C91"/>
-    <mergeCell ref="C92:C95"/>
-    <mergeCell ref="C96:C99"/>
-    <mergeCell ref="C100:C103"/>
-    <mergeCell ref="C70:C73"/>
-    <mergeCell ref="C76:C78"/>
-    <mergeCell ref="C74:C75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5548,11 +5557,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C4" s="169" t="s">
+      <c r="C4" s="171" t="s">
         <v>171</v>
       </c>
-      <c r="D4" s="170"/>
-      <c r="E4" s="171"/>
+      <c r="D4" s="172"/>
+      <c r="E4" s="173"/>
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.35">
@@ -5568,10 +5577,10 @@
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C7" s="172" t="s">
+      <c r="C7" s="174" t="s">
         <v>145</v>
       </c>
-      <c r="D7" s="172"/>
+      <c r="D7" s="174"/>
       <c r="E7" s="3"/>
       <c r="F7" s="93"/>
     </row>
@@ -5626,11 +5635,11 @@
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C14" s="173" t="s">
+      <c r="C14" s="175" t="s">
         <v>152</v>
       </c>
-      <c r="D14" s="174"/>
-      <c r="E14" s="175"/>
+      <c r="D14" s="176"/>
+      <c r="E14" s="177"/>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.35">
@@ -5716,11 +5725,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C4" s="169" t="s">
+      <c r="C4" s="171" t="s">
         <v>184</v>
       </c>
-      <c r="D4" s="170"/>
-      <c r="E4" s="171"/>
+      <c r="D4" s="172"/>
+      <c r="E4" s="173"/>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C5" s="3"/>
@@ -5740,18 +5749,18 @@
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C8" s="176" t="s">
+      <c r="C8" s="178" t="s">
         <v>122</v>
       </c>
-      <c r="D8" s="176"/>
+      <c r="D8" s="178"/>
       <c r="E8" s="3"/>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C9" s="173" t="s">
+      <c r="C9" s="175" t="s">
         <v>152</v>
       </c>
-      <c r="D9" s="174"/>
-      <c r="E9" s="175"/>
+      <c r="D9" s="176"/>
+      <c r="E9" s="177"/>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.35">
       <c r="C10" s="3"/>
@@ -5864,350 +5873,350 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B2" s="187" t="s">
+      <c r="B2" s="179" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="188"/>
-      <c r="D2" s="188"/>
-      <c r="E2" s="188"/>
-      <c r="F2" s="189"/>
+      <c r="C2" s="180"/>
+      <c r="D2" s="180"/>
+      <c r="E2" s="180"/>
+      <c r="F2" s="181"/>
     </row>
     <row r="4" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B4" s="178" t="s">
+      <c r="B4" s="182" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="178"/>
-      <c r="D4" s="177" t="s">
+      <c r="C4" s="182"/>
+      <c r="D4" s="189" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="177"/>
-      <c r="F4" s="177"/>
-      <c r="G4" s="177"/>
-      <c r="H4" s="177"/>
-      <c r="I4" s="177"/>
-      <c r="J4" s="177"/>
-      <c r="K4" s="177"/>
-      <c r="L4" s="177"/>
-      <c r="M4" s="177"/>
-      <c r="N4" s="177"/>
-      <c r="O4" s="177"/>
-      <c r="P4" s="177"/>
-      <c r="Q4" s="177"/>
-      <c r="R4" s="177"/>
-      <c r="S4" s="177"/>
-      <c r="T4" s="177"/>
-      <c r="U4" s="177"/>
-      <c r="V4" s="177"/>
-      <c r="W4" s="177"/>
-      <c r="X4" s="177"/>
+      <c r="E4" s="189"/>
+      <c r="F4" s="189"/>
+      <c r="G4" s="189"/>
+      <c r="H4" s="189"/>
+      <c r="I4" s="189"/>
+      <c r="J4" s="189"/>
+      <c r="K4" s="189"/>
+      <c r="L4" s="189"/>
+      <c r="M4" s="189"/>
+      <c r="N4" s="189"/>
+      <c r="O4" s="189"/>
+      <c r="P4" s="189"/>
+      <c r="Q4" s="189"/>
+      <c r="R4" s="189"/>
+      <c r="S4" s="189"/>
+      <c r="T4" s="189"/>
+      <c r="U4" s="189"/>
+      <c r="V4" s="189"/>
+      <c r="W4" s="189"/>
+      <c r="X4" s="189"/>
     </row>
     <row r="5" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B5" s="179"/>
-      <c r="C5" s="179"/>
-      <c r="D5" s="177"/>
-      <c r="E5" s="177"/>
-      <c r="F5" s="177"/>
-      <c r="G5" s="177"/>
-      <c r="H5" s="177"/>
-      <c r="I5" s="177"/>
-      <c r="J5" s="177"/>
-      <c r="K5" s="177"/>
-      <c r="L5" s="177"/>
-      <c r="M5" s="177"/>
-      <c r="N5" s="177"/>
-      <c r="O5" s="177"/>
-      <c r="P5" s="177"/>
-      <c r="Q5" s="177"/>
-      <c r="R5" s="177"/>
-      <c r="S5" s="177"/>
-      <c r="T5" s="177"/>
-      <c r="U5" s="177"/>
-      <c r="V5" s="177"/>
-      <c r="W5" s="177"/>
-      <c r="X5" s="177"/>
+      <c r="B5" s="188"/>
+      <c r="C5" s="188"/>
+      <c r="D5" s="189"/>
+      <c r="E5" s="189"/>
+      <c r="F5" s="189"/>
+      <c r="G5" s="189"/>
+      <c r="H5" s="189"/>
+      <c r="I5" s="189"/>
+      <c r="J5" s="189"/>
+      <c r="K5" s="189"/>
+      <c r="L5" s="189"/>
+      <c r="M5" s="189"/>
+      <c r="N5" s="189"/>
+      <c r="O5" s="189"/>
+      <c r="P5" s="189"/>
+      <c r="Q5" s="189"/>
+      <c r="R5" s="189"/>
+      <c r="S5" s="189"/>
+      <c r="T5" s="189"/>
+      <c r="U5" s="189"/>
+      <c r="V5" s="189"/>
+      <c r="W5" s="189"/>
+      <c r="X5" s="189"/>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B6" s="180" t="s">
+      <c r="B6" s="191" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="180"/>
-      <c r="D6" s="177" t="s">
+      <c r="C6" s="191"/>
+      <c r="D6" s="189" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="177"/>
-      <c r="F6" s="177"/>
-      <c r="G6" s="177"/>
-      <c r="H6" s="177"/>
-      <c r="I6" s="177"/>
-      <c r="J6" s="177"/>
-      <c r="K6" s="177"/>
-      <c r="L6" s="177"/>
-      <c r="M6" s="177"/>
-      <c r="N6" s="177"/>
-      <c r="O6" s="177"/>
-      <c r="P6" s="177"/>
-      <c r="Q6" s="177"/>
-      <c r="R6" s="177"/>
-      <c r="S6" s="177"/>
-      <c r="T6" s="177"/>
-      <c r="U6" s="177"/>
-      <c r="V6" s="177"/>
-      <c r="W6" s="177"/>
-      <c r="X6" s="177"/>
+      <c r="E6" s="189"/>
+      <c r="F6" s="189"/>
+      <c r="G6" s="189"/>
+      <c r="H6" s="189"/>
+      <c r="I6" s="189"/>
+      <c r="J6" s="189"/>
+      <c r="K6" s="189"/>
+      <c r="L6" s="189"/>
+      <c r="M6" s="189"/>
+      <c r="N6" s="189"/>
+      <c r="O6" s="189"/>
+      <c r="P6" s="189"/>
+      <c r="Q6" s="189"/>
+      <c r="R6" s="189"/>
+      <c r="S6" s="189"/>
+      <c r="T6" s="189"/>
+      <c r="U6" s="189"/>
+      <c r="V6" s="189"/>
+      <c r="W6" s="189"/>
+      <c r="X6" s="189"/>
     </row>
     <row r="7" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B7" s="181" t="s">
+      <c r="B7" s="192" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="181"/>
-      <c r="D7" s="177" t="s">
+      <c r="C7" s="192"/>
+      <c r="D7" s="189" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="177"/>
-      <c r="F7" s="177"/>
-      <c r="G7" s="177"/>
-      <c r="H7" s="177"/>
-      <c r="I7" s="177"/>
-      <c r="J7" s="177"/>
-      <c r="K7" s="177"/>
-      <c r="L7" s="177"/>
-      <c r="M7" s="177"/>
-      <c r="N7" s="177"/>
-      <c r="O7" s="177"/>
-      <c r="P7" s="177"/>
-      <c r="Q7" s="177"/>
-      <c r="R7" s="177"/>
-      <c r="S7" s="177"/>
-      <c r="T7" s="177"/>
-      <c r="U7" s="177"/>
-      <c r="V7" s="177"/>
-      <c r="W7" s="177"/>
-      <c r="X7" s="177"/>
+      <c r="E7" s="189"/>
+      <c r="F7" s="189"/>
+      <c r="G7" s="189"/>
+      <c r="H7" s="189"/>
+      <c r="I7" s="189"/>
+      <c r="J7" s="189"/>
+      <c r="K7" s="189"/>
+      <c r="L7" s="189"/>
+      <c r="M7" s="189"/>
+      <c r="N7" s="189"/>
+      <c r="O7" s="189"/>
+      <c r="P7" s="189"/>
+      <c r="Q7" s="189"/>
+      <c r="R7" s="189"/>
+      <c r="S7" s="189"/>
+      <c r="T7" s="189"/>
+      <c r="U7" s="189"/>
+      <c r="V7" s="189"/>
+      <c r="W7" s="189"/>
+      <c r="X7" s="189"/>
     </row>
     <row r="8" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B8" s="169"/>
-      <c r="C8" s="171"/>
-      <c r="D8" s="182"/>
-      <c r="E8" s="183"/>
-      <c r="F8" s="183"/>
-      <c r="G8" s="183"/>
-      <c r="H8" s="183"/>
-      <c r="I8" s="183"/>
-      <c r="J8" s="183"/>
-      <c r="K8" s="183"/>
-      <c r="L8" s="183"/>
-      <c r="M8" s="183"/>
-      <c r="N8" s="183"/>
-      <c r="O8" s="183"/>
-      <c r="P8" s="183"/>
-      <c r="Q8" s="183"/>
-      <c r="R8" s="183"/>
-      <c r="S8" s="183"/>
-      <c r="T8" s="183"/>
-      <c r="U8" s="183"/>
-      <c r="V8" s="183"/>
-      <c r="W8" s="183"/>
-      <c r="X8" s="184"/>
+      <c r="B8" s="171"/>
+      <c r="C8" s="173"/>
+      <c r="D8" s="185"/>
+      <c r="E8" s="186"/>
+      <c r="F8" s="186"/>
+      <c r="G8" s="186"/>
+      <c r="H8" s="186"/>
+      <c r="I8" s="186"/>
+      <c r="J8" s="186"/>
+      <c r="K8" s="186"/>
+      <c r="L8" s="186"/>
+      <c r="M8" s="186"/>
+      <c r="N8" s="186"/>
+      <c r="O8" s="186"/>
+      <c r="P8" s="186"/>
+      <c r="Q8" s="186"/>
+      <c r="R8" s="186"/>
+      <c r="S8" s="186"/>
+      <c r="T8" s="186"/>
+      <c r="U8" s="186"/>
+      <c r="V8" s="186"/>
+      <c r="W8" s="186"/>
+      <c r="X8" s="187"/>
     </row>
     <row r="9" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B9" s="185" t="s">
+      <c r="B9" s="193" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="186"/>
-      <c r="D9" s="182"/>
-      <c r="E9" s="183"/>
-      <c r="F9" s="183"/>
-      <c r="G9" s="183"/>
-      <c r="H9" s="183"/>
-      <c r="I9" s="183"/>
-      <c r="J9" s="183"/>
-      <c r="K9" s="183"/>
-      <c r="L9" s="183"/>
-      <c r="M9" s="183"/>
-      <c r="N9" s="183"/>
-      <c r="O9" s="183"/>
-      <c r="P9" s="183"/>
-      <c r="Q9" s="183"/>
-      <c r="R9" s="183"/>
-      <c r="S9" s="183"/>
-      <c r="T9" s="183"/>
-      <c r="U9" s="183"/>
-      <c r="V9" s="183"/>
-      <c r="W9" s="183"/>
-      <c r="X9" s="184"/>
+      <c r="C9" s="194"/>
+      <c r="D9" s="185"/>
+      <c r="E9" s="186"/>
+      <c r="F9" s="186"/>
+      <c r="G9" s="186"/>
+      <c r="H9" s="186"/>
+      <c r="I9" s="186"/>
+      <c r="J9" s="186"/>
+      <c r="K9" s="186"/>
+      <c r="L9" s="186"/>
+      <c r="M9" s="186"/>
+      <c r="N9" s="186"/>
+      <c r="O9" s="186"/>
+      <c r="P9" s="186"/>
+      <c r="Q9" s="186"/>
+      <c r="R9" s="186"/>
+      <c r="S9" s="186"/>
+      <c r="T9" s="186"/>
+      <c r="U9" s="186"/>
+      <c r="V9" s="186"/>
+      <c r="W9" s="186"/>
+      <c r="X9" s="187"/>
     </row>
     <row r="10" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B10" s="169"/>
-      <c r="C10" s="171"/>
-      <c r="D10" s="182"/>
-      <c r="E10" s="183"/>
-      <c r="F10" s="183"/>
-      <c r="G10" s="183"/>
-      <c r="H10" s="183"/>
-      <c r="I10" s="183"/>
-      <c r="J10" s="183"/>
-      <c r="K10" s="183"/>
-      <c r="L10" s="183"/>
-      <c r="M10" s="183"/>
-      <c r="N10" s="183"/>
-      <c r="O10" s="183"/>
-      <c r="P10" s="183"/>
-      <c r="Q10" s="183"/>
-      <c r="R10" s="183"/>
-      <c r="S10" s="183"/>
-      <c r="T10" s="183"/>
-      <c r="U10" s="183"/>
-      <c r="V10" s="183"/>
-      <c r="W10" s="183"/>
-      <c r="X10" s="184"/>
+      <c r="B10" s="171"/>
+      <c r="C10" s="173"/>
+      <c r="D10" s="185"/>
+      <c r="E10" s="186"/>
+      <c r="F10" s="186"/>
+      <c r="G10" s="186"/>
+      <c r="H10" s="186"/>
+      <c r="I10" s="186"/>
+      <c r="J10" s="186"/>
+      <c r="K10" s="186"/>
+      <c r="L10" s="186"/>
+      <c r="M10" s="186"/>
+      <c r="N10" s="186"/>
+      <c r="O10" s="186"/>
+      <c r="P10" s="186"/>
+      <c r="Q10" s="186"/>
+      <c r="R10" s="186"/>
+      <c r="S10" s="186"/>
+      <c r="T10" s="186"/>
+      <c r="U10" s="186"/>
+      <c r="V10" s="186"/>
+      <c r="W10" s="186"/>
+      <c r="X10" s="187"/>
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B11" s="192" t="s">
+      <c r="B11" s="190" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="192"/>
-      <c r="D11" s="177" t="s">
+      <c r="C11" s="190"/>
+      <c r="D11" s="189" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="177"/>
-      <c r="F11" s="177"/>
-      <c r="G11" s="177"/>
-      <c r="H11" s="177"/>
-      <c r="I11" s="177"/>
-      <c r="J11" s="177"/>
-      <c r="K11" s="177"/>
-      <c r="L11" s="177"/>
-      <c r="M11" s="177"/>
-      <c r="N11" s="177"/>
-      <c r="O11" s="177"/>
-      <c r="P11" s="177"/>
-      <c r="Q11" s="177"/>
-      <c r="R11" s="177"/>
-      <c r="S11" s="177"/>
-      <c r="T11" s="177"/>
-      <c r="U11" s="177"/>
-      <c r="V11" s="177"/>
-      <c r="W11" s="177"/>
-      <c r="X11" s="177"/>
+      <c r="E11" s="189"/>
+      <c r="F11" s="189"/>
+      <c r="G11" s="189"/>
+      <c r="H11" s="189"/>
+      <c r="I11" s="189"/>
+      <c r="J11" s="189"/>
+      <c r="K11" s="189"/>
+      <c r="L11" s="189"/>
+      <c r="M11" s="189"/>
+      <c r="N11" s="189"/>
+      <c r="O11" s="189"/>
+      <c r="P11" s="189"/>
+      <c r="Q11" s="189"/>
+      <c r="R11" s="189"/>
+      <c r="S11" s="189"/>
+      <c r="T11" s="189"/>
+      <c r="U11" s="189"/>
+      <c r="V11" s="189"/>
+      <c r="W11" s="189"/>
+      <c r="X11" s="189"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B12" s="191" t="s">
+      <c r="B12" s="184" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="191"/>
-      <c r="D12" s="177" t="s">
+      <c r="C12" s="184"/>
+      <c r="D12" s="189" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="177"/>
-      <c r="F12" s="177"/>
-      <c r="G12" s="177"/>
-      <c r="H12" s="177"/>
-      <c r="I12" s="177"/>
-      <c r="J12" s="177"/>
-      <c r="K12" s="177"/>
-      <c r="L12" s="177"/>
-      <c r="M12" s="177"/>
-      <c r="N12" s="177"/>
-      <c r="O12" s="177"/>
-      <c r="P12" s="177"/>
-      <c r="Q12" s="177"/>
-      <c r="R12" s="177"/>
-      <c r="S12" s="177"/>
-      <c r="T12" s="177"/>
-      <c r="U12" s="177"/>
-      <c r="V12" s="177"/>
-      <c r="W12" s="177"/>
-      <c r="X12" s="177"/>
+      <c r="E12" s="189"/>
+      <c r="F12" s="189"/>
+      <c r="G12" s="189"/>
+      <c r="H12" s="189"/>
+      <c r="I12" s="189"/>
+      <c r="J12" s="189"/>
+      <c r="K12" s="189"/>
+      <c r="L12" s="189"/>
+      <c r="M12" s="189"/>
+      <c r="N12" s="189"/>
+      <c r="O12" s="189"/>
+      <c r="P12" s="189"/>
+      <c r="Q12" s="189"/>
+      <c r="R12" s="189"/>
+      <c r="S12" s="189"/>
+      <c r="T12" s="189"/>
+      <c r="U12" s="189"/>
+      <c r="V12" s="189"/>
+      <c r="W12" s="189"/>
+      <c r="X12" s="189"/>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B13" s="190" t="s">
+      <c r="B13" s="183" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="190"/>
-      <c r="D13" s="177" t="s">
+      <c r="C13" s="183"/>
+      <c r="D13" s="189" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="177"/>
-      <c r="F13" s="177"/>
-      <c r="G13" s="177"/>
-      <c r="H13" s="177"/>
-      <c r="I13" s="177"/>
-      <c r="J13" s="177"/>
-      <c r="K13" s="177"/>
-      <c r="L13" s="177"/>
-      <c r="M13" s="177"/>
-      <c r="N13" s="177"/>
-      <c r="O13" s="177"/>
-      <c r="P13" s="177"/>
-      <c r="Q13" s="177"/>
-      <c r="R13" s="177"/>
-      <c r="S13" s="177"/>
-      <c r="T13" s="177"/>
-      <c r="U13" s="177"/>
-      <c r="V13" s="177"/>
-      <c r="W13" s="177"/>
-      <c r="X13" s="177"/>
+      <c r="E13" s="189"/>
+      <c r="F13" s="189"/>
+      <c r="G13" s="189"/>
+      <c r="H13" s="189"/>
+      <c r="I13" s="189"/>
+      <c r="J13" s="189"/>
+      <c r="K13" s="189"/>
+      <c r="L13" s="189"/>
+      <c r="M13" s="189"/>
+      <c r="N13" s="189"/>
+      <c r="O13" s="189"/>
+      <c r="P13" s="189"/>
+      <c r="Q13" s="189"/>
+      <c r="R13" s="189"/>
+      <c r="S13" s="189"/>
+      <c r="T13" s="189"/>
+      <c r="U13" s="189"/>
+      <c r="V13" s="189"/>
+      <c r="W13" s="189"/>
+      <c r="X13" s="189"/>
     </row>
     <row r="14" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B14" s="179"/>
-      <c r="C14" s="179"/>
-      <c r="D14" s="177"/>
-      <c r="E14" s="177"/>
-      <c r="F14" s="177"/>
-      <c r="G14" s="177"/>
-      <c r="H14" s="177"/>
-      <c r="I14" s="177"/>
-      <c r="J14" s="177"/>
-      <c r="K14" s="177"/>
-      <c r="L14" s="177"/>
-      <c r="M14" s="177"/>
-      <c r="N14" s="177"/>
-      <c r="O14" s="177"/>
-      <c r="P14" s="177"/>
-      <c r="Q14" s="177"/>
-      <c r="R14" s="177"/>
-      <c r="S14" s="177"/>
-      <c r="T14" s="177"/>
-      <c r="U14" s="177"/>
-      <c r="V14" s="177"/>
-      <c r="W14" s="177"/>
-      <c r="X14" s="177"/>
+      <c r="B14" s="188"/>
+      <c r="C14" s="188"/>
+      <c r="D14" s="189"/>
+      <c r="E14" s="189"/>
+      <c r="F14" s="189"/>
+      <c r="G14" s="189"/>
+      <c r="H14" s="189"/>
+      <c r="I14" s="189"/>
+      <c r="J14" s="189"/>
+      <c r="K14" s="189"/>
+      <c r="L14" s="189"/>
+      <c r="M14" s="189"/>
+      <c r="N14" s="189"/>
+      <c r="O14" s="189"/>
+      <c r="P14" s="189"/>
+      <c r="Q14" s="189"/>
+      <c r="R14" s="189"/>
+      <c r="S14" s="189"/>
+      <c r="T14" s="189"/>
+      <c r="U14" s="189"/>
+      <c r="V14" s="189"/>
+      <c r="W14" s="189"/>
+      <c r="X14" s="189"/>
     </row>
     <row r="15" spans="2:24" x14ac:dyDescent="0.3">
-      <c r="B15" s="178" t="s">
+      <c r="B15" s="182" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="178"/>
-      <c r="D15" s="177" t="s">
+      <c r="C15" s="182"/>
+      <c r="D15" s="189" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="177"/>
-      <c r="F15" s="177"/>
-      <c r="G15" s="177"/>
-      <c r="H15" s="177"/>
-      <c r="I15" s="177"/>
-      <c r="J15" s="177"/>
-      <c r="K15" s="177"/>
-      <c r="L15" s="177"/>
-      <c r="M15" s="177"/>
-      <c r="N15" s="177"/>
-      <c r="O15" s="177"/>
-      <c r="P15" s="177"/>
-      <c r="Q15" s="177"/>
-      <c r="R15" s="177"/>
-      <c r="S15" s="177"/>
-      <c r="T15" s="177"/>
-      <c r="U15" s="177"/>
-      <c r="V15" s="177"/>
-      <c r="W15" s="177"/>
-      <c r="X15" s="177"/>
+      <c r="E15" s="189"/>
+      <c r="F15" s="189"/>
+      <c r="G15" s="189"/>
+      <c r="H15" s="189"/>
+      <c r="I15" s="189"/>
+      <c r="J15" s="189"/>
+      <c r="K15" s="189"/>
+      <c r="L15" s="189"/>
+      <c r="M15" s="189"/>
+      <c r="N15" s="189"/>
+      <c r="O15" s="189"/>
+      <c r="P15" s="189"/>
+      <c r="Q15" s="189"/>
+      <c r="R15" s="189"/>
+      <c r="S15" s="189"/>
+      <c r="T15" s="189"/>
+      <c r="U15" s="189"/>
+      <c r="V15" s="189"/>
+      <c r="W15" s="189"/>
+      <c r="X15" s="189"/>
     </row>
     <row r="17" spans="3:67" x14ac:dyDescent="0.3">
-      <c r="D17" s="178" t="s">
+      <c r="D17" s="182" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="178"/>
-      <c r="F17" s="178"/>
+      <c r="E17" s="182"/>
+      <c r="F17" s="182"/>
       <c r="G17" s="84" t="s">
         <v>0</v>
       </c>
@@ -6266,21 +6275,21 @@
       <c r="BF17" s="83" t="s">
         <v>9</v>
       </c>
-      <c r="BG17" s="191" t="s">
+      <c r="BG17" s="184" t="s">
         <v>7</v>
       </c>
-      <c r="BH17" s="191"/>
-      <c r="BI17" s="191"/>
-      <c r="BJ17" s="191"/>
-      <c r="BK17" s="190" t="s">
+      <c r="BH17" s="184"/>
+      <c r="BI17" s="184"/>
+      <c r="BJ17" s="184"/>
+      <c r="BK17" s="183" t="s">
         <v>5</v>
       </c>
-      <c r="BL17" s="190"/>
-      <c r="BM17" s="178" t="s">
+      <c r="BL17" s="183"/>
+      <c r="BM17" s="182" t="s">
         <v>6</v>
       </c>
-      <c r="BN17" s="178"/>
-      <c r="BO17" s="178"/>
+      <c r="BN17" s="182"/>
+      <c r="BO17" s="182"/>
     </row>
     <row r="18" spans="3:67" x14ac:dyDescent="0.3">
       <c r="C18" s="95" t="s">
@@ -6480,57 +6489,57 @@
       </c>
     </row>
     <row r="20" spans="3:67" x14ac:dyDescent="0.3">
-      <c r="I20" s="169" t="s">
+      <c r="I20" s="171" t="s">
         <v>168</v>
       </c>
-      <c r="J20" s="170"/>
-      <c r="K20" s="170"/>
-      <c r="L20" s="170"/>
-      <c r="M20" s="170"/>
-      <c r="N20" s="170"/>
-      <c r="O20" s="170"/>
-      <c r="P20" s="170"/>
-      <c r="Q20" s="170"/>
-      <c r="R20" s="170"/>
-      <c r="S20" s="170"/>
-      <c r="T20" s="170"/>
-      <c r="U20" s="170"/>
-      <c r="V20" s="170"/>
-      <c r="W20" s="170"/>
-      <c r="X20" s="170"/>
-      <c r="Y20" s="170"/>
-      <c r="Z20" s="170"/>
-      <c r="AA20" s="170"/>
-      <c r="AB20" s="170"/>
-      <c r="AC20" s="170"/>
-      <c r="AD20" s="170"/>
-      <c r="AE20" s="170"/>
-      <c r="AF20" s="170"/>
-      <c r="AG20" s="170"/>
-      <c r="AH20" s="170"/>
-      <c r="AI20" s="170"/>
-      <c r="AJ20" s="170"/>
-      <c r="AK20" s="170"/>
-      <c r="AL20" s="170"/>
-      <c r="AM20" s="170"/>
-      <c r="AN20" s="170"/>
-      <c r="AO20" s="170"/>
-      <c r="AP20" s="170"/>
-      <c r="AQ20" s="170"/>
-      <c r="AR20" s="170"/>
-      <c r="AS20" s="170"/>
-      <c r="AT20" s="170"/>
-      <c r="AU20" s="170"/>
-      <c r="AV20" s="170"/>
-      <c r="AW20" s="170"/>
-      <c r="AX20" s="170"/>
-      <c r="AY20" s="170"/>
-      <c r="AZ20" s="170"/>
-      <c r="BA20" s="170"/>
-      <c r="BB20" s="170"/>
-      <c r="BC20" s="170"/>
-      <c r="BD20" s="170"/>
-      <c r="BE20" s="171"/>
+      <c r="J20" s="172"/>
+      <c r="K20" s="172"/>
+      <c r="L20" s="172"/>
+      <c r="M20" s="172"/>
+      <c r="N20" s="172"/>
+      <c r="O20" s="172"/>
+      <c r="P20" s="172"/>
+      <c r="Q20" s="172"/>
+      <c r="R20" s="172"/>
+      <c r="S20" s="172"/>
+      <c r="T20" s="172"/>
+      <c r="U20" s="172"/>
+      <c r="V20" s="172"/>
+      <c r="W20" s="172"/>
+      <c r="X20" s="172"/>
+      <c r="Y20" s="172"/>
+      <c r="Z20" s="172"/>
+      <c r="AA20" s="172"/>
+      <c r="AB20" s="172"/>
+      <c r="AC20" s="172"/>
+      <c r="AD20" s="172"/>
+      <c r="AE20" s="172"/>
+      <c r="AF20" s="172"/>
+      <c r="AG20" s="172"/>
+      <c r="AH20" s="172"/>
+      <c r="AI20" s="172"/>
+      <c r="AJ20" s="172"/>
+      <c r="AK20" s="172"/>
+      <c r="AL20" s="172"/>
+      <c r="AM20" s="172"/>
+      <c r="AN20" s="172"/>
+      <c r="AO20" s="172"/>
+      <c r="AP20" s="172"/>
+      <c r="AQ20" s="172"/>
+      <c r="AR20" s="172"/>
+      <c r="AS20" s="172"/>
+      <c r="AT20" s="172"/>
+      <c r="AU20" s="172"/>
+      <c r="AV20" s="172"/>
+      <c r="AW20" s="172"/>
+      <c r="AX20" s="172"/>
+      <c r="AY20" s="172"/>
+      <c r="AZ20" s="172"/>
+      <c r="BA20" s="172"/>
+      <c r="BB20" s="172"/>
+      <c r="BC20" s="172"/>
+      <c r="BD20" s="172"/>
+      <c r="BE20" s="173"/>
     </row>
     <row r="21" spans="3:67" x14ac:dyDescent="0.3">
       <c r="I21" s="126">
@@ -6683,6 +6692,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="I20:BE20"/>
+    <mergeCell ref="D13:X13"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:X4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:X5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:X6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:X7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="D8:X8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="D9:X9"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="D17:F17"/>
     <mergeCell ref="BK17:BL17"/>
@@ -6699,20 +6722,6 @@
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="D12:X12"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="I20:BE20"/>
-    <mergeCell ref="D13:X13"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:X4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:X5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:X6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:X7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="D8:X8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="D9:X9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6739,17 +6748,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="169" t="s">
+      <c r="B2" s="171" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="171"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="173"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="172" t="s">
+      <c r="B5" s="174" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="172"/>
+      <c r="C5" s="174"/>
       <c r="E5" s="93"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
@@ -6828,10 +6837,10 @@
       <c r="H10" s="76"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="172" t="s">
+      <c r="B12" s="174" t="s">
         <v>145</v>
       </c>
-      <c r="C12" s="172"/>
+      <c r="C12" s="174"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="14">
@@ -6890,11 +6899,11 @@
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="173" t="s">
+      <c r="B21" s="175" t="s">
         <v>152</v>
       </c>
-      <c r="C21" s="174"/>
-      <c r="D21" s="175"/>
+      <c r="C21" s="176"/>
+      <c r="D21" s="177"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -6924,11 +6933,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2" s="193" t="s">
+      <c r="B2" s="195" t="s">
         <v>122</v>
       </c>
-      <c r="C2" s="193"/>
-      <c r="D2" s="193"/>
+      <c r="C2" s="195"/>
+      <c r="D2" s="195"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B4" s="14">
@@ -7013,111 +7022,111 @@
       <c r="B5" s="25">
         <v>5</v>
       </c>
-      <c r="C5" s="194" t="s">
+      <c r="C5" s="196" t="s">
         <v>119</v>
       </c>
       <c r="D5" s="97" t="s">
         <v>78</v>
       </c>
-      <c r="F5" s="206" t="s">
+      <c r="F5" s="208" t="s">
         <v>151</v>
       </c>
-      <c r="G5" s="207"/>
-      <c r="H5" s="208"/>
+      <c r="G5" s="209"/>
+      <c r="H5" s="210"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="25">
         <v>6</v>
       </c>
-      <c r="C6" s="195"/>
+      <c r="C6" s="197"/>
       <c r="D6" s="98" t="s">
         <v>79</v>
       </c>
-      <c r="F6" s="209" t="s">
+      <c r="F6" s="211" t="s">
         <v>154</v>
       </c>
-      <c r="G6" s="210"/>
-      <c r="H6" s="211"/>
+      <c r="G6" s="212"/>
+      <c r="H6" s="213"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="25">
         <v>7</v>
       </c>
-      <c r="C7" s="195"/>
+      <c r="C7" s="197"/>
       <c r="D7" s="98" t="s">
         <v>81</v>
       </c>
-      <c r="F7" s="209" t="s">
+      <c r="F7" s="211" t="s">
         <v>155</v>
       </c>
-      <c r="G7" s="210"/>
-      <c r="H7" s="211"/>
+      <c r="G7" s="212"/>
+      <c r="H7" s="213"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="25">
         <v>8</v>
       </c>
-      <c r="C8" s="196"/>
+      <c r="C8" s="198"/>
       <c r="D8" s="99" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="212" t="s">
+      <c r="F8" s="214" t="s">
         <v>156</v>
       </c>
-      <c r="G8" s="213"/>
-      <c r="H8" s="214"/>
+      <c r="G8" s="215"/>
+      <c r="H8" s="216"/>
     </row>
     <row r="9" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="25">
         <v>9</v>
       </c>
-      <c r="C9" s="203" t="s">
+      <c r="C9" s="205" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="100" t="s">
         <v>78</v>
       </c>
-      <c r="F9" s="197" t="s">
+      <c r="F9" s="199" t="s">
         <v>153</v>
       </c>
-      <c r="G9" s="198"/>
-      <c r="H9" s="199"/>
+      <c r="G9" s="200"/>
+      <c r="H9" s="201"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="25">
         <v>10</v>
       </c>
-      <c r="C10" s="204"/>
+      <c r="C10" s="206"/>
       <c r="D10" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="F10" s="197"/>
-      <c r="G10" s="198"/>
-      <c r="H10" s="199"/>
+      <c r="F10" s="199"/>
+      <c r="G10" s="200"/>
+      <c r="H10" s="201"/>
     </row>
     <row r="11" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="25">
         <v>11</v>
       </c>
-      <c r="C11" s="204"/>
+      <c r="C11" s="206"/>
       <c r="D11" s="101" t="s">
         <v>81</v>
       </c>
-      <c r="F11" s="197"/>
-      <c r="G11" s="198"/>
-      <c r="H11" s="199"/>
+      <c r="F11" s="199"/>
+      <c r="G11" s="200"/>
+      <c r="H11" s="201"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="25">
         <v>12</v>
       </c>
-      <c r="C12" s="205"/>
+      <c r="C12" s="207"/>
       <c r="D12" s="102" t="s">
         <v>80</v>
       </c>
-      <c r="F12" s="197"/>
-      <c r="G12" s="198"/>
-      <c r="H12" s="199"/>
+      <c r="F12" s="199"/>
+      <c r="G12" s="200"/>
+      <c r="H12" s="201"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="25">
@@ -7127,9 +7136,9 @@
         <v>0</v>
       </c>
       <c r="D13" s="104"/>
-      <c r="F13" s="197"/>
-      <c r="G13" s="198"/>
-      <c r="H13" s="199"/>
+      <c r="F13" s="199"/>
+      <c r="G13" s="200"/>
+      <c r="H13" s="201"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="25">
@@ -7139,9 +7148,9 @@
         <v>20</v>
       </c>
       <c r="D14" s="106"/>
-      <c r="F14" s="200"/>
-      <c r="G14" s="201"/>
-      <c r="H14" s="202"/>
+      <c r="F14" s="202"/>
+      <c r="G14" s="203"/>
+      <c r="H14" s="204"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -7177,10 +7186,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="169" t="s">
+      <c r="B3" s="171" t="s">
         <v>173</v>
       </c>
-      <c r="C3" s="171"/>
+      <c r="C3" s="173"/>
       <c r="D3" s="94"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
@@ -7413,17 +7422,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B2" s="169" t="s">
+      <c r="B2" s="171" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="170"/>
-      <c r="D2" s="171"/>
+      <c r="C2" s="172"/>
+      <c r="D2" s="173"/>
     </row>
     <row r="5" spans="2:9" ht="14.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="172" t="s">
+      <c r="B5" s="174" t="s">
         <v>145</v>
       </c>
-      <c r="C5" s="172"/>
+      <c r="C5" s="174"/>
       <c r="E5" s="93"/>
       <c r="F5" s="93"/>
     </row>
@@ -7437,10 +7446,10 @@
       <c r="D6" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="215" t="s">
+      <c r="F6" s="217" t="s">
         <v>123</v>
       </c>
-      <c r="G6" s="215"/>
+      <c r="G6" s="217"/>
       <c r="H6" s="4"/>
       <c r="I6" s="72"/>
     </row>
@@ -7525,10 +7534,10 @@
       <c r="G12" s="42"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="176" t="s">
+      <c r="B13" s="178" t="s">
         <v>122</v>
       </c>
-      <c r="C13" s="176"/>
+      <c r="C13" s="178"/>
       <c r="F13" s="12" t="s">
         <v>182</v>
       </c>
@@ -7538,11 +7547,11 @@
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="173" t="s">
+      <c r="B14" s="175" t="s">
         <v>152</v>
       </c>
-      <c r="C14" s="174"/>
-      <c r="D14" s="175"/>
+      <c r="C14" s="176"/>
+      <c r="D14" s="177"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="14">

</xml_diff>